<commit_message>
date_cataloged mappings for DUKE, NCSU
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.unc.edu\lib\common\LMS\TRLN Discovery\data-documentation\map_to_argot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\data-documentation\argot\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="5910" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="5910" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
-    <sheet name="issues_fields" sheetId="4" r:id="rId2"/>
+    <sheet name="fields_issues" sheetId="4" r:id="rId2"/>
     <sheet name="mappings" sheetId="2" r:id="rId3"/>
-    <sheet name="issues_maps" sheetId="3" r:id="rId4"/>
+    <sheet name="mappings_issues" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="205">
   <si>
     <t>subject_chronological_facet</t>
   </si>
@@ -359,9 +359,6 @@
     <t>Transform to standard date format; map to desired date ranges (last week, last month, etc)</t>
   </si>
   <si>
-    <t>Need institutional mappings for Duke, NCSU, NCCU</t>
-  </si>
-  <si>
     <t>languages</t>
   </si>
   <si>
@@ -627,6 +624,24 @@
   </si>
   <si>
     <t>calculated</t>
+  </si>
+  <si>
+    <t>DUKE</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>NCSU</t>
+  </si>
+  <si>
+    <t>NCCU</t>
+  </si>
+  <si>
+    <t>date_catalogedNCCU...</t>
+  </si>
+  <si>
+    <t>Need to find out where this is in their data.</t>
   </si>
 </sst>
 </file>
@@ -901,8 +916,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="issuesfield" displayName="issuesfield" ref="A1:C10" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:C10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="issuesfield" displayName="issuesfield" ref="A1:C9" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:C9"/>
   <tableColumns count="3">
     <tableColumn id="1" name="field" dataDxfId="8"/>
     <tableColumn id="3" name="desc" dataDxfId="7"/>
@@ -913,10 +928,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="mappings" displayName="mappings" ref="A1:M66" totalsRowShown="0">
-  <autoFilter ref="A1:M66"/>
-  <sortState ref="A2:K60">
-    <sortCondition ref="D1:D60"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="mappings" displayName="mappings" ref="A1:M69" totalsRowShown="0">
+  <autoFilter ref="A1:M69"/>
+  <sortState ref="A2:M69">
+    <sortCondition ref="A2:A69"/>
+    <sortCondition ref="C2:C69"/>
+    <sortCondition ref="D2:D69"/>
+    <sortCondition ref="B2:B69"/>
+    <sortCondition ref="E2:E69"/>
   </sortState>
   <tableColumns count="13">
     <tableColumn id="1" name="field"/>
@@ -944,8 +963,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="issuesmap" displayName="issuesmap" ref="A1:D7" totalsRowShown="0">
-  <autoFilter ref="A1:D7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="issuesmap" displayName="issuesmap" ref="A1:D8" totalsRowShown="0">
+  <autoFilter ref="A1:D8"/>
   <tableColumns count="4">
     <tableColumn id="1" name="mappingID"/>
     <tableColumn id="2" name="element"/>
@@ -1222,7 +1241,7 @@
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,10 +1307,10 @@
         <v>80</v>
       </c>
       <c r="P1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -1562,16 +1581,16 @@
       </c>
       <c r="P6">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q6">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
@@ -1589,31 +1608,31 @@
         <v>2</v>
       </c>
       <c r="G7" t="s">
+        <v>111</v>
+      </c>
+      <c r="H7" t="s">
         <v>112</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>113</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>114</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>115</v>
-      </c>
-      <c r="K7" t="s">
-        <v>116</v>
       </c>
       <c r="L7" t="s">
         <v>83</v>
       </c>
       <c r="M7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N7" t="s">
         <v>6</v>
       </c>
       <c r="O7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P7">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -1626,7 +1645,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -1644,7 +1663,7 @@
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H8" t="s">
         <v>82</v>
@@ -1653,16 +1672,16 @@
         <v>83</v>
       </c>
       <c r="J8" t="s">
+        <v>119</v>
+      </c>
+      <c r="K8" t="s">
         <v>120</v>
-      </c>
-      <c r="K8" t="s">
-        <v>121</v>
       </c>
       <c r="L8" t="s">
         <v>86</v>
       </c>
       <c r="M8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N8" t="s">
         <v>6</v>
@@ -1681,7 +1700,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -1708,10 +1727,10 @@
         <v>83</v>
       </c>
       <c r="J9" t="s">
+        <v>123</v>
+      </c>
+      <c r="K9" t="s">
         <v>124</v>
-      </c>
-      <c r="K9" t="s">
-        <v>125</v>
       </c>
       <c r="L9" t="s">
         <v>86</v>
@@ -1736,7 +1755,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B10" t="s">
         <v>86</v>
@@ -1757,13 +1776,13 @@
         <v>6</v>
       </c>
       <c r="H10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I10" t="s">
         <v>127</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>128</v>
-      </c>
-      <c r="J10" t="s">
-        <v>129</v>
       </c>
       <c r="P10">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -1776,7 +1795,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
@@ -1797,28 +1816,28 @@
         <v>6</v>
       </c>
       <c r="H11" t="s">
+        <v>170</v>
+      </c>
+      <c r="I11" t="s">
         <v>171</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>172</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>173</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
+        <v>6</v>
+      </c>
+      <c r="M11" t="s">
         <v>174</v>
       </c>
-      <c r="L11" t="s">
-        <v>6</v>
-      </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O11" t="s">
         <v>175</v>
-      </c>
-      <c r="N11" t="s">
-        <v>6</v>
-      </c>
-      <c r="O11" t="s">
-        <v>176</v>
       </c>
       <c r="P11" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -1831,7 +1850,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
@@ -1858,22 +1877,22 @@
         <v>6</v>
       </c>
       <c r="J12" t="s">
+        <v>165</v>
+      </c>
+      <c r="K12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M12" t="s">
         <v>166</v>
       </c>
-      <c r="K12" t="s">
-        <v>6</v>
-      </c>
-      <c r="L12" t="s">
-        <v>6</v>
-      </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O12" t="s">
         <v>167</v>
-      </c>
-      <c r="N12" t="s">
-        <v>6</v>
-      </c>
-      <c r="O12" t="s">
-        <v>168</v>
       </c>
       <c r="P12" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -1886,7 +1905,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
@@ -1907,28 +1926,28 @@
         <v>6</v>
       </c>
       <c r="H13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I13" t="s">
+        <v>178</v>
+      </c>
+      <c r="J13" t="s">
         <v>179</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>180</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M13" t="s">
         <v>181</v>
       </c>
-      <c r="L13" t="s">
-        <v>6</v>
-      </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>182</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>183</v>
-      </c>
-      <c r="O13" t="s">
-        <v>184</v>
       </c>
       <c r="P13" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -1941,7 +1960,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
@@ -1962,28 +1981,28 @@
         <v>6</v>
       </c>
       <c r="H14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I14" t="s">
+        <v>186</v>
+      </c>
+      <c r="J14" t="s">
         <v>187</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>188</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
+        <v>6</v>
+      </c>
+      <c r="M14" t="s">
         <v>189</v>
       </c>
-      <c r="L14" t="s">
-        <v>6</v>
-      </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
+        <v>6</v>
+      </c>
+      <c r="O14" t="s">
         <v>190</v>
-      </c>
-      <c r="N14" t="s">
-        <v>6</v>
-      </c>
-      <c r="O14" t="s">
-        <v>191</v>
       </c>
       <c r="P14" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -1996,7 +2015,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
@@ -2023,22 +2042,22 @@
         <v>6</v>
       </c>
       <c r="J15" t="s">
+        <v>194</v>
+      </c>
+      <c r="K15" t="s">
+        <v>191</v>
+      </c>
+      <c r="L15" t="s">
+        <v>6</v>
+      </c>
+      <c r="M15" t="s">
+        <v>192</v>
+      </c>
+      <c r="N15" t="s">
+        <v>6</v>
+      </c>
+      <c r="O15" t="s">
         <v>195</v>
-      </c>
-      <c r="K15" t="s">
-        <v>192</v>
-      </c>
-      <c r="L15" t="s">
-        <v>6</v>
-      </c>
-      <c r="M15" t="s">
-        <v>193</v>
-      </c>
-      <c r="N15" t="s">
-        <v>6</v>
-      </c>
-      <c r="O15" t="s">
-        <v>196</v>
       </c>
       <c r="P15" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2051,7 +2070,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="P16" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2064,7 +2083,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P17" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2077,7 +2096,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="P18" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2090,7 +2109,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P19" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2103,7 +2122,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P20" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2116,7 +2135,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P21" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2129,7 +2148,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P22" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2142,7 +2161,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P23" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2155,7 +2174,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P24" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2168,7 +2187,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="P25" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2181,7 +2200,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P26" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2202,10 +2221,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2219,18 +2238,18 @@
         <v>68</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -2241,7 +2260,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>6</v>
@@ -2249,10 +2268,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>6</v>
@@ -2303,24 +2322,13 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="C10" s="6"/>
+      <c r="A9" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="C9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2332,9 +2340,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M66"/>
+  <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2376,178 +2384,178 @@
         <v>66</v>
       </c>
       <c r="L1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>193</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>142</v>
+        <v>3</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="E2" s="1">
-        <v>600</v>
+        <v>999</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
+        <v>185</v>
       </c>
       <c r="G2" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="H2" t="s">
-        <v>5</v>
+        <v>198</v>
       </c>
       <c r="I2" t="s">
-        <v>6</v>
+        <v>197</v>
       </c>
       <c r="J2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN600yi2=0 OR (i2=7 AND $2=lcsh)</v>
-      </c>
-      <c r="L2">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M2">
+      <c r="K2" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>circulation_countUNC999oi1=9 AND i2=1</v>
+      </c>
+      <c r="L2" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>142</v>
+        <v>199</v>
       </c>
       <c r="E3" s="1">
-        <v>610</v>
+        <v>946</v>
       </c>
       <c r="F3" t="s">
-        <v>3</v>
+        <v>200</v>
       </c>
       <c r="G3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H3" t="s">
         <v>5</v>
       </c>
       <c r="I3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="J3" t="s">
         <v>6</v>
       </c>
-      <c r="K3" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN610yi2=0 OR (i2=7 AND $2=lcsh)</v>
-      </c>
-      <c r="L3">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+      <c r="K3" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>date_catalogedDUKE946b.</v>
+      </c>
+      <c r="L3" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>142</v>
+        <v>201</v>
       </c>
       <c r="E4" s="1">
-        <v>611</v>
+        <v>909</v>
       </c>
       <c r="F4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H4" t="s">
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="J4" t="s">
         <v>6</v>
       </c>
-      <c r="K4" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN611yi2=0 OR (i2=7 AND $2=lcsh)</v>
-      </c>
-      <c r="L4">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+      <c r="K4" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>date_catalogedNCSU909a.</v>
+      </c>
+      <c r="L4" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>142</v>
+        <v>54</v>
       </c>
       <c r="E5" s="1">
-        <v>630</v>
+        <v>999</v>
       </c>
       <c r="F5" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="H5" t="s">
         <v>5</v>
       </c>
       <c r="I5" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="J5" t="s">
         <v>6</v>
       </c>
       <c r="K5" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN630yi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>date_catalogedUNC999ai1=0 AND i2=0</v>
       </c>
       <c r="L5">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -2555,74 +2563,71 @@
       </c>
       <c r="M5">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>142</v>
-      </c>
-      <c r="E6" s="1">
-        <v>648</v>
+        <v>202</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" t="s">
-        <v>9</v>
-      </c>
-      <c r="K6" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN648ai2=0 OR (i2=7 AND $2=~/lcsh|fast/)</v>
-      </c>
-      <c r="L6">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+        <v>56</v>
+      </c>
+      <c r="K6" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>date_catalogedNCCU...</v>
+      </c>
+      <c r="L6" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>1</v>
+      </c>
+      <c r="M6" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>142</v>
+        <v>54</v>
       </c>
       <c r="E7" s="1">
-        <v>650</v>
+        <v>999</v>
       </c>
       <c r="F7" t="s">
-        <v>3</v>
+        <v>176</v>
       </c>
       <c r="G7" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="H7" t="s">
         <v>5</v>
@@ -2631,42 +2636,42 @@
         <v>6</v>
       </c>
       <c r="J7" t="s">
-        <v>6</v>
-      </c>
-      <c r="K7" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN650yi2=0 OR (i2=7 AND $2=lcsh)</v>
-      </c>
-      <c r="L7">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+        <v>177</v>
+      </c>
+      <c r="K7" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>item_due_dateUNC999di1=9 AND i2=1</v>
+      </c>
+      <c r="L7" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>152</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
       </c>
-      <c r="D8" t="s">
-        <v>142</v>
+      <c r="D8" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="E8" s="1">
-        <v>651</v>
+        <v>999</v>
       </c>
       <c r="F8" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="G8" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="H8" t="s">
         <v>5</v>
@@ -2677,40 +2682,40 @@
       <c r="J8" t="s">
         <v>6</v>
       </c>
-      <c r="K8" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN651yi2=0 OR (i2=7 AND $2=lcsh)</v>
-      </c>
-      <c r="L8">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+      <c r="K8" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>item_locationUNC999li1=9 AND i2=1</v>
+      </c>
+      <c r="L8" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>153</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
       </c>
-      <c r="D9" t="s">
-        <v>142</v>
+      <c r="D9" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="E9" s="1">
-        <v>655</v>
+        <v>999</v>
       </c>
       <c r="F9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="H9" t="s">
         <v>5</v>
@@ -2721,40 +2726,40 @@
       <c r="J9" t="s">
         <v>6</v>
       </c>
-      <c r="K9" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN655yi2=0 OR (i2=7 AND $2=lcsh)</v>
-      </c>
-      <c r="L9">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+      <c r="K9" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>item_public_noteUNC999ni1=9 AND i2=1</v>
+      </c>
+      <c r="L9" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>151</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>142</v>
+        <v>54</v>
       </c>
       <c r="E10" s="1">
-        <v>600</v>
+        <v>999</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>168</v>
       </c>
       <c r="G10" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="H10" t="s">
         <v>5</v>
@@ -2765,22 +2770,22 @@
       <c r="J10" t="s">
         <v>6</v>
       </c>
-      <c r="K10" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN600vi2=0 OR (i2=7 AND $2=lcsh)</v>
-      </c>
-      <c r="L10">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>2</v>
+      <c r="K10" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>item_record_idUNC999ii1=9 AND i2=1</v>
+      </c>
+      <c r="L10" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
@@ -2789,13 +2794,13 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E11" s="1">
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="F11" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="G11" t="s">
         <v>4</v>
@@ -2811,7 +2816,7 @@
       </c>
       <c r="K11" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN610vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_chronological_facetGEN600yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L11">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -2819,12 +2824,12 @@
       </c>
       <c r="M11">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -2833,13 +2838,13 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E12" s="1">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="G12" t="s">
         <v>4</v>
@@ -2855,7 +2860,7 @@
       </c>
       <c r="K12" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN611vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_chronological_facetGEN610yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L12">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -2863,12 +2868,12 @@
       </c>
       <c r="M12">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
@@ -2877,29 +2882,29 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E13" s="1">
-        <v>6</v>
-      </c>
-      <c r="F13">
-        <v>16</v>
+        <v>611</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
       </c>
       <c r="G13" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H13" t="s">
         <v>5</v>
       </c>
       <c r="I13" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J13" t="s">
         <v>6</v>
       </c>
       <c r="K13" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN616LDR/06 = a AND LDR/07 =~ [acdm] AND 006/00 =~ [at]</v>
+        <v>subject_chronological_facetGEN611yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L13">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -2907,12 +2912,12 @@
       </c>
       <c r="M13">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
@@ -2921,29 +2926,29 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E14" s="1">
-        <v>6</v>
-      </c>
-      <c r="F14">
-        <v>17</v>
+        <v>630</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3</v>
       </c>
       <c r="G14" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H14" t="s">
         <v>5</v>
       </c>
       <c r="I14" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="J14" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="K14" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN617LDR/06 = a AND LDR/07 =~ [acdm] AND 006/00 =~ [at]</v>
+        <v>subject_chronological_facetGEN630yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L14">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -2951,12 +2956,12 @@
       </c>
       <c r="M14">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
@@ -2965,13 +2970,13 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E15" s="1">
-        <v>630</v>
+        <v>650</v>
       </c>
       <c r="F15" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="G15" t="s">
         <v>4</v>
@@ -2987,7 +2992,7 @@
       </c>
       <c r="K15" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN630vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_chronological_facetGEN650yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L15">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -2995,27 +3000,27 @@
       </c>
       <c r="M15">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
       </c>
       <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>141</v>
+      </c>
+      <c r="E16" s="1">
+        <v>651</v>
+      </c>
+      <c r="F16" t="s">
         <v>3</v>
-      </c>
-      <c r="D16" t="s">
-        <v>142</v>
-      </c>
-      <c r="E16" s="1">
-        <v>647</v>
-      </c>
-      <c r="F16" t="s">
-        <v>16</v>
       </c>
       <c r="G16" t="s">
         <v>4</v>
@@ -3027,11 +3032,11 @@
         <v>6</v>
       </c>
       <c r="J16" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="K16" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN647vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_chronological_facetGEN651yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L16">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3039,27 +3044,27 @@
       </c>
       <c r="M16">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
       </c>
       <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>141</v>
+      </c>
+      <c r="E17" s="1">
+        <v>655</v>
+      </c>
+      <c r="F17" t="s">
         <v>3</v>
-      </c>
-      <c r="D17" t="s">
-        <v>142</v>
-      </c>
-      <c r="E17" s="1">
-        <v>648</v>
-      </c>
-      <c r="F17" t="s">
-        <v>16</v>
       </c>
       <c r="G17" t="s">
         <v>4</v>
@@ -3071,11 +3076,11 @@
         <v>6</v>
       </c>
       <c r="J17" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="K17" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN648vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_chronological_facetGEN655yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L17">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3083,30 +3088,30 @@
       </c>
       <c r="M17">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E18" s="1">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="F18" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G18" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H18" t="s">
         <v>5</v>
@@ -3115,11 +3120,11 @@
         <v>6</v>
       </c>
       <c r="J18" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K18" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN650vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_chronological_facetGEN648ai2=0 OR (i2=7 AND $2=~/lcsh|fast/)</v>
       </c>
       <c r="L18">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3127,7 +3132,7 @@
       </c>
       <c r="M18">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -3141,29 +3146,29 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E19" s="1">
-        <v>651</v>
-      </c>
-      <c r="F19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19">
         <v>16</v>
       </c>
       <c r="G19" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="H19" t="s">
         <v>5</v>
       </c>
       <c r="I19" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="J19" t="s">
         <v>6</v>
       </c>
       <c r="K19" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN651vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN616LDR/06 = a AND LDR/07 =~ [acdm] AND 006/00 =~ [at]</v>
       </c>
       <c r="L19">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3182,32 +3187,32 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E20" s="1">
-        <v>655</v>
-      </c>
-      <c r="F20" t="s">
-        <v>19</v>
+        <v>6</v>
+      </c>
+      <c r="F20">
+        <v>17</v>
       </c>
       <c r="G20" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="H20" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I20" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="J20" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="K20" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655axi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN617LDR/06 = a AND LDR/07 =~ [acdm] AND 006/00 =~ [at]</v>
       </c>
       <c r="L20">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3226,32 +3231,32 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E21" s="1">
-        <v>655</v>
-      </c>
-      <c r="F21" t="s">
-        <v>19</v>
+        <v>8</v>
+      </c>
+      <c r="F21">
+        <v>33</v>
       </c>
       <c r="G21" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H21" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I21" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="J21" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="K21" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655axi2=7 AND $2=lcgft</v>
+        <v>subject_genre_facetGEN833LDR/06 = a AND LDR/07 =~ [acdm]</v>
       </c>
       <c r="L21">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3270,32 +3275,32 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E22" s="1">
-        <v>655</v>
-      </c>
-      <c r="F22" t="s">
-        <v>19</v>
+        <v>8</v>
+      </c>
+      <c r="F22">
+        <v>34</v>
       </c>
       <c r="G22" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="H22" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I22" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="J22" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="K22" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655axi2=7 AND $2=rbbin</v>
+        <v>subject_genre_facetGEN834LDR/06 = a AND LDR/07 =~ [acdm]</v>
       </c>
       <c r="L22">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3314,32 +3319,32 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E23" s="1">
-        <v>655</v>
+        <v>600</v>
       </c>
       <c r="F23" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G23" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="H23" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I23" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="J23" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="K23" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655axi2=7 AND $2=rbgenr</v>
+        <v>subject_genre_facetGEN600vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L23">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3358,32 +3363,32 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E24" s="1">
-        <v>655</v>
+        <v>610</v>
       </c>
       <c r="F24" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G24" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="H24" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I24" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="J24" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="K24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655axi2=7 AND $2=rbprov</v>
+        <v>subject_genre_facetGEN610vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3405,10 +3410,10 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E25" s="1">
-        <v>655</v>
+        <v>611</v>
       </c>
       <c r="F25" t="s">
         <v>16</v>
@@ -3427,7 +3432,7 @@
       </c>
       <c r="K25" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN611vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L25">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3446,19 +3451,19 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E26" s="1">
-        <v>655</v>
+        <v>630</v>
       </c>
       <c r="F26" t="s">
         <v>16</v>
       </c>
       <c r="G26" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="H26" t="s">
         <v>5</v>
@@ -3467,11 +3472,11 @@
         <v>6</v>
       </c>
       <c r="J26" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="K26" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655vi2=7 AND $2=lcgft</v>
+        <v>subject_genre_facetGEN630vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L26">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3490,19 +3495,19 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E27" s="1">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="F27" t="s">
         <v>16</v>
       </c>
       <c r="G27" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="H27" t="s">
         <v>5</v>
@@ -3511,11 +3516,11 @@
         <v>6</v>
       </c>
       <c r="J27" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="K27" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655vi2=7 AND $2=rbbin</v>
+        <v>subject_genre_facetGEN650vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L27">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3534,19 +3539,19 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E28" s="1">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="F28" t="s">
         <v>16</v>
       </c>
       <c r="G28" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="H28" t="s">
         <v>5</v>
@@ -3555,11 +3560,11 @@
         <v>6</v>
       </c>
       <c r="J28" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="K28" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655vi2=7 AND $2=rbgenr</v>
+        <v>subject_genre_facetGEN651vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L28">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3578,10 +3583,10 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E29" s="1">
         <v>655</v>
@@ -3590,7 +3595,7 @@
         <v>16</v>
       </c>
       <c r="G29" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="H29" t="s">
         <v>5</v>
@@ -3599,11 +3604,11 @@
         <v>6</v>
       </c>
       <c r="J29" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="K29" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655vi2=7 AND $2=rbprov</v>
+        <v>subject_genre_facetGEN655vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L29">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3625,16 +3630,16 @@
         <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E30" s="1">
-        <v>656</v>
+        <v>647</v>
       </c>
       <c r="F30" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="G30" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="H30" t="s">
         <v>5</v>
@@ -3643,11 +3648,11 @@
         <v>6</v>
       </c>
       <c r="J30" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="K30" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN656kvi2=7 AND $2=lcsh</v>
+        <v>subject_genre_facetGEN647vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L30">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3669,16 +3674,16 @@
         <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E31" s="1">
-        <v>657</v>
+        <v>648</v>
       </c>
       <c r="F31" t="s">
         <v>16</v>
       </c>
       <c r="G31" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="H31" t="s">
         <v>5</v>
@@ -3687,11 +3692,11 @@
         <v>6</v>
       </c>
       <c r="J31" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="K31" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN657vi2=7 AND $2=lcsh</v>
+        <v>subject_genre_facetGEN648vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L31">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3710,32 +3715,32 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E32" s="1">
-        <v>8</v>
-      </c>
-      <c r="F32">
-        <v>33</v>
+        <v>655</v>
+      </c>
+      <c r="F32" t="s">
+        <v>19</v>
       </c>
       <c r="G32" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="H32" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I32" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="J32" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="K32" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN833LDR/06 = a AND LDR/07 =~ [acdm]</v>
+        <v>subject_genre_facetGEN655axi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L32">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3754,32 +3759,32 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E33" s="1">
-        <v>8</v>
-      </c>
-      <c r="F33">
-        <v>34</v>
+        <v>655</v>
+      </c>
+      <c r="F33" t="s">
+        <v>19</v>
       </c>
       <c r="G33" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="H33" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I33" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="J33" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="K33" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN834LDR/06 = a AND LDR/07 =~ [acdm]</v>
+        <v>subject_genre_facetGEN655axi2=7 AND $2=lcgft</v>
       </c>
       <c r="L33">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3792,38 +3797,38 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B34" t="s">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E34" s="1">
-        <v>600</v>
+        <v>655</v>
       </c>
       <c r="F34" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="G34" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="H34" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I34" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="J34" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="K34" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN600zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN655axi2=7 AND $2=rbbin</v>
       </c>
       <c r="L34">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3831,43 +3836,43 @@
       </c>
       <c r="M34">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B35" t="s">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D35" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E35" s="1">
-        <v>610</v>
+        <v>655</v>
       </c>
       <c r="F35" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="G35" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="H35" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I35" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="J35" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K35" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN610zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN655axi2=7 AND $2=rbgenr</v>
       </c>
       <c r="L35">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3875,43 +3880,43 @@
       </c>
       <c r="M35">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B36" t="s">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E36" s="1">
-        <v>611</v>
+        <v>655</v>
       </c>
       <c r="F36" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="G36" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="H36" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I36" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="J36" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="K36" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN611zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN655axi2=7 AND $2=rbprov</v>
       </c>
       <c r="L36">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3919,30 +3924,30 @@
       </c>
       <c r="M36">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B37" t="s">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E37" s="1">
-        <v>630</v>
+        <v>655</v>
       </c>
       <c r="F37" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="G37" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="H37" t="s">
         <v>5</v>
@@ -3951,11 +3956,11 @@
         <v>6</v>
       </c>
       <c r="J37" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="K37" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN630zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN655vi2=7 AND $2=lcgft</v>
       </c>
       <c r="L37">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3963,12 +3968,12 @@
       </c>
       <c r="M37">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B38" t="s">
         <v>1</v>
@@ -3977,16 +3982,16 @@
         <v>3</v>
       </c>
       <c r="D38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E38" s="1">
-        <v>648</v>
+        <v>655</v>
       </c>
       <c r="F38" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="G38" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="H38" t="s">
         <v>5</v>
@@ -3995,11 +4000,11 @@
         <v>6</v>
       </c>
       <c r="J38" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="K38" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN648zi2=0 OR (i2=7 AND $2=~/lcsh|fast/)</v>
+        <v>subject_genre_facetGEN655vi2=7 AND $2=rbbin</v>
       </c>
       <c r="L38">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4007,30 +4012,30 @@
       </c>
       <c r="M38">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E39" s="1">
-        <v>650</v>
+        <v>655</v>
       </c>
       <c r="F39" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="G39" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="H39" t="s">
         <v>5</v>
@@ -4039,11 +4044,11 @@
         <v>6</v>
       </c>
       <c r="J39" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K39" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN650zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN655vi2=7 AND $2=rbgenr</v>
       </c>
       <c r="L39">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4051,30 +4056,30 @@
       </c>
       <c r="M39">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B40" t="s">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E40" s="1">
-        <v>651</v>
+        <v>655</v>
       </c>
       <c r="F40" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="G40" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="H40" t="s">
         <v>5</v>
@@ -4083,11 +4088,11 @@
         <v>6</v>
       </c>
       <c r="J40" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="K40" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN651zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN655vi2=7 AND $2=rbprov</v>
       </c>
       <c r="L40">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4095,30 +4100,30 @@
       </c>
       <c r="M40">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B41" t="s">
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E41" s="1">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="F41" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G41" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="H41" t="s">
         <v>5</v>
@@ -4127,11 +4132,11 @@
         <v>6</v>
       </c>
       <c r="J41" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="K41" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN655zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN656kvi2=7 AND $2=lcsh</v>
       </c>
       <c r="L41">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4139,43 +4144,43 @@
       </c>
       <c r="M41">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="B42" t="s">
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E42" s="1">
-        <v>600</v>
+        <v>657</v>
       </c>
       <c r="F42" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="G42" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="H42" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I42" t="s">
         <v>6</v>
       </c>
       <c r="J42" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="K42" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN600abcdfghjklmnopqrstui2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN657vi2=7 AND $2=lcsh</v>
       </c>
       <c r="L42">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4183,12 +4188,12 @@
       </c>
       <c r="M42">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B43" t="s">
         <v>1</v>
@@ -4197,13 +4202,13 @@
         <v>2</v>
       </c>
       <c r="D43" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E43" s="1">
         <v>600</v>
       </c>
       <c r="F43" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G43" t="s">
         <v>4</v>
@@ -4219,7 +4224,7 @@
       </c>
       <c r="K43" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN600xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN600zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L43">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4232,7 +4237,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B44" t="s">
         <v>1</v>
@@ -4241,29 +4246,29 @@
         <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E44" s="1">
         <v>610</v>
       </c>
       <c r="F44" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G44" t="s">
         <v>4</v>
       </c>
       <c r="H44" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I44" t="s">
         <v>6</v>
       </c>
       <c r="J44" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="K44" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN610abcdfghklmnoprstui2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN610zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L44">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4276,7 +4281,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B45" t="s">
         <v>1</v>
@@ -4285,13 +4290,13 @@
         <v>2</v>
       </c>
       <c r="D45" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E45" s="1">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="F45" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G45" t="s">
         <v>4</v>
@@ -4307,7 +4312,7 @@
       </c>
       <c r="K45" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN610xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN611zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L45">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4320,7 +4325,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B46" t="s">
         <v>1</v>
@@ -4329,29 +4334,29 @@
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E46" s="1">
-        <v>611</v>
+        <v>630</v>
       </c>
       <c r="F46" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G46" t="s">
         <v>4</v>
       </c>
       <c r="H46" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I46" t="s">
         <v>6</v>
       </c>
       <c r="J46" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="K46" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN611acdefghklnpqstui2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN630zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L46">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4364,7 +4369,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B47" t="s">
         <v>1</v>
@@ -4373,13 +4378,13 @@
         <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E47" s="1">
-        <v>611</v>
+        <v>650</v>
       </c>
       <c r="F47" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G47" t="s">
         <v>4</v>
@@ -4395,7 +4400,7 @@
       </c>
       <c r="K47" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN611xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN650zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L47">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4408,7 +4413,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B48" t="s">
         <v>1</v>
@@ -4417,29 +4422,29 @@
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E48" s="1">
-        <v>630</v>
+        <v>651</v>
       </c>
       <c r="F48" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="G48" t="s">
         <v>4</v>
       </c>
       <c r="H48" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I48" t="s">
         <v>6</v>
       </c>
       <c r="J48" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="K48" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN630adfghklmnoprsti2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN651zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L48">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4452,7 +4457,7 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B49" t="s">
         <v>1</v>
@@ -4461,13 +4466,13 @@
         <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E49" s="1">
-        <v>630</v>
+        <v>655</v>
       </c>
       <c r="F49" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G49" t="s">
         <v>4</v>
@@ -4483,7 +4488,7 @@
       </c>
       <c r="K49" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN630xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN655zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L49">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4496,7 +4501,7 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B50" t="s">
         <v>1</v>
@@ -4505,29 +4510,29 @@
         <v>3</v>
       </c>
       <c r="D50" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E50" s="1">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="F50" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="G50" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H50" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I50" t="s">
         <v>6</v>
       </c>
       <c r="J50" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K50" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN647acdgi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN648zi2=0 OR (i2=7 AND $2=~/lcsh|fast/)</v>
       </c>
       <c r="L50">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4546,36 +4551,36 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E51" s="1">
-        <v>655</v>
+        <v>600</v>
       </c>
       <c r="F51" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G51" t="s">
         <v>4</v>
       </c>
       <c r="H51" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I51" t="s">
         <v>6</v>
       </c>
       <c r="J51" t="s">
-        <v>6</v>
-      </c>
-      <c r="K51" s="8" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN655xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>40</v>
+      </c>
+      <c r="K51" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>subject_topic_lcsh_facetGEN600abcdfghjklmnopqrstui2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L51">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M51">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
@@ -4590,13 +4595,13 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E52" s="1">
-        <v>647</v>
+        <v>600</v>
       </c>
       <c r="F52" t="s">
         <v>41</v>
@@ -4611,11 +4616,11 @@
         <v>6</v>
       </c>
       <c r="J52" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="K52" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN647xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN600xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L52">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4634,32 +4639,32 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E53" s="1">
-        <v>648</v>
+        <v>610</v>
       </c>
       <c r="F53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G53" t="s">
         <v>4</v>
       </c>
       <c r="H53" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I53" t="s">
         <v>6</v>
       </c>
       <c r="J53" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="K53" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN648xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN610abcdfghklmnoprstui2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L53">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4681,19 +4686,19 @@
         <v>2</v>
       </c>
       <c r="D54" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E54" s="1">
-        <v>650</v>
+        <v>610</v>
       </c>
       <c r="F54" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G54" t="s">
         <v>4</v>
       </c>
       <c r="H54" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I54" t="s">
         <v>6</v>
@@ -4703,7 +4708,7 @@
       </c>
       <c r="K54" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN650abcdgi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN610xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L54">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4725,29 +4730,29 @@
         <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E55" s="1">
-        <v>650</v>
+        <v>611</v>
       </c>
       <c r="F55" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G55" t="s">
         <v>4</v>
       </c>
       <c r="H55" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I55" t="s">
         <v>6</v>
       </c>
       <c r="J55" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="K55" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN650xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN611acdefghklnpqstui2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L55">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4769,10 +4774,10 @@
         <v>2</v>
       </c>
       <c r="D56" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E56" s="1">
-        <v>651</v>
+        <v>611</v>
       </c>
       <c r="F56" t="s">
         <v>41</v>
@@ -4791,7 +4796,7 @@
       </c>
       <c r="K56" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN651xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN611xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L56">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4810,32 +4815,32 @@
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E57" s="1">
-        <v>656</v>
+        <v>630</v>
       </c>
       <c r="F57" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="G57" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="H57" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I57" t="s">
         <v>6</v>
       </c>
       <c r="J57" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K57" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN656ai2=7 AND $2=lcsh</v>
+        <v>subject_topic_lcsh_facetGEN630adfghklmnoprsti2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L57">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4854,19 +4859,19 @@
         <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D58" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E58" s="1">
-        <v>656</v>
+        <v>630</v>
       </c>
       <c r="F58" t="s">
         <v>41</v>
       </c>
       <c r="G58" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="H58" t="s">
         <v>5</v>
@@ -4875,11 +4880,11 @@
         <v>6</v>
       </c>
       <c r="J58" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="K58" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN656xi2=7 AND $2=lcsh</v>
+        <v>subject_topic_lcsh_facetGEN630xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L58">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4898,32 +4903,32 @@
         <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D59" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E59" s="1">
-        <v>657</v>
+        <v>650</v>
       </c>
       <c r="F59" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="G59" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="H59" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I59" t="s">
         <v>6</v>
       </c>
       <c r="J59" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="K59" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN657ai2=7 AND $2=lcsh</v>
+        <v>subject_topic_lcsh_facetGEN650abcdgi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L59">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4942,19 +4947,19 @@
         <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D60" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E60" s="1">
-        <v>657</v>
+        <v>650</v>
       </c>
       <c r="F60" t="s">
         <v>41</v>
       </c>
       <c r="G60" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="H60" t="s">
         <v>5</v>
@@ -4963,11 +4968,11 @@
         <v>6</v>
       </c>
       <c r="J60" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="K60" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN657xi2=7 AND $2=lcsh</v>
+        <v>subject_topic_lcsh_facetGEN650xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L60">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4980,38 +4985,38 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B61" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="C61" t="s">
         <v>2</v>
       </c>
       <c r="D61" t="s">
-        <v>54</v>
+        <v>141</v>
       </c>
       <c r="E61" s="1">
-        <v>999</v>
+        <v>651</v>
       </c>
       <c r="F61" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="G61" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="H61" t="s">
         <v>5</v>
       </c>
       <c r="I61" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="J61" t="s">
         <v>6</v>
       </c>
       <c r="K61" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>date_catalogedUNC999ai1=0 AND i2=0</v>
+        <v>subject_topic_lcsh_facetGEN651xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L61">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5024,69 +5029,69 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>152</v>
+        <v>38</v>
       </c>
       <c r="B62" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D62" t="s">
-        <v>54</v>
+        <v>141</v>
       </c>
       <c r="E62" s="1">
-        <v>999</v>
+        <v>647</v>
       </c>
       <c r="F62" t="s">
-        <v>169</v>
+        <v>48</v>
       </c>
       <c r="G62" t="s">
-        <v>170</v>
+        <v>4</v>
       </c>
       <c r="H62" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I62" t="s">
         <v>6</v>
       </c>
       <c r="J62" t="s">
-        <v>6</v>
-      </c>
-      <c r="K62" s="8" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_record_idUNC999ii1=9 AND i2=1</v>
-      </c>
-      <c r="L62" s="8">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M62" s="8">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="K62" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>subject_topic_lcsh_facetGEN647acdgi2=0 OR (i2=7 AND $2=lcsh)</v>
+      </c>
+      <c r="L62">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M62">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>151</v>
+        <v>38</v>
       </c>
       <c r="B63" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D63" t="s">
-        <v>54</v>
+        <v>141</v>
       </c>
       <c r="E63" s="1">
-        <v>999</v>
+        <v>647</v>
       </c>
       <c r="F63" t="s">
-        <v>177</v>
+        <v>41</v>
       </c>
       <c r="G63" t="s">
-        <v>170</v>
+        <v>4</v>
       </c>
       <c r="H63" t="s">
         <v>5</v>
@@ -5095,42 +5100,42 @@
         <v>6</v>
       </c>
       <c r="J63" t="s">
-        <v>178</v>
-      </c>
-      <c r="K63" s="8" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_due_dateUNC999di1=9 AND i2=1</v>
-      </c>
-      <c r="L63" s="8">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M63" s="8">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="K63" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>subject_topic_lcsh_facetGEN647xi2=0 OR (i2=7 AND $2=lcsh)</v>
+      </c>
+      <c r="L63">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M63">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>153</v>
+        <v>38</v>
       </c>
       <c r="B64" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>2</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>54</v>
+        <v>3</v>
+      </c>
+      <c r="D64" t="s">
+        <v>141</v>
       </c>
       <c r="E64" s="1">
-        <v>999</v>
+        <v>648</v>
       </c>
       <c r="F64" t="s">
-        <v>185</v>
+        <v>41</v>
       </c>
       <c r="G64" t="s">
-        <v>170</v>
+        <v>4</v>
       </c>
       <c r="H64" t="s">
         <v>5</v>
@@ -5139,42 +5144,42 @@
         <v>6</v>
       </c>
       <c r="J64" t="s">
-        <v>6</v>
-      </c>
-      <c r="K64" s="8" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_locationUNC999li1=9 AND i2=1</v>
-      </c>
-      <c r="L64" s="8">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M64" s="8">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="K64" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>subject_topic_lcsh_facetGEN648xi2=0 OR (i2=7 AND $2=lcsh)</v>
+      </c>
+      <c r="L64">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M64">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="B65" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>2</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>54</v>
+        <v>3</v>
+      </c>
+      <c r="D65" t="s">
+        <v>141</v>
       </c>
       <c r="E65" s="1">
-        <v>999</v>
+        <v>655</v>
       </c>
       <c r="F65" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="G65" t="s">
-        <v>170</v>
+        <v>4</v>
       </c>
       <c r="H65" t="s">
         <v>5</v>
@@ -5187,57 +5192,189 @@
       </c>
       <c r="K65" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_public_noteUNC999ni1=9 AND i2=1</v>
-      </c>
-      <c r="L65" s="8">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M65" s="8">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>0</v>
+        <v>subject_topic_lcsh_facetGEN655xi2=0 OR (i2=7 AND $2=lcsh)</v>
+      </c>
+      <c r="L65">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>1</v>
+      </c>
+      <c r="M65">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>194</v>
+        <v>38</v>
       </c>
       <c r="B66" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="C66" t="s">
         <v>3</v>
       </c>
-      <c r="D66" s="9" t="s">
-        <v>54</v>
+      <c r="D66" t="s">
+        <v>141</v>
       </c>
       <c r="E66" s="1">
-        <v>999</v>
+        <v>656</v>
       </c>
       <c r="F66" t="s">
-        <v>186</v>
+        <v>7</v>
       </c>
       <c r="G66" t="s">
-        <v>170</v>
+        <v>34</v>
       </c>
       <c r="H66" t="s">
-        <v>199</v>
+        <v>5</v>
       </c>
       <c r="I66" t="s">
-        <v>198</v>
+        <v>6</v>
       </c>
       <c r="J66" t="s">
-        <v>6</v>
-      </c>
-      <c r="K66" s="8" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>circulation_countUNC999oi1=9 AND i2=1</v>
-      </c>
-      <c r="L66" s="8">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M66" s="8">
+        <v>50</v>
+      </c>
+      <c r="K66" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>subject_topic_lcsh_facetGEN656ai2=7 AND $2=lcsh</v>
+      </c>
+      <c r="L66">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M66">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>38</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" t="s">
+        <v>3</v>
+      </c>
+      <c r="D67" t="s">
+        <v>141</v>
+      </c>
+      <c r="E67" s="1">
+        <v>656</v>
+      </c>
+      <c r="F67" t="s">
+        <v>41</v>
+      </c>
+      <c r="G67" t="s">
+        <v>34</v>
+      </c>
+      <c r="H67" t="s">
+        <v>5</v>
+      </c>
+      <c r="I67" t="s">
+        <v>6</v>
+      </c>
+      <c r="J67" t="s">
+        <v>35</v>
+      </c>
+      <c r="K67" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>subject_topic_lcsh_facetGEN656xi2=7 AND $2=lcsh</v>
+      </c>
+      <c r="L67">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M67">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>38</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>3</v>
+      </c>
+      <c r="D68" t="s">
+        <v>141</v>
+      </c>
+      <c r="E68" s="1">
+        <v>657</v>
+      </c>
+      <c r="F68" t="s">
+        <v>7</v>
+      </c>
+      <c r="G68" t="s">
+        <v>34</v>
+      </c>
+      <c r="H68" t="s">
+        <v>5</v>
+      </c>
+      <c r="I68" t="s">
+        <v>6</v>
+      </c>
+      <c r="J68" t="s">
+        <v>51</v>
+      </c>
+      <c r="K68" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>subject_topic_lcsh_facetGEN657ai2=7 AND $2=lcsh</v>
+      </c>
+      <c r="L68">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M68">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>38</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69" t="s">
+        <v>3</v>
+      </c>
+      <c r="D69" t="s">
+        <v>141</v>
+      </c>
+      <c r="E69" s="1">
+        <v>657</v>
+      </c>
+      <c r="F69" t="s">
+        <v>41</v>
+      </c>
+      <c r="G69" t="s">
+        <v>34</v>
+      </c>
+      <c r="H69" t="s">
+        <v>5</v>
+      </c>
+      <c r="I69" t="s">
+        <v>6</v>
+      </c>
+      <c r="J69" t="s">
+        <v>51</v>
+      </c>
+      <c r="K69" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>subject_topic_lcsh_facetGEN657xi2=7 AND $2=lcsh</v>
+      </c>
+      <c r="L69">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M69">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
         <v>1</v>
       </c>
@@ -5256,10 +5393,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5272,21 +5409,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" t="s">
         <v>130</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>131</v>
-      </c>
-      <c r="D1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B2">
         <v>655</v>
@@ -5295,7 +5432,7 @@
         <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5309,7 +5446,7 @@
         <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5323,7 +5460,7 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5337,7 +5474,7 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5348,10 +5485,10 @@
         <v>46</v>
       </c>
       <c r="C6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" t="s">
         <v>140</v>
-      </c>
-      <c r="D6" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5365,7 +5502,21 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>141</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>203</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -5373,8 +5524,9 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Adding items and holdings data fields; UNC mappings
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="5910" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="5910"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="260">
   <si>
     <t>subject_chronological_facet</t>
   </si>
@@ -374,12 +374,6 @@
     <t>Language(s) of the content in the material(s) described by the record</t>
   </si>
   <si>
-    <t xml:space="preserve">Limit/narrow results by language. Many resources are in more than one language. Users studying languages should be able to find materials that are in "English and French" </t>
-  </si>
-  <si>
-    <t>Language codes need to be mapped to preferred display terms -- http://id.loc.gov/vocabulary/languages.html or http://www.loc.gov/standards/codelists/languages.xml</t>
-  </si>
-  <si>
     <t>subject_topic_mesh_facet</t>
   </si>
   <si>
@@ -488,51 +482,27 @@
     <t>item_location</t>
   </si>
   <si>
-    <t>item_public_note</t>
-  </si>
-  <si>
     <t>item_call_number</t>
   </si>
   <si>
-    <t>item_call_number_scheme</t>
-  </si>
-  <si>
     <t>item_status</t>
   </si>
   <si>
     <t>item_type</t>
   </si>
   <si>
-    <t>item_volume_designator</t>
-  </si>
-  <si>
-    <t>holdings_summary_statement</t>
-  </si>
-  <si>
-    <t>holdings_location</t>
-  </si>
-  <si>
     <t>holdings_record_id</t>
   </si>
   <si>
     <t>holdings_call_number</t>
   </si>
   <si>
-    <t>holdings_call_number_scheme</t>
-  </si>
-  <si>
-    <t>holdings_public_note</t>
-  </si>
-  <si>
     <t>Unique identifier for an item record in host institution's ILS. Could be record number or barcode.</t>
   </si>
   <si>
     <t>Item ID</t>
   </si>
   <si>
-    <t>Each item record has only 1 value for this field. Depending on how you implement this, if there are multiple item records, this could end up being a multivalued field.</t>
-  </si>
-  <si>
     <t>i</t>
   </si>
   <si>
@@ -542,9 +512,6 @@
     <t>brief record, full record</t>
   </si>
   <si>
-    <t>Status: Due $date</t>
-  </si>
-  <si>
     <t>Item due date</t>
   </si>
   <si>
@@ -563,9 +530,6 @@
     <t>Will be blank if item is NOT checked out</t>
   </si>
   <si>
-    <t>Location:</t>
-  </si>
-  <si>
     <t>Shelving location code for item</t>
   </si>
   <si>
@@ -587,21 +551,12 @@
     <t>o</t>
   </si>
   <si>
-    <t>Notes:</t>
-  </si>
-  <si>
-    <t>Notes from the item record, intended for public view.</t>
-  </si>
-  <si>
     <t>Provide specific information at the copy or volume level. Assist in select and obtain user tasks</t>
   </si>
   <si>
     <t>ItemNotes</t>
   </si>
   <si>
-    <t>An item may have more than one item note.</t>
-  </si>
-  <si>
     <t>Used to sort by popularity</t>
   </si>
   <si>
@@ -642,6 +597,216 @@
   </si>
   <si>
     <t>Need to find out where this is in their data.</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>Limit/narrow results by language. Many resources are in more than one language. Users studying languages should be able to find materials that are in "English and French" ;;; Display language names in record</t>
+  </si>
+  <si>
+    <t>Of possible use for requesting or other features</t>
+  </si>
+  <si>
+    <t>(none)</t>
+  </si>
+  <si>
+    <t>Status: Due #{date}</t>
+  </si>
+  <si>
+    <t>item_note</t>
+  </si>
+  <si>
+    <t>call number</t>
+  </si>
+  <si>
+    <t>Full call number from item record (classification number + shelving cutter + shelf marks + volume/copy designators)</t>
+  </si>
+  <si>
+    <t>Library building/branch/larger location in which the shelving location is found</t>
+  </si>
+  <si>
+    <t>Inform user what library building or main section/area to go to in order to find the item</t>
+  </si>
+  <si>
+    <t>Libraries</t>
+  </si>
+  <si>
+    <t>Subjects;;;Subject Headings</t>
+  </si>
+  <si>
+    <t>Display in record (in order); adaptive hyperlinking for browsing/exploring; feed into autosuggest and/or "related titles" features</t>
+  </si>
+  <si>
+    <t>subject heading</t>
+  </si>
+  <si>
+    <t>Scheme (LCC, DDC, NLM, SUDOC, etc) from which item_call_number was assigned</t>
+  </si>
+  <si>
+    <t>Obtain resource</t>
+  </si>
+  <si>
+    <t>Support/control features behind the scenes -- gives info on further processing of this info into other fields</t>
+  </si>
+  <si>
+    <t>Call Number</t>
+  </si>
+  <si>
+    <t>item_classification_scheme</t>
+  </si>
+  <si>
+    <t>999Class (prepipeline field)</t>
+  </si>
+  <si>
+    <t>An item may have more than one item note. They should be displayed in order.</t>
+  </si>
+  <si>
+    <t>Empty if not checked out</t>
+  </si>
+  <si>
+    <t>documentation</t>
+  </si>
+  <si>
+    <t>Map language codes to preferred language terms for display (if not storage/indexing) -- http://id.loc.gov/vocabulary/languages.html or http://www.loc.gov/standards/codelists/languages.xml ;;; Retain order because 008 language code is the "main" or first language in the item; in 041, codes are assigned in order of importance/amount of content</t>
+  </si>
+  <si>
+    <t>https://github.com/trln/data-documentation/blob/master/argot/processing_rules_and_procedures.md#all-fields-that-become-facet-values</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>items</t>
+  </si>
+  <si>
+    <t>item_requestable</t>
+  </si>
+  <si>
+    <t>Status of individual item</t>
+  </si>
+  <si>
+    <t>Shows user whether item is available, library use only, checked out (and when due), missing, etc. Feeds into bib availability value</t>
+  </si>
+  <si>
+    <t>Statuses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Develop/agree upon a standard set of statuses, and how they map to bib_availability value? </t>
+  </si>
+  <si>
+    <t>Type/format for individual item</t>
+  </si>
+  <si>
+    <t>Do we need this in Argot/Argon? Will any features use it? Not sure if any do in Endeca.</t>
+  </si>
+  <si>
+    <t>ItemTypes</t>
+  </si>
+  <si>
+    <t>Placeholder for possibility of representing this in data/index instead of on-the-fly</t>
+  </si>
+  <si>
+    <t>holdings</t>
+  </si>
+  <si>
+    <t>holdings_note</t>
+  </si>
+  <si>
+    <t>item_location_library</t>
+  </si>
+  <si>
+    <t>item_location_shelf</t>
+  </si>
+  <si>
+    <t>holdings_location_library</t>
+  </si>
+  <si>
+    <t>holdings_location_shelf</t>
+  </si>
+  <si>
+    <t>resource_type</t>
+  </si>
+  <si>
+    <t>search limit?</t>
+  </si>
+  <si>
+    <t>in advanced search options?</t>
+  </si>
+  <si>
+    <t>Broad category of resources that might be helpful for limiting searches.</t>
+  </si>
+  <si>
+    <t>The analogous Endeca property looks like it is only used by NCSU, but it could have broader use</t>
+  </si>
+  <si>
+    <t>DocType</t>
+  </si>
+  <si>
+    <t>in Endeca, categories include "Gov Doc" and "Reference"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collaboratively maintain a vocabulary/set of types to use here, to avoid bizarre behavior after "expand to..." </t>
+  </si>
+  <si>
+    <t>Use case for this? Does NCSU still need? Anyone else?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For serials (and for some institutions, monographic series or sets), statement indicating what the library/location has for the title (volumes/years held, gaps, etc) </t>
+  </si>
+  <si>
+    <t>institution- and/or format-specific decision (brief record, full record)</t>
+  </si>
+  <si>
+    <t>Obtain resource; sort items in display into a logical order</t>
+  </si>
+  <si>
+    <t>See what the library/location has without having to look through all the individual items/volumes</t>
+  </si>
+  <si>
+    <t>SerialHoldingsSummary &gt; Serial Summary</t>
+  </si>
+  <si>
+    <t>Inform user what library building or main section/area to go to in order to find the items covered by holdings statement</t>
+  </si>
+  <si>
+    <t>SerialHoldingsSummary &gt; Library</t>
+  </si>
+  <si>
+    <t>Shelving location code for items covered by the holdings statement</t>
+  </si>
+  <si>
+    <t>Inform user what section/area of stacks to go to in order to find the items covered by holdings statement</t>
+  </si>
+  <si>
+    <t>SerialHoldingsSummary &gt; Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique identifier for source data holdings record in host institution's ILS. </t>
+  </si>
+  <si>
+    <t>Of possible use for requesting or other features;;;UNC uses this to link to "Latest Received" display from our Sierra OPAC</t>
+  </si>
+  <si>
+    <t>Full call number from holdings record (classification number + shelving cutter + shelf marks + volume/copy designators)</t>
+  </si>
+  <si>
+    <t>SerialHoldingsSummary &gt; Call #</t>
+  </si>
+  <si>
+    <t>holdings_summary</t>
+  </si>
+  <si>
+    <t>Public notes from the item record</t>
+  </si>
+  <si>
+    <t>Public notes from the holdings record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provide information on the run/span of items described that cannot be recorded elsewhere in holdings record. </t>
+  </si>
+  <si>
+    <t>SerialHoldingsSummary &gt; Item Note</t>
   </si>
 </sst>
 </file>
@@ -886,12 +1051,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="fields" displayName="fields" ref="A1:Q26" totalsRowShown="0">
-  <autoFilter ref="A1:Q26"/>
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="fields" displayName="fields" ref="A1:T28" totalsRowShown="0">
+  <autoFilter ref="A1:T28"/>
+  <tableColumns count="20">
     <tableColumn id="2" name="field"/>
     <tableColumn id="1" name="provisional"/>
     <tableColumn id="3" name="local"/>
+    <tableColumn id="18" name="parent"/>
+    <tableColumn id="19" name="required"/>
     <tableColumn id="4" name="multivalued?"/>
     <tableColumn id="5" name="searchable in"/>
     <tableColumn id="6" name="retain order"/>
@@ -904,6 +1071,7 @@
     <tableColumn id="13" name="endeca equivalent"/>
     <tableColumn id="14" name="notes"/>
     <tableColumn id="15" name="implementation details"/>
+    <tableColumn id="20" name="documentation"/>
     <tableColumn id="16" name="issue ct" dataDxfId="11">
       <calculatedColumnFormula>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</calculatedColumnFormula>
     </tableColumn>
@@ -916,8 +1084,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="issuesfield" displayName="issuesfield" ref="A1:C9" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:C9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="issuesfield" displayName="issuesfield" ref="A1:C11" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:C11"/>
   <tableColumns count="3">
     <tableColumn id="1" name="field" dataDxfId="8"/>
     <tableColumn id="3" name="desc" dataDxfId="7"/>
@@ -1238,29 +1406,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.42578125" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="5" max="6" width="14.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1"/>
-    <col min="13" max="13" width="34.5703125" customWidth="1"/>
-    <col min="14" max="14" width="19.5703125" customWidth="1"/>
-    <col min="16" max="16" width="24" customWidth="1"/>
-    <col min="17" max="17" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="12" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" customWidth="1"/>
+    <col min="17" max="17" width="24.85546875" customWidth="1"/>
+    <col min="18" max="18" width="17" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.5703125" customWidth="1"/>
+    <col min="21" max="21" width="24" customWidth="1"/>
+    <col min="22" max="22" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -1271,49 +1443,58 @@
         <v>69</v>
       </c>
       <c r="D1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F1" t="s">
         <v>70</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>71</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>72</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>73</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>74</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>75</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>76</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>77</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>78</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>79</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>65</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>80</v>
       </c>
-      <c r="P1" t="s">
-        <v>149</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" t="s">
+        <v>212</v>
+      </c>
+      <c r="S1" t="s">
+        <v>147</v>
+      </c>
+      <c r="T1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1324,51 +1505,57 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>158</v>
       </c>
       <c r="F2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
         <v>81</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>82</v>
       </c>
-      <c r="I2" t="s">
-        <v>83</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" t="s">
         <v>84</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>85</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>86</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>87</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>88</v>
       </c>
-      <c r="O2" t="s">
-        <v>6</v>
-      </c>
-      <c r="P2">
+      <c r="Q2" t="s">
+        <v>214</v>
+      </c>
+      <c r="S2">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>1</v>
       </c>
-      <c r="Q2">
+      <c r="T2">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1379,51 +1566,57 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>2</v>
+        <v>158</v>
       </c>
       <c r="F3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
         <v>90</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>82</v>
       </c>
-      <c r="I3" t="s">
-        <v>83</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" t="s">
         <v>91</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>92</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>86</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>93</v>
       </c>
-      <c r="N3" t="s">
+      <c r="P3" t="s">
         <v>94</v>
       </c>
-      <c r="O3" t="s">
-        <v>6</v>
-      </c>
-      <c r="P3">
+      <c r="Q3" t="s">
+        <v>214</v>
+      </c>
+      <c r="S3">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>2</v>
       </c>
-      <c r="Q3">
+      <c r="T3">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1434,51 +1627,57 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>2</v>
+        <v>158</v>
       </c>
       <c r="F4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
         <v>95</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>82</v>
       </c>
-      <c r="I4" t="s">
-        <v>83</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" t="s">
         <v>96</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>97</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>86</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>98</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>99</v>
       </c>
-      <c r="O4" t="s">
-        <v>6</v>
-      </c>
-      <c r="P4">
+      <c r="Q4" t="s">
+        <v>214</v>
+      </c>
+      <c r="S4">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>1</v>
       </c>
-      <c r="Q4">
+      <c r="T4">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1489,51 +1688,57 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>2</v>
+        <v>158</v>
       </c>
       <c r="F5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" t="s">
         <v>100</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>82</v>
       </c>
-      <c r="I5" t="s">
-        <v>83</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" t="s">
         <v>101</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>102</v>
       </c>
-      <c r="L5" t="s">
+      <c r="N5" t="s">
         <v>86</v>
       </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>103</v>
       </c>
-      <c r="N5" t="s">
+      <c r="P5" t="s">
         <v>99</v>
       </c>
-      <c r="O5" t="s">
-        <v>6</v>
-      </c>
-      <c r="P5">
+      <c r="Q5" t="s">
+        <v>214</v>
+      </c>
+      <c r="S5">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>1</v>
       </c>
-      <c r="Q5">
+      <c r="T5">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -1544,51 +1749,57 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>2</v>
+        <v>158</v>
       </c>
       <c r="F6" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" t="s">
         <v>104</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>105</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M6" t="s">
+        <v>107</v>
+      </c>
+      <c r="N6" t="s">
         <v>83</v>
       </c>
-      <c r="J6" t="s">
-        <v>106</v>
-      </c>
-      <c r="K6" t="s">
-        <v>107</v>
-      </c>
-      <c r="L6" t="s">
-        <v>83</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>108</v>
       </c>
-      <c r="N6" t="s">
-        <v>6</v>
-      </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q6" t="s">
         <v>109</v>
       </c>
-      <c r="P6">
+      <c r="S6">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>0</v>
       </c>
-      <c r="Q6">
+      <c r="T6">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>110</v>
       </c>
@@ -1599,614 +1810,1348 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>2</v>
+        <v>158</v>
       </c>
       <c r="F7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" t="s">
         <v>111</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>112</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>113</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>114</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
+        <v>191</v>
+      </c>
+      <c r="N7" t="s">
+        <v>83</v>
+      </c>
+      <c r="O7" t="s">
+        <v>111</v>
+      </c>
+      <c r="P7" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>213</v>
+      </c>
+      <c r="S7">
+        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>115</v>
       </c>
-      <c r="L7" t="s">
-        <v>83</v>
-      </c>
-      <c r="M7" t="s">
-        <v>111</v>
-      </c>
-      <c r="N7" t="s">
-        <v>6</v>
-      </c>
-      <c r="O7" t="s">
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" t="s">
+        <v>158</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" t="s">
         <v>116</v>
       </c>
-      <c r="P7">
+      <c r="J8" t="s">
+        <v>82</v>
+      </c>
+      <c r="K8" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" t="s">
+        <v>117</v>
+      </c>
+      <c r="M8" t="s">
+        <v>118</v>
+      </c>
+      <c r="N8" t="s">
+        <v>86</v>
+      </c>
+      <c r="O8" t="s">
+        <v>119</v>
+      </c>
+      <c r="P8" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>6</v>
+      </c>
+      <c r="S8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="T8">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>117</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" t="s">
-        <v>118</v>
-      </c>
-      <c r="H8" t="s">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
+        <v>158</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" t="s">
+        <v>81</v>
+      </c>
+      <c r="J9" t="s">
         <v>82</v>
       </c>
-      <c r="I8" t="s">
-        <v>83</v>
-      </c>
-      <c r="J8" t="s">
-        <v>119</v>
-      </c>
-      <c r="K8" t="s">
-        <v>120</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="K9" t="s">
+        <v>41</v>
+      </c>
+      <c r="L9" t="s">
+        <v>121</v>
+      </c>
+      <c r="M9" t="s">
+        <v>122</v>
+      </c>
+      <c r="N9" t="s">
         <v>86</v>
       </c>
-      <c r="M8" t="s">
-        <v>121</v>
-      </c>
-      <c r="N8" t="s">
-        <v>6</v>
-      </c>
-      <c r="O8" t="s">
-        <v>6</v>
-      </c>
-      <c r="P8">
+      <c r="O9" t="s">
+        <v>87</v>
+      </c>
+      <c r="P9" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>6</v>
+      </c>
+      <c r="S9">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>1</v>
       </c>
-      <c r="Q8">
+      <c r="T9">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>122</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" t="s">
-        <v>81</v>
-      </c>
-      <c r="H9" t="s">
-        <v>82</v>
-      </c>
-      <c r="I9" t="s">
-        <v>83</v>
-      </c>
-      <c r="J9" t="s">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>123</v>
       </c>
-      <c r="K9" t="s">
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>158</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>203</v>
+      </c>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" t="s">
         <v>124</v>
       </c>
-      <c r="L9" t="s">
+      <c r="K10" t="s">
+        <v>125</v>
+      </c>
+      <c r="L10" t="s">
+        <v>126</v>
+      </c>
+      <c r="M10" t="s">
+        <v>202</v>
+      </c>
+      <c r="O10" t="s">
+        <v>201</v>
+      </c>
+      <c r="P10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>6</v>
+      </c>
+      <c r="S10">
+        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>216</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" t="s">
+        <v>160</v>
+      </c>
+      <c r="K11" t="s">
+        <v>194</v>
+      </c>
+      <c r="L11" t="s">
+        <v>161</v>
+      </c>
+      <c r="M11" t="s">
+        <v>162</v>
+      </c>
+      <c r="N11" t="s">
+        <v>41</v>
+      </c>
+      <c r="O11" t="s">
+        <v>163</v>
+      </c>
+      <c r="P11" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>164</v>
+      </c>
+      <c r="S11" s="8">
+        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>216</v>
+      </c>
+      <c r="E12" t="s">
+        <v>173</v>
+      </c>
+      <c r="F12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" t="s">
+        <v>41</v>
+      </c>
+      <c r="L12" t="s">
+        <v>156</v>
+      </c>
+      <c r="M12" t="s">
+        <v>192</v>
+      </c>
+      <c r="N12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O12" t="s">
+        <v>157</v>
+      </c>
+      <c r="P12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>41</v>
+      </c>
+      <c r="S12" s="8">
+        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>228</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>216</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" t="s">
+        <v>160</v>
+      </c>
+      <c r="K13" t="s">
+        <v>193</v>
+      </c>
+      <c r="L13" t="s">
+        <v>198</v>
+      </c>
+      <c r="M13" t="s">
+        <v>199</v>
+      </c>
+      <c r="N13" t="s">
+        <v>41</v>
+      </c>
+      <c r="O13" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>171</v>
+      </c>
+      <c r="S13" s="8">
+        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>229</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>216</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" t="s">
+        <v>160</v>
+      </c>
+      <c r="K14" t="s">
+        <v>193</v>
+      </c>
+      <c r="L14" t="s">
+        <v>167</v>
+      </c>
+      <c r="M14" t="s">
+        <v>168</v>
+      </c>
+      <c r="N14" t="s">
+        <v>41</v>
+      </c>
+      <c r="O14" t="s">
+        <v>169</v>
+      </c>
+      <c r="P14" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>171</v>
+      </c>
+      <c r="S14" s="8">
+        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>195</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>216</v>
+      </c>
+      <c r="E15" t="s">
+        <v>173</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" t="s">
+        <v>41</v>
+      </c>
+      <c r="J15" t="s">
+        <v>160</v>
+      </c>
+      <c r="K15" t="s">
+        <v>193</v>
+      </c>
+      <c r="L15" t="s">
+        <v>256</v>
+      </c>
+      <c r="M15" t="s">
+        <v>174</v>
+      </c>
+      <c r="N15" t="s">
+        <v>41</v>
+      </c>
+      <c r="O15" t="s">
+        <v>175</v>
+      </c>
+      <c r="P15" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>210</v>
+      </c>
+      <c r="S15" s="8">
+        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>178</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" t="s">
         <v>86</v>
       </c>
-      <c r="M9" t="s">
-        <v>87</v>
-      </c>
-      <c r="N9" t="s">
-        <v>6</v>
-      </c>
-      <c r="O9" t="s">
-        <v>6</v>
-      </c>
-      <c r="P9">
+      <c r="F16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" t="s">
+        <v>41</v>
+      </c>
+      <c r="J16" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" t="s">
+        <v>41</v>
+      </c>
+      <c r="L16" t="s">
+        <v>179</v>
+      </c>
+      <c r="M16" t="s">
+        <v>176</v>
+      </c>
+      <c r="N16" t="s">
+        <v>41</v>
+      </c>
+      <c r="O16" t="s">
+        <v>177</v>
+      </c>
+      <c r="P16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>180</v>
+      </c>
+      <c r="S16" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>1</v>
       </c>
-      <c r="Q9">
+      <c r="T16">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>125</v>
-      </c>
-      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>216</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>196</v>
+      </c>
+      <c r="H17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I17" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" t="s">
+        <v>160</v>
+      </c>
+      <c r="K17" t="s">
+        <v>193</v>
+      </c>
+      <c r="L17" t="s">
+        <v>197</v>
+      </c>
+      <c r="M17" t="s">
+        <v>243</v>
+      </c>
+      <c r="N17" t="s">
+        <v>6</v>
+      </c>
+      <c r="O17" t="s">
+        <v>207</v>
+      </c>
+      <c r="S17" s="8">
+        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>208</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>216</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" t="s">
+        <v>41</v>
+      </c>
+      <c r="J18" t="s">
+        <v>41</v>
+      </c>
+      <c r="K18" t="s">
+        <v>41</v>
+      </c>
+      <c r="L18" t="s">
+        <v>204</v>
+      </c>
+      <c r="M18" t="s">
+        <v>206</v>
+      </c>
+      <c r="N18" t="s">
+        <v>41</v>
+      </c>
+      <c r="O18" t="s">
+        <v>209</v>
+      </c>
+      <c r="P18" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>41</v>
+      </c>
+      <c r="S18" s="8">
+        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>216</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19" t="s">
+        <v>41</v>
+      </c>
+      <c r="I19" t="s">
+        <v>41</v>
+      </c>
+      <c r="J19" t="s">
+        <v>160</v>
+      </c>
+      <c r="K19" t="s">
+        <v>193</v>
+      </c>
+      <c r="L19" t="s">
+        <v>218</v>
+      </c>
+      <c r="M19" t="s">
+        <v>219</v>
+      </c>
+      <c r="N19" t="s">
+        <v>41</v>
+      </c>
+      <c r="O19" t="s">
+        <v>220</v>
+      </c>
+      <c r="P19" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>221</v>
+      </c>
+      <c r="S19" s="8">
+        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>153</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>216</v>
+      </c>
+      <c r="E20" t="s">
         <v>86</v>
       </c>
-      <c r="C10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" t="s">
-        <v>126</v>
-      </c>
-      <c r="I10" t="s">
-        <v>127</v>
-      </c>
-      <c r="J10" t="s">
-        <v>128</v>
-      </c>
-      <c r="P10">
+      <c r="F20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" t="s">
+        <v>41</v>
+      </c>
+      <c r="H20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20" t="s">
+        <v>41</v>
+      </c>
+      <c r="J20" t="s">
+        <v>86</v>
+      </c>
+      <c r="K20" t="s">
+        <v>86</v>
+      </c>
+      <c r="L20" t="s">
+        <v>222</v>
+      </c>
+      <c r="M20" t="s">
+        <v>86</v>
+      </c>
+      <c r="N20" t="s">
+        <v>41</v>
+      </c>
+      <c r="O20" t="s">
+        <v>224</v>
+      </c>
+      <c r="P20" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>6</v>
+      </c>
+      <c r="R20" t="s">
+        <v>6</v>
+      </c>
+      <c r="S20" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="T20">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>150</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11" t="s">
-        <v>170</v>
-      </c>
-      <c r="I11" t="s">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>217</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>216</v>
+      </c>
+      <c r="E21" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" t="s">
+        <v>41</v>
+      </c>
+      <c r="H21" t="s">
+        <v>41</v>
+      </c>
+      <c r="I21" t="s">
+        <v>41</v>
+      </c>
+      <c r="J21" t="s">
+        <v>41</v>
+      </c>
+      <c r="K21" t="s">
+        <v>41</v>
+      </c>
+      <c r="L21" t="s">
+        <v>225</v>
+      </c>
+      <c r="M21" t="s">
+        <v>6</v>
+      </c>
+      <c r="N21" t="s">
+        <v>41</v>
+      </c>
+      <c r="O21" t="s">
+        <v>41</v>
+      </c>
+      <c r="P21" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>6</v>
+      </c>
+      <c r="R21" t="s">
+        <v>6</v>
+      </c>
+      <c r="S21" s="8">
+        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>255</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>226</v>
+      </c>
+      <c r="E22" t="s">
+        <v>173</v>
+      </c>
+      <c r="F22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22" t="s">
+        <v>41</v>
+      </c>
+      <c r="J22" t="s">
+        <v>242</v>
+      </c>
+      <c r="K22" t="s">
+        <v>193</v>
+      </c>
+      <c r="L22" t="s">
+        <v>241</v>
+      </c>
+      <c r="M22" t="s">
+        <v>244</v>
+      </c>
+      <c r="N22" t="s">
+        <v>41</v>
+      </c>
+      <c r="O22" t="s">
+        <v>245</v>
+      </c>
+      <c r="P22" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>6</v>
+      </c>
+      <c r="R22" t="s">
+        <v>6</v>
+      </c>
+      <c r="S22" s="8">
+        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>230</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>226</v>
+      </c>
+      <c r="E23" t="s">
+        <v>173</v>
+      </c>
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H23" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" t="s">
+        <v>41</v>
+      </c>
+      <c r="J23" t="s">
+        <v>242</v>
+      </c>
+      <c r="K23" t="s">
+        <v>193</v>
+      </c>
+      <c r="L23" t="s">
+        <v>198</v>
+      </c>
+      <c r="M23" t="s">
+        <v>246</v>
+      </c>
+      <c r="N23" t="s">
+        <v>41</v>
+      </c>
+      <c r="O23" t="s">
+        <v>247</v>
+      </c>
+      <c r="P23" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q23" t="s">
         <v>171</v>
       </c>
-      <c r="J11" t="s">
-        <v>172</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="R23" t="s">
+        <v>6</v>
+      </c>
+      <c r="S23" s="8">
+        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>231</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>226</v>
+      </c>
+      <c r="E24" t="s">
         <v>173</v>
       </c>
-      <c r="L11" t="s">
-        <v>6</v>
-      </c>
-      <c r="M11" t="s">
-        <v>174</v>
-      </c>
-      <c r="N11" t="s">
-        <v>6</v>
-      </c>
-      <c r="O11" t="s">
-        <v>175</v>
-      </c>
-      <c r="P11" s="8">
+      <c r="F24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" t="s">
+        <v>41</v>
+      </c>
+      <c r="H24" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" t="s">
+        <v>41</v>
+      </c>
+      <c r="J24" t="s">
+        <v>242</v>
+      </c>
+      <c r="K24" t="s">
+        <v>193</v>
+      </c>
+      <c r="L24" t="s">
+        <v>248</v>
+      </c>
+      <c r="M24" t="s">
+        <v>249</v>
+      </c>
+      <c r="N24" t="s">
+        <v>41</v>
+      </c>
+      <c r="O24" t="s">
+        <v>250</v>
+      </c>
+      <c r="P24" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>171</v>
+      </c>
+      <c r="R24" t="s">
+        <v>6</v>
+      </c>
+      <c r="S24" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>0</v>
       </c>
-      <c r="Q11">
+      <c r="T24">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>151</v>
-      </c>
-      <c r="B12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12" t="s">
-        <v>6</v>
-      </c>
-      <c r="I12" t="s">
-        <v>6</v>
-      </c>
-      <c r="J12" t="s">
-        <v>165</v>
-      </c>
-      <c r="K12" t="s">
-        <v>6</v>
-      </c>
-      <c r="L12" t="s">
-        <v>6</v>
-      </c>
-      <c r="M12" t="s">
-        <v>166</v>
-      </c>
-      <c r="N12" t="s">
-        <v>6</v>
-      </c>
-      <c r="O12" t="s">
-        <v>167</v>
-      </c>
-      <c r="P12" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>154</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>226</v>
+      </c>
+      <c r="E25" t="s">
+        <v>173</v>
+      </c>
+      <c r="F25" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" t="s">
+        <v>41</v>
+      </c>
+      <c r="H25" t="s">
+        <v>41</v>
+      </c>
+      <c r="I25" t="s">
+        <v>41</v>
+      </c>
+      <c r="J25" t="s">
+        <v>41</v>
+      </c>
+      <c r="K25" t="s">
+        <v>41</v>
+      </c>
+      <c r="L25" t="s">
+        <v>251</v>
+      </c>
+      <c r="M25" t="s">
+        <v>252</v>
+      </c>
+      <c r="N25" t="s">
+        <v>41</v>
+      </c>
+      <c r="O25" t="s">
+        <v>41</v>
+      </c>
+      <c r="P25" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>6</v>
+      </c>
+      <c r="R25" t="s">
+        <v>6</v>
+      </c>
+      <c r="S25" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>0</v>
       </c>
-      <c r="Q12">
+      <c r="T25">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>152</v>
-      </c>
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H13" t="s">
-        <v>170</v>
-      </c>
-      <c r="I13" t="s">
-        <v>178</v>
-      </c>
-      <c r="J13" t="s">
-        <v>179</v>
-      </c>
-      <c r="K13" t="s">
-        <v>180</v>
-      </c>
-      <c r="L13" t="s">
-        <v>6</v>
-      </c>
-      <c r="M13" t="s">
-        <v>181</v>
-      </c>
-      <c r="N13" t="s">
-        <v>182</v>
-      </c>
-      <c r="O13" t="s">
-        <v>183</v>
-      </c>
-      <c r="P13" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>155</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>226</v>
+      </c>
+      <c r="E26" t="s">
+        <v>173</v>
+      </c>
+      <c r="F26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" t="s">
+        <v>196</v>
+      </c>
+      <c r="H26" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" t="s">
+        <v>41</v>
+      </c>
+      <c r="J26" t="s">
+        <v>242</v>
+      </c>
+      <c r="K26" t="s">
+        <v>193</v>
+      </c>
+      <c r="L26" t="s">
+        <v>253</v>
+      </c>
+      <c r="M26" t="s">
+        <v>205</v>
+      </c>
+      <c r="N26" t="s">
+        <v>41</v>
+      </c>
+      <c r="O26" t="s">
+        <v>254</v>
+      </c>
+      <c r="P26" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>6</v>
+      </c>
+      <c r="R26" t="s">
+        <v>6</v>
+      </c>
+      <c r="S26" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>0</v>
       </c>
-      <c r="Q13">
+      <c r="T26">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>153</v>
-      </c>
-      <c r="B14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" t="s">
-        <v>170</v>
-      </c>
-      <c r="I14" t="s">
-        <v>186</v>
-      </c>
-      <c r="J14" t="s">
-        <v>187</v>
-      </c>
-      <c r="K14" t="s">
-        <v>188</v>
-      </c>
-      <c r="L14" t="s">
-        <v>6</v>
-      </c>
-      <c r="M14" t="s">
-        <v>189</v>
-      </c>
-      <c r="N14" t="s">
-        <v>6</v>
-      </c>
-      <c r="O14" t="s">
-        <v>190</v>
-      </c>
-      <c r="P14" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>227</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>226</v>
+      </c>
+      <c r="E27" t="s">
+        <v>173</v>
+      </c>
+      <c r="F27" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" t="s">
+        <v>41</v>
+      </c>
+      <c r="H27" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" t="s">
+        <v>41</v>
+      </c>
+      <c r="J27" t="s">
+        <v>242</v>
+      </c>
+      <c r="K27" t="s">
+        <v>193</v>
+      </c>
+      <c r="L27" t="s">
+        <v>257</v>
+      </c>
+      <c r="M27" t="s">
+        <v>258</v>
+      </c>
+      <c r="N27" t="s">
+        <v>41</v>
+      </c>
+      <c r="O27" t="s">
+        <v>259</v>
+      </c>
+      <c r="P27" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>6</v>
+      </c>
+      <c r="R27" t="s">
+        <v>6</v>
+      </c>
+      <c r="S27" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>0</v>
       </c>
-      <c r="Q14">
+      <c r="T27">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>193</v>
-      </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" t="s">
-        <v>6</v>
-      </c>
-      <c r="H15" t="s">
-        <v>6</v>
-      </c>
-      <c r="I15" t="s">
-        <v>6</v>
-      </c>
-      <c r="J15" t="s">
-        <v>194</v>
-      </c>
-      <c r="K15" t="s">
-        <v>191</v>
-      </c>
-      <c r="L15" t="s">
-        <v>6</v>
-      </c>
-      <c r="M15" t="s">
-        <v>192</v>
-      </c>
-      <c r="N15" t="s">
-        <v>6</v>
-      </c>
-      <c r="O15" t="s">
-        <v>195</v>
-      </c>
-      <c r="P15" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>232</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" t="s">
+        <v>173</v>
+      </c>
+      <c r="F28" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" t="s">
+        <v>233</v>
+      </c>
+      <c r="H28" t="s">
+        <v>2</v>
+      </c>
+      <c r="I28" t="s">
+        <v>41</v>
+      </c>
+      <c r="J28" t="s">
+        <v>234</v>
+      </c>
+      <c r="K28" t="s">
+        <v>6</v>
+      </c>
+      <c r="L28" t="s">
+        <v>235</v>
+      </c>
+      <c r="M28" t="s">
+        <v>236</v>
+      </c>
+      <c r="N28" t="s">
+        <v>41</v>
+      </c>
+      <c r="O28" t="s">
+        <v>237</v>
+      </c>
+      <c r="P28" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>239</v>
+      </c>
+      <c r="R28" t="s">
+        <v>6</v>
+      </c>
+      <c r="S28" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>1</v>
       </c>
-      <c r="Q15">
-        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>154</v>
-      </c>
-      <c r="P16" s="8">
-        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>155</v>
-      </c>
-      <c r="P17" s="8">
-        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>156</v>
-      </c>
-      <c r="P18" s="8">
-        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>157</v>
-      </c>
-      <c r="P19" s="8">
-        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>158</v>
-      </c>
-      <c r="P20" s="8">
-        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>159</v>
-      </c>
-      <c r="P21" s="8">
-        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>160</v>
-      </c>
-      <c r="P22" s="8">
-        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q22">
-        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>161</v>
-      </c>
-      <c r="P23" s="8">
-        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q23">
-        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>162</v>
-      </c>
-      <c r="P24" s="8">
-        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q24">
-        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>163</v>
-      </c>
-      <c r="P25" s="8">
-        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q25">
-        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>164</v>
-      </c>
-      <c r="P26" s="8">
-        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q26">
+      <c r="T28">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
         <v>0</v>
       </c>
@@ -2221,10 +3166,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2238,18 +3183,18 @@
         <v>68</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -2260,7 +3205,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>6</v>
@@ -2268,10 +3213,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>6</v>
@@ -2323,12 +3268,30 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="C11" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2342,7 +3305,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2384,15 +3349,15 @@
         <v>66</v>
       </c>
       <c r="L1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="M1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="B2" t="s">
         <v>53</v>
@@ -2407,16 +3372,16 @@
         <v>999</v>
       </c>
       <c r="F2" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="G2" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="H2" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="I2" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="J2" t="s">
         <v>6</v>
@@ -2445,13 +3410,13 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="E3" s="1">
         <v>946</v>
       </c>
       <c r="F3" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
@@ -2489,7 +3454,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="E4" s="1">
         <v>909</v>
@@ -2577,7 +3542,7 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>6</v>
@@ -2609,7 +3574,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B7" t="s">
         <v>53</v>
@@ -2624,10 +3589,10 @@
         <v>999</v>
       </c>
       <c r="F7" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="G7" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="H7" t="s">
         <v>5</v>
@@ -2636,7 +3601,7 @@
         <v>6</v>
       </c>
       <c r="J7" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="K7" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
@@ -2653,7 +3618,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B8" t="s">
         <v>53</v>
@@ -2668,10 +3633,10 @@
         <v>999</v>
       </c>
       <c r="F8" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="G8" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="H8" t="s">
         <v>5</v>
@@ -2697,7 +3662,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>153</v>
+        <v>195</v>
       </c>
       <c r="B9" t="s">
         <v>53</v>
@@ -2715,7 +3680,7 @@
         <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="H9" t="s">
         <v>5</v>
@@ -2728,7 +3693,7 @@
       </c>
       <c r="K9" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_public_noteUNC999ni1=9 AND i2=1</v>
+        <v>item_noteUNC999ni1=9 AND i2=1</v>
       </c>
       <c r="L9" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -2741,7 +3706,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B10" t="s">
         <v>53</v>
@@ -2756,10 +3721,10 @@
         <v>999</v>
       </c>
       <c r="F10" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="G10" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="H10" t="s">
         <v>5</v>
@@ -2794,7 +3759,7 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E11" s="1">
         <v>600</v>
@@ -2838,7 +3803,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E12" s="1">
         <v>610</v>
@@ -2882,7 +3847,7 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E13" s="1">
         <v>611</v>
@@ -2926,7 +3891,7 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E14" s="1">
         <v>630</v>
@@ -2970,7 +3935,7 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E15" s="1">
         <v>650</v>
@@ -3014,7 +3979,7 @@
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E16" s="1">
         <v>651</v>
@@ -3058,7 +4023,7 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E17" s="1">
         <v>655</v>
@@ -3102,7 +4067,7 @@
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E18" s="1">
         <v>648</v>
@@ -3146,7 +4111,7 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E19" s="1">
         <v>6</v>
@@ -3190,7 +4155,7 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E20" s="1">
         <v>6</v>
@@ -3234,7 +4199,7 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E21" s="1">
         <v>8</v>
@@ -3278,7 +4243,7 @@
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E22" s="1">
         <v>8</v>
@@ -3322,7 +4287,7 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E23" s="1">
         <v>600</v>
@@ -3366,7 +4331,7 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E24" s="1">
         <v>610</v>
@@ -3410,7 +4375,7 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E25" s="1">
         <v>611</v>
@@ -3454,7 +4419,7 @@
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E26" s="1">
         <v>630</v>
@@ -3498,7 +4463,7 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E27" s="1">
         <v>650</v>
@@ -3542,7 +4507,7 @@
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E28" s="1">
         <v>651</v>
@@ -3586,7 +4551,7 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E29" s="1">
         <v>655</v>
@@ -3630,7 +4595,7 @@
         <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E30" s="1">
         <v>647</v>
@@ -3674,7 +4639,7 @@
         <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E31" s="1">
         <v>648</v>
@@ -3718,7 +4683,7 @@
         <v>3</v>
       </c>
       <c r="D32" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E32" s="1">
         <v>655</v>
@@ -3762,7 +4727,7 @@
         <v>3</v>
       </c>
       <c r="D33" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E33" s="1">
         <v>655</v>
@@ -3806,7 +4771,7 @@
         <v>3</v>
       </c>
       <c r="D34" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E34" s="1">
         <v>655</v>
@@ -3850,7 +4815,7 @@
         <v>3</v>
       </c>
       <c r="D35" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E35" s="1">
         <v>655</v>
@@ -3894,7 +4859,7 @@
         <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E36" s="1">
         <v>655</v>
@@ -3938,7 +4903,7 @@
         <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E37" s="1">
         <v>655</v>
@@ -3982,7 +4947,7 @@
         <v>3</v>
       </c>
       <c r="D38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E38" s="1">
         <v>655</v>
@@ -4026,7 +4991,7 @@
         <v>3</v>
       </c>
       <c r="D39" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E39" s="1">
         <v>655</v>
@@ -4070,7 +5035,7 @@
         <v>3</v>
       </c>
       <c r="D40" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E40" s="1">
         <v>655</v>
@@ -4114,7 +5079,7 @@
         <v>3</v>
       </c>
       <c r="D41" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E41" s="1">
         <v>656</v>
@@ -4158,7 +5123,7 @@
         <v>3</v>
       </c>
       <c r="D42" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E42" s="1">
         <v>657</v>
@@ -4202,7 +5167,7 @@
         <v>2</v>
       </c>
       <c r="D43" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E43" s="1">
         <v>600</v>
@@ -4246,7 +5211,7 @@
         <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E44" s="1">
         <v>610</v>
@@ -4290,7 +5255,7 @@
         <v>2</v>
       </c>
       <c r="D45" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E45" s="1">
         <v>611</v>
@@ -4334,7 +5299,7 @@
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E46" s="1">
         <v>630</v>
@@ -4378,7 +5343,7 @@
         <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E47" s="1">
         <v>650</v>
@@ -4422,7 +5387,7 @@
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E48" s="1">
         <v>651</v>
@@ -4466,7 +5431,7 @@
         <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E49" s="1">
         <v>655</v>
@@ -4510,7 +5475,7 @@
         <v>3</v>
       </c>
       <c r="D50" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E50" s="1">
         <v>648</v>
@@ -4554,7 +5519,7 @@
         <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E51" s="1">
         <v>600</v>
@@ -4598,7 +5563,7 @@
         <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E52" s="1">
         <v>600</v>
@@ -4642,7 +5607,7 @@
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E53" s="1">
         <v>610</v>
@@ -4686,7 +5651,7 @@
         <v>2</v>
       </c>
       <c r="D54" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E54" s="1">
         <v>610</v>
@@ -4730,7 +5695,7 @@
         <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E55" s="1">
         <v>611</v>
@@ -4774,7 +5739,7 @@
         <v>2</v>
       </c>
       <c r="D56" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E56" s="1">
         <v>611</v>
@@ -4818,7 +5783,7 @@
         <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E57" s="1">
         <v>630</v>
@@ -4862,7 +5827,7 @@
         <v>2</v>
       </c>
       <c r="D58" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E58" s="1">
         <v>630</v>
@@ -4906,7 +5871,7 @@
         <v>2</v>
       </c>
       <c r="D59" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E59" s="1">
         <v>650</v>
@@ -4950,7 +5915,7 @@
         <v>2</v>
       </c>
       <c r="D60" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E60" s="1">
         <v>650</v>
@@ -4994,7 +5959,7 @@
         <v>2</v>
       </c>
       <c r="D61" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E61" s="1">
         <v>651</v>
@@ -5038,7 +6003,7 @@
         <v>3</v>
       </c>
       <c r="D62" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E62" s="1">
         <v>647</v>
@@ -5082,7 +6047,7 @@
         <v>3</v>
       </c>
       <c r="D63" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E63" s="1">
         <v>647</v>
@@ -5126,7 +6091,7 @@
         <v>3</v>
       </c>
       <c r="D64" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E64" s="1">
         <v>648</v>
@@ -5170,7 +6135,7 @@
         <v>3</v>
       </c>
       <c r="D65" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E65" s="1">
         <v>655</v>
@@ -5214,7 +6179,7 @@
         <v>3</v>
       </c>
       <c r="D66" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E66" s="1">
         <v>656</v>
@@ -5258,7 +6223,7 @@
         <v>3</v>
       </c>
       <c r="D67" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E67" s="1">
         <v>656</v>
@@ -5302,7 +6267,7 @@
         <v>3</v>
       </c>
       <c r="D68" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E68" s="1">
         <v>657</v>
@@ -5346,7 +6311,7 @@
         <v>3</v>
       </c>
       <c r="D69" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E69" s="1">
         <v>657</v>
@@ -5395,8 +6360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5409,21 +6374,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" t="s">
         <v>129</v>
-      </c>
-      <c r="C1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B2">
         <v>655</v>
@@ -5432,7 +6397,7 @@
         <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5446,7 +6411,7 @@
         <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5460,7 +6425,7 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5474,7 +6439,7 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5485,10 +6450,10 @@
         <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5502,12 +6467,12 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -5516,7 +6481,7 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mapping/docs for location facet and display
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="5910" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12570" windowHeight="5910" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="279">
   <si>
     <t>subject_chronological_facet</t>
   </si>
@@ -846,6 +846,24 @@
   </si>
   <si>
     <t>See maps/location_shelf_to_location_library.json["UNC"]</t>
+  </si>
+  <si>
+    <t>bib_locations_hierarchical</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Higher-level (library, etc.) locations housing volumes/copies of the resource described in the bib record </t>
+  </si>
+  <si>
+    <t>Support for hierarchical location facet; polyhierarchy already existing in Endeca</t>
+  </si>
+  <si>
+    <t>Recommended: limit to physical places people can go -- Online and E-resource are NOT locations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Determine best way to derive/represent data; I've provided something that seems to make sense to me... </t>
   </si>
 </sst>
 </file>
@@ -1093,14 +1111,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="fields" displayName="fields" ref="A1:T28" totalsRowShown="0">
-  <autoFilter ref="A1:T28">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="items"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="fields" displayName="fields" ref="A1:T29" totalsRowShown="0">
+  <autoFilter ref="A1:T29"/>
   <tableColumns count="20">
     <tableColumn id="2" name="field"/>
     <tableColumn id="1" name="provisional"/>
@@ -1132,8 +1144,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="issuesfield" displayName="issuesfield" ref="A1:C11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:C11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="issuesfield" displayName="issuesfield" ref="A1:C13" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:C13"/>
   <tableColumns count="3">
     <tableColumn id="1" name="field" dataDxfId="9"/>
     <tableColumn id="3" name="desc" dataDxfId="8"/>
@@ -1144,8 +1156,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="mappings" displayName="mappings" ref="A1:N76" totalsRowShown="0">
-  <autoFilter ref="A1:N76"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="mappings" displayName="mappings" ref="A1:N77" totalsRowShown="0">
+  <autoFilter ref="A1:N77"/>
   <sortState ref="A2:N70">
     <sortCondition ref="A2:A70"/>
     <sortCondition ref="C2:C70"/>
@@ -1457,11 +1469,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T28"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A13" sqref="A13"/>
+      <selection pane="topRight" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1545,7 +1557,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1609,7 +1621,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1673,7 +1685,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1737,7 +1749,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1801,7 +1813,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -1865,7 +1877,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>110</v>
       </c>
@@ -1929,7 +1941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -1993,7 +2005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>120</v>
       </c>
@@ -2057,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>123</v>
       </c>
@@ -2438,7 +2450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>177</v>
       </c>
@@ -2816,7 +2828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>254</v>
       </c>
@@ -2880,7 +2892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>229</v>
       </c>
@@ -2944,7 +2956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>230</v>
       </c>
@@ -3008,7 +3020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>153</v>
       </c>
@@ -3072,7 +3084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>154</v>
       </c>
@@ -3136,7 +3148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>226</v>
       </c>
@@ -3200,7 +3212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>231</v>
       </c>
@@ -3262,6 +3274,61 @@
       <c r="T28">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>273</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" t="s">
+        <v>73</v>
+      </c>
+      <c r="H29" t="s">
+        <v>2</v>
+      </c>
+      <c r="I29" t="s">
+        <v>274</v>
+      </c>
+      <c r="J29" t="s">
+        <v>82</v>
+      </c>
+      <c r="K29" t="s">
+        <v>41</v>
+      </c>
+      <c r="L29" t="s">
+        <v>275</v>
+      </c>
+      <c r="M29" t="s">
+        <v>276</v>
+      </c>
+      <c r="N29" t="s">
+        <v>41</v>
+      </c>
+      <c r="O29" t="s">
+        <v>274</v>
+      </c>
+      <c r="S29" s="8">
+        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
+        <v>2</v>
+      </c>
+      <c r="T29">
+        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3274,10 +3341,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3401,6 +3468,24 @@
       </c>
       <c r="C11" s="6"/>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="C13" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3411,10 +3496,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N76"/>
+  <dimension ref="A1:N77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3468,7 +3553,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>177</v>
+        <v>273</v>
       </c>
       <c r="B2" t="s">
         <v>53</v>
@@ -3476,30 +3561,13 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="1">
-        <v>999</v>
-      </c>
-      <c r="F2" t="s">
-        <v>172</v>
-      </c>
-      <c r="G2" t="s">
-        <v>158</v>
-      </c>
-      <c r="H2" t="s">
-        <v>182</v>
-      </c>
-      <c r="I2" t="s">
-        <v>181</v>
-      </c>
-      <c r="J2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E2" s="1"/>
       <c r="K2" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>circulation_countUNC999oi1=9 AND i2=1</v>
+        <v>bib_locations_hierarchicalUNC</v>
       </c>
       <c r="L2" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3507,7 +3575,7 @@
       </c>
       <c r="M2" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N2" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -3516,38 +3584,38 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>177</v>
       </c>
       <c r="B3" t="s">
         <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>183</v>
+        <v>3</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="E3" s="1">
-        <v>946</v>
+        <v>999</v>
       </c>
       <c r="F3" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>158</v>
       </c>
       <c r="H3" t="s">
-        <v>5</v>
+        <v>182</v>
       </c>
       <c r="I3" t="s">
-        <v>56</v>
+        <v>181</v>
       </c>
       <c r="J3" t="s">
         <v>6</v>
       </c>
       <c r="K3" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>date_catalogedDUKE946b.</v>
+        <v>circulation_countUNC999oi1=9 AND i2=1</v>
       </c>
       <c r="L3" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3555,7 +3623,7 @@
       </c>
       <c r="M3" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -3573,13 +3641,13 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E4" s="1">
-        <v>909</v>
+        <v>946</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>184</v>
       </c>
       <c r="G4" t="s">
         <v>6</v>
@@ -3595,7 +3663,7 @@
       </c>
       <c r="K4" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>date_catalogedNCSU909a.</v>
+        <v>date_catalogedDUKE946b.</v>
       </c>
       <c r="L4" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3621,16 +3689,16 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>185</v>
       </c>
       <c r="E5" s="1">
-        <v>999</v>
+        <v>909</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="H5" t="s">
         <v>5</v>
@@ -3641,15 +3709,15 @@
       <c r="J5" t="s">
         <v>6</v>
       </c>
-      <c r="K5" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>date_catalogedUNC999ai1=0 AND i2=0</v>
-      </c>
-      <c r="L5">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M5">
+      <c r="K5" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>date_catalogedNCSU909a.</v>
+      </c>
+      <c r="L5" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
         <v>0</v>
       </c>
@@ -3666,35 +3734,38 @@
         <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>186</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>6</v>
+        <v>54</v>
+      </c>
+      <c r="E6" s="1">
+        <v>999</v>
       </c>
       <c r="F6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="H6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I6" t="s">
         <v>56</v>
       </c>
-      <c r="K6" s="8" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>date_catalogedNCCU...</v>
-      </c>
-      <c r="L6" s="8">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>1</v>
-      </c>
-      <c r="M6" s="8">
+      <c r="J6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>date_catalogedUNC999ai1=0 AND i2=0</v>
+      </c>
+      <c r="L6">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M6">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
         <v>0</v>
       </c>
@@ -3705,42 +3776,39 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
         <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="1">
-        <v>999</v>
+        <v>186</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>260</v>
+        <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>158</v>
+        <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="I7" t="s">
-        <v>262</v>
-      </c>
-      <c r="J7" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="K7" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_call_numberUNC999qvci1=9 AND i2=1</v>
+        <v>date_catalogedNCCU...</v>
       </c>
       <c r="L7" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
@@ -3753,7 +3821,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B8" t="s">
         <v>53</v>
@@ -3768,23 +3836,23 @@
         <v>999</v>
       </c>
       <c r="F8" t="s">
-        <v>164</v>
+        <v>260</v>
       </c>
       <c r="G8" t="s">
-        <v>263</v>
+        <v>158</v>
       </c>
       <c r="H8" t="s">
-        <v>264</v>
+        <v>20</v>
       </c>
       <c r="I8" t="s">
-        <v>6</v>
+        <v>262</v>
       </c>
       <c r="J8" t="s">
         <v>6</v>
       </c>
       <c r="K8" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_statusUNC999di1=9 AND i2=1 and $d IS NOT blank</v>
+        <v>item_call_numberUNC999qvci1=9 AND i2=1</v>
       </c>
       <c r="L8" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3816,23 +3884,23 @@
         <v>999</v>
       </c>
       <c r="F9" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="G9" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="H9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I9" t="s">
-        <v>267</v>
+        <v>6</v>
       </c>
       <c r="J9" t="s">
         <v>6</v>
       </c>
       <c r="K9" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_statusUNC999si1=9 AND i2=1 and $d IS blank</v>
+        <v>item_statusUNC999di1=9 AND i2=1 and $d IS NOT blank</v>
       </c>
       <c r="L9" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3864,23 +3932,23 @@
         <v>999</v>
       </c>
       <c r="F10" t="s">
-        <v>7</v>
+        <v>189</v>
       </c>
       <c r="G10" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H10" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="I10" t="s">
-        <v>6</v>
+        <v>267</v>
       </c>
       <c r="J10" t="s">
-        <v>270</v>
+        <v>6</v>
       </c>
       <c r="K10" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_statusUNC999ai1=9 AND i2=4 AND NOT EXIST (tag=999 AND i1=9 and i2=1)</v>
+        <v>item_statusUNC999si1=9 AND i2=1 and $d IS blank</v>
       </c>
       <c r="L10" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3897,7 +3965,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B11" t="s">
         <v>53</v>
@@ -3912,23 +3980,23 @@
         <v>999</v>
       </c>
       <c r="F11" t="s">
-        <v>164</v>
+        <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>158</v>
+        <v>268</v>
       </c>
       <c r="H11" t="s">
-        <v>5</v>
+        <v>269</v>
       </c>
       <c r="I11" t="s">
         <v>6</v>
       </c>
       <c r="J11" t="s">
-        <v>165</v>
+        <v>270</v>
       </c>
       <c r="K11" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_due_dateUNC999di1=9 AND i2=1</v>
+        <v>item_statusUNC999ai1=9 AND i2=4 AND NOT EXIST (tag=999 AND i1=9 and i2=1)</v>
       </c>
       <c r="L11" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -3945,7 +4013,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>228</v>
+        <v>148</v>
       </c>
       <c r="B12" t="s">
         <v>53</v>
@@ -3953,14 +4021,14 @@
       <c r="C12" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" t="s">
         <v>54</v>
       </c>
       <c r="E12" s="1">
         <v>999</v>
       </c>
       <c r="F12" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G12" t="s">
         <v>158</v>
@@ -3972,11 +4040,11 @@
         <v>6</v>
       </c>
       <c r="J12" t="s">
-        <v>6</v>
+        <v>165</v>
       </c>
       <c r="K12" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_location_shelfUNC999li1=9 AND i2=1</v>
+        <v>item_due_dateUNC999di1=9 AND i2=1</v>
       </c>
       <c r="L12" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4008,10 +4076,10 @@
         <v>999</v>
       </c>
       <c r="F13" t="s">
-        <v>271</v>
+        <v>171</v>
       </c>
       <c r="G13" t="s">
-        <v>268</v>
+        <v>158</v>
       </c>
       <c r="H13" t="s">
         <v>5</v>
@@ -4024,7 +4092,7 @@
       </c>
       <c r="K13" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_location_shelfUNC999fi1=9 AND i2=4 AND NOT EXIST (tag=999 AND i1=9 and i2=1)</v>
+        <v>item_location_shelfUNC999li1=9 AND i2=1</v>
       </c>
       <c r="L13" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4041,7 +4109,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B14" t="s">
         <v>53</v>
@@ -4056,23 +4124,23 @@
         <v>999</v>
       </c>
       <c r="F14" t="s">
-        <v>171</v>
+        <v>271</v>
       </c>
       <c r="G14" t="s">
-        <v>158</v>
+        <v>268</v>
       </c>
       <c r="H14" t="s">
-        <v>265</v>
+        <v>5</v>
       </c>
       <c r="I14" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="J14" t="s">
         <v>6</v>
       </c>
       <c r="K14" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_location_libraryUNC999li1=9 AND i2=1</v>
+        <v>item_location_shelfUNC999fi1=9 AND i2=4 AND NOT EXIST (tag=999 AND i1=9 and i2=1)</v>
       </c>
       <c r="L14" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4104,10 +4172,10 @@
         <v>999</v>
       </c>
       <c r="F15" t="s">
-        <v>271</v>
+        <v>171</v>
       </c>
       <c r="G15" t="s">
-        <v>268</v>
+        <v>158</v>
       </c>
       <c r="H15" t="s">
         <v>265</v>
@@ -4120,7 +4188,7 @@
       </c>
       <c r="K15" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_location_libraryUNC999fi1=9 AND i2=4 AND NOT EXIST (tag=999 AND i1=9 and i2=1)</v>
+        <v>item_location_libraryUNC999li1=9 AND i2=1</v>
       </c>
       <c r="L15" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4137,7 +4205,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>195</v>
+        <v>227</v>
       </c>
       <c r="B16" t="s">
         <v>53</v>
@@ -4152,23 +4220,23 @@
         <v>999</v>
       </c>
       <c r="F16" t="s">
-        <v>2</v>
+        <v>271</v>
       </c>
       <c r="G16" t="s">
-        <v>158</v>
+        <v>268</v>
       </c>
       <c r="H16" t="s">
-        <v>5</v>
+        <v>265</v>
       </c>
       <c r="I16" t="s">
-        <v>6</v>
+        <v>272</v>
       </c>
       <c r="J16" t="s">
         <v>6</v>
       </c>
       <c r="K16" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_noteUNC999ni1=9 AND i2=1</v>
+        <v>item_location_libraryUNC999fi1=9 AND i2=4 AND NOT EXIST (tag=999 AND i1=9 and i2=1)</v>
       </c>
       <c r="L16" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4185,7 +4253,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>195</v>
       </c>
       <c r="B17" t="s">
         <v>53</v>
@@ -4193,14 +4261,14 @@
       <c r="C17" t="s">
         <v>2</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="9" t="s">
         <v>54</v>
       </c>
       <c r="E17" s="1">
         <v>999</v>
       </c>
       <c r="F17" t="s">
-        <v>157</v>
+        <v>2</v>
       </c>
       <c r="G17" t="s">
         <v>158</v>
@@ -4216,7 +4284,7 @@
       </c>
       <c r="K17" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_record_idUNC999ii1=9 AND i2=1</v>
+        <v>item_noteUNC999ni1=9 AND i2=1</v>
       </c>
       <c r="L17" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4233,25 +4301,25 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>0</v>
+        <v>149</v>
       </c>
       <c r="B18" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>139</v>
+        <v>54</v>
       </c>
       <c r="E18" s="1">
-        <v>600</v>
+        <v>999</v>
       </c>
       <c r="F18" t="s">
-        <v>3</v>
+        <v>157</v>
       </c>
       <c r="G18" t="s">
-        <v>4</v>
+        <v>158</v>
       </c>
       <c r="H18" t="s">
         <v>5</v>
@@ -4262,17 +4330,17 @@
       <c r="J18" t="s">
         <v>6</v>
       </c>
-      <c r="K18" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN600yi2=0 OR (i2=7 AND $2=lcsh)</v>
-      </c>
-      <c r="L18">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+      <c r="K18" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>item_record_idUNC999ii1=9 AND i2=1</v>
+      </c>
+      <c r="L18" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M18" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
       </c>
       <c r="N18" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -4293,7 +4361,7 @@
         <v>139</v>
       </c>
       <c r="E19" s="1">
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="F19" t="s">
         <v>3</v>
@@ -4312,7 +4380,7 @@
       </c>
       <c r="K19" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN610yi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_chronological_facetGEN600yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L19">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4341,7 +4409,7 @@
         <v>139</v>
       </c>
       <c r="E20" s="1">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F20" t="s">
         <v>3</v>
@@ -4360,7 +4428,7 @@
       </c>
       <c r="K20" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN611yi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_chronological_facetGEN610yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L20">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4389,7 +4457,7 @@
         <v>139</v>
       </c>
       <c r="E21" s="1">
-        <v>630</v>
+        <v>611</v>
       </c>
       <c r="F21" t="s">
         <v>3</v>
@@ -4408,7 +4476,7 @@
       </c>
       <c r="K21" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN630yi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_chronological_facetGEN611yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L21">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4437,7 +4505,7 @@
         <v>139</v>
       </c>
       <c r="E22" s="1">
-        <v>650</v>
+        <v>630</v>
       </c>
       <c r="F22" t="s">
         <v>3</v>
@@ -4456,7 +4524,7 @@
       </c>
       <c r="K22" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN650yi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_chronological_facetGEN630yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L22">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4485,7 +4553,7 @@
         <v>139</v>
       </c>
       <c r="E23" s="1">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="F23" t="s">
         <v>3</v>
@@ -4504,7 +4572,7 @@
       </c>
       <c r="K23" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN651yi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_chronological_facetGEN650yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L23">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4533,7 +4601,7 @@
         <v>139</v>
       </c>
       <c r="E24" s="1">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="F24" t="s">
         <v>3</v>
@@ -4552,7 +4620,7 @@
       </c>
       <c r="K24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN655yi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_chronological_facetGEN651yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4575,19 +4643,19 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D25" t="s">
         <v>139</v>
       </c>
       <c r="E25" s="1">
-        <v>648</v>
+        <v>655</v>
       </c>
       <c r="F25" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G25" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H25" t="s">
         <v>5</v>
@@ -4596,11 +4664,11 @@
         <v>6</v>
       </c>
       <c r="J25" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K25" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN648ai2=0 OR (i2=7 AND $2=~/lcsh|fast/)</v>
+        <v>subject_chronological_facetGEN655yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L25">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4617,38 +4685,38 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D26" t="s">
         <v>139</v>
       </c>
       <c r="E26" s="1">
-        <v>6</v>
-      </c>
-      <c r="F26">
-        <v>16</v>
+        <v>648</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
       </c>
       <c r="G26" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H26" t="s">
         <v>5</v>
       </c>
       <c r="I26" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J26" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K26" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN616LDR/06 = a AND LDR/07 =~ [acdm] AND 006/00 =~ [at]</v>
+        <v>subject_chronological_facetGEN648ai2=0 OR (i2=7 AND $2=~/lcsh|fast/)</v>
       </c>
       <c r="L26">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4656,7 +4724,7 @@
       </c>
       <c r="M26">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N26" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -4680,7 +4748,7 @@
         <v>6</v>
       </c>
       <c r="F27">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G27" t="s">
         <v>11</v>
@@ -4689,14 +4757,14 @@
         <v>5</v>
       </c>
       <c r="I27" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J27" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="K27" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN617LDR/06 = a AND LDR/07 =~ [acdm] AND 006/00 =~ [at]</v>
+        <v>subject_genre_facetGEN616LDR/06 = a AND LDR/07 =~ [acdm] AND 006/00 =~ [at]</v>
       </c>
       <c r="L27">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4725,26 +4793,26 @@
         <v>139</v>
       </c>
       <c r="E28" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F28">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="G28" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H28" t="s">
         <v>5</v>
       </c>
       <c r="I28" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J28" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="K28" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN833LDR/06 = a AND LDR/07 =~ [acdm]</v>
+        <v>subject_genre_facetGEN617LDR/06 = a AND LDR/07 =~ [acdm] AND 006/00 =~ [at]</v>
       </c>
       <c r="L28">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4776,7 +4844,7 @@
         <v>8</v>
       </c>
       <c r="F29">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G29" t="s">
         <v>15</v>
@@ -4785,14 +4853,14 @@
         <v>5</v>
       </c>
       <c r="I29" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J29" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="K29" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN834LDR/06 = a AND LDR/07 =~ [acdm]</v>
+        <v>subject_genre_facetGEN833LDR/06 = a AND LDR/07 =~ [acdm]</v>
       </c>
       <c r="L29">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4821,26 +4889,26 @@
         <v>139</v>
       </c>
       <c r="E30" s="1">
-        <v>600</v>
-      </c>
-      <c r="F30" t="s">
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="F30">
+        <v>34</v>
       </c>
       <c r="G30" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="H30" t="s">
         <v>5</v>
       </c>
       <c r="I30" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="J30" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="K30" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN600vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN834LDR/06 = a AND LDR/07 =~ [acdm]</v>
       </c>
       <c r="L30">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4869,7 +4937,7 @@
         <v>139</v>
       </c>
       <c r="E31" s="1">
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="F31" t="s">
         <v>16</v>
@@ -4888,7 +4956,7 @@
       </c>
       <c r="K31" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN610vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN600vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L31">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4917,7 +4985,7 @@
         <v>139</v>
       </c>
       <c r="E32" s="1">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F32" t="s">
         <v>16</v>
@@ -4936,7 +5004,7 @@
       </c>
       <c r="K32" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN611vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN610vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L32">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -4965,7 +5033,7 @@
         <v>139</v>
       </c>
       <c r="E33" s="1">
-        <v>630</v>
+        <v>611</v>
       </c>
       <c r="F33" t="s">
         <v>16</v>
@@ -4984,7 +5052,7 @@
       </c>
       <c r="K33" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN630vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN611vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L33">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5013,7 +5081,7 @@
         <v>139</v>
       </c>
       <c r="E34" s="1">
-        <v>650</v>
+        <v>630</v>
       </c>
       <c r="F34" t="s">
         <v>16</v>
@@ -5032,7 +5100,7 @@
       </c>
       <c r="K34" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN650vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN630vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L34">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5061,7 +5129,7 @@
         <v>139</v>
       </c>
       <c r="E35" s="1">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="F35" t="s">
         <v>16</v>
@@ -5080,7 +5148,7 @@
       </c>
       <c r="K35" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN651vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN650vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L35">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5109,7 +5177,7 @@
         <v>139</v>
       </c>
       <c r="E36" s="1">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="F36" t="s">
         <v>16</v>
@@ -5128,7 +5196,7 @@
       </c>
       <c r="K36" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN651vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L36">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5151,13 +5219,13 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D37" t="s">
         <v>139</v>
       </c>
       <c r="E37" s="1">
-        <v>647</v>
+        <v>655</v>
       </c>
       <c r="F37" t="s">
         <v>16</v>
@@ -5172,11 +5240,11 @@
         <v>6</v>
       </c>
       <c r="J37" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="K37" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN647vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN655vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L37">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5205,7 +5273,7 @@
         <v>139</v>
       </c>
       <c r="E38" s="1">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F38" t="s">
         <v>16</v>
@@ -5220,11 +5288,11 @@
         <v>6</v>
       </c>
       <c r="J38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K38" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN648vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN647vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L38">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5253,26 +5321,26 @@
         <v>139</v>
       </c>
       <c r="E39" s="1">
-        <v>655</v>
+        <v>648</v>
       </c>
       <c r="F39" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G39" t="s">
         <v>4</v>
       </c>
       <c r="H39" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I39" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="J39" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="K39" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655axi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN648vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L39">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5307,7 +5375,7 @@
         <v>19</v>
       </c>
       <c r="G40" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="H40" t="s">
         <v>20</v>
@@ -5316,11 +5384,11 @@
         <v>21</v>
       </c>
       <c r="J40" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K40" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655axi2=7 AND $2=lcgft</v>
+        <v>subject_genre_facetGEN655axi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L40">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5355,7 +5423,7 @@
         <v>19</v>
       </c>
       <c r="G41" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H41" t="s">
         <v>20</v>
@@ -5364,11 +5432,11 @@
         <v>21</v>
       </c>
       <c r="J41" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K41" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655axi2=7 AND $2=rbbin</v>
+        <v>subject_genre_facetGEN655axi2=7 AND $2=lcgft</v>
       </c>
       <c r="L41">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5403,7 +5471,7 @@
         <v>19</v>
       </c>
       <c r="G42" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H42" t="s">
         <v>20</v>
@@ -5412,11 +5480,11 @@
         <v>21</v>
       </c>
       <c r="J42" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K42" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655axi2=7 AND $2=rbgenr</v>
+        <v>subject_genre_facetGEN655axi2=7 AND $2=rbbin</v>
       </c>
       <c r="L42">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5451,20 +5519,20 @@
         <v>19</v>
       </c>
       <c r="G43" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H43" t="s">
         <v>20</v>
       </c>
       <c r="I43" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="J43" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K43" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655axi2=7 AND $2=rbprov</v>
+        <v>subject_genre_facetGEN655axi2=7 AND $2=rbgenr</v>
       </c>
       <c r="L43">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5496,23 +5564,23 @@
         <v>655</v>
       </c>
       <c r="F44" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G44" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="H44" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I44" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="J44" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="K44" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655vi2=7 AND $2=lcgft</v>
+        <v>subject_genre_facetGEN655axi2=7 AND $2=rbprov</v>
       </c>
       <c r="L44">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5547,7 +5615,7 @@
         <v>16</v>
       </c>
       <c r="G45" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H45" t="s">
         <v>5</v>
@@ -5556,11 +5624,11 @@
         <v>6</v>
       </c>
       <c r="J45" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K45" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655vi2=7 AND $2=rbbin</v>
+        <v>subject_genre_facetGEN655vi2=7 AND $2=lcgft</v>
       </c>
       <c r="L45">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5595,7 +5663,7 @@
         <v>16</v>
       </c>
       <c r="G46" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H46" t="s">
         <v>5</v>
@@ -5604,11 +5672,11 @@
         <v>6</v>
       </c>
       <c r="J46" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K46" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655vi2=7 AND $2=rbgenr</v>
+        <v>subject_genre_facetGEN655vi2=7 AND $2=rbbin</v>
       </c>
       <c r="L46">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5643,7 +5711,7 @@
         <v>16</v>
       </c>
       <c r="G47" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H47" t="s">
         <v>5</v>
@@ -5652,11 +5720,11 @@
         <v>6</v>
       </c>
       <c r="J47" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K47" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655vi2=7 AND $2=rbprov</v>
+        <v>subject_genre_facetGEN655vi2=7 AND $2=rbgenr</v>
       </c>
       <c r="L47">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5685,13 +5753,13 @@
         <v>139</v>
       </c>
       <c r="E48" s="1">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="F48" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="G48" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H48" t="s">
         <v>5</v>
@@ -5700,11 +5768,11 @@
         <v>6</v>
       </c>
       <c r="J48" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K48" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN656kvi2=7 AND $2=lcsh</v>
+        <v>subject_genre_facetGEN655vi2=7 AND $2=rbprov</v>
       </c>
       <c r="L48">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5733,10 +5801,10 @@
         <v>139</v>
       </c>
       <c r="E49" s="1">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F49" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="G49" t="s">
         <v>34</v>
@@ -5752,7 +5820,7 @@
       </c>
       <c r="K49" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN657vi2=7 AND $2=lcsh</v>
+        <v>subject_genre_facetGEN656kvi2=7 AND $2=lcsh</v>
       </c>
       <c r="L49">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5769,25 +5837,25 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B50" t="s">
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D50" t="s">
         <v>139</v>
       </c>
       <c r="E50" s="1">
-        <v>600</v>
+        <v>657</v>
       </c>
       <c r="F50" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="G50" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="H50" t="s">
         <v>5</v>
@@ -5796,11 +5864,11 @@
         <v>6</v>
       </c>
       <c r="J50" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="K50" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN600zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN657vi2=7 AND $2=lcsh</v>
       </c>
       <c r="L50">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5808,7 +5876,7 @@
       </c>
       <c r="M50">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N50" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -5829,7 +5897,7 @@
         <v>139</v>
       </c>
       <c r="E51" s="1">
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="F51" t="s">
         <v>37</v>
@@ -5848,7 +5916,7 @@
       </c>
       <c r="K51" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN610zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN600zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L51">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5877,7 +5945,7 @@
         <v>139</v>
       </c>
       <c r="E52" s="1">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F52" t="s">
         <v>37</v>
@@ -5896,7 +5964,7 @@
       </c>
       <c r="K52" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN611zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN610zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L52">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5925,7 +5993,7 @@
         <v>139</v>
       </c>
       <c r="E53" s="1">
-        <v>630</v>
+        <v>611</v>
       </c>
       <c r="F53" t="s">
         <v>37</v>
@@ -5944,7 +6012,7 @@
       </c>
       <c r="K53" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN630zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN611zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L53">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5973,7 +6041,7 @@
         <v>139</v>
       </c>
       <c r="E54" s="1">
-        <v>650</v>
+        <v>630</v>
       </c>
       <c r="F54" t="s">
         <v>37</v>
@@ -5992,7 +6060,7 @@
       </c>
       <c r="K54" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN650zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN630zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L54">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6021,7 +6089,7 @@
         <v>139</v>
       </c>
       <c r="E55" s="1">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="F55" t="s">
         <v>37</v>
@@ -6040,7 +6108,7 @@
       </c>
       <c r="K55" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN651zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN650zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L55">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6069,7 +6137,7 @@
         <v>139</v>
       </c>
       <c r="E56" s="1">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="F56" t="s">
         <v>37</v>
@@ -6088,7 +6156,7 @@
       </c>
       <c r="K56" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN655zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN651zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L56">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6111,19 +6179,19 @@
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D57" t="s">
         <v>139</v>
       </c>
       <c r="E57" s="1">
-        <v>648</v>
+        <v>655</v>
       </c>
       <c r="F57" t="s">
         <v>37</v>
       </c>
       <c r="G57" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H57" t="s">
         <v>5</v>
@@ -6132,11 +6200,11 @@
         <v>6</v>
       </c>
       <c r="J57" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="K57" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN648zi2=0 OR (i2=7 AND $2=~/lcsh|fast/)</v>
+        <v>subject_geographic_facetGEN655zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L57">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6153,38 +6221,38 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B58" t="s">
         <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D58" t="s">
         <v>139</v>
       </c>
       <c r="E58" s="1">
-        <v>600</v>
+        <v>648</v>
       </c>
       <c r="F58" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G58" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H58" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I58" t="s">
         <v>6</v>
       </c>
       <c r="J58" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="K58" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN600abcdfghjklmnopqrstui2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN648zi2=0 OR (i2=7 AND $2=~/lcsh|fast/)</v>
       </c>
       <c r="L58">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6216,23 +6284,23 @@
         <v>600</v>
       </c>
       <c r="F59" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G59" t="s">
         <v>4</v>
       </c>
       <c r="H59" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I59" t="s">
         <v>6</v>
       </c>
       <c r="J59" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="K59" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN600xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN600abcdfghjklmnopqrstui2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L59">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6261,26 +6329,26 @@
         <v>139</v>
       </c>
       <c r="E60" s="1">
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="F60" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G60" t="s">
         <v>4</v>
       </c>
       <c r="H60" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I60" t="s">
         <v>6</v>
       </c>
       <c r="J60" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="K60" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN610abcdfghklmnoprstui2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN600xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L60">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6312,23 +6380,23 @@
         <v>610</v>
       </c>
       <c r="F61" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G61" t="s">
         <v>4</v>
       </c>
       <c r="H61" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I61" t="s">
         <v>6</v>
       </c>
       <c r="J61" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="K61" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN610xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN610abcdfghklmnoprstui2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L61">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6357,26 +6425,26 @@
         <v>139</v>
       </c>
       <c r="E62" s="1">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F62" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G62" t="s">
         <v>4</v>
       </c>
       <c r="H62" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I62" t="s">
         <v>6</v>
       </c>
       <c r="J62" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="K62" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN611acdefghklnpqstui2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN610xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L62">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6408,23 +6476,23 @@
         <v>611</v>
       </c>
       <c r="F63" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G63" t="s">
         <v>4</v>
       </c>
       <c r="H63" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I63" t="s">
         <v>6</v>
       </c>
       <c r="J63" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="K63" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN611xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN611acdefghklnpqstui2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L63">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6453,26 +6521,26 @@
         <v>139</v>
       </c>
       <c r="E64" s="1">
-        <v>630</v>
+        <v>611</v>
       </c>
       <c r="F64" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G64" t="s">
         <v>4</v>
       </c>
       <c r="H64" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I64" t="s">
         <v>6</v>
       </c>
       <c r="J64" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="K64" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN630adfghklmnoprsti2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN611xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L64">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6504,23 +6572,23 @@
         <v>630</v>
       </c>
       <c r="F65" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G65" t="s">
         <v>4</v>
       </c>
       <c r="H65" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I65" t="s">
         <v>6</v>
       </c>
       <c r="J65" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="K65" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN630xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN630adfghklmnoprsti2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L65">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6549,16 +6617,16 @@
         <v>139</v>
       </c>
       <c r="E66" s="1">
-        <v>650</v>
+        <v>630</v>
       </c>
       <c r="F66" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G66" t="s">
         <v>4</v>
       </c>
       <c r="H66" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I66" t="s">
         <v>6</v>
@@ -6568,7 +6636,7 @@
       </c>
       <c r="K66" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN650abcdgi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN630xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L66">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6600,13 +6668,13 @@
         <v>650</v>
       </c>
       <c r="F67" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="G67" t="s">
         <v>4</v>
       </c>
       <c r="H67" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I67" t="s">
         <v>6</v>
@@ -6616,7 +6684,7 @@
       </c>
       <c r="K67" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN650xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN650abcdgi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L67">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6645,7 +6713,7 @@
         <v>139</v>
       </c>
       <c r="E68" s="1">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="F68" t="s">
         <v>41</v>
@@ -6664,7 +6732,7 @@
       </c>
       <c r="K68" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN651xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN650xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L68">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6687,32 +6755,32 @@
         <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D69" t="s">
         <v>139</v>
       </c>
       <c r="E69" s="1">
-        <v>647</v>
+        <v>651</v>
       </c>
       <c r="F69" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G69" t="s">
         <v>4</v>
       </c>
       <c r="H69" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I69" t="s">
         <v>6</v>
       </c>
       <c r="J69" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="K69" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN647acdgi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN651xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L69">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6744,13 +6812,13 @@
         <v>647</v>
       </c>
       <c r="F70" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G70" t="s">
         <v>4</v>
       </c>
       <c r="H70" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I70" t="s">
         <v>6</v>
@@ -6760,7 +6828,7 @@
       </c>
       <c r="K70" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN647xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN647acdgi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L70">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6789,7 +6857,7 @@
         <v>139</v>
       </c>
       <c r="E71" s="1">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F71" t="s">
         <v>41</v>
@@ -6804,11 +6872,11 @@
         <v>6</v>
       </c>
       <c r="J71" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K71" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN648xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN647xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L71">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6837,7 +6905,7 @@
         <v>139</v>
       </c>
       <c r="E72" s="1">
-        <v>655</v>
+        <v>648</v>
       </c>
       <c r="F72" t="s">
         <v>41</v>
@@ -6852,15 +6920,15 @@
         <v>6</v>
       </c>
       <c r="J72" t="s">
-        <v>6</v>
-      </c>
-      <c r="K72" s="8" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN655xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>18</v>
+      </c>
+      <c r="K72" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>subject_topic_lcsh_facetGEN648xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L72">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M72">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
@@ -6885,13 +6953,13 @@
         <v>139</v>
       </c>
       <c r="E73" s="1">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="F73" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="G73" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="H73" t="s">
         <v>5</v>
@@ -6900,15 +6968,15 @@
         <v>6</v>
       </c>
       <c r="J73" t="s">
-        <v>50</v>
-      </c>
-      <c r="K73" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN656ai2=7 AND $2=lcsh</v>
+        <v>6</v>
+      </c>
+      <c r="K73" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>subject_topic_lcsh_facetGEN655xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L73">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M73">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
@@ -6936,7 +7004,7 @@
         <v>656</v>
       </c>
       <c r="F74" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="G74" t="s">
         <v>34</v>
@@ -6948,11 +7016,11 @@
         <v>6</v>
       </c>
       <c r="J74" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="K74" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN656xi2=7 AND $2=lcsh</v>
+        <v>subject_topic_lcsh_facetGEN656ai2=7 AND $2=lcsh</v>
       </c>
       <c r="L74">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6981,10 +7049,10 @@
         <v>139</v>
       </c>
       <c r="E75" s="1">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F75" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="G75" t="s">
         <v>34</v>
@@ -6996,11 +7064,11 @@
         <v>6</v>
       </c>
       <c r="J75" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="K75" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN657ai2=7 AND $2=lcsh</v>
+        <v>subject_topic_lcsh_facetGEN656xi2=7 AND $2=lcsh</v>
       </c>
       <c r="L75">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -7032,7 +7100,7 @@
         <v>657</v>
       </c>
       <c r="F76" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="G76" t="s">
         <v>34</v>
@@ -7048,23 +7116,71 @@
       </c>
       <c r="K76" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>subject_topic_lcsh_facetGEN657ai2=7 AND $2=lcsh</v>
+      </c>
+      <c r="L76">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M76">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>1</v>
+      </c>
+      <c r="N76" s="8" t="str">
+        <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
+        <v>y</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>38</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" t="s">
+        <v>3</v>
+      </c>
+      <c r="D77" t="s">
+        <v>139</v>
+      </c>
+      <c r="E77" s="1">
+        <v>657</v>
+      </c>
+      <c r="F77" t="s">
+        <v>41</v>
+      </c>
+      <c r="G77" t="s">
+        <v>34</v>
+      </c>
+      <c r="H77" t="s">
+        <v>5</v>
+      </c>
+      <c r="I77" t="s">
+        <v>6</v>
+      </c>
+      <c r="J77" t="s">
+        <v>51</v>
+      </c>
+      <c r="K77" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
         <v>subject_topic_lcsh_facetGEN657xi2=7 AND $2=lcsh</v>
       </c>
-      <c r="L76">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M76">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
-      </c>
-      <c r="N76" s="8" t="str">
+      <c r="L77">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M77">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>1</v>
+      </c>
+      <c r="N77" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
         <v>y</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K2:K66">
+  <conditionalFormatting sqref="K3:K67">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
sort mappings by field
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1794" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1794" uniqueCount="376">
   <si>
     <t>subject_chronological_facet</t>
   </si>
@@ -1152,6 +1152,9 @@
   </si>
   <si>
     <t>lz</t>
+  </si>
+  <si>
+    <t>(i1=9 AND i2=2) AND $c &gt; 0</t>
   </si>
 </sst>
 </file>
@@ -1471,12 +1474,12 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="mappings" displayName="mappings" ref="A1:N104" totalsRowShown="0">
   <autoFilter ref="A1:N104"/>
-  <sortState ref="A2:N99">
-    <sortCondition ref="A2:A99"/>
-    <sortCondition ref="C2:C99"/>
-    <sortCondition ref="D2:D99"/>
-    <sortCondition ref="B2:B99"/>
-    <sortCondition ref="E2:E99"/>
+  <sortState ref="A2:N104">
+    <sortCondition ref="A2:A104"/>
+    <sortCondition ref="C2:C104"/>
+    <sortCondition ref="D2:D104"/>
+    <sortCondition ref="B2:B104"/>
+    <sortCondition ref="E2:E104"/>
   </sortState>
   <tableColumns count="14">
     <tableColumn id="1" name="field"/>
@@ -4917,8 +4920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B104" sqref="B104"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6122,7 +6125,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B26" t="s">
         <v>53</v>
@@ -6137,23 +6140,23 @@
         <v>999</v>
       </c>
       <c r="F26" t="s">
-        <v>261</v>
+        <v>372</v>
       </c>
       <c r="G26" t="s">
-        <v>158</v>
+        <v>373</v>
       </c>
       <c r="H26" t="s">
         <v>20</v>
       </c>
       <c r="I26" t="s">
-        <v>263</v>
+        <v>41</v>
       </c>
       <c r="J26" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="K26" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_call_numberUNC999qvci1=9 AND i2=1</v>
+        <v>holdings_call_numberUNC999hijkmi1=9 AND i2=3 AND $0=#{holdings_record_id} AND $2='852'</v>
       </c>
       <c r="L26" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6170,7 +6173,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>148</v>
+        <v>230</v>
       </c>
       <c r="B27" t="s">
         <v>53</v>
@@ -6185,23 +6188,23 @@
         <v>999</v>
       </c>
       <c r="F27" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
       <c r="G27" t="s">
-        <v>158</v>
+        <v>368</v>
       </c>
       <c r="H27" t="s">
-        <v>5</v>
+        <v>362</v>
       </c>
       <c r="I27" t="s">
-        <v>6</v>
+        <v>370</v>
       </c>
       <c r="J27" t="s">
-        <v>165</v>
+        <v>41</v>
       </c>
       <c r="K27" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_due_dateUNC999di1=9 AND i2=1</v>
+        <v>holdings_location_libraryUNC999bi1=9 and i2=2</v>
       </c>
       <c r="L27" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6218,7 +6221,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B28" t="s">
         <v>53</v>
@@ -6226,30 +6229,27 @@
       <c r="C28" t="s">
         <v>2</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" t="s">
         <v>54</v>
       </c>
       <c r="E28" s="1">
         <v>999</v>
       </c>
       <c r="F28" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="G28" t="s">
-        <v>158</v>
+        <v>368</v>
       </c>
       <c r="H28" t="s">
-        <v>266</v>
+        <v>5</v>
       </c>
       <c r="I28" t="s">
         <v>369</v>
       </c>
-      <c r="J28" t="s">
-        <v>6</v>
-      </c>
       <c r="K28" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_location_libraryUNC999li1=9 AND i2=1</v>
+        <v>holdings_location_shelfUNC999bi1=9 and i2=2</v>
       </c>
       <c r="L28" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6266,7 +6266,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B29" t="s">
         <v>53</v>
@@ -6274,30 +6274,30 @@
       <c r="C29" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" t="s">
         <v>54</v>
       </c>
       <c r="E29" s="1">
         <v>999</v>
       </c>
       <c r="F29" t="s">
-        <v>272</v>
+        <v>374</v>
       </c>
       <c r="G29" t="s">
-        <v>269</v>
+        <v>373</v>
       </c>
       <c r="H29" t="s">
-        <v>266</v>
+        <v>5</v>
       </c>
       <c r="I29" t="s">
-        <v>369</v>
+        <v>41</v>
       </c>
       <c r="J29" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="K29" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_location_libraryUNC999fi1=9 AND i2=4 AND NOT EXIST (tag=999 AND i1=9 and i2=1)</v>
+        <v>holdings_noteUNC999lzi1=9 AND i2=3 AND $0=#{holdings_record_id} AND $2='852'</v>
       </c>
       <c r="L29" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6314,7 +6314,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>229</v>
+        <v>153</v>
       </c>
       <c r="B30" t="s">
         <v>53</v>
@@ -6322,30 +6322,30 @@
       <c r="C30" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" t="s">
         <v>54</v>
       </c>
       <c r="E30" s="1">
         <v>999</v>
       </c>
       <c r="F30" t="s">
-        <v>171</v>
+        <v>7</v>
       </c>
       <c r="G30" t="s">
-        <v>158</v>
+        <v>375</v>
       </c>
       <c r="H30" t="s">
         <v>5</v>
       </c>
       <c r="I30" t="s">
-        <v>369</v>
+        <v>41</v>
       </c>
       <c r="J30" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="K30" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_location_shelfUNC999li1=9 AND i2=1</v>
+        <v>holdings_record_idUNC999a(i1=9 AND i2=2) AND $c &gt; 0</v>
       </c>
       <c r="L30" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6362,7 +6362,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>229</v>
+        <v>255</v>
       </c>
       <c r="B31" t="s">
         <v>53</v>
@@ -6370,30 +6370,30 @@
       <c r="C31" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" t="s">
         <v>54</v>
       </c>
       <c r="E31" s="1">
         <v>999</v>
       </c>
       <c r="F31" t="s">
-        <v>272</v>
+        <v>7</v>
       </c>
       <c r="G31" t="s">
-        <v>269</v>
+        <v>371</v>
       </c>
       <c r="H31" t="s">
         <v>5</v>
       </c>
       <c r="I31" t="s">
-        <v>369</v>
+        <v>41</v>
       </c>
       <c r="J31" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="K31" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_location_shelfUNC999fi1=9 AND i2=4 AND NOT EXIST (tag=999 AND i1=9 and i2=1)</v>
+        <v>holdings_summaryUNC999ai1=9 AND i2=3 AND $0=#{holdings_record_id} AND $2='866'</v>
       </c>
       <c r="L31" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6410,7 +6410,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>195</v>
+        <v>150</v>
       </c>
       <c r="B32" t="s">
         <v>53</v>
@@ -6418,30 +6418,30 @@
       <c r="C32" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" t="s">
         <v>54</v>
       </c>
       <c r="E32" s="1">
         <v>999</v>
       </c>
       <c r="F32" t="s">
-        <v>2</v>
+        <v>261</v>
       </c>
       <c r="G32" t="s">
         <v>158</v>
       </c>
       <c r="H32" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I32" t="s">
-        <v>6</v>
+        <v>263</v>
       </c>
       <c r="J32" t="s">
         <v>6</v>
       </c>
       <c r="K32" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_noteUNC999ni1=9 AND i2=1</v>
+        <v>item_call_numberUNC999qvci1=9 AND i2=1</v>
       </c>
       <c r="L32" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6458,7 +6458,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B33" t="s">
         <v>53</v>
@@ -6473,7 +6473,7 @@
         <v>999</v>
       </c>
       <c r="F33" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="G33" t="s">
         <v>158</v>
@@ -6485,11 +6485,11 @@
         <v>6</v>
       </c>
       <c r="J33" t="s">
-        <v>6</v>
+        <v>165</v>
       </c>
       <c r="K33" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_record_idUNC999ii1=9 AND i2=1</v>
+        <v>item_due_dateUNC999di1=9 AND i2=1</v>
       </c>
       <c r="L33" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6506,7 +6506,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>151</v>
+        <v>228</v>
       </c>
       <c r="B34" t="s">
         <v>53</v>
@@ -6514,30 +6514,30 @@
       <c r="C34" t="s">
         <v>2</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="9" t="s">
         <v>54</v>
       </c>
       <c r="E34" s="1">
         <v>999</v>
       </c>
       <c r="F34" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="G34" t="s">
-        <v>264</v>
+        <v>158</v>
       </c>
       <c r="H34" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="I34" t="s">
-        <v>6</v>
+        <v>369</v>
       </c>
       <c r="J34" t="s">
         <v>6</v>
       </c>
       <c r="K34" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_statusUNC999di1=9 AND i2=1 and $d IS NOT blank</v>
+        <v>item_location_libraryUNC999li1=9 AND i2=1</v>
       </c>
       <c r="L34" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6554,7 +6554,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>151</v>
+        <v>228</v>
       </c>
       <c r="B35" t="s">
         <v>53</v>
@@ -6562,30 +6562,30 @@
       <c r="C35" t="s">
         <v>2</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="9" t="s">
         <v>54</v>
       </c>
       <c r="E35" s="1">
         <v>999</v>
       </c>
       <c r="F35" t="s">
-        <v>189</v>
+        <v>272</v>
       </c>
       <c r="G35" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="H35" t="s">
         <v>266</v>
       </c>
       <c r="I35" t="s">
-        <v>268</v>
+        <v>369</v>
       </c>
       <c r="J35" t="s">
         <v>6</v>
       </c>
       <c r="K35" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_statusUNC999si1=9 AND i2=1 and $d IS blank</v>
+        <v>item_location_libraryUNC999fi1=9 AND i2=4 AND NOT EXIST (tag=999 AND i1=9 and i2=1)</v>
       </c>
       <c r="L35" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6602,7 +6602,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>151</v>
+        <v>229</v>
       </c>
       <c r="B36" t="s">
         <v>53</v>
@@ -6610,30 +6610,30 @@
       <c r="C36" t="s">
         <v>2</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="9" t="s">
         <v>54</v>
       </c>
       <c r="E36" s="1">
         <v>999</v>
       </c>
       <c r="F36" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="G36" t="s">
-        <v>269</v>
+        <v>158</v>
       </c>
       <c r="H36" t="s">
-        <v>270</v>
+        <v>5</v>
       </c>
       <c r="I36" t="s">
-        <v>6</v>
+        <v>369</v>
       </c>
       <c r="J36" t="s">
-        <v>271</v>
+        <v>6</v>
       </c>
       <c r="K36" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_statusUNC999ai1=9 AND i2=4 AND NOT EXIST (tag=999 AND i1=9 and i2=1)</v>
+        <v>item_location_shelfUNC999li1=9 AND i2=1</v>
       </c>
       <c r="L36" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6650,46 +6650,46 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>0</v>
+        <v>229</v>
       </c>
       <c r="B37" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C37" t="s">
         <v>2</v>
       </c>
-      <c r="D37" t="s">
-        <v>139</v>
+      <c r="D37" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="E37" s="1">
-        <v>600</v>
+        <v>999</v>
       </c>
       <c r="F37" t="s">
-        <v>3</v>
+        <v>272</v>
       </c>
       <c r="G37" t="s">
-        <v>4</v>
+        <v>269</v>
       </c>
       <c r="H37" t="s">
         <v>5</v>
       </c>
       <c r="I37" t="s">
-        <v>6</v>
+        <v>369</v>
       </c>
       <c r="J37" t="s">
         <v>6</v>
       </c>
-      <c r="K37" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN600yi2=0 OR (i2=7 AND $2=lcsh)</v>
-      </c>
-      <c r="L37">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M37">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+      <c r="K37" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>item_location_shelfUNC999fi1=9 AND i2=4 AND NOT EXIST (tag=999 AND i1=9 and i2=1)</v>
+      </c>
+      <c r="L37" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M37" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
       </c>
       <c r="N37" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -6698,25 +6698,25 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>0</v>
+        <v>195</v>
       </c>
       <c r="B38" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C38" t="s">
         <v>2</v>
       </c>
-      <c r="D38" t="s">
-        <v>139</v>
+      <c r="D38" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="E38" s="1">
-        <v>610</v>
+        <v>999</v>
       </c>
       <c r="F38" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G38" t="s">
-        <v>4</v>
+        <v>158</v>
       </c>
       <c r="H38" t="s">
         <v>5</v>
@@ -6727,17 +6727,17 @@
       <c r="J38" t="s">
         <v>6</v>
       </c>
-      <c r="K38" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN610yi2=0 OR (i2=7 AND $2=lcsh)</v>
-      </c>
-      <c r="L38">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M38">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+      <c r="K38" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>item_noteUNC999ni1=9 AND i2=1</v>
+      </c>
+      <c r="L38" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M38" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
       </c>
       <c r="N38" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -6746,25 +6746,25 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>0</v>
+        <v>149</v>
       </c>
       <c r="B39" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C39" t="s">
         <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>139</v>
+        <v>54</v>
       </c>
       <c r="E39" s="1">
-        <v>611</v>
+        <v>999</v>
       </c>
       <c r="F39" t="s">
-        <v>3</v>
+        <v>157</v>
       </c>
       <c r="G39" t="s">
-        <v>4</v>
+        <v>158</v>
       </c>
       <c r="H39" t="s">
         <v>5</v>
@@ -6775,17 +6775,17 @@
       <c r="J39" t="s">
         <v>6</v>
       </c>
-      <c r="K39" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN611yi2=0 OR (i2=7 AND $2=lcsh)</v>
-      </c>
-      <c r="L39">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M39">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+      <c r="K39" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>item_record_idUNC999ii1=9 AND i2=1</v>
+      </c>
+      <c r="L39" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M39" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
       </c>
       <c r="N39" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -6794,28 +6794,28 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>0</v>
+        <v>151</v>
       </c>
       <c r="B40" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C40" t="s">
         <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>139</v>
+        <v>54</v>
       </c>
       <c r="E40" s="1">
-        <v>630</v>
+        <v>999</v>
       </c>
       <c r="F40" t="s">
-        <v>3</v>
+        <v>164</v>
       </c>
       <c r="G40" t="s">
-        <v>4</v>
+        <v>264</v>
       </c>
       <c r="H40" t="s">
-        <v>5</v>
+        <v>265</v>
       </c>
       <c r="I40" t="s">
         <v>6</v>
@@ -6823,17 +6823,17 @@
       <c r="J40" t="s">
         <v>6</v>
       </c>
-      <c r="K40" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN630yi2=0 OR (i2=7 AND $2=lcsh)</v>
-      </c>
-      <c r="L40">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M40">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+      <c r="K40" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>item_statusUNC999di1=9 AND i2=1 and $d IS NOT blank</v>
+      </c>
+      <c r="L40" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M40" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
       </c>
       <c r="N40" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -6842,46 +6842,46 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>0</v>
+        <v>151</v>
       </c>
       <c r="B41" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C41" t="s">
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>139</v>
+        <v>54</v>
       </c>
       <c r="E41" s="1">
-        <v>650</v>
+        <v>999</v>
       </c>
       <c r="F41" t="s">
-        <v>3</v>
+        <v>189</v>
       </c>
       <c r="G41" t="s">
-        <v>4</v>
+        <v>267</v>
       </c>
       <c r="H41" t="s">
-        <v>5</v>
+        <v>266</v>
       </c>
       <c r="I41" t="s">
-        <v>6</v>
+        <v>268</v>
       </c>
       <c r="J41" t="s">
         <v>6</v>
       </c>
-      <c r="K41" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN650yi2=0 OR (i2=7 AND $2=lcsh)</v>
-      </c>
-      <c r="L41">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M41">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+      <c r="K41" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>item_statusUNC999si1=9 AND i2=1 and $d IS blank</v>
+      </c>
+      <c r="L41" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M41" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
       </c>
       <c r="N41" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -6890,46 +6890,46 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>0</v>
+        <v>151</v>
       </c>
       <c r="B42" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C42" t="s">
         <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>139</v>
+        <v>54</v>
       </c>
       <c r="E42" s="1">
-        <v>651</v>
+        <v>999</v>
       </c>
       <c r="F42" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G42" t="s">
-        <v>4</v>
+        <v>269</v>
       </c>
       <c r="H42" t="s">
-        <v>5</v>
+        <v>270</v>
       </c>
       <c r="I42" t="s">
         <v>6</v>
       </c>
       <c r="J42" t="s">
-        <v>6</v>
-      </c>
-      <c r="K42" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN651yi2=0 OR (i2=7 AND $2=lcsh)</v>
-      </c>
-      <c r="L42">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M42">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+        <v>271</v>
+      </c>
+      <c r="K42" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>item_statusUNC999ai1=9 AND i2=4 AND NOT EXIST (tag=999 AND i1=9 and i2=1)</v>
+      </c>
+      <c r="L42" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M42" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
       </c>
       <c r="N42" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -6950,7 +6950,7 @@
         <v>139</v>
       </c>
       <c r="E43" s="1">
-        <v>655</v>
+        <v>600</v>
       </c>
       <c r="F43" t="s">
         <v>3</v>
@@ -6969,7 +6969,7 @@
       </c>
       <c r="K43" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN655yi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_chronological_facetGEN600yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L43">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6992,19 +6992,19 @@
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D44" t="s">
         <v>139</v>
       </c>
       <c r="E44" s="1">
-        <v>648</v>
+        <v>610</v>
       </c>
       <c r="F44" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G44" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H44" t="s">
         <v>5</v>
@@ -7013,11 +7013,11 @@
         <v>6</v>
       </c>
       <c r="J44" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K44" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN648ai2=0 OR (i2=7 AND $2=~/lcsh|fast/)</v>
+        <v>subject_chronological_facetGEN610yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L44">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -7034,7 +7034,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B45" t="s">
         <v>1</v>
@@ -7046,26 +7046,26 @@
         <v>139</v>
       </c>
       <c r="E45" s="1">
-        <v>6</v>
-      </c>
-      <c r="F45">
-        <v>16</v>
+        <v>611</v>
+      </c>
+      <c r="F45" t="s">
+        <v>3</v>
       </c>
       <c r="G45" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H45" t="s">
         <v>5</v>
       </c>
       <c r="I45" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J45" t="s">
         <v>6</v>
       </c>
       <c r="K45" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN616LDR/06 = a AND LDR/07 =~ [acdm] AND 006/00 =~ [at]</v>
+        <v>subject_chronological_facetGEN611yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L45">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -7073,7 +7073,7 @@
       </c>
       <c r="M45">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N45" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -7082,7 +7082,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B46" t="s">
         <v>1</v>
@@ -7094,26 +7094,26 @@
         <v>139</v>
       </c>
       <c r="E46" s="1">
-        <v>6</v>
-      </c>
-      <c r="F46">
-        <v>17</v>
+        <v>630</v>
+      </c>
+      <c r="F46" t="s">
+        <v>3</v>
       </c>
       <c r="G46" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H46" t="s">
         <v>5</v>
       </c>
       <c r="I46" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="J46" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="K46" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN617LDR/06 = a AND LDR/07 =~ [acdm] AND 006/00 =~ [at]</v>
+        <v>subject_chronological_facetGEN630yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L46">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -7121,7 +7121,7 @@
       </c>
       <c r="M46">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N46" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -7130,7 +7130,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B47" t="s">
         <v>1</v>
@@ -7142,26 +7142,26 @@
         <v>139</v>
       </c>
       <c r="E47" s="1">
-        <v>8</v>
-      </c>
-      <c r="F47">
-        <v>33</v>
+        <v>650</v>
+      </c>
+      <c r="F47" t="s">
+        <v>3</v>
       </c>
       <c r="G47" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="H47" t="s">
         <v>5</v>
       </c>
       <c r="I47" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J47" t="s">
         <v>6</v>
       </c>
       <c r="K47" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN833LDR/06 = a AND LDR/07 =~ [acdm]</v>
+        <v>subject_chronological_facetGEN650yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L47">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -7169,7 +7169,7 @@
       </c>
       <c r="M47">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N47" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -7178,7 +7178,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B48" t="s">
         <v>1</v>
@@ -7190,26 +7190,26 @@
         <v>139</v>
       </c>
       <c r="E48" s="1">
-        <v>8</v>
-      </c>
-      <c r="F48">
-        <v>34</v>
+        <v>651</v>
+      </c>
+      <c r="F48" t="s">
+        <v>3</v>
       </c>
       <c r="G48" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="H48" t="s">
         <v>5</v>
       </c>
       <c r="I48" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="J48" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="K48" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN834LDR/06 = a AND LDR/07 =~ [acdm]</v>
+        <v>subject_chronological_facetGEN651yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L48">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -7217,7 +7217,7 @@
       </c>
       <c r="M48">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N48" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -7226,7 +7226,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B49" t="s">
         <v>1</v>
@@ -7238,10 +7238,10 @@
         <v>139</v>
       </c>
       <c r="E49" s="1">
-        <v>600</v>
+        <v>655</v>
       </c>
       <c r="F49" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="G49" t="s">
         <v>4</v>
@@ -7257,7 +7257,7 @@
       </c>
       <c r="K49" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN600vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_chronological_facetGEN655yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L49">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -7265,7 +7265,7 @@
       </c>
       <c r="M49">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N49" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -7274,25 +7274,25 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B50" t="s">
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D50" t="s">
         <v>139</v>
       </c>
       <c r="E50" s="1">
-        <v>610</v>
+        <v>648</v>
       </c>
       <c r="F50" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G50" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H50" t="s">
         <v>5</v>
@@ -7301,11 +7301,11 @@
         <v>6</v>
       </c>
       <c r="J50" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K50" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN610vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_chronological_facetGEN648ai2=0 OR (i2=7 AND $2=~/lcsh|fast/)</v>
       </c>
       <c r="L50">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -7313,7 +7313,7 @@
       </c>
       <c r="M50">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N50" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -7334,26 +7334,26 @@
         <v>139</v>
       </c>
       <c r="E51" s="1">
-        <v>611</v>
-      </c>
-      <c r="F51" t="s">
+        <v>6</v>
+      </c>
+      <c r="F51">
         <v>16</v>
       </c>
       <c r="G51" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="H51" t="s">
         <v>5</v>
       </c>
       <c r="I51" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="J51" t="s">
         <v>6</v>
       </c>
       <c r="K51" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN611vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN616LDR/06 = a AND LDR/07 =~ [acdm] AND 006/00 =~ [at]</v>
       </c>
       <c r="L51">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -7382,26 +7382,26 @@
         <v>139</v>
       </c>
       <c r="E52" s="1">
-        <v>630</v>
-      </c>
-      <c r="F52" t="s">
-        <v>16</v>
+        <v>6</v>
+      </c>
+      <c r="F52">
+        <v>17</v>
       </c>
       <c r="G52" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="H52" t="s">
         <v>5</v>
       </c>
       <c r="I52" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="J52" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="K52" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN630vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN617LDR/06 = a AND LDR/07 =~ [acdm] AND 006/00 =~ [at]</v>
       </c>
       <c r="L52">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -7430,26 +7430,26 @@
         <v>139</v>
       </c>
       <c r="E53" s="1">
-        <v>650</v>
-      </c>
-      <c r="F53" t="s">
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="F53">
+        <v>33</v>
       </c>
       <c r="G53" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="H53" t="s">
         <v>5</v>
       </c>
       <c r="I53" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="J53" t="s">
         <v>6</v>
       </c>
       <c r="K53" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN650vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN833LDR/06 = a AND LDR/07 =~ [acdm]</v>
       </c>
       <c r="L53">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -7478,26 +7478,26 @@
         <v>139</v>
       </c>
       <c r="E54" s="1">
-        <v>651</v>
-      </c>
-      <c r="F54" t="s">
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="F54">
+        <v>34</v>
       </c>
       <c r="G54" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="H54" t="s">
         <v>5</v>
       </c>
       <c r="I54" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="J54" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="K54" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN651vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN834LDR/06 = a AND LDR/07 =~ [acdm]</v>
       </c>
       <c r="L54">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -7526,7 +7526,7 @@
         <v>139</v>
       </c>
       <c r="E55" s="1">
-        <v>655</v>
+        <v>600</v>
       </c>
       <c r="F55" t="s">
         <v>16</v>
@@ -7545,7 +7545,7 @@
       </c>
       <c r="K55" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN600vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L55">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -7568,13 +7568,13 @@
         <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D56" t="s">
         <v>139</v>
       </c>
       <c r="E56" s="1">
-        <v>647</v>
+        <v>610</v>
       </c>
       <c r="F56" t="s">
         <v>16</v>
@@ -7589,11 +7589,11 @@
         <v>6</v>
       </c>
       <c r="J56" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="K56" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN647vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN610vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L56">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -7616,13 +7616,13 @@
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D57" t="s">
         <v>139</v>
       </c>
       <c r="E57" s="1">
-        <v>648</v>
+        <v>611</v>
       </c>
       <c r="F57" t="s">
         <v>16</v>
@@ -7637,11 +7637,11 @@
         <v>6</v>
       </c>
       <c r="J57" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="K57" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN648vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN611vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L57">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -7664,32 +7664,32 @@
         <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D58" t="s">
         <v>139</v>
       </c>
       <c r="E58" s="1">
-        <v>655</v>
+        <v>630</v>
       </c>
       <c r="F58" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G58" t="s">
         <v>4</v>
       </c>
       <c r="H58" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I58" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="J58" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="K58" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655axi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN630vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L58">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -7712,32 +7712,32 @@
         <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D59" t="s">
         <v>139</v>
       </c>
       <c r="E59" s="1">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="F59" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G59" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="H59" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I59" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="J59" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="K59" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655axi2=7 AND $2=lcgft</v>
+        <v>subject_genre_facetGEN650vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L59">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -7760,32 +7760,32 @@
         <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D60" t="s">
         <v>139</v>
       </c>
       <c r="E60" s="1">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="F60" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G60" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="H60" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I60" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="J60" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="K60" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655axi2=7 AND $2=rbbin</v>
+        <v>subject_genre_facetGEN651vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L60">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -7808,7 +7808,7 @@
         <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D61" t="s">
         <v>139</v>
@@ -7817,23 +7817,23 @@
         <v>655</v>
       </c>
       <c r="F61" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G61" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="H61" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I61" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="J61" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="K61" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655axi2=7 AND $2=rbgenr</v>
+        <v>subject_genre_facetGEN655vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L61">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -7862,26 +7862,26 @@
         <v>139</v>
       </c>
       <c r="E62" s="1">
-        <v>655</v>
+        <v>647</v>
       </c>
       <c r="F62" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G62" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="H62" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I62" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="J62" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="K62" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655axi2=7 AND $2=rbprov</v>
+        <v>subject_genre_facetGEN647vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L62">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -7910,13 +7910,13 @@
         <v>139</v>
       </c>
       <c r="E63" s="1">
-        <v>655</v>
+        <v>648</v>
       </c>
       <c r="F63" t="s">
         <v>16</v>
       </c>
       <c r="G63" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="H63" t="s">
         <v>5</v>
@@ -7925,11 +7925,11 @@
         <v>6</v>
       </c>
       <c r="J63" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="K63" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655vi2=7 AND $2=lcgft</v>
+        <v>subject_genre_facetGEN648vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L63">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -7961,23 +7961,23 @@
         <v>655</v>
       </c>
       <c r="F64" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G64" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="H64" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I64" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="J64" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="K64" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655vi2=7 AND $2=rbbin</v>
+        <v>subject_genre_facetGEN655axi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L64">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8009,23 +8009,23 @@
         <v>655</v>
       </c>
       <c r="F65" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G65" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="H65" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I65" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="J65" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="K65" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655vi2=7 AND $2=rbgenr</v>
+        <v>subject_genre_facetGEN655axi2=7 AND $2=lcgft</v>
       </c>
       <c r="L65">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8057,23 +8057,23 @@
         <v>655</v>
       </c>
       <c r="F66" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G66" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H66" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I66" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="J66" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="K66" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655vi2=7 AND $2=rbprov</v>
+        <v>subject_genre_facetGEN655axi2=7 AND $2=rbbin</v>
       </c>
       <c r="L66">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8102,26 +8102,26 @@
         <v>139</v>
       </c>
       <c r="E67" s="1">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="F67" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="G67" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H67" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I67" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="J67" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="K67" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN656kvi2=7 AND $2=lcsh</v>
+        <v>subject_genre_facetGEN655axi2=7 AND $2=rbgenr</v>
       </c>
       <c r="L67">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8150,26 +8150,26 @@
         <v>139</v>
       </c>
       <c r="E68" s="1">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="F68" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G68" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H68" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I68" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="J68" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K68" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN657vi2=7 AND $2=lcsh</v>
+        <v>subject_genre_facetGEN655axi2=7 AND $2=rbprov</v>
       </c>
       <c r="L68">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8186,25 +8186,25 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B69" t="s">
         <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D69" t="s">
         <v>139</v>
       </c>
       <c r="E69" s="1">
-        <v>600</v>
+        <v>655</v>
       </c>
       <c r="F69" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="G69" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="H69" t="s">
         <v>5</v>
@@ -8213,11 +8213,11 @@
         <v>6</v>
       </c>
       <c r="J69" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="K69" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN600zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN655vi2=7 AND $2=lcgft</v>
       </c>
       <c r="L69">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8225,7 +8225,7 @@
       </c>
       <c r="M69">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N69" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -8234,25 +8234,25 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B70" t="s">
         <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D70" t="s">
         <v>139</v>
       </c>
       <c r="E70" s="1">
-        <v>610</v>
+        <v>655</v>
       </c>
       <c r="F70" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="G70" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="H70" t="s">
         <v>5</v>
@@ -8261,11 +8261,11 @@
         <v>6</v>
       </c>
       <c r="J70" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="K70" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN610zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN655vi2=7 AND $2=rbbin</v>
       </c>
       <c r="L70">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8273,7 +8273,7 @@
       </c>
       <c r="M70">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N70" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -8282,25 +8282,25 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B71" t="s">
         <v>1</v>
       </c>
       <c r="C71" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D71" t="s">
         <v>139</v>
       </c>
       <c r="E71" s="1">
-        <v>611</v>
+        <v>655</v>
       </c>
       <c r="F71" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="G71" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="H71" t="s">
         <v>5</v>
@@ -8309,11 +8309,11 @@
         <v>6</v>
       </c>
       <c r="J71" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K71" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN611zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN655vi2=7 AND $2=rbgenr</v>
       </c>
       <c r="L71">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8321,7 +8321,7 @@
       </c>
       <c r="M71">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N71" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -8330,25 +8330,25 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B72" t="s">
         <v>1</v>
       </c>
       <c r="C72" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D72" t="s">
         <v>139</v>
       </c>
       <c r="E72" s="1">
-        <v>630</v>
+        <v>655</v>
       </c>
       <c r="F72" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="G72" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="H72" t="s">
         <v>5</v>
@@ -8357,11 +8357,11 @@
         <v>6</v>
       </c>
       <c r="J72" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="K72" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN630zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN655vi2=7 AND $2=rbprov</v>
       </c>
       <c r="L72">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8369,7 +8369,7 @@
       </c>
       <c r="M72">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N72" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -8378,25 +8378,25 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B73" t="s">
         <v>1</v>
       </c>
       <c r="C73" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D73" t="s">
         <v>139</v>
       </c>
       <c r="E73" s="1">
-        <v>650</v>
+        <v>656</v>
       </c>
       <c r="F73" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G73" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="H73" t="s">
         <v>5</v>
@@ -8405,11 +8405,11 @@
         <v>6</v>
       </c>
       <c r="J73" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="K73" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN650zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN656kvi2=7 AND $2=lcsh</v>
       </c>
       <c r="L73">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8417,7 +8417,7 @@
       </c>
       <c r="M73">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N73" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -8426,25 +8426,25 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B74" t="s">
         <v>1</v>
       </c>
       <c r="C74" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D74" t="s">
         <v>139</v>
       </c>
       <c r="E74" s="1">
-        <v>651</v>
+        <v>657</v>
       </c>
       <c r="F74" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="G74" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="H74" t="s">
         <v>5</v>
@@ -8453,11 +8453,11 @@
         <v>6</v>
       </c>
       <c r="J74" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="K74" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN651zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN657vi2=7 AND $2=lcsh</v>
       </c>
       <c r="L74">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8465,7 +8465,7 @@
       </c>
       <c r="M74">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N74" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -8486,7 +8486,7 @@
         <v>139</v>
       </c>
       <c r="E75" s="1">
-        <v>655</v>
+        <v>600</v>
       </c>
       <c r="F75" t="s">
         <v>37</v>
@@ -8505,7 +8505,7 @@
       </c>
       <c r="K75" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN655zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN600zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L75">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8528,19 +8528,19 @@
         <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D76" t="s">
         <v>139</v>
       </c>
       <c r="E76" s="1">
-        <v>648</v>
+        <v>610</v>
       </c>
       <c r="F76" t="s">
         <v>37</v>
       </c>
       <c r="G76" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H76" t="s">
         <v>5</v>
@@ -8549,11 +8549,11 @@
         <v>6</v>
       </c>
       <c r="J76" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="K76" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN648zi2=0 OR (i2=7 AND $2=~/lcsh|fast/)</v>
+        <v>subject_geographic_facetGEN610zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L76">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8570,7 +8570,7 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B77" t="s">
         <v>1</v>
@@ -8582,26 +8582,26 @@
         <v>139</v>
       </c>
       <c r="E77" s="1">
-        <v>600</v>
+        <v>611</v>
       </c>
       <c r="F77" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G77" t="s">
         <v>4</v>
       </c>
       <c r="H77" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I77" t="s">
         <v>6</v>
       </c>
       <c r="J77" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="K77" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN600abcdfghjklmnopqrstui2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN611zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L77">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8618,7 +8618,7 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B78" t="s">
         <v>1</v>
@@ -8630,10 +8630,10 @@
         <v>139</v>
       </c>
       <c r="E78" s="1">
-        <v>600</v>
+        <v>630</v>
       </c>
       <c r="F78" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G78" t="s">
         <v>4</v>
@@ -8649,7 +8649,7 @@
       </c>
       <c r="K78" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN600xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN630zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L78">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8666,7 +8666,7 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B79" t="s">
         <v>1</v>
@@ -8678,26 +8678,26 @@
         <v>139</v>
       </c>
       <c r="E79" s="1">
-        <v>610</v>
+        <v>650</v>
       </c>
       <c r="F79" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G79" t="s">
         <v>4</v>
       </c>
       <c r="H79" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I79" t="s">
         <v>6</v>
       </c>
       <c r="J79" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="K79" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN610abcdfghklmnoprstui2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN650zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L79">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8714,7 +8714,7 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B80" t="s">
         <v>1</v>
@@ -8726,10 +8726,10 @@
         <v>139</v>
       </c>
       <c r="E80" s="1">
-        <v>610</v>
+        <v>651</v>
       </c>
       <c r="F80" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G80" t="s">
         <v>4</v>
@@ -8745,7 +8745,7 @@
       </c>
       <c r="K80" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN610xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN651zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L80">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8762,7 +8762,7 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B81" t="s">
         <v>1</v>
@@ -8774,26 +8774,26 @@
         <v>139</v>
       </c>
       <c r="E81" s="1">
-        <v>611</v>
+        <v>655</v>
       </c>
       <c r="F81" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G81" t="s">
         <v>4</v>
       </c>
       <c r="H81" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I81" t="s">
         <v>6</v>
       </c>
       <c r="J81" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="K81" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN611acdefghklnpqstui2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN655zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L81">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8810,25 +8810,25 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B82" t="s">
         <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D82" t="s">
         <v>139</v>
       </c>
       <c r="E82" s="1">
-        <v>611</v>
+        <v>648</v>
       </c>
       <c r="F82" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G82" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H82" t="s">
         <v>5</v>
@@ -8837,11 +8837,11 @@
         <v>6</v>
       </c>
       <c r="J82" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="K82" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN611xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN648zi2=0 OR (i2=7 AND $2=~/lcsh|fast/)</v>
       </c>
       <c r="L82">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8870,10 +8870,10 @@
         <v>139</v>
       </c>
       <c r="E83" s="1">
-        <v>630</v>
+        <v>600</v>
       </c>
       <c r="F83" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G83" t="s">
         <v>4</v>
@@ -8885,11 +8885,11 @@
         <v>6</v>
       </c>
       <c r="J83" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="K83" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN630adfghklmnoprsti2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN600abcdfghjklmnopqrstui2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L83">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8918,7 +8918,7 @@
         <v>139</v>
       </c>
       <c r="E84" s="1">
-        <v>630</v>
+        <v>600</v>
       </c>
       <c r="F84" t="s">
         <v>41</v>
@@ -8937,7 +8937,7 @@
       </c>
       <c r="K84" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN630xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN600xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L84">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8966,10 +8966,10 @@
         <v>139</v>
       </c>
       <c r="E85" s="1">
-        <v>650</v>
+        <v>610</v>
       </c>
       <c r="F85" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G85" t="s">
         <v>4</v>
@@ -8981,11 +8981,11 @@
         <v>6</v>
       </c>
       <c r="J85" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="K85" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN650abcdgi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN610abcdfghklmnoprstui2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L85">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9014,7 +9014,7 @@
         <v>139</v>
       </c>
       <c r="E86" s="1">
-        <v>650</v>
+        <v>610</v>
       </c>
       <c r="F86" t="s">
         <v>41</v>
@@ -9033,7 +9033,7 @@
       </c>
       <c r="K86" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN650xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN610xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L86">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9062,26 +9062,26 @@
         <v>139</v>
       </c>
       <c r="E87" s="1">
-        <v>651</v>
+        <v>611</v>
       </c>
       <c r="F87" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G87" t="s">
         <v>4</v>
       </c>
       <c r="H87" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I87" t="s">
         <v>6</v>
       </c>
       <c r="J87" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="K87" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN651xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN611acdefghklnpqstui2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L87">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9104,32 +9104,32 @@
         <v>1</v>
       </c>
       <c r="C88" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D88" t="s">
         <v>139</v>
       </c>
       <c r="E88" s="1">
-        <v>647</v>
+        <v>611</v>
       </c>
       <c r="F88" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G88" t="s">
         <v>4</v>
       </c>
       <c r="H88" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I88" t="s">
         <v>6</v>
       </c>
       <c r="J88" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="K88" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN647acdgi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN611xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L88">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9152,32 +9152,32 @@
         <v>1</v>
       </c>
       <c r="C89" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D89" t="s">
         <v>139</v>
       </c>
       <c r="E89" s="1">
-        <v>647</v>
+        <v>630</v>
       </c>
       <c r="F89" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G89" t="s">
         <v>4</v>
       </c>
       <c r="H89" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I89" t="s">
         <v>6</v>
       </c>
       <c r="J89" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="K89" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN647xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN630adfghklmnoprsti2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L89">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9200,13 +9200,13 @@
         <v>1</v>
       </c>
       <c r="C90" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D90" t="s">
         <v>139</v>
       </c>
       <c r="E90" s="1">
-        <v>648</v>
+        <v>630</v>
       </c>
       <c r="F90" t="s">
         <v>41</v>
@@ -9221,11 +9221,11 @@
         <v>6</v>
       </c>
       <c r="J90" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="K90" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN648xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN630xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L90">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9248,22 +9248,22 @@
         <v>1</v>
       </c>
       <c r="C91" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D91" t="s">
         <v>139</v>
       </c>
       <c r="E91" s="1">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="F91" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="G91" t="s">
         <v>4</v>
       </c>
       <c r="H91" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I91" t="s">
         <v>6</v>
@@ -9271,13 +9271,13 @@
       <c r="J91" t="s">
         <v>6</v>
       </c>
-      <c r="K91" s="8" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN655xi2=0 OR (i2=7 AND $2=lcsh)</v>
+      <c r="K91" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>subject_topic_lcsh_facetGEN650abcdgi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L91">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M91">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
@@ -9296,19 +9296,19 @@
         <v>1</v>
       </c>
       <c r="C92" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D92" t="s">
         <v>139</v>
       </c>
       <c r="E92" s="1">
-        <v>656</v>
+        <v>650</v>
       </c>
       <c r="F92" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="G92" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="H92" t="s">
         <v>5</v>
@@ -9317,11 +9317,11 @@
         <v>6</v>
       </c>
       <c r="J92" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="K92" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN656ai2=7 AND $2=lcsh</v>
+        <v>subject_topic_lcsh_facetGEN650xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L92">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9344,19 +9344,19 @@
         <v>1</v>
       </c>
       <c r="C93" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D93" t="s">
         <v>139</v>
       </c>
       <c r="E93" s="1">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="F93" t="s">
         <v>41</v>
       </c>
       <c r="G93" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="H93" t="s">
         <v>5</v>
@@ -9365,11 +9365,11 @@
         <v>6</v>
       </c>
       <c r="J93" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="K93" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN656xi2=7 AND $2=lcsh</v>
+        <v>subject_topic_lcsh_facetGEN651xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L93">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9398,26 +9398,26 @@
         <v>139</v>
       </c>
       <c r="E94" s="1">
-        <v>657</v>
+        <v>647</v>
       </c>
       <c r="F94" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="G94" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="H94" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I94" t="s">
         <v>6</v>
       </c>
       <c r="J94" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="K94" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN657ai2=7 AND $2=lcsh</v>
+        <v>subject_topic_lcsh_facetGEN647acdgi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L94">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9446,13 +9446,13 @@
         <v>139</v>
       </c>
       <c r="E95" s="1">
-        <v>657</v>
+        <v>647</v>
       </c>
       <c r="F95" t="s">
         <v>41</v>
       </c>
       <c r="G95" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="H95" t="s">
         <v>5</v>
@@ -9461,11 +9461,11 @@
         <v>6</v>
       </c>
       <c r="J95" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="K95" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN657xi2=7 AND $2=lcsh</v>
+        <v>subject_topic_lcsh_facetGEN647xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L95">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9482,46 +9482,46 @@
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>321</v>
+        <v>38</v>
       </c>
       <c r="B96" t="s">
         <v>1</v>
       </c>
       <c r="C96" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D96" t="s">
         <v>139</v>
       </c>
       <c r="E96" s="1">
-        <v>100</v>
+        <v>648</v>
       </c>
       <c r="F96" t="s">
-        <v>330</v>
+        <v>41</v>
       </c>
       <c r="G96" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H96" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I96" t="s">
-        <v>335</v>
+        <v>6</v>
       </c>
       <c r="J96" t="s">
-        <v>328</v>
-      </c>
-      <c r="K96" s="8" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>uniform_titleGEN100f(g)klnpt.</v>
-      </c>
-      <c r="L96" s="8">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M96" s="8">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="K96" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>subject_topic_lcsh_facetGEN648xi2=0 OR (i2=7 AND $2=lcsh)</v>
+      </c>
+      <c r="L96">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M96">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>1</v>
       </c>
       <c r="N96" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -9530,46 +9530,46 @@
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>321</v>
+        <v>38</v>
       </c>
       <c r="B97" t="s">
         <v>1</v>
       </c>
       <c r="C97" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D97" t="s">
         <v>139</v>
       </c>
       <c r="E97" s="1">
-        <v>110</v>
+        <v>655</v>
       </c>
       <c r="F97" t="s">
-        <v>334</v>
+        <v>41</v>
       </c>
       <c r="G97" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H97" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I97" t="s">
-        <v>336</v>
+        <v>6</v>
       </c>
       <c r="J97" t="s">
-        <v>328</v>
+        <v>6</v>
       </c>
       <c r="K97" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>uniform_titleGEN110f(g)kl(n)pt.</v>
-      </c>
-      <c r="L97" s="8">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M97" s="8">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>0</v>
+        <v>subject_topic_lcsh_facetGEN655xi2=0 OR (i2=7 AND $2=lcsh)</v>
+      </c>
+      <c r="L97">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>1</v>
+      </c>
+      <c r="M97">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>1</v>
       </c>
       <c r="N97" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -9578,46 +9578,46 @@
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>321</v>
+        <v>38</v>
       </c>
       <c r="B98" t="s">
         <v>1</v>
       </c>
       <c r="C98" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D98" t="s">
         <v>139</v>
       </c>
       <c r="E98" s="1">
-        <v>111</v>
+        <v>656</v>
       </c>
       <c r="F98" t="s">
-        <v>334</v>
+        <v>7</v>
       </c>
       <c r="G98" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="H98" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I98" t="s">
-        <v>336</v>
+        <v>6</v>
       </c>
       <c r="J98" t="s">
-        <v>328</v>
-      </c>
-      <c r="K98" s="8" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>uniform_titleGEN111f(g)kl(n)pt.</v>
-      </c>
-      <c r="L98" s="8">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M98" s="8">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>0</v>
+        <v>50</v>
+      </c>
+      <c r="K98" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>subject_topic_lcsh_facetGEN656ai2=7 AND $2=lcsh</v>
+      </c>
+      <c r="L98">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M98">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>1</v>
       </c>
       <c r="N98" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -9626,46 +9626,46 @@
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>255</v>
+        <v>38</v>
       </c>
       <c r="B99" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="C99" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D99" t="s">
-        <v>54</v>
+        <v>139</v>
       </c>
       <c r="E99" s="1">
-        <v>999</v>
+        <v>656</v>
       </c>
       <c r="F99" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="G99" t="s">
-        <v>371</v>
+        <v>34</v>
       </c>
       <c r="H99" t="s">
         <v>5</v>
       </c>
       <c r="I99" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="J99" t="s">
-        <v>41</v>
-      </c>
-      <c r="K99" s="8" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>holdings_summaryUNC999ai1=9 AND i2=3 AND $0=#{holdings_record_id} AND $2='866'</v>
-      </c>
-      <c r="L99" s="8">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M99" s="8">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>0</v>
+        <v>35</v>
+      </c>
+      <c r="K99" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>subject_topic_lcsh_facetGEN656xi2=7 AND $2=lcsh</v>
+      </c>
+      <c r="L99">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M99">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>1</v>
       </c>
       <c r="N99" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -9674,46 +9674,46 @@
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>230</v>
+        <v>38</v>
       </c>
       <c r="B100" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="C100" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D100" t="s">
-        <v>54</v>
+        <v>139</v>
       </c>
       <c r="E100" s="1">
-        <v>999</v>
+        <v>657</v>
       </c>
       <c r="F100" t="s">
-        <v>184</v>
+        <v>7</v>
       </c>
       <c r="G100" t="s">
-        <v>368</v>
+        <v>34</v>
       </c>
       <c r="H100" t="s">
-        <v>362</v>
+        <v>5</v>
       </c>
       <c r="I100" t="s">
-        <v>370</v>
+        <v>6</v>
       </c>
       <c r="J100" t="s">
-        <v>41</v>
-      </c>
-      <c r="K100" s="8" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>holdings_location_libraryUNC999bi1=9 and i2=2</v>
-      </c>
-      <c r="L100" s="8">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M100" s="8">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>0</v>
+        <v>51</v>
+      </c>
+      <c r="K100" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>subject_topic_lcsh_facetGEN657ai2=7 AND $2=lcsh</v>
+      </c>
+      <c r="L100">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M100">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>1</v>
       </c>
       <c r="N100" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -9722,43 +9722,46 @@
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>231</v>
+        <v>38</v>
       </c>
       <c r="B101" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="C101" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D101" t="s">
-        <v>54</v>
+        <v>139</v>
       </c>
       <c r="E101" s="1">
-        <v>999</v>
+        <v>657</v>
       </c>
       <c r="F101" t="s">
-        <v>184</v>
+        <v>41</v>
       </c>
       <c r="G101" t="s">
-        <v>368</v>
+        <v>34</v>
       </c>
       <c r="H101" t="s">
         <v>5</v>
       </c>
       <c r="I101" t="s">
-        <v>369</v>
-      </c>
-      <c r="K101" s="8" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>holdings_location_shelfUNC999bi1=9 and i2=2</v>
-      </c>
-      <c r="L101" s="8">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M101" s="8">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="J101" t="s">
+        <v>51</v>
+      </c>
+      <c r="K101" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>subject_topic_lcsh_facetGEN657xi2=7 AND $2=lcsh</v>
+      </c>
+      <c r="L101">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M101">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>1</v>
       </c>
       <c r="N101" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -9767,38 +9770,38 @@
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>153</v>
+        <v>321</v>
       </c>
       <c r="B102" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="C102" t="s">
         <v>2</v>
       </c>
       <c r="D102" t="s">
-        <v>54</v>
+        <v>139</v>
       </c>
       <c r="E102" s="1">
-        <v>999</v>
+        <v>100</v>
       </c>
       <c r="F102" t="s">
-        <v>7</v>
+        <v>330</v>
       </c>
       <c r="G102" t="s">
-        <v>368</v>
+        <v>6</v>
       </c>
       <c r="H102" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I102" t="s">
-        <v>41</v>
+        <v>335</v>
       </c>
       <c r="J102" t="s">
-        <v>41</v>
+        <v>328</v>
       </c>
       <c r="K102" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>holdings_record_idUNC999ai1=9 and i2=2</v>
+        <v>uniform_titleGEN100f(g)klnpt.</v>
       </c>
       <c r="L102" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9815,38 +9818,38 @@
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>154</v>
+        <v>321</v>
       </c>
       <c r="B103" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="C103" t="s">
         <v>2</v>
       </c>
       <c r="D103" t="s">
-        <v>54</v>
+        <v>139</v>
       </c>
       <c r="E103" s="1">
-        <v>999</v>
+        <v>110</v>
       </c>
       <c r="F103" t="s">
-        <v>372</v>
+        <v>334</v>
       </c>
       <c r="G103" t="s">
-        <v>373</v>
+        <v>6</v>
       </c>
       <c r="H103" t="s">
         <v>20</v>
       </c>
       <c r="I103" t="s">
-        <v>41</v>
+        <v>336</v>
       </c>
       <c r="J103" t="s">
-        <v>41</v>
+        <v>328</v>
       </c>
       <c r="K103" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>holdings_call_numberUNC999hijkmi1=9 AND i2=3 AND $0=#{holdings_record_id} AND $2='852'</v>
+        <v>uniform_titleGEN110f(g)kl(n)pt.</v>
       </c>
       <c r="L103" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9863,38 +9866,38 @@
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>227</v>
+        <v>321</v>
       </c>
       <c r="B104" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="C104" t="s">
         <v>2</v>
       </c>
       <c r="D104" t="s">
-        <v>54</v>
+        <v>139</v>
       </c>
       <c r="E104" s="1">
-        <v>999</v>
+        <v>111</v>
       </c>
       <c r="F104" t="s">
-        <v>374</v>
+        <v>334</v>
       </c>
       <c r="G104" t="s">
-        <v>373</v>
+        <v>6</v>
       </c>
       <c r="H104" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I104" t="s">
-        <v>41</v>
+        <v>336</v>
       </c>
       <c r="J104" t="s">
-        <v>41</v>
+        <v>328</v>
       </c>
       <c r="K104" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>holdings_noteUNC999lzi1=9 AND i2=3 AND $0=#{holdings_record_id} AND $2='852'</v>
+        <v>uniform_titleGEN111f(g)kl(n)pt.</v>
       </c>
       <c r="L104" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>

</xml_diff>

<commit_message>
update author_facet mapping processing instructions
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="381">
   <si>
     <t>subject_chronological_facet</t>
   </si>
@@ -1154,9 +1154,6 @@
     <t>i2!=2 AND (NO $t OR $k) AND (relator_category.include?('creator'))</t>
   </si>
   <si>
-    <t>relator category: look up $e/$4 values in argot/maps/_relator_categories.json ;;; https://github.com/trln/data-documentation/blob/master/argot/processing_rules_and_procedures.md#all-fields-that-become-facet-values</t>
-  </si>
-  <si>
     <t>(creators not part of name-title entries)</t>
   </si>
   <si>
@@ -1164,6 +1161,15 @@
   </si>
   <si>
     <t>i2!=2 AND (NO $t OR $k) AND ($e = (editor OR editor of compilation OR director OR film director) OR $4 = (edt OR edc OR drt OR fmd))</t>
+  </si>
+  <si>
+    <t>subfield g included in creator_main if there is NO $t or $k, or if it occurs BEFORE any $t/$k present ;;; https://github.com/trln/data-documentation/blob/master/argot/processing_rules_and_procedures.md#all-fields-that-become-facet-values</t>
+  </si>
+  <si>
+    <t>$g and/or $n included in creator_main if there is NO $t or $k, or if it occurs BEFORE any $t/$k present ;;; https://github.com/trln/data-documentation/blob/master/argot/processing_rules_and_procedures.md#all-fields-that-become-facet-values</t>
+  </si>
+  <si>
+    <t>subfield g included in creator_main if there is NO $t or $k, or if it occurs BEFORE any $t/$k present ;;; relator category: look up $e/$4 values in argot/maps/_relator_categories.json ;;; https://github.com/trln/data-documentation/blob/master/argot/processing_rules_and_procedures.md#all-fields-that-become-facet-values</t>
   </si>
 </sst>
 </file>
@@ -1185,6 +1191,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1296,16 +1303,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -1319,6 +1316,16 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1498,22 +1505,22 @@
     <tableColumn id="2" name="source data format"/>
     <tableColumn id="11" name="provisional?"/>
     <tableColumn id="3" name="institution"/>
-    <tableColumn id="4" name="element/field" dataDxfId="6"/>
+    <tableColumn id="4" name="element/field" dataDxfId="5"/>
     <tableColumn id="5" name="subelement/field(s)"/>
     <tableColumn id="6" name="constraints"/>
     <tableColumn id="7" name="processing_type"/>
     <tableColumn id="8" name="processing instructions"/>
     <tableColumn id="9" name="notes"/>
-    <tableColumn id="10" name="mapping_id" dataDxfId="5">
+    <tableColumn id="10" name="mapping_id" dataDxfId="4">
       <calculatedColumnFormula>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="mapping issue ct" dataDxfId="4">
+    <tableColumn id="12" name="mapping issue ct" dataDxfId="3">
       <calculatedColumnFormula>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="field issue ct" dataDxfId="3">
+    <tableColumn id="13" name="field issue ct" dataDxfId="2">
       <calculatedColumnFormula>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="field defined?" dataDxfId="2">
+    <tableColumn id="14" name="field defined?" dataDxfId="1">
       <calculatedColumnFormula>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4849,7 +4856,7 @@
   <dimension ref="A1:N103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4929,7 +4936,7 @@
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>213</v>
+        <v>378</v>
       </c>
       <c r="J2" t="s">
         <v>41</v>
@@ -4977,7 +4984,7 @@
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>213</v>
+        <v>379</v>
       </c>
       <c r="J3" t="s">
         <v>41</v>
@@ -5025,7 +5032,7 @@
         <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>213</v>
+        <v>379</v>
       </c>
       <c r="J4" t="s">
         <v>41</v>
@@ -5073,7 +5080,7 @@
         <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>213</v>
+        <v>378</v>
       </c>
       <c r="J5" t="s">
         <v>372</v>
@@ -5121,7 +5128,7 @@
         <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>213</v>
+        <v>378</v>
       </c>
       <c r="J6" t="s">
         <v>373</v>
@@ -5169,10 +5176,10 @@
         <v>20</v>
       </c>
       <c r="I7" t="s">
+        <v>380</v>
+      </c>
+      <c r="J7" t="s">
         <v>375</v>
-      </c>
-      <c r="J7" t="s">
-        <v>376</v>
       </c>
       <c r="K7" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
@@ -5211,16 +5218,16 @@
         <v>326</v>
       </c>
       <c r="G8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H8" t="s">
         <v>20</v>
       </c>
       <c r="I8" t="s">
-        <v>213</v>
+        <v>378</v>
       </c>
       <c r="J8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="K8" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
@@ -9795,7 +9802,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K3:K65">
-    <cfRule type="duplicateValues" dxfId="0" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -9935,7 +9942,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
remove field names from processing instructions
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="382">
   <si>
     <t>subject_chronological_facet</t>
   </si>
@@ -1013,24 +1013,12 @@
     <t>f(g)klnpt</t>
   </si>
   <si>
-    <t>subfield g included in creator_main if there is NO $t or $k, or if it occurs BEFORE any $t/$k present</t>
-  </si>
-  <si>
     <t>abcd(g)(n)u</t>
   </si>
   <si>
-    <t>$g and/or $n included in creator_main if there is NO $t or $k, or if it occurs BEFORE any $t/$k present</t>
-  </si>
-  <si>
     <t>f(g)kl(n)pt</t>
   </si>
   <si>
-    <t>$g included in uniform_title if it occurs AFTER a $t or $k</t>
-  </si>
-  <si>
-    <t>$g and/or $n included in uniform_title if it occurs AFTER a $t or $k</t>
-  </si>
-  <si>
     <t>acde(g)(n)qu</t>
   </si>
   <si>
@@ -1163,13 +1151,28 @@
     <t>i2!=2 AND (NO $t OR $k) AND ($e = (editor OR editor of compilation OR director OR film director) OR $4 = (edt OR edc OR drt OR fmd))</t>
   </si>
   <si>
-    <t>subfield g included in creator_main if there is NO $t or $k, or if it occurs BEFORE any $t/$k present ;;; https://github.com/trln/data-documentation/blob/master/argot/processing_rules_and_procedures.md#all-fields-that-become-facet-values</t>
-  </si>
-  <si>
-    <t>$g and/or $n included in creator_main if there is NO $t or $k, or if it occurs BEFORE any $t/$k present ;;; https://github.com/trln/data-documentation/blob/master/argot/processing_rules_and_procedures.md#all-fields-that-become-facet-values</t>
-  </si>
-  <si>
-    <t>subfield g included in creator_main if there is NO $t or $k, or if it occurs BEFORE any $t/$k present ;;; relator category: look up $e/$4 values in argot/maps/_relator_categories.json ;;; https://github.com/trln/data-documentation/blob/master/argot/processing_rules_and_procedures.md#all-fields-that-become-facet-values</t>
+    <t>subfield g included if there is NO $t or $k, or if it occurs BEFORE any $t/$k present ;;; https://github.com/trln/data-documentation/blob/master/argot/processing_rules_and_procedures.md#all-fields-that-become-facet-values</t>
+  </si>
+  <si>
+    <t>$g and/or $n included if there is NO $t or $k, or if it occurs BEFORE any $t/$k present ;;; https://github.com/trln/data-documentation/blob/master/argot/processing_rules_and_procedures.md#all-fields-that-become-facet-values</t>
+  </si>
+  <si>
+    <t>subfield g included if there is NO $t or $k, or if it occurs BEFORE any $t/$k present ;;; relator category: look up $e/$4 values in argot/maps/_relator_categories.json ;;; https://github.com/trln/data-documentation/blob/master/argot/processing_rules_and_procedures.md#all-fields-that-become-facet-values</t>
+  </si>
+  <si>
+    <t>subfield g included if there is NO $t or $k, or if it occurs BEFORE any $t/$k present</t>
+  </si>
+  <si>
+    <t>$g and/or $n included if there is NO $t or $k, or if it occurs BEFORE any $t/$k present</t>
+  </si>
+  <si>
+    <t>$g and/or $n included there is NO $t or $k, or if it occurs BEFORE any $t/$k present</t>
+  </si>
+  <si>
+    <t>$g included if it occurs AFTER a $t or $k</t>
+  </si>
+  <si>
+    <t>$g and/or $n included if it occurs AFTER a $t or $k</t>
   </si>
 </sst>
 </file>
@@ -1933,7 +1936,7 @@
         <v>6</v>
       </c>
       <c r="M2" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="N2" t="s">
         <v>6</v>
@@ -2117,7 +2120,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B6" t="s">
         <v>294</v>
@@ -2173,7 +2176,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B8" t="s">
         <v>294</v>
@@ -2228,7 +2231,7 @@
         <v>41</v>
       </c>
       <c r="J9" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K9" t="s">
         <v>6</v>
@@ -2262,7 +2265,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B10" t="s">
         <v>294</v>
@@ -2470,7 +2473,7 @@
         <v>3</v>
       </c>
       <c r="J14" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K14" t="s">
         <v>6</v>
@@ -2479,19 +2482,19 @@
         <v>6</v>
       </c>
       <c r="M14" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="N14" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="O14" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="P14" t="s">
         <v>313</v>
       </c>
       <c r="Q14" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="R14" t="s">
         <v>6</v>
@@ -2562,28 +2565,28 @@
         <v>3</v>
       </c>
       <c r="J16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K16" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="L16" t="s">
         <v>6</v>
       </c>
       <c r="M16" t="s">
+        <v>345</v>
+      </c>
+      <c r="N16" t="s">
+        <v>346</v>
+      </c>
+      <c r="O16" t="s">
         <v>349</v>
-      </c>
-      <c r="N16" t="s">
-        <v>350</v>
-      </c>
-      <c r="O16" t="s">
-        <v>353</v>
       </c>
       <c r="P16" t="s">
         <v>312</v>
       </c>
       <c r="Q16" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="R16" t="s">
         <v>6</v>
@@ -3844,7 +3847,7 @@
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B38" t="s">
         <v>294</v>
@@ -4581,19 +4584,19 @@
         <v>6</v>
       </c>
       <c r="M52" t="s">
+        <v>350</v>
+      </c>
+      <c r="N52" t="s">
+        <v>351</v>
+      </c>
+      <c r="O52" t="s">
+        <v>352</v>
+      </c>
+      <c r="P52" t="s">
+        <v>353</v>
+      </c>
+      <c r="Q52" t="s">
         <v>354</v>
-      </c>
-      <c r="N52" t="s">
-        <v>355</v>
-      </c>
-      <c r="O52" t="s">
-        <v>356</v>
-      </c>
-      <c r="P52" t="s">
-        <v>357</v>
-      </c>
-      <c r="Q52" t="s">
-        <v>358</v>
       </c>
       <c r="R52" t="s">
         <v>6</v>
@@ -4855,9 +4858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4936,7 +4937,7 @@
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="J2" t="s">
         <v>41</v>
@@ -4975,7 +4976,7 @@
         <v>110</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
@@ -4984,7 +4985,7 @@
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="J3" t="s">
         <v>41</v>
@@ -5023,7 +5024,7 @@
         <v>111</v>
       </c>
       <c r="F4" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="G4" t="s">
         <v>6</v>
@@ -5032,7 +5033,7 @@
         <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="J4" t="s">
         <v>41</v>
@@ -5074,16 +5075,16 @@
         <v>326</v>
       </c>
       <c r="G5" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="H5" t="s">
         <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="J5" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="K5" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
@@ -5122,16 +5123,16 @@
         <v>326</v>
       </c>
       <c r="G6" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="H6" t="s">
         <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="J6" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="K6" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
@@ -5170,16 +5171,16 @@
         <v>326</v>
       </c>
       <c r="G7" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="H7" t="s">
         <v>20</v>
       </c>
       <c r="I7" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="J7" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="K7" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
@@ -5218,16 +5219,16 @@
         <v>326</v>
       </c>
       <c r="G8" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="H8" t="s">
         <v>20</v>
       </c>
       <c r="I8" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="J8" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="K8" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
@@ -5320,7 +5321,7 @@
         <v>20</v>
       </c>
       <c r="I10" t="s">
-        <v>328</v>
+        <v>377</v>
       </c>
       <c r="J10" t="s">
         <v>41</v>
@@ -5359,7 +5360,7 @@
         <v>110</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G11" t="s">
         <v>6</v>
@@ -5368,7 +5369,7 @@
         <v>20</v>
       </c>
       <c r="I11" t="s">
-        <v>330</v>
+        <v>378</v>
       </c>
       <c r="J11" t="s">
         <v>41</v>
@@ -5407,7 +5408,7 @@
         <v>111</v>
       </c>
       <c r="F12" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="G12" t="s">
         <v>6</v>
@@ -5416,7 +5417,7 @@
         <v>20</v>
       </c>
       <c r="I12" t="s">
-        <v>330</v>
+        <v>379</v>
       </c>
       <c r="J12" t="s">
         <v>41</v>
@@ -5440,7 +5441,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
@@ -5455,7 +5456,7 @@
         <v>100</v>
       </c>
       <c r="F13" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="G13" t="s">
         <v>6</v>
@@ -5464,7 +5465,7 @@
         <v>5</v>
       </c>
       <c r="I13" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="J13" t="s">
         <v>41</v>
@@ -5488,7 +5489,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
@@ -5503,7 +5504,7 @@
         <v>110</v>
       </c>
       <c r="F14" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="G14" t="s">
         <v>6</v>
@@ -5512,7 +5513,7 @@
         <v>5</v>
       </c>
       <c r="I14" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="J14" t="s">
         <v>41</v>
@@ -5536,7 +5537,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
@@ -5551,7 +5552,7 @@
         <v>111</v>
       </c>
       <c r="F15" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="G15" t="s">
         <v>6</v>
@@ -5560,7 +5561,7 @@
         <v>5</v>
       </c>
       <c r="I15" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="J15" t="s">
         <v>41</v>
@@ -5791,16 +5792,16 @@
         <v>326</v>
       </c>
       <c r="G20" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="H20" t="s">
         <v>5</v>
       </c>
       <c r="I20" t="s">
-        <v>328</v>
+        <v>377</v>
       </c>
       <c r="J20" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="K20" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
@@ -5839,13 +5840,13 @@
         <v>326</v>
       </c>
       <c r="G21" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="H21" t="s">
         <v>5</v>
       </c>
       <c r="I21" t="s">
-        <v>328</v>
+        <v>377</v>
       </c>
       <c r="J21" t="s">
         <v>41</v>
@@ -5884,16 +5885,16 @@
         <v>710</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G22" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="H22" t="s">
         <v>5</v>
       </c>
       <c r="I22" t="s">
-        <v>330</v>
+        <v>378</v>
       </c>
       <c r="J22" t="s">
         <v>41</v>
@@ -5935,16 +5936,16 @@
         <v>326</v>
       </c>
       <c r="G23" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="H23" t="s">
         <v>5</v>
       </c>
       <c r="I23" t="s">
-        <v>330</v>
+        <v>378</v>
       </c>
       <c r="J23" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="K23" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
@@ -5983,13 +5984,13 @@
         <v>326</v>
       </c>
       <c r="G24" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="H24" t="s">
         <v>5</v>
       </c>
       <c r="I24" t="s">
-        <v>330</v>
+        <v>378</v>
       </c>
       <c r="J24" t="s">
         <v>41</v>
@@ -6028,10 +6029,10 @@
         <v>999</v>
       </c>
       <c r="F25" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="G25" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="H25" t="s">
         <v>20</v>
@@ -6079,13 +6080,13 @@
         <v>184</v>
       </c>
       <c r="G26" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="H26" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="I26" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="J26" t="s">
         <v>41</v>
@@ -6127,13 +6128,13 @@
         <v>184</v>
       </c>
       <c r="G27" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="H27" t="s">
         <v>5</v>
       </c>
       <c r="I27" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="K27" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
@@ -6169,10 +6170,10 @@
         <v>999</v>
       </c>
       <c r="F28" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="G28" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="H28" t="s">
         <v>5</v>
@@ -6220,7 +6221,7 @@
         <v>7</v>
       </c>
       <c r="G29" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="H29" t="s">
         <v>5</v>
@@ -6268,7 +6269,7 @@
         <v>7</v>
       </c>
       <c r="G30" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="H30" t="s">
         <v>5</v>
@@ -6418,7 +6419,7 @@
         <v>266</v>
       </c>
       <c r="I33" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="J33" t="s">
         <v>6</v>
@@ -6466,7 +6467,7 @@
         <v>266</v>
       </c>
       <c r="I34" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="J34" t="s">
         <v>6</v>
@@ -6514,7 +6515,7 @@
         <v>5</v>
       </c>
       <c r="I35" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="J35" t="s">
         <v>6</v>
@@ -6562,7 +6563,7 @@
         <v>5</v>
       </c>
       <c r="I36" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="J36" t="s">
         <v>6</v>
@@ -9682,7 +9683,7 @@
         <v>20</v>
       </c>
       <c r="I101" t="s">
-        <v>332</v>
+        <v>380</v>
       </c>
       <c r="J101" t="s">
         <v>325</v>
@@ -9721,7 +9722,7 @@
         <v>110</v>
       </c>
       <c r="F102" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G102" t="s">
         <v>6</v>
@@ -9730,7 +9731,7 @@
         <v>20</v>
       </c>
       <c r="I102" t="s">
-        <v>333</v>
+        <v>381</v>
       </c>
       <c r="J102" t="s">
         <v>325</v>
@@ -9769,7 +9770,7 @@
         <v>111</v>
       </c>
       <c r="F103" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G103" t="s">
         <v>6</v>
@@ -9778,7 +9779,7 @@
         <v>20</v>
       </c>
       <c r="I103" t="s">
-        <v>333</v>
+        <v>381</v>
       </c>
       <c r="J103" t="s">
         <v>325</v>

</xml_diff>

<commit_message>
additional relators for director, editor
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -1043,12 +1043,6 @@
     <t>j4</t>
   </si>
   <si>
-    <t>$e = director OR $4 = drt</t>
-  </si>
-  <si>
-    <t>$e = editor OR $4 = edt</t>
-  </si>
-  <si>
     <t xml:space="preserve">Main author/creatorship is assumed when name is recorded in 1xx, and may not always be represented by explicit relator term/code. Director is a "contributor" role, not a "creator role". There is no good way to tell if "1xx Doe, John$edirector") really means "writer and director" or if the name *should* have been recorded in 7xx field because the person only was in a contributor role. We err on the side of treating it as if the name has two roles. </t>
   </si>
   <si>
@@ -1173,6 +1167,12 @@
   </si>
   <si>
     <t>$g and/or $n included if it occurs AFTER a $t or $k</t>
+  </si>
+  <si>
+    <t>$e = ('director' OR 'film director') OR $4 = ('drt' OR 'fmd')</t>
+  </si>
+  <si>
+    <t>$e = ('editor' OR 'editor of compilation') OR $4 = ('edt' OR 'edc')</t>
   </si>
 </sst>
 </file>
@@ -1936,7 +1936,7 @@
         <v>6</v>
       </c>
       <c r="M2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="N2" t="s">
         <v>6</v>
@@ -2231,7 +2231,7 @@
         <v>41</v>
       </c>
       <c r="J9" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="K9" t="s">
         <v>6</v>
@@ -2473,7 +2473,7 @@
         <v>3</v>
       </c>
       <c r="J14" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="K14" t="s">
         <v>6</v>
@@ -2482,19 +2482,19 @@
         <v>6</v>
       </c>
       <c r="M14" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="N14" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="O14" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="P14" t="s">
         <v>313</v>
       </c>
       <c r="Q14" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="R14" t="s">
         <v>6</v>
@@ -2565,28 +2565,28 @@
         <v>3</v>
       </c>
       <c r="J16" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="K16" t="s">
+        <v>342</v>
+      </c>
+      <c r="L16" t="s">
+        <v>6</v>
+      </c>
+      <c r="M16" t="s">
+        <v>343</v>
+      </c>
+      <c r="N16" t="s">
         <v>344</v>
       </c>
-      <c r="L16" t="s">
-        <v>6</v>
-      </c>
-      <c r="M16" t="s">
-        <v>345</v>
-      </c>
-      <c r="N16" t="s">
-        <v>346</v>
-      </c>
       <c r="O16" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="P16" t="s">
         <v>312</v>
       </c>
       <c r="Q16" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="R16" t="s">
         <v>6</v>
@@ -4584,19 +4584,19 @@
         <v>6</v>
       </c>
       <c r="M52" t="s">
+        <v>348</v>
+      </c>
+      <c r="N52" t="s">
+        <v>349</v>
+      </c>
+      <c r="O52" t="s">
         <v>350</v>
       </c>
-      <c r="N52" t="s">
+      <c r="P52" t="s">
         <v>351</v>
       </c>
-      <c r="O52" t="s">
+      <c r="Q52" t="s">
         <v>352</v>
-      </c>
-      <c r="P52" t="s">
-        <v>353</v>
-      </c>
-      <c r="Q52" t="s">
-        <v>354</v>
       </c>
       <c r="R52" t="s">
         <v>6</v>
@@ -4858,7 +4858,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4937,7 +4939,7 @@
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="J2" t="s">
         <v>41</v>
@@ -4985,7 +4987,7 @@
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="J3" t="s">
         <v>41</v>
@@ -5033,7 +5035,7 @@
         <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="J4" t="s">
         <v>41</v>
@@ -5075,16 +5077,16 @@
         <v>326</v>
       </c>
       <c r="G5" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="H5" t="s">
         <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="J5" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="K5" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
@@ -5123,16 +5125,16 @@
         <v>326</v>
       </c>
       <c r="G6" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="H6" t="s">
         <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="J6" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="K6" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
@@ -5171,16 +5173,16 @@
         <v>326</v>
       </c>
       <c r="G7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="H7" t="s">
         <v>20</v>
       </c>
       <c r="I7" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="J7" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="K7" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
@@ -5219,16 +5221,16 @@
         <v>326</v>
       </c>
       <c r="G8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="H8" t="s">
         <v>20</v>
       </c>
       <c r="I8" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="J8" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K8" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
@@ -5321,7 +5323,7 @@
         <v>20</v>
       </c>
       <c r="I10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="J10" t="s">
         <v>41</v>
@@ -5369,7 +5371,7 @@
         <v>20</v>
       </c>
       <c r="I11" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="J11" t="s">
         <v>41</v>
@@ -5417,7 +5419,7 @@
         <v>20</v>
       </c>
       <c r="I12" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="J12" t="s">
         <v>41</v>
@@ -5792,20 +5794,20 @@
         <v>326</v>
       </c>
       <c r="G20" t="s">
-        <v>338</v>
+        <v>380</v>
       </c>
       <c r="H20" t="s">
         <v>5</v>
       </c>
       <c r="I20" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="J20" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="K20" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>directorGEN100abcd(g)jqu$e = director OR $4 = drt</v>
+        <v>directorGEN100abcd(g)jqu$e = ('director' OR 'film director') OR $4 = ('drt' OR 'fmd')</v>
       </c>
       <c r="L20" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5840,20 +5842,20 @@
         <v>326</v>
       </c>
       <c r="G21" t="s">
-        <v>338</v>
+        <v>380</v>
       </c>
       <c r="H21" t="s">
         <v>5</v>
       </c>
       <c r="I21" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="J21" t="s">
         <v>41</v>
       </c>
       <c r="K21" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>directorGEN700abcd(g)jqu$e = director OR $4 = drt</v>
+        <v>directorGEN700abcd(g)jqu$e = ('director' OR 'film director') OR $4 = ('drt' OR 'fmd')</v>
       </c>
       <c r="L21" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5888,20 +5890,20 @@
         <v>328</v>
       </c>
       <c r="G22" t="s">
-        <v>338</v>
+        <v>380</v>
       </c>
       <c r="H22" t="s">
         <v>5</v>
       </c>
       <c r="I22" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="J22" t="s">
         <v>41</v>
       </c>
       <c r="K22" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>directorGEN710abcd(g)(n)u$e = director OR $4 = drt</v>
+        <v>directorGEN710abcd(g)(n)u$e = ('director' OR 'film director') OR $4 = ('drt' OR 'fmd')</v>
       </c>
       <c r="L22" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5936,20 +5938,20 @@
         <v>326</v>
       </c>
       <c r="G23" t="s">
-        <v>339</v>
+        <v>381</v>
       </c>
       <c r="H23" t="s">
         <v>5</v>
       </c>
       <c r="I23" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="J23" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="K23" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>editorGEN100abcd(g)jqu$e = editor OR $4 = edt</v>
+        <v>editorGEN100abcd(g)jqu$e = ('editor' OR 'editor of compilation') OR $4 = ('edt' OR 'edc')</v>
       </c>
       <c r="L23" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5984,20 +5986,20 @@
         <v>326</v>
       </c>
       <c r="G24" t="s">
-        <v>339</v>
+        <v>381</v>
       </c>
       <c r="H24" t="s">
         <v>5</v>
       </c>
       <c r="I24" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="J24" t="s">
         <v>41</v>
       </c>
       <c r="K24" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>editorGEN700abcd(g)jqu$e = editor OR $4 = edt</v>
+        <v>editorGEN700abcd(g)jqu$e = ('editor' OR 'editor of compilation') OR $4 = ('edt' OR 'edc')</v>
       </c>
       <c r="L24" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6029,10 +6031,10 @@
         <v>999</v>
       </c>
       <c r="F25" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G25" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="H25" t="s">
         <v>20</v>
@@ -6080,13 +6082,13 @@
         <v>184</v>
       </c>
       <c r="G26" t="s">
+        <v>356</v>
+      </c>
+      <c r="H26" t="s">
+        <v>353</v>
+      </c>
+      <c r="I26" t="s">
         <v>358</v>
-      </c>
-      <c r="H26" t="s">
-        <v>355</v>
-      </c>
-      <c r="I26" t="s">
-        <v>360</v>
       </c>
       <c r="J26" t="s">
         <v>41</v>
@@ -6128,13 +6130,13 @@
         <v>184</v>
       </c>
       <c r="G27" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="H27" t="s">
         <v>5</v>
       </c>
       <c r="I27" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="K27" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
@@ -6170,10 +6172,10 @@
         <v>999</v>
       </c>
       <c r="F28" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G28" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="H28" t="s">
         <v>5</v>
@@ -6221,7 +6223,7 @@
         <v>7</v>
       </c>
       <c r="G29" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="H29" t="s">
         <v>5</v>
@@ -6269,7 +6271,7 @@
         <v>7</v>
       </c>
       <c r="G30" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="H30" t="s">
         <v>5</v>
@@ -6419,7 +6421,7 @@
         <v>266</v>
       </c>
       <c r="I33" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="J33" t="s">
         <v>6</v>
@@ -6467,7 +6469,7 @@
         <v>266</v>
       </c>
       <c r="I34" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="J34" t="s">
         <v>6</v>
@@ -6515,7 +6517,7 @@
         <v>5</v>
       </c>
       <c r="I35" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="J35" t="s">
         <v>6</v>
@@ -6563,7 +6565,7 @@
         <v>5</v>
       </c>
       <c r="I36" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="J36" t="s">
         <v>6</v>
@@ -9683,7 +9685,7 @@
         <v>20</v>
       </c>
       <c r="I101" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="J101" t="s">
         <v>325</v>
@@ -9731,7 +9733,7 @@
         <v>20</v>
       </c>
       <c r="I102" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="J102" t="s">
         <v>325</v>
@@ -9779,7 +9781,7 @@
         <v>20</v>
       </c>
       <c r="I103" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="J103" t="s">
         <v>325</v>

</xml_diff>

<commit_message>
Shorten and align item and holding subelement names
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -9,7 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="5910" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="5910"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20265" windowHeight="6450"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1735" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1713" uniqueCount="369">
   <si>
     <t>subject_chronological_facet</t>
   </si>
@@ -473,27 +474,6 @@
     <t>issue ct</t>
   </si>
   <si>
-    <t>item_due_date</t>
-  </si>
-  <si>
-    <t>item_record_id</t>
-  </si>
-  <si>
-    <t>item_call_number</t>
-  </si>
-  <si>
-    <t>item_status</t>
-  </si>
-  <si>
-    <t>item_type</t>
-  </si>
-  <si>
-    <t>holdings_record_id</t>
-  </si>
-  <si>
-    <t>holdings_call_number</t>
-  </si>
-  <si>
     <t>Unique identifier for an item record in host institution's ILS. Could be record number or barcode.</t>
   </si>
   <si>
@@ -527,21 +507,12 @@
     <t>Will be blank if item is NOT checked out</t>
   </si>
   <si>
-    <t>Shelving location code for item</t>
-  </si>
-  <si>
     <t>Inform user what section/area of stacks to go to in order to find the item</t>
   </si>
   <si>
     <t>Location_property</t>
   </si>
   <si>
-    <t>CODE, not display value</t>
-  </si>
-  <si>
-    <t>Map to readable label for display</t>
-  </si>
-  <si>
     <t>l</t>
   </si>
   <si>
@@ -590,18 +561,12 @@
     <t>Status: Due #{date}</t>
   </si>
   <si>
-    <t>item_note</t>
-  </si>
-  <si>
     <t>call number</t>
   </si>
   <si>
     <t>Full call number from item record (classification number + shelving cutter + shelf marks + volume/copy designators)</t>
   </si>
   <si>
-    <t>Library building/branch/larger location in which the shelving location is found</t>
-  </si>
-  <si>
     <t>Inform user what library building or main section/area to go to in order to find the item</t>
   </si>
   <si>
@@ -629,15 +594,9 @@
     <t>Call Number</t>
   </si>
   <si>
-    <t>item_classification_scheme</t>
-  </si>
-  <si>
     <t>An item may have more than one item note. They should be displayed in order.</t>
   </si>
   <si>
-    <t>Empty if not checked out</t>
-  </si>
-  <si>
     <t>documentation</t>
   </si>
   <si>
@@ -656,9 +615,6 @@
     <t>items</t>
   </si>
   <si>
-    <t>item_requestable</t>
-  </si>
-  <si>
     <t>Status of individual item</t>
   </si>
   <si>
@@ -668,39 +624,15 @@
     <t>Statuses</t>
   </si>
   <si>
-    <t xml:space="preserve">Develop/agree upon a standard set of statuses, and how they map to bib_availability value? </t>
-  </si>
-  <si>
     <t>Type/format for individual item</t>
   </si>
   <si>
-    <t>Do we need this in Argot/Argon? Will any features use it? Not sure if any do in Endeca.</t>
-  </si>
-  <si>
     <t>ItemTypes</t>
   </si>
   <si>
-    <t>Placeholder for possibility of representing this in data/index instead of on-the-fly</t>
-  </si>
-  <si>
     <t>holdings</t>
   </si>
   <si>
-    <t>holdings_note</t>
-  </si>
-  <si>
-    <t>item_location_library</t>
-  </si>
-  <si>
-    <t>item_location_shelf</t>
-  </si>
-  <si>
-    <t>holdings_location_library</t>
-  </si>
-  <si>
-    <t>holdings_location_shelf</t>
-  </si>
-  <si>
     <t>resource_type</t>
   </si>
   <si>
@@ -749,9 +681,6 @@
     <t>SerialHoldingsSummary &gt; Library</t>
   </si>
   <si>
-    <t>Shelving location code for items covered by the holdings statement</t>
-  </si>
-  <si>
     <t>Inform user what section/area of stacks to go to in order to find the items covered by holdings statement</t>
   </si>
   <si>
@@ -770,9 +699,6 @@
     <t>SerialHoldingsSummary &gt; Call #</t>
   </si>
   <si>
-    <t>holdings_summary</t>
-  </si>
-  <si>
     <t>Public notes from the item record</t>
   </si>
   <si>
@@ -824,39 +750,18 @@
     <t>f</t>
   </si>
   <si>
-    <t>bib_locations_hierarchical</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
     <t xml:space="preserve">Higher-level (library, etc.) locations housing volumes/copies of the resource described in the bib record </t>
   </si>
   <si>
-    <t>Support for hierarchical location facet; polyhierarchy already existing in Endeca</t>
-  </si>
-  <si>
-    <t>Recommended: limit to physical places people can go -- Online and E-resource are NOT locations</t>
-  </si>
-  <si>
-    <t>Determine best way to derive/represent data; I've provided something that seems to make sense to me and serves as an example of what we are doing now with polyhierarchy and "sublocations", that we need to still be able to do</t>
-  </si>
-  <si>
     <t>jira ref</t>
   </si>
   <si>
     <t>https://trlnmain.atlassian.net/browse/TD-370</t>
   </si>
   <si>
-    <t>https://github.com/trln/data-documentation/blob/master/argot/questions_issues/location.md</t>
-  </si>
-  <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-363</t>
-  </si>
-  <si>
-    <t>https://trlnmain.atlassian.net/browse/TD-371</t>
-  </si>
-  <si>
     <t>creator_main</t>
   </si>
   <si>
@@ -1146,6 +1051,90 @@
   </si>
   <si>
     <t>$e = ('editor' OR 'editor of compilation') OR $4 = ('edt' OR 'edc')</t>
+  </si>
+  <si>
+    <t>call_no (holdings)</t>
+  </si>
+  <si>
+    <t>loc_b (holdings)</t>
+  </si>
+  <si>
+    <t>loc_n (holdings)</t>
+  </si>
+  <si>
+    <t>rec_id (holdings)</t>
+  </si>
+  <si>
+    <t>summary (holdings)</t>
+  </si>
+  <si>
+    <t>notes (holdings)</t>
+  </si>
+  <si>
+    <t>Broad location: Library building/branch/larger location in which the shelving location is found</t>
+  </si>
+  <si>
+    <t>Narrow location: Area of library, shelving location, etc. code for items covered by the holdings statement</t>
+  </si>
+  <si>
+    <t>ILS code. Do not translate to human-readable label in MARC-to-Argot</t>
+  </si>
+  <si>
+    <t>https://github.com/trln/data-documentation/blob/master/argot/examples/holdings.md</t>
+  </si>
+  <si>
+    <t>call_no (items)</t>
+  </si>
+  <si>
+    <t>cn_scheme (items)</t>
+  </si>
+  <si>
+    <t>due_date (items)</t>
+  </si>
+  <si>
+    <t>loc_b (items)</t>
+  </si>
+  <si>
+    <t>loc_n (items)</t>
+  </si>
+  <si>
+    <t>notes (items)</t>
+  </si>
+  <si>
+    <t>rec_id (items)</t>
+  </si>
+  <si>
+    <t>status (items)</t>
+  </si>
+  <si>
+    <t>type (items)</t>
+  </si>
+  <si>
+    <t>Narrow location: Area of library, shelving location code for item</t>
+  </si>
+  <si>
+    <t>Only populated if item status = Checked out</t>
+  </si>
+  <si>
+    <t>Output human-readable status. Institution-specific status messages are output at item level. These will be mapped to a standardized, central set of broader "status" categories for use outside individual item display</t>
+  </si>
+  <si>
+    <t>https://github.com/trln/data-documentation/blob/master/argot/examples/items.md</t>
+  </si>
+  <si>
+    <t>Currently defined as single value. Have asked Adam if it is ever multivalued for NCSU -- 2017-10-25</t>
+  </si>
+  <si>
+    <t>Slack DM</t>
+  </si>
+  <si>
+    <t>location_facet</t>
+  </si>
+  <si>
+    <t>Support for abstract, polyhierarchical location facet. Facet limits/excludes BIB records.</t>
+  </si>
+  <si>
+    <t>Create documentation in this repo</t>
   </si>
 </sst>
 </file>
@@ -1155,7 +1144,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1176,6 +1165,12 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1244,7 +1239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1256,10 +1251,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1415,11 +1412,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="fields" displayName="fields" ref="A1:U52" totalsRowShown="0">
-  <autoFilter ref="A1:U52"/>
-  <sortState ref="A2:U56">
-    <sortCondition ref="A2:A56"/>
-  </sortState>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="fields" displayName="fields" ref="A1:U51" totalsRowShown="0">
+  <autoFilter ref="A1:U51"/>
   <tableColumns count="21">
     <tableColumn id="2" name="field"/>
     <tableColumn id="22" name="category"/>
@@ -1452,8 +1446,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="issuesfield" displayName="issuesfield" ref="A1:D12" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:D12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="issuesfield" displayName="issuesfield" ref="A1:D11" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:D11"/>
   <tableColumns count="4">
     <tableColumn id="1" name="field" dataDxfId="10"/>
     <tableColumn id="3" name="desc" dataDxfId="9"/>
@@ -1778,11 +1772,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U52"/>
+  <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A4" sqref="A4:XFD4"/>
+      <selection pane="topRight" activeCell="A3" sqref="A3"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <pane xSplit="1" ySplit="15" topLeftCell="N16" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1809,7 +1809,7 @@
         <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="C1" t="s">
         <v>67</v>
@@ -1818,10 +1818,10 @@
         <v>69</v>
       </c>
       <c r="E1" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="F1" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="G1" t="s">
         <v>70</v>
@@ -1860,7 +1860,7 @@
         <v>80</v>
       </c>
       <c r="S1" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="T1" t="s">
         <v>147</v>
@@ -1871,10 +1871,10 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>286</v>
+        <v>254</v>
       </c>
       <c r="B2" t="s">
-        <v>285</v>
+        <v>253</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -1898,7 +1898,7 @@
         <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>306</v>
+        <v>274</v>
       </c>
       <c r="K2" t="s">
         <v>82</v>
@@ -1907,7 +1907,7 @@
         <v>6</v>
       </c>
       <c r="M2" t="s">
-        <v>346</v>
+        <v>314</v>
       </c>
       <c r="N2" t="s">
         <v>6</v>
@@ -1916,13 +1916,13 @@
         <v>6</v>
       </c>
       <c r="P2" t="s">
-        <v>306</v>
+        <v>274</v>
       </c>
       <c r="Q2" t="s">
         <v>41</v>
       </c>
       <c r="R2" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="S2" t="s">
         <v>6</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>265</v>
+        <v>366</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -1965,7 +1965,7 @@
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>266</v>
+        <v>240</v>
       </c>
       <c r="K3" t="s">
         <v>82</v>
@@ -1974,20 +1974,29 @@
         <v>41</v>
       </c>
       <c r="M3" t="s">
-        <v>267</v>
+        <v>241</v>
       </c>
       <c r="N3" t="s">
-        <v>268</v>
+        <v>367</v>
       </c>
       <c r="O3" t="s">
         <v>41</v>
       </c>
       <c r="P3" t="s">
-        <v>266</v>
+        <v>240</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3" t="s">
+        <v>41</v>
+      </c>
+      <c r="S3" t="s">
+        <v>6</v>
       </c>
       <c r="T3" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U3">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
@@ -1996,10 +2005,10 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>280</v>
+        <v>248</v>
       </c>
       <c r="B4" t="s">
-        <v>285</v>
+        <v>253</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -2011,7 +2020,7 @@
         <v>41</v>
       </c>
       <c r="P4" t="s">
-        <v>303</v>
+        <v>271</v>
       </c>
       <c r="T4" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2024,10 +2033,10 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>325</v>
+        <v>293</v>
       </c>
       <c r="B5" t="s">
-        <v>285</v>
+        <v>253</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -2052,10 +2061,10 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>277</v>
+        <v>245</v>
       </c>
       <c r="B6" t="s">
-        <v>285</v>
+        <v>253</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -2067,7 +2076,7 @@
         <v>41</v>
       </c>
       <c r="P6" t="s">
-        <v>303</v>
+        <v>271</v>
       </c>
       <c r="T6" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2080,10 +2089,10 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>324</v>
+        <v>292</v>
       </c>
       <c r="B7" t="s">
-        <v>285</v>
+        <v>253</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -2108,10 +2117,10 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>276</v>
+        <v>244</v>
       </c>
       <c r="B8" t="s">
-        <v>285</v>
+        <v>253</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -2129,13 +2138,13 @@
         <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>311</v>
+        <v>279</v>
       </c>
       <c r="I8" t="s">
         <v>41</v>
       </c>
       <c r="J8" t="s">
-        <v>345</v>
+        <v>313</v>
       </c>
       <c r="K8" t="s">
         <v>6</v>
@@ -2144,16 +2153,16 @@
         <v>6</v>
       </c>
       <c r="M8" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="N8" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="O8" t="s">
         <v>6</v>
       </c>
       <c r="P8" t="s">
-        <v>307</v>
+        <v>275</v>
       </c>
       <c r="Q8" t="s">
         <v>41</v>
@@ -2169,10 +2178,10 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>323</v>
+        <v>291</v>
       </c>
       <c r="B9" t="s">
-        <v>285</v>
+        <v>253</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
@@ -2205,10 +2214,10 @@
         <v>6</v>
       </c>
       <c r="M9" t="s">
-        <v>314</v>
+        <v>282</v>
       </c>
       <c r="N9" t="s">
-        <v>315</v>
+        <v>283</v>
       </c>
       <c r="O9" t="s">
         <v>41</v>
@@ -2242,7 +2251,7 @@
         <v>41</v>
       </c>
       <c r="F10" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="G10" t="s">
         <v>2</v>
@@ -2294,10 +2303,10 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>295</v>
+        <v>263</v>
       </c>
       <c r="B11" t="s">
-        <v>293</v>
+        <v>261</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -2309,7 +2318,7 @@
         <v>41</v>
       </c>
       <c r="P11" t="s">
-        <v>301</v>
+        <v>269</v>
       </c>
       <c r="T11" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2322,10 +2331,10 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="B12" t="s">
-        <v>293</v>
+        <v>261</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -2350,10 +2359,10 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>278</v>
+        <v>246</v>
       </c>
       <c r="B13" t="s">
-        <v>285</v>
+        <v>253</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
@@ -2365,19 +2374,19 @@
         <v>41</v>
       </c>
       <c r="F13" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="G13" t="s">
         <v>3</v>
       </c>
       <c r="H13" t="s">
-        <v>311</v>
+        <v>279</v>
       </c>
       <c r="I13" t="s">
         <v>3</v>
       </c>
       <c r="J13" t="s">
-        <v>345</v>
+        <v>313</v>
       </c>
       <c r="K13" t="s">
         <v>6</v>
@@ -2386,19 +2395,19 @@
         <v>6</v>
       </c>
       <c r="M13" t="s">
-        <v>331</v>
+        <v>299</v>
       </c>
       <c r="N13" t="s">
-        <v>332</v>
+        <v>300</v>
       </c>
       <c r="O13" t="s">
-        <v>338</v>
+        <v>306</v>
       </c>
       <c r="P13" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q13" t="s">
         <v>304</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>336</v>
       </c>
       <c r="R13" t="s">
         <v>6</v>
@@ -2414,10 +2423,10 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>296</v>
+        <v>264</v>
       </c>
       <c r="B14" t="s">
-        <v>285</v>
+        <v>253</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
@@ -2429,7 +2438,7 @@
         <v>41</v>
       </c>
       <c r="P14" t="s">
-        <v>305</v>
+        <v>273</v>
       </c>
       <c r="T14" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2442,10 +2451,10 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>279</v>
+        <v>247</v>
       </c>
       <c r="B15" t="s">
-        <v>285</v>
+        <v>253</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
@@ -2457,40 +2466,40 @@
         <v>41</v>
       </c>
       <c r="F15" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="G15" t="s">
         <v>3</v>
       </c>
       <c r="H15" t="s">
-        <v>311</v>
+        <v>279</v>
       </c>
       <c r="I15" t="s">
         <v>3</v>
       </c>
       <c r="J15" t="s">
-        <v>345</v>
+        <v>313</v>
       </c>
       <c r="K15" t="s">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="L15" t="s">
         <v>6</v>
       </c>
       <c r="M15" t="s">
-        <v>334</v>
+        <v>302</v>
       </c>
       <c r="N15" t="s">
-        <v>335</v>
+        <v>303</v>
       </c>
       <c r="O15" t="s">
-        <v>338</v>
+        <v>306</v>
       </c>
       <c r="P15" t="s">
-        <v>303</v>
+        <v>271</v>
       </c>
       <c r="Q15" t="s">
-        <v>337</v>
+        <v>305</v>
       </c>
       <c r="R15" t="s">
         <v>6</v>
@@ -2506,10 +2515,10 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>341</v>
       </c>
       <c r="B16" t="s">
-        <v>284</v>
+        <v>252</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
@@ -2518,16 +2527,16 @@
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="F16" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="G16" t="s">
         <v>2</v>
       </c>
       <c r="H16" t="s">
-        <v>188</v>
+        <v>41</v>
       </c>
       <c r="I16" t="s">
         <v>6</v>
@@ -2536,22 +2545,22 @@
         <v>41</v>
       </c>
       <c r="K16" t="s">
-        <v>234</v>
+        <v>211</v>
       </c>
       <c r="L16" t="s">
+        <v>175</v>
+      </c>
+      <c r="M16" t="s">
+        <v>221</v>
+      </c>
+      <c r="N16" t="s">
         <v>185</v>
       </c>
-      <c r="M16" t="s">
-        <v>245</v>
-      </c>
-      <c r="N16" t="s">
-        <v>197</v>
-      </c>
       <c r="O16" t="s">
         <v>41</v>
       </c>
       <c r="P16" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="Q16" t="s">
         <v>41</v>
@@ -2560,7 +2569,7 @@
         <v>6</v>
       </c>
       <c r="S16" t="s">
-        <v>6</v>
+        <v>350</v>
       </c>
       <c r="T16" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2573,10 +2582,10 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>222</v>
+        <v>342</v>
       </c>
       <c r="B17" t="s">
-        <v>284</v>
+        <v>252</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -2585,10 +2594,10 @@
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="F17" t="s">
-        <v>172</v>
+        <v>3</v>
       </c>
       <c r="G17" t="s">
         <v>2</v>
@@ -2603,31 +2612,31 @@
         <v>41</v>
       </c>
       <c r="K17" t="s">
-        <v>234</v>
+        <v>211</v>
       </c>
       <c r="L17" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="M17" t="s">
-        <v>190</v>
+        <v>347</v>
       </c>
       <c r="N17" t="s">
-        <v>238</v>
+        <v>215</v>
       </c>
       <c r="O17" t="s">
         <v>41</v>
       </c>
       <c r="P17" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="Q17" t="s">
         <v>41</v>
       </c>
       <c r="R17" t="s">
-        <v>170</v>
+        <v>349</v>
       </c>
       <c r="S17" t="s">
-        <v>6</v>
+        <v>350</v>
       </c>
       <c r="T17" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2640,10 +2649,10 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>223</v>
+        <v>343</v>
       </c>
       <c r="B18" t="s">
-        <v>284</v>
+        <v>252</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
@@ -2652,49 +2661,49 @@
         <v>3</v>
       </c>
       <c r="E18" t="s">
+        <v>200</v>
+      </c>
+      <c r="F18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" t="s">
+        <v>41</v>
+      </c>
+      <c r="K18" t="s">
+        <v>211</v>
+      </c>
+      <c r="L18" t="s">
+        <v>175</v>
+      </c>
+      <c r="M18" t="s">
+        <v>348</v>
+      </c>
+      <c r="N18" t="s">
+        <v>217</v>
+      </c>
+      <c r="O18" t="s">
+        <v>41</v>
+      </c>
+      <c r="P18" t="s">
         <v>218</v>
       </c>
-      <c r="F18" t="s">
-        <v>172</v>
-      </c>
-      <c r="G18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H18" t="s">
-        <v>41</v>
-      </c>
-      <c r="I18" t="s">
-        <v>6</v>
-      </c>
-      <c r="J18" t="s">
-        <v>41</v>
-      </c>
-      <c r="K18" t="s">
-        <v>234</v>
-      </c>
-      <c r="L18" t="s">
-        <v>185</v>
-      </c>
-      <c r="M18" t="s">
-        <v>240</v>
-      </c>
-      <c r="N18" t="s">
-        <v>241</v>
-      </c>
-      <c r="O18" t="s">
-        <v>41</v>
-      </c>
-      <c r="P18" t="s">
-        <v>242</v>
-      </c>
       <c r="Q18" t="s">
         <v>41</v>
       </c>
       <c r="R18" t="s">
-        <v>170</v>
+        <v>349</v>
       </c>
       <c r="S18" t="s">
-        <v>6</v>
+        <v>350</v>
       </c>
       <c r="T18" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2707,10 +2716,10 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>219</v>
+        <v>346</v>
       </c>
       <c r="B19" t="s">
-        <v>284</v>
+        <v>252</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
@@ -2719,10 +2728,10 @@
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="F19" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="G19" t="s">
         <v>3</v>
@@ -2737,22 +2746,22 @@
         <v>41</v>
       </c>
       <c r="K19" t="s">
-        <v>234</v>
+        <v>211</v>
       </c>
       <c r="L19" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="M19" t="s">
-        <v>249</v>
+        <v>224</v>
       </c>
       <c r="N19" t="s">
-        <v>250</v>
+        <v>225</v>
       </c>
       <c r="O19" t="s">
         <v>41</v>
       </c>
       <c r="P19" t="s">
-        <v>251</v>
+        <v>226</v>
       </c>
       <c r="Q19" t="s">
         <v>41</v>
@@ -2761,7 +2770,7 @@
         <v>6</v>
       </c>
       <c r="S19" t="s">
-        <v>6</v>
+        <v>350</v>
       </c>
       <c r="T19" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2774,10 +2783,10 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>153</v>
+        <v>344</v>
       </c>
       <c r="B20" t="s">
-        <v>284</v>
+        <v>252</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
@@ -2786,10 +2795,10 @@
         <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="F20" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="G20" t="s">
         <v>2</v>
@@ -2798,7 +2807,7 @@
         <v>41</v>
       </c>
       <c r="I20" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="J20" t="s">
         <v>41</v>
@@ -2810,10 +2819,10 @@
         <v>41</v>
       </c>
       <c r="M20" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="N20" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
       <c r="O20" t="s">
         <v>41</v>
@@ -2828,7 +2837,7 @@
         <v>6</v>
       </c>
       <c r="S20" t="s">
-        <v>6</v>
+        <v>350</v>
       </c>
       <c r="T20" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2841,10 +2850,10 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>247</v>
+        <v>345</v>
       </c>
       <c r="B21" t="s">
-        <v>284</v>
+        <v>252</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -2853,10 +2862,10 @@
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="F21" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="G21" t="s">
         <v>2</v>
@@ -2871,22 +2880,22 @@
         <v>41</v>
       </c>
       <c r="K21" t="s">
-        <v>234</v>
+        <v>211</v>
       </c>
       <c r="L21" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="M21" t="s">
-        <v>233</v>
+        <v>210</v>
       </c>
       <c r="N21" t="s">
-        <v>236</v>
+        <v>213</v>
       </c>
       <c r="O21" t="s">
         <v>41</v>
       </c>
       <c r="P21" t="s">
-        <v>237</v>
+        <v>214</v>
       </c>
       <c r="Q21" t="s">
         <v>41</v>
@@ -2895,7 +2904,7 @@
         <v>6</v>
       </c>
       <c r="S21" t="s">
-        <v>6</v>
+        <v>350</v>
       </c>
       <c r="T21" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2908,10 +2917,10 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>291</v>
+        <v>259</v>
       </c>
       <c r="B22" t="s">
-        <v>293</v>
+        <v>261</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
@@ -2923,7 +2932,7 @@
         <v>41</v>
       </c>
       <c r="P22" t="s">
-        <v>301</v>
+        <v>269</v>
       </c>
       <c r="T22" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2936,10 +2945,10 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>298</v>
+        <v>266</v>
       </c>
       <c r="B23" t="s">
-        <v>293</v>
+        <v>261</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
@@ -2964,10 +2973,10 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>287</v>
+        <v>255</v>
       </c>
       <c r="B24" t="s">
-        <v>285</v>
+        <v>253</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
@@ -2979,7 +2988,7 @@
         <v>41</v>
       </c>
       <c r="P24" t="s">
-        <v>303</v>
+        <v>271</v>
       </c>
       <c r="T24" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2992,10 +3001,10 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>150</v>
+        <v>351</v>
       </c>
       <c r="B25" t="s">
-        <v>283</v>
+        <v>251</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
@@ -3004,16 +3013,16 @@
         <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="F25" t="s">
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="G25" t="s">
         <v>2</v>
       </c>
       <c r="H25" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="I25" t="s">
         <v>41</v>
@@ -3022,25 +3031,25 @@
         <v>41</v>
       </c>
       <c r="K25" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="L25" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="M25" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="N25" t="s">
-        <v>235</v>
+        <v>212</v>
       </c>
       <c r="O25" t="s">
         <v>6</v>
       </c>
       <c r="P25" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="S25" t="s">
-        <v>6</v>
+        <v>363</v>
       </c>
       <c r="T25" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3053,10 +3062,10 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>200</v>
+        <v>352</v>
       </c>
       <c r="B26" t="s">
-        <v>283</v>
+        <v>251</v>
       </c>
       <c r="C26" t="s">
         <v>2</v>
@@ -3065,10 +3074,10 @@
         <v>3</v>
       </c>
       <c r="E26" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="F26" t="s">
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="G26" t="s">
         <v>2</v>
@@ -3089,16 +3098,16 @@
         <v>41</v>
       </c>
       <c r="M26" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="N26" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="O26" t="s">
         <v>41</v>
       </c>
       <c r="P26" t="s">
-        <v>254</v>
+        <v>229</v>
       </c>
       <c r="Q26" t="s">
         <v>41</v>
@@ -3107,7 +3116,7 @@
         <v>41</v>
       </c>
       <c r="S26" t="s">
-        <v>6</v>
+        <v>363</v>
       </c>
       <c r="T26" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3120,10 +3129,10 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>148</v>
+        <v>353</v>
       </c>
       <c r="B27" t="s">
-        <v>283</v>
+        <v>251</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
@@ -3132,10 +3141,10 @@
         <v>3</v>
       </c>
       <c r="E27" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="F27" t="s">
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="G27" t="s">
         <v>2</v>
@@ -3150,31 +3159,31 @@
         <v>41</v>
       </c>
       <c r="K27" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="L27" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="M27" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="N27" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="O27" t="s">
         <v>41</v>
       </c>
       <c r="P27" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="Q27" t="s">
-        <v>202</v>
+        <v>361</v>
       </c>
       <c r="R27" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="S27" t="s">
-        <v>6</v>
+        <v>363</v>
       </c>
       <c r="T27" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3187,10 +3196,10 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>220</v>
+        <v>354</v>
       </c>
       <c r="B28" t="s">
-        <v>283</v>
+        <v>251</v>
       </c>
       <c r="C28" t="s">
         <v>2</v>
@@ -3199,7 +3208,7 @@
         <v>3</v>
       </c>
       <c r="E28" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="F28" t="s">
         <v>3</v>
@@ -3217,31 +3226,31 @@
         <v>41</v>
       </c>
       <c r="K28" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="L28" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="M28" t="s">
-        <v>190</v>
+        <v>347</v>
       </c>
       <c r="N28" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="O28" t="s">
         <v>41</v>
       </c>
       <c r="P28" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="Q28" t="s">
         <v>41</v>
       </c>
       <c r="R28" t="s">
-        <v>170</v>
+        <v>349</v>
       </c>
       <c r="S28" t="s">
-        <v>6</v>
+        <v>363</v>
       </c>
       <c r="T28" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3254,10 +3263,10 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>221</v>
+        <v>355</v>
       </c>
       <c r="B29" t="s">
-        <v>283</v>
+        <v>251</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
@@ -3266,7 +3275,7 @@
         <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="F29" t="s">
         <v>3</v>
@@ -3284,31 +3293,31 @@
         <v>41</v>
       </c>
       <c r="K29" t="s">
+        <v>152</v>
+      </c>
+      <c r="L29" t="s">
+        <v>175</v>
+      </c>
+      <c r="M29" t="s">
+        <v>360</v>
+      </c>
+      <c r="N29" t="s">
         <v>159</v>
       </c>
-      <c r="L29" t="s">
-        <v>185</v>
-      </c>
-      <c r="M29" t="s">
-        <v>166</v>
-      </c>
-      <c r="N29" t="s">
-        <v>167</v>
-      </c>
       <c r="O29" t="s">
         <v>41</v>
       </c>
       <c r="P29" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="Q29" t="s">
-        <v>169</v>
+        <v>41</v>
       </c>
       <c r="R29" t="s">
-        <v>170</v>
+        <v>349</v>
       </c>
       <c r="S29" t="s">
-        <v>6</v>
+        <v>363</v>
       </c>
       <c r="T29" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3321,10 +3330,10 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>187</v>
+        <v>356</v>
       </c>
       <c r="B30" t="s">
-        <v>283</v>
+        <v>251</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
@@ -3333,10 +3342,10 @@
         <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="F30" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="G30" t="s">
         <v>3</v>
@@ -3351,31 +3360,31 @@
         <v>41</v>
       </c>
       <c r="K30" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="L30" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="M30" t="s">
-        <v>248</v>
+        <v>223</v>
       </c>
       <c r="N30" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="O30" t="s">
         <v>41</v>
       </c>
       <c r="P30" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="Q30" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="R30" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="S30" t="s">
-        <v>6</v>
+        <v>363</v>
       </c>
       <c r="T30" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3388,10 +3397,10 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>149</v>
+        <v>357</v>
       </c>
       <c r="B31" t="s">
-        <v>283</v>
+        <v>251</v>
       </c>
       <c r="C31" t="s">
         <v>2</v>
@@ -3400,10 +3409,10 @@
         <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="F31" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="G31" t="s">
         <v>2</v>
@@ -3424,16 +3433,16 @@
         <v>41</v>
       </c>
       <c r="M31" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="N31" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="O31" t="s">
         <v>41</v>
       </c>
       <c r="P31" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="Q31" t="s">
         <v>41</v>
@@ -3442,7 +3451,7 @@
         <v>41</v>
       </c>
       <c r="S31" t="s">
-        <v>6</v>
+        <v>363</v>
       </c>
       <c r="T31" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3455,25 +3464,25 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>209</v>
+        <v>358</v>
       </c>
       <c r="B32" t="s">
-        <v>283</v>
+        <v>251</v>
       </c>
       <c r="C32" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D32" t="s">
         <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="F32" t="s">
-        <v>86</v>
+        <v>3</v>
       </c>
       <c r="G32" t="s">
-        <v>86</v>
+        <v>2</v>
       </c>
       <c r="H32" t="s">
         <v>41</v>
@@ -3485,31 +3494,31 @@
         <v>41</v>
       </c>
       <c r="K32" t="s">
-        <v>41</v>
+        <v>152</v>
       </c>
       <c r="L32" t="s">
-        <v>41</v>
+        <v>175</v>
       </c>
       <c r="M32" t="s">
-        <v>217</v>
+        <v>195</v>
       </c>
       <c r="N32" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="O32" t="s">
         <v>41</v>
       </c>
       <c r="P32" t="s">
-        <v>41</v>
+        <v>197</v>
       </c>
       <c r="Q32" t="s">
         <v>41</v>
       </c>
       <c r="R32" t="s">
-        <v>6</v>
+        <v>362</v>
       </c>
       <c r="S32" t="s">
-        <v>6</v>
+        <v>363</v>
       </c>
       <c r="T32" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3517,15 +3526,15 @@
       </c>
       <c r="U32">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>151</v>
+        <v>359</v>
       </c>
       <c r="B33" t="s">
-        <v>283</v>
+        <v>251</v>
       </c>
       <c r="C33" t="s">
         <v>2</v>
@@ -3534,10 +3543,10 @@
         <v>3</v>
       </c>
       <c r="E33" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="F33" t="s">
-        <v>3</v>
+        <v>162</v>
       </c>
       <c r="G33" t="s">
         <v>2</v>
@@ -3552,102 +3561,102 @@
         <v>41</v>
       </c>
       <c r="K33" t="s">
-        <v>159</v>
+        <v>86</v>
       </c>
       <c r="L33" t="s">
-        <v>185</v>
+        <v>86</v>
       </c>
       <c r="M33" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="N33" t="s">
-        <v>211</v>
+        <v>86</v>
       </c>
       <c r="O33" t="s">
         <v>41</v>
       </c>
       <c r="P33" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="Q33" t="s">
         <v>41</v>
       </c>
       <c r="R33" t="s">
-        <v>213</v>
+        <v>6</v>
       </c>
       <c r="S33" t="s">
-        <v>6</v>
+        <v>363</v>
       </c>
       <c r="T33" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U33">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>152</v>
+        <v>110</v>
       </c>
       <c r="B34" t="s">
-        <v>283</v>
+        <v>6</v>
       </c>
       <c r="C34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" t="s">
+        <v>150</v>
+      </c>
+      <c r="G34" t="s">
         <v>3</v>
       </c>
-      <c r="D34" t="s">
+      <c r="H34" t="s">
+        <v>73</v>
+      </c>
+      <c r="I34" t="s">
         <v>3</v>
       </c>
-      <c r="E34" t="s">
-        <v>208</v>
-      </c>
-      <c r="F34" t="s">
-        <v>86</v>
-      </c>
-      <c r="G34" t="s">
-        <v>86</v>
-      </c>
-      <c r="H34" t="s">
-        <v>41</v>
-      </c>
-      <c r="I34" t="s">
-        <v>41</v>
-      </c>
       <c r="J34" t="s">
-        <v>41</v>
+        <v>111</v>
       </c>
       <c r="K34" t="s">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="L34" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="M34" t="s">
-        <v>214</v>
+        <v>114</v>
       </c>
       <c r="N34" t="s">
-        <v>86</v>
+        <v>173</v>
       </c>
       <c r="O34" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="P34" t="s">
-        <v>216</v>
+        <v>111</v>
       </c>
       <c r="Q34" t="s">
         <v>41</v>
       </c>
       <c r="R34" t="s">
-        <v>6</v>
+        <v>190</v>
       </c>
       <c r="S34" t="s">
         <v>6</v>
       </c>
-      <c r="T34" s="8">
+      <c r="T34">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U34">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
@@ -3656,10 +3665,10 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>110</v>
+        <v>249</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>253</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
@@ -3670,49 +3679,10 @@
       <c r="E35" t="s">
         <v>41</v>
       </c>
-      <c r="F35" t="s">
-        <v>157</v>
-      </c>
-      <c r="G35" t="s">
-        <v>3</v>
-      </c>
-      <c r="H35" t="s">
-        <v>73</v>
-      </c>
-      <c r="I35" t="s">
-        <v>3</v>
-      </c>
-      <c r="J35" t="s">
-        <v>111</v>
-      </c>
-      <c r="K35" t="s">
-        <v>112</v>
-      </c>
-      <c r="L35" t="s">
-        <v>113</v>
-      </c>
-      <c r="M35" t="s">
-        <v>114</v>
-      </c>
-      <c r="N35" t="s">
-        <v>183</v>
-      </c>
-      <c r="O35" t="s">
-        <v>83</v>
-      </c>
       <c r="P35" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>41</v>
-      </c>
-      <c r="R35" t="s">
-        <v>204</v>
-      </c>
-      <c r="S35" t="s">
-        <v>6</v>
-      </c>
-      <c r="T35">
+        <v>271</v>
+      </c>
+      <c r="T35" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>0</v>
       </c>
@@ -3723,10 +3693,10 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>281</v>
+        <v>294</v>
       </c>
       <c r="B36" t="s">
-        <v>285</v>
+        <v>253</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
@@ -3738,7 +3708,7 @@
         <v>41</v>
       </c>
       <c r="P36" t="s">
-        <v>303</v>
+        <v>41</v>
       </c>
       <c r="T36" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3751,10 +3721,10 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>326</v>
+        <v>260</v>
       </c>
       <c r="B37" t="s">
-        <v>285</v>
+        <v>261</v>
       </c>
       <c r="C37" t="s">
         <v>2</v>
@@ -3766,7 +3736,7 @@
         <v>41</v>
       </c>
       <c r="P37" t="s">
-        <v>41</v>
+        <v>269</v>
       </c>
       <c r="T37" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3779,10 +3749,10 @@
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>292</v>
+        <v>267</v>
       </c>
       <c r="B38" t="s">
-        <v>293</v>
+        <v>261</v>
       </c>
       <c r="C38" t="s">
         <v>2</v>
@@ -3794,7 +3764,7 @@
         <v>41</v>
       </c>
       <c r="P38" t="s">
-        <v>301</v>
+        <v>41</v>
       </c>
       <c r="T38" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3807,10 +3777,10 @@
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>299</v>
+        <v>256</v>
       </c>
       <c r="B39" t="s">
-        <v>293</v>
+        <v>253</v>
       </c>
       <c r="C39" t="s">
         <v>2</v>
@@ -3822,7 +3792,7 @@
         <v>41</v>
       </c>
       <c r="P39" t="s">
-        <v>41</v>
+        <v>271</v>
       </c>
       <c r="T39" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3835,26 +3805,65 @@
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>288</v>
+        <v>201</v>
       </c>
       <c r="B40" t="s">
-        <v>285</v>
+        <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D40" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E40" t="s">
         <v>41</v>
       </c>
+      <c r="F40" t="s">
+        <v>162</v>
+      </c>
+      <c r="G40" t="s">
+        <v>3</v>
+      </c>
+      <c r="H40" t="s">
+        <v>202</v>
+      </c>
+      <c r="I40" t="s">
+        <v>2</v>
+      </c>
+      <c r="J40" t="s">
+        <v>41</v>
+      </c>
+      <c r="K40" t="s">
+        <v>203</v>
+      </c>
+      <c r="L40" t="s">
+        <v>6</v>
+      </c>
+      <c r="M40" t="s">
+        <v>204</v>
+      </c>
+      <c r="N40" t="s">
+        <v>205</v>
+      </c>
+      <c r="O40" t="s">
+        <v>41</v>
+      </c>
       <c r="P40" t="s">
-        <v>303</v>
+        <v>206</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>207</v>
+      </c>
+      <c r="R40" t="s">
+        <v>208</v>
+      </c>
+      <c r="S40" t="s">
+        <v>6</v>
       </c>
       <c r="T40" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U40">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
@@ -3863,77 +3872,77 @@
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>224</v>
+        <v>0</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>250</v>
       </c>
       <c r="C41" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E41" t="s">
         <v>41</v>
       </c>
       <c r="F41" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="G41" t="s">
         <v>3</v>
       </c>
       <c r="H41" t="s">
-        <v>225</v>
+        <v>73</v>
       </c>
       <c r="I41" t="s">
         <v>2</v>
       </c>
       <c r="J41" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="K41" t="s">
-        <v>226</v>
+        <v>82</v>
       </c>
       <c r="L41" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="M41" t="s">
-        <v>227</v>
+        <v>96</v>
       </c>
       <c r="N41" t="s">
-        <v>228</v>
+        <v>97</v>
       </c>
       <c r="O41" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="P41" t="s">
-        <v>229</v>
+        <v>98</v>
       </c>
       <c r="Q41" t="s">
-        <v>230</v>
+        <v>99</v>
       </c>
       <c r="R41" t="s">
-        <v>231</v>
+        <v>191</v>
       </c>
       <c r="S41" t="s">
         <v>6</v>
       </c>
-      <c r="T41" s="8">
+      <c r="T41">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>1</v>
       </c>
       <c r="U41">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>282</v>
+        <v>250</v>
       </c>
       <c r="C42" t="s">
         <v>2</v>
@@ -3945,7 +3954,7 @@
         <v>41</v>
       </c>
       <c r="F42" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="G42" t="s">
         <v>3</v>
@@ -3957,7 +3966,7 @@
         <v>2</v>
       </c>
       <c r="J42" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="K42" t="s">
         <v>82</v>
@@ -3966,41 +3975,41 @@
         <v>41</v>
       </c>
       <c r="M42" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="N42" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="O42" t="s">
         <v>86</v>
       </c>
       <c r="P42" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="Q42" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="R42" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="S42" t="s">
         <v>6</v>
       </c>
       <c r="T42">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U42">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B43" t="s">
-        <v>282</v>
+        <v>250</v>
       </c>
       <c r="C43" t="s">
         <v>2</v>
@@ -4012,7 +4021,7 @@
         <v>41</v>
       </c>
       <c r="F43" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="G43" t="s">
         <v>3</v>
@@ -4024,7 +4033,7 @@
         <v>2</v>
       </c>
       <c r="J43" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="K43" t="s">
         <v>82</v>
@@ -4033,41 +4042,41 @@
         <v>41</v>
       </c>
       <c r="M43" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="N43" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="O43" t="s">
         <v>86</v>
       </c>
       <c r="P43" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="Q43" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="R43" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="S43" t="s">
         <v>6</v>
       </c>
       <c r="T43">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U43">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>36</v>
+        <v>123</v>
       </c>
       <c r="B44" t="s">
-        <v>282</v>
+        <v>250</v>
       </c>
       <c r="C44" t="s">
         <v>2</v>
@@ -4079,62 +4088,59 @@
         <v>41</v>
       </c>
       <c r="F44" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="G44" t="s">
         <v>3</v>
       </c>
       <c r="H44" t="s">
-        <v>73</v>
+        <v>183</v>
       </c>
       <c r="I44" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J44" t="s">
-        <v>100</v>
+        <v>41</v>
       </c>
       <c r="K44" t="s">
-        <v>82</v>
+        <v>124</v>
       </c>
       <c r="L44" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="M44" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="N44" t="s">
-        <v>102</v>
-      </c>
-      <c r="O44" t="s">
-        <v>86</v>
+        <v>182</v>
       </c>
       <c r="P44" t="s">
-        <v>103</v>
+        <v>181</v>
       </c>
       <c r="Q44" t="s">
-        <v>99</v>
+        <v>6</v>
       </c>
       <c r="R44" t="s">
-        <v>205</v>
+        <v>6</v>
       </c>
       <c r="S44" t="s">
         <v>6</v>
       </c>
       <c r="T44">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U44">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>123</v>
+        <v>38</v>
       </c>
       <c r="B45" t="s">
-        <v>282</v>
+        <v>250</v>
       </c>
       <c r="C45" t="s">
         <v>2</v>
@@ -4146,62 +4152,65 @@
         <v>41</v>
       </c>
       <c r="F45" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="G45" t="s">
         <v>3</v>
       </c>
       <c r="H45" t="s">
-        <v>195</v>
+        <v>73</v>
       </c>
       <c r="I45" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J45" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="K45" t="s">
-        <v>124</v>
+        <v>82</v>
       </c>
       <c r="L45" t="s">
-        <v>125</v>
+        <v>41</v>
       </c>
       <c r="M45" t="s">
-        <v>126</v>
+        <v>84</v>
       </c>
       <c r="N45" t="s">
-        <v>194</v>
+        <v>85</v>
+      </c>
+      <c r="O45" t="s">
+        <v>86</v>
       </c>
       <c r="P45" t="s">
-        <v>193</v>
+        <v>87</v>
       </c>
       <c r="Q45" t="s">
-        <v>6</v>
+        <v>88</v>
       </c>
       <c r="R45" t="s">
-        <v>6</v>
+        <v>191</v>
       </c>
       <c r="S45" t="s">
         <v>6</v>
       </c>
       <c r="T45">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U45">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>38</v>
+        <v>115</v>
       </c>
       <c r="B46" t="s">
-        <v>282</v>
+        <v>250</v>
       </c>
       <c r="C46" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D46" t="s">
         <v>2</v>
@@ -4210,7 +4219,7 @@
         <v>41</v>
       </c>
       <c r="F46" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="G46" t="s">
         <v>3</v>
@@ -4222,7 +4231,7 @@
         <v>2</v>
       </c>
       <c r="J46" t="s">
-        <v>81</v>
+        <v>116</v>
       </c>
       <c r="K46" t="s">
         <v>82</v>
@@ -4231,22 +4240,22 @@
         <v>41</v>
       </c>
       <c r="M46" t="s">
-        <v>84</v>
+        <v>117</v>
       </c>
       <c r="N46" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="O46" t="s">
         <v>86</v>
       </c>
       <c r="P46" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="Q46" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="R46" t="s">
-        <v>205</v>
+        <v>6</v>
       </c>
       <c r="S46" t="s">
         <v>6</v>
@@ -4257,15 +4266,15 @@
       </c>
       <c r="U46">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="B47" t="s">
-        <v>282</v>
+        <v>250</v>
       </c>
       <c r="C47" t="s">
         <v>3</v>
@@ -4277,7 +4286,7 @@
         <v>41</v>
       </c>
       <c r="F47" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="G47" t="s">
         <v>3</v>
@@ -4289,7 +4298,7 @@
         <v>2</v>
       </c>
       <c r="J47" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="K47" t="s">
         <v>82</v>
@@ -4298,16 +4307,16 @@
         <v>41</v>
       </c>
       <c r="M47" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="N47" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="O47" t="s">
         <v>86</v>
       </c>
       <c r="P47" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="Q47" t="s">
         <v>41</v>
@@ -4329,13 +4338,13 @@
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>120</v>
+        <v>262</v>
       </c>
       <c r="B48" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="C48" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D48" t="s">
         <v>2</v>
@@ -4343,51 +4352,12 @@
       <c r="E48" t="s">
         <v>41</v>
       </c>
-      <c r="F48" t="s">
-        <v>157</v>
-      </c>
-      <c r="G48" t="s">
-        <v>3</v>
-      </c>
-      <c r="H48" t="s">
-        <v>73</v>
-      </c>
-      <c r="I48" t="s">
-        <v>2</v>
-      </c>
-      <c r="J48" t="s">
-        <v>81</v>
-      </c>
-      <c r="K48" t="s">
-        <v>82</v>
-      </c>
-      <c r="L48" t="s">
-        <v>41</v>
-      </c>
-      <c r="M48" t="s">
-        <v>121</v>
-      </c>
-      <c r="N48" t="s">
-        <v>122</v>
-      </c>
-      <c r="O48" t="s">
-        <v>86</v>
-      </c>
       <c r="P48" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q48" t="s">
-        <v>41</v>
-      </c>
-      <c r="R48" t="s">
-        <v>6</v>
-      </c>
-      <c r="S48" t="s">
-        <v>6</v>
-      </c>
-      <c r="T48">
+        <v>276</v>
+      </c>
+      <c r="T48" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U48">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
@@ -4396,10 +4366,10 @@
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>294</v>
+        <v>257</v>
       </c>
       <c r="B49" t="s">
-        <v>300</v>
+        <v>253</v>
       </c>
       <c r="C49" t="s">
         <v>2</v>
@@ -4411,7 +4381,7 @@
         <v>41</v>
       </c>
       <c r="P49" t="s">
-        <v>308</v>
+        <v>270</v>
       </c>
       <c r="T49" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -4424,10 +4394,10 @@
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="B50" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="C50" t="s">
         <v>2</v>
@@ -4438,8 +4408,47 @@
       <c r="E50" t="s">
         <v>41</v>
       </c>
+      <c r="F50" t="s">
+        <v>3</v>
+      </c>
+      <c r="G50" t="s">
+        <v>2</v>
+      </c>
+      <c r="H50" t="s">
+        <v>268</v>
+      </c>
+      <c r="I50" t="s">
+        <v>41</v>
+      </c>
+      <c r="J50" t="s">
+        <v>41</v>
+      </c>
+      <c r="K50" t="s">
+        <v>6</v>
+      </c>
+      <c r="L50" t="s">
+        <v>6</v>
+      </c>
+      <c r="M50" t="s">
+        <v>307</v>
+      </c>
+      <c r="N50" t="s">
+        <v>308</v>
+      </c>
+      <c r="O50" t="s">
+        <v>309</v>
+      </c>
       <c r="P50" t="s">
-        <v>302</v>
+        <v>310</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>311</v>
+      </c>
+      <c r="R50" t="s">
+        <v>6</v>
+      </c>
+      <c r="S50" t="s">
+        <v>6</v>
       </c>
       <c r="T50" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -4447,15 +4456,15 @@
       </c>
       <c r="U50">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>309</v>
+        <v>258</v>
       </c>
       <c r="B51" t="s">
-        <v>300</v>
+        <v>261</v>
       </c>
       <c r="C51" t="s">
         <v>2</v>
@@ -4466,81 +4475,14 @@
       <c r="E51" t="s">
         <v>41</v>
       </c>
-      <c r="F51" t="s">
-        <v>3</v>
-      </c>
-      <c r="G51" t="s">
-        <v>2</v>
-      </c>
-      <c r="H51" t="s">
-        <v>300</v>
-      </c>
-      <c r="I51" t="s">
-        <v>41</v>
-      </c>
-      <c r="J51" t="s">
-        <v>41</v>
-      </c>
-      <c r="K51" t="s">
-        <v>6</v>
-      </c>
-      <c r="L51" t="s">
-        <v>6</v>
-      </c>
-      <c r="M51" t="s">
-        <v>339</v>
-      </c>
-      <c r="N51" t="s">
-        <v>340</v>
-      </c>
-      <c r="O51" t="s">
-        <v>341</v>
-      </c>
       <c r="P51" t="s">
-        <v>342</v>
-      </c>
-      <c r="Q51" t="s">
-        <v>343</v>
-      </c>
-      <c r="R51" t="s">
-        <v>6</v>
-      </c>
-      <c r="S51" t="s">
-        <v>6</v>
+        <v>278</v>
       </c>
       <c r="T51" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>0</v>
       </c>
       <c r="U51">
-        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>290</v>
-      </c>
-      <c r="B52" t="s">
-        <v>293</v>
-      </c>
-      <c r="C52" t="s">
-        <v>2</v>
-      </c>
-      <c r="D52" t="s">
-        <v>2</v>
-      </c>
-      <c r="E52" t="s">
-        <v>41</v>
-      </c>
-      <c r="P52" t="s">
-        <v>310</v>
-      </c>
-      <c r="T52" s="8">
-        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="U52">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
         <v>0</v>
       </c>
@@ -4555,11 +4497,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4578,7 +4521,7 @@
         <v>140</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>271</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4592,7 +4535,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>272</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4680,14 +4623,14 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>215</v>
+      <c r="A9" t="s">
+        <v>359</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>364</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>6</v>
+        <v>365</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>6</v>
@@ -4695,10 +4638,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>232</v>
+        <v>209</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>6</v>
@@ -4708,32 +4651,14 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>274</v>
-      </c>
+      <c r="A11" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4748,9 +4673,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4800,12 +4726,12 @@
         <v>144</v>
       </c>
       <c r="N1" t="s">
-        <v>252</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>286</v>
+        <v>254</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -4820,7 +4746,7 @@
         <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>317</v>
+        <v>285</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
@@ -4829,7 +4755,7 @@
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>363</v>
+        <v>331</v>
       </c>
       <c r="J2" t="s">
         <v>41</v>
@@ -4853,7 +4779,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>286</v>
+        <v>254</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -4867,8 +4793,8 @@
       <c r="E3" s="1">
         <v>110</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>319</v>
+      <c r="F3" s="11" t="s">
+        <v>287</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
@@ -4877,7 +4803,7 @@
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>364</v>
+        <v>332</v>
       </c>
       <c r="J3" t="s">
         <v>41</v>
@@ -4901,7 +4827,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>286</v>
+        <v>254</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -4916,7 +4842,7 @@
         <v>111</v>
       </c>
       <c r="F4" t="s">
-        <v>321</v>
+        <v>289</v>
       </c>
       <c r="G4" t="s">
         <v>6</v>
@@ -4925,7 +4851,7 @@
         <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>364</v>
+        <v>332</v>
       </c>
       <c r="J4" t="s">
         <v>41</v>
@@ -4949,7 +4875,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>286</v>
+        <v>254</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -4964,19 +4890,19 @@
         <v>700</v>
       </c>
       <c r="F5" t="s">
-        <v>317</v>
+        <v>285</v>
       </c>
       <c r="G5" t="s">
-        <v>355</v>
+        <v>323</v>
       </c>
       <c r="H5" t="s">
         <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>363</v>
+        <v>331</v>
       </c>
       <c r="J5" t="s">
-        <v>357</v>
+        <v>325</v>
       </c>
       <c r="K5" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
@@ -4997,7 +4923,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>286</v>
+        <v>254</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -5012,19 +4938,19 @@
         <v>700</v>
       </c>
       <c r="F6" t="s">
-        <v>317</v>
+        <v>285</v>
       </c>
       <c r="G6" t="s">
-        <v>356</v>
+        <v>324</v>
       </c>
       <c r="H6" t="s">
         <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>363</v>
+        <v>331</v>
       </c>
       <c r="J6" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="K6" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
@@ -5045,7 +4971,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>286</v>
+        <v>254</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -5060,19 +4986,19 @@
         <v>700</v>
       </c>
       <c r="F7" t="s">
-        <v>317</v>
+        <v>285</v>
       </c>
       <c r="G7" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="H7" t="s">
         <v>20</v>
       </c>
       <c r="I7" t="s">
-        <v>365</v>
+        <v>333</v>
       </c>
       <c r="J7" t="s">
-        <v>360</v>
+        <v>328</v>
       </c>
       <c r="K7" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
@@ -5093,7 +5019,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>286</v>
+        <v>254</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
@@ -5108,19 +5034,19 @@
         <v>700</v>
       </c>
       <c r="F8" t="s">
-        <v>317</v>
+        <v>285</v>
       </c>
       <c r="G8" t="s">
-        <v>362</v>
+        <v>330</v>
       </c>
       <c r="H8" t="s">
         <v>20</v>
       </c>
       <c r="I8" t="s">
-        <v>363</v>
+        <v>331</v>
       </c>
       <c r="J8" t="s">
-        <v>361</v>
+        <v>329</v>
       </c>
       <c r="K8" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
@@ -5141,7 +5067,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>276</v>
+        <v>244</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -5156,7 +5082,7 @@
         <v>100</v>
       </c>
       <c r="F9" t="s">
-        <v>317</v>
+        <v>285</v>
       </c>
       <c r="G9" t="s">
         <v>6</v>
@@ -5165,7 +5091,7 @@
         <v>20</v>
       </c>
       <c r="I9" t="s">
-        <v>366</v>
+        <v>334</v>
       </c>
       <c r="J9" t="s">
         <v>41</v>
@@ -5189,7 +5115,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>276</v>
+        <v>244</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
@@ -5203,8 +5129,8 @@
       <c r="E10" s="1">
         <v>110</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>319</v>
+      <c r="F10" s="11" t="s">
+        <v>287</v>
       </c>
       <c r="G10" t="s">
         <v>6</v>
@@ -5213,7 +5139,7 @@
         <v>20</v>
       </c>
       <c r="I10" t="s">
-        <v>367</v>
+        <v>335</v>
       </c>
       <c r="J10" t="s">
         <v>41</v>
@@ -5237,7 +5163,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>276</v>
+        <v>244</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
@@ -5252,7 +5178,7 @@
         <v>111</v>
       </c>
       <c r="F11" t="s">
-        <v>321</v>
+        <v>289</v>
       </c>
       <c r="G11" t="s">
         <v>6</v>
@@ -5261,7 +5187,7 @@
         <v>20</v>
       </c>
       <c r="I11" t="s">
-        <v>368</v>
+        <v>336</v>
       </c>
       <c r="J11" t="s">
         <v>41</v>
@@ -5285,7 +5211,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>323</v>
+        <v>291</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -5300,7 +5226,7 @@
         <v>100</v>
       </c>
       <c r="F12" t="s">
-        <v>322</v>
+        <v>290</v>
       </c>
       <c r="G12" t="s">
         <v>6</v>
@@ -5309,7 +5235,7 @@
         <v>5</v>
       </c>
       <c r="I12" t="s">
-        <v>327</v>
+        <v>295</v>
       </c>
       <c r="J12" t="s">
         <v>41</v>
@@ -5333,7 +5259,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>323</v>
+        <v>291</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
@@ -5348,7 +5274,7 @@
         <v>110</v>
       </c>
       <c r="F13" t="s">
-        <v>322</v>
+        <v>290</v>
       </c>
       <c r="G13" t="s">
         <v>6</v>
@@ -5357,7 +5283,7 @@
         <v>5</v>
       </c>
       <c r="I13" t="s">
-        <v>327</v>
+        <v>295</v>
       </c>
       <c r="J13" t="s">
         <v>41</v>
@@ -5381,7 +5307,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>323</v>
+        <v>291</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
@@ -5396,7 +5322,7 @@
         <v>111</v>
       </c>
       <c r="F14" t="s">
-        <v>328</v>
+        <v>296</v>
       </c>
       <c r="G14" t="s">
         <v>6</v>
@@ -5405,7 +5331,7 @@
         <v>5</v>
       </c>
       <c r="I14" t="s">
-        <v>327</v>
+        <v>295</v>
       </c>
       <c r="J14" t="s">
         <v>41</v>
@@ -5438,13 +5364,13 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="E15" s="1">
         <v>946</v>
       </c>
       <c r="F15" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="G15" t="s">
         <v>6</v>
@@ -5486,7 +5412,7 @@
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="E16" s="1">
         <v>909</v>
@@ -5582,7 +5508,7 @@
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>6</v>
@@ -5618,7 +5544,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>278</v>
+        <v>246</v>
       </c>
       <c r="B19" t="s">
         <v>1</v>
@@ -5633,19 +5559,19 @@
         <v>100</v>
       </c>
       <c r="F19" t="s">
-        <v>317</v>
+        <v>285</v>
       </c>
       <c r="G19" t="s">
-        <v>371</v>
+        <v>339</v>
       </c>
       <c r="H19" t="s">
         <v>5</v>
       </c>
       <c r="I19" t="s">
-        <v>366</v>
+        <v>334</v>
       </c>
       <c r="J19" t="s">
-        <v>329</v>
+        <v>297</v>
       </c>
       <c r="K19" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
@@ -5666,7 +5592,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>278</v>
+        <v>246</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
@@ -5681,16 +5607,16 @@
         <v>700</v>
       </c>
       <c r="F20" t="s">
-        <v>317</v>
+        <v>285</v>
       </c>
       <c r="G20" t="s">
-        <v>371</v>
+        <v>339</v>
       </c>
       <c r="H20" t="s">
         <v>5</v>
       </c>
       <c r="I20" t="s">
-        <v>366</v>
+        <v>334</v>
       </c>
       <c r="J20" t="s">
         <v>41</v>
@@ -5714,7 +5640,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>278</v>
+        <v>246</v>
       </c>
       <c r="B21" t="s">
         <v>1</v>
@@ -5728,17 +5654,17 @@
       <c r="E21" s="1">
         <v>710</v>
       </c>
-      <c r="F21" s="12" t="s">
-        <v>319</v>
+      <c r="F21" s="11" t="s">
+        <v>287</v>
       </c>
       <c r="G21" t="s">
-        <v>371</v>
+        <v>339</v>
       </c>
       <c r="H21" t="s">
         <v>5</v>
       </c>
       <c r="I21" t="s">
-        <v>367</v>
+        <v>335</v>
       </c>
       <c r="J21" t="s">
         <v>41</v>
@@ -5762,7 +5688,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>279</v>
+        <v>247</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
@@ -5777,19 +5703,19 @@
         <v>100</v>
       </c>
       <c r="F22" t="s">
-        <v>317</v>
+        <v>285</v>
       </c>
       <c r="G22" t="s">
-        <v>372</v>
+        <v>340</v>
       </c>
       <c r="H22" t="s">
         <v>5</v>
       </c>
       <c r="I22" t="s">
-        <v>367</v>
+        <v>335</v>
       </c>
       <c r="J22" t="s">
-        <v>330</v>
+        <v>298</v>
       </c>
       <c r="K22" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
@@ -5810,7 +5736,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>279</v>
+        <v>247</v>
       </c>
       <c r="B23" t="s">
         <v>1</v>
@@ -5825,16 +5751,16 @@
         <v>700</v>
       </c>
       <c r="F23" t="s">
-        <v>317</v>
+        <v>285</v>
       </c>
       <c r="G23" t="s">
-        <v>372</v>
+        <v>340</v>
       </c>
       <c r="H23" t="s">
         <v>5</v>
       </c>
       <c r="I23" t="s">
-        <v>367</v>
+        <v>335</v>
       </c>
       <c r="J23" t="s">
         <v>41</v>
@@ -5858,7 +5784,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>154</v>
+        <v>341</v>
       </c>
       <c r="B24" t="s">
         <v>53</v>
@@ -5873,10 +5799,10 @@
         <v>999</v>
       </c>
       <c r="F24" t="s">
-        <v>351</v>
+        <v>319</v>
       </c>
       <c r="G24" t="s">
-        <v>352</v>
+        <v>320</v>
       </c>
       <c r="H24" t="s">
         <v>20</v>
@@ -5889,7 +5815,7 @@
       </c>
       <c r="K24" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>holdings_call_numberUNC999hijkmi1=9 AND i2=3 AND $0=#{holdings_record_id} AND $2='852'</v>
+        <v>call_no (holdings)UNC999hijkmi1=9 AND i2=3 AND $0=#{holdings_record_id} AND $2='852'</v>
       </c>
       <c r="L24" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5906,7 +5832,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>222</v>
+        <v>342</v>
       </c>
       <c r="B25" t="s">
         <v>53</v>
@@ -5921,23 +5847,23 @@
         <v>999</v>
       </c>
       <c r="F25" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="G25" t="s">
-        <v>347</v>
+        <v>315</v>
       </c>
       <c r="H25" t="s">
-        <v>344</v>
+        <v>312</v>
       </c>
       <c r="I25" t="s">
-        <v>349</v>
+        <v>317</v>
       </c>
       <c r="J25" t="s">
         <v>41</v>
       </c>
       <c r="K25" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>holdings_location_libraryUNC999bi1=9 and i2=2</v>
+        <v>loc_b (holdings)UNC999bi1=9 and i2=2</v>
       </c>
       <c r="L25" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5954,7 +5880,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>223</v>
+        <v>343</v>
       </c>
       <c r="B26" t="s">
         <v>53</v>
@@ -5969,20 +5895,20 @@
         <v>999</v>
       </c>
       <c r="F26" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="G26" t="s">
-        <v>347</v>
+        <v>315</v>
       </c>
       <c r="H26" t="s">
         <v>5</v>
       </c>
       <c r="I26" t="s">
-        <v>348</v>
+        <v>316</v>
       </c>
       <c r="K26" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>holdings_location_shelfUNC999bi1=9 and i2=2</v>
+        <v>loc_n (holdings)UNC999bi1=9 and i2=2</v>
       </c>
       <c r="L26" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -5999,7 +5925,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>219</v>
+        <v>346</v>
       </c>
       <c r="B27" t="s">
         <v>53</v>
@@ -6014,10 +5940,10 @@
         <v>999</v>
       </c>
       <c r="F27" t="s">
-        <v>353</v>
+        <v>321</v>
       </c>
       <c r="G27" t="s">
-        <v>352</v>
+        <v>320</v>
       </c>
       <c r="H27" t="s">
         <v>5</v>
@@ -6030,7 +5956,7 @@
       </c>
       <c r="K27" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>holdings_noteUNC999lzi1=9 AND i2=3 AND $0=#{holdings_record_id} AND $2='852'</v>
+        <v>notes (holdings)UNC999lzi1=9 AND i2=3 AND $0=#{holdings_record_id} AND $2='852'</v>
       </c>
       <c r="L27" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6047,7 +5973,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>153</v>
+        <v>344</v>
       </c>
       <c r="B28" t="s">
         <v>53</v>
@@ -6065,7 +5991,7 @@
         <v>7</v>
       </c>
       <c r="G28" t="s">
-        <v>354</v>
+        <v>322</v>
       </c>
       <c r="H28" t="s">
         <v>5</v>
@@ -6078,7 +6004,7 @@
       </c>
       <c r="K28" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>holdings_record_idUNC999a(i1=9 AND i2=2) AND $c &gt; 0</v>
+        <v>rec_id (holdings)UNC999a(i1=9 AND i2=2) AND $c &gt; 0</v>
       </c>
       <c r="L28" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6095,7 +6021,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>247</v>
+        <v>345</v>
       </c>
       <c r="B29" t="s">
         <v>53</v>
@@ -6113,7 +6039,7 @@
         <v>7</v>
       </c>
       <c r="G29" t="s">
-        <v>350</v>
+        <v>318</v>
       </c>
       <c r="H29" t="s">
         <v>5</v>
@@ -6126,7 +6052,7 @@
       </c>
       <c r="K29" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>holdings_summaryUNC999ai1=9 AND i2=3 AND $0=#{holdings_record_id} AND $2='866'</v>
+        <v>summary (holdings)UNC999ai1=9 AND i2=3 AND $0=#{holdings_record_id} AND $2='866'</v>
       </c>
       <c r="L29" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6143,7 +6069,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>150</v>
+        <v>351</v>
       </c>
       <c r="B30" t="s">
         <v>53</v>
@@ -6158,23 +6084,23 @@
         <v>999</v>
       </c>
       <c r="F30" t="s">
-        <v>253</v>
+        <v>228</v>
       </c>
       <c r="G30" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="H30" t="s">
         <v>20</v>
       </c>
       <c r="I30" t="s">
-        <v>255</v>
+        <v>230</v>
       </c>
       <c r="J30" t="s">
         <v>6</v>
       </c>
       <c r="K30" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_call_numberUNC999qvci1=9 AND i2=1</v>
+        <v>call_no (items)UNC999qvci1=9 AND i2=1</v>
       </c>
       <c r="L30" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6191,7 +6117,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>148</v>
+        <v>353</v>
       </c>
       <c r="B31" t="s">
         <v>53</v>
@@ -6206,10 +6132,10 @@
         <v>999</v>
       </c>
       <c r="F31" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="G31" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="H31" t="s">
         <v>5</v>
@@ -6218,11 +6144,11 @@
         <v>6</v>
       </c>
       <c r="J31" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="K31" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_due_dateUNC999di1=9 AND i2=1</v>
+        <v>due_date (items)UNC999di1=9 AND i2=1</v>
       </c>
       <c r="L31" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6239,7 +6165,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>220</v>
+        <v>354</v>
       </c>
       <c r="B32" t="s">
         <v>53</v>
@@ -6254,23 +6180,23 @@
         <v>999</v>
       </c>
       <c r="F32" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="G32" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="H32" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
       <c r="I32" t="s">
-        <v>348</v>
+        <v>316</v>
       </c>
       <c r="J32" t="s">
         <v>6</v>
       </c>
       <c r="K32" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_location_libraryUNC999li1=9 AND i2=1</v>
+        <v>loc_b (items)UNC999li1=9 AND i2=1</v>
       </c>
       <c r="L32" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6287,7 +6213,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>220</v>
+        <v>354</v>
       </c>
       <c r="B33" t="s">
         <v>53</v>
@@ -6302,23 +6228,23 @@
         <v>999</v>
       </c>
       <c r="F33" t="s">
-        <v>264</v>
+        <v>239</v>
       </c>
       <c r="G33" t="s">
-        <v>261</v>
+        <v>236</v>
       </c>
       <c r="H33" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
       <c r="I33" t="s">
-        <v>348</v>
+        <v>316</v>
       </c>
       <c r="J33" t="s">
         <v>6</v>
       </c>
       <c r="K33" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_location_libraryUNC999fi1=9 AND i2=4 AND NOT EXIST (tag=999 AND i1=9 and i2=1)</v>
+        <v>loc_b (items)UNC999fi1=9 AND i2=4 AND NOT EXIST (tag=999 AND i1=9 and i2=1)</v>
       </c>
       <c r="L33" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6335,7 +6261,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>221</v>
+        <v>355</v>
       </c>
       <c r="B34" t="s">
         <v>53</v>
@@ -6350,23 +6276,23 @@
         <v>999</v>
       </c>
       <c r="F34" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="G34" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="H34" t="s">
         <v>5</v>
       </c>
       <c r="I34" t="s">
-        <v>348</v>
+        <v>316</v>
       </c>
       <c r="J34" t="s">
         <v>6</v>
       </c>
       <c r="K34" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_location_shelfUNC999li1=9 AND i2=1</v>
+        <v>loc_n (items)UNC999li1=9 AND i2=1</v>
       </c>
       <c r="L34" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6383,7 +6309,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>221</v>
+        <v>355</v>
       </c>
       <c r="B35" t="s">
         <v>53</v>
@@ -6398,23 +6324,23 @@
         <v>999</v>
       </c>
       <c r="F35" t="s">
-        <v>264</v>
+        <v>239</v>
       </c>
       <c r="G35" t="s">
-        <v>261</v>
+        <v>236</v>
       </c>
       <c r="H35" t="s">
         <v>5</v>
       </c>
       <c r="I35" t="s">
-        <v>348</v>
+        <v>316</v>
       </c>
       <c r="J35" t="s">
         <v>6</v>
       </c>
       <c r="K35" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_location_shelfUNC999fi1=9 AND i2=4 AND NOT EXIST (tag=999 AND i1=9 and i2=1)</v>
+        <v>loc_n (items)UNC999fi1=9 AND i2=4 AND NOT EXIST (tag=999 AND i1=9 and i2=1)</v>
       </c>
       <c r="L35" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6431,7 +6357,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>187</v>
+        <v>356</v>
       </c>
       <c r="B36" t="s">
         <v>53</v>
@@ -6449,7 +6375,7 @@
         <v>2</v>
       </c>
       <c r="G36" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="H36" t="s">
         <v>5</v>
@@ -6462,7 +6388,7 @@
       </c>
       <c r="K36" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_noteUNC999ni1=9 AND i2=1</v>
+        <v>notes (items)UNC999ni1=9 AND i2=1</v>
       </c>
       <c r="L36" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6479,7 +6405,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>149</v>
+        <v>357</v>
       </c>
       <c r="B37" t="s">
         <v>53</v>
@@ -6494,10 +6420,10 @@
         <v>999</v>
       </c>
       <c r="F37" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="G37" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="H37" t="s">
         <v>5</v>
@@ -6510,7 +6436,7 @@
       </c>
       <c r="K37" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_record_idUNC999ii1=9 AND i2=1</v>
+        <v>rec_id (items)UNC999ii1=9 AND i2=1</v>
       </c>
       <c r="L37" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6527,7 +6453,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>151</v>
+        <v>358</v>
       </c>
       <c r="B38" t="s">
         <v>53</v>
@@ -6542,13 +6468,13 @@
         <v>999</v>
       </c>
       <c r="F38" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="G38" t="s">
-        <v>256</v>
+        <v>231</v>
       </c>
       <c r="H38" t="s">
-        <v>257</v>
+        <v>232</v>
       </c>
       <c r="I38" t="s">
         <v>6</v>
@@ -6558,7 +6484,7 @@
       </c>
       <c r="K38" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_statusUNC999di1=9 AND i2=1 and $d IS NOT blank</v>
+        <v>status (items)UNC999di1=9 AND i2=1 and $d IS NOT blank</v>
       </c>
       <c r="L38" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6575,7 +6501,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>151</v>
+        <v>358</v>
       </c>
       <c r="B39" t="s">
         <v>53</v>
@@ -6590,23 +6516,23 @@
         <v>999</v>
       </c>
       <c r="F39" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="G39" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="H39" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
       <c r="I39" t="s">
-        <v>260</v>
+        <v>235</v>
       </c>
       <c r="J39" t="s">
         <v>6</v>
       </c>
       <c r="K39" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_statusUNC999si1=9 AND i2=1 and $d IS blank</v>
+        <v>status (items)UNC999si1=9 AND i2=1 and $d IS blank</v>
       </c>
       <c r="L39" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6623,7 +6549,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>151</v>
+        <v>358</v>
       </c>
       <c r="B40" t="s">
         <v>53</v>
@@ -6641,20 +6567,20 @@
         <v>7</v>
       </c>
       <c r="G40" t="s">
-        <v>261</v>
+        <v>236</v>
       </c>
       <c r="H40" t="s">
-        <v>262</v>
+        <v>237</v>
       </c>
       <c r="I40" t="s">
         <v>6</v>
       </c>
       <c r="J40" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
       <c r="K40" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>item_statusUNC999ai1=9 AND i2=4 AND NOT EXIST (tag=999 AND i1=9 and i2=1)</v>
+        <v>status (items)UNC999ai1=9 AND i2=4 AND NOT EXIST (tag=999 AND i1=9 and i2=1)</v>
       </c>
       <c r="L40" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9503,7 +9429,7 @@
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>309</v>
+        <v>277</v>
       </c>
       <c r="B100" t="s">
         <v>1</v>
@@ -9518,7 +9444,7 @@
         <v>100</v>
       </c>
       <c r="F100" t="s">
-        <v>318</v>
+        <v>286</v>
       </c>
       <c r="G100" t="s">
         <v>6</v>
@@ -9527,10 +9453,10 @@
         <v>20</v>
       </c>
       <c r="I100" t="s">
-        <v>369</v>
+        <v>337</v>
       </c>
       <c r="J100" t="s">
-        <v>316</v>
+        <v>284</v>
       </c>
       <c r="K100" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
@@ -9551,7 +9477,7 @@
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>309</v>
+        <v>277</v>
       </c>
       <c r="B101" t="s">
         <v>1</v>
@@ -9566,7 +9492,7 @@
         <v>110</v>
       </c>
       <c r="F101" t="s">
-        <v>320</v>
+        <v>288</v>
       </c>
       <c r="G101" t="s">
         <v>6</v>
@@ -9575,10 +9501,10 @@
         <v>20</v>
       </c>
       <c r="I101" t="s">
-        <v>370</v>
+        <v>338</v>
       </c>
       <c r="J101" t="s">
-        <v>316</v>
+        <v>284</v>
       </c>
       <c r="K101" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
@@ -9599,7 +9525,7 @@
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>309</v>
+        <v>277</v>
       </c>
       <c r="B102" t="s">
         <v>1</v>
@@ -9614,7 +9540,7 @@
         <v>111</v>
       </c>
       <c r="F102" t="s">
-        <v>320</v>
+        <v>288</v>
       </c>
       <c r="G102" t="s">
         <v>6</v>
@@ -9623,10 +9549,10 @@
         <v>20</v>
       </c>
       <c r="I102" t="s">
-        <v>370</v>
+        <v>338</v>
       </c>
       <c r="J102" t="s">
-        <v>316</v>
+        <v>284</v>
       </c>
       <c r="K102" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
@@ -9661,9 +9587,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9773,7 +9700,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -9782,7 +9709,7 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add top level items and holdings fields
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -10,7 +10,6 @@
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="5910"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20265" windowHeight="6450"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1713" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="371">
   <si>
     <t>subject_chronological_facet</t>
   </si>
@@ -1135,6 +1134,12 @@
   </si>
   <si>
     <t>Create documentation in this repo</t>
+  </si>
+  <si>
+    <t>Array of holdings elements, each representing a holdings record attached to the bib. Each holdings element is an an escaped JSON string</t>
+  </si>
+  <si>
+    <t>Array of item elements, each representing an item record attached to the bib. Each item element is an an escaped JSON string</t>
   </si>
 </sst>
 </file>
@@ -1412,8 +1417,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="fields" displayName="fields" ref="A1:U51" totalsRowShown="0">
-  <autoFilter ref="A1:U51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="fields" displayName="fields" ref="A1:U53" totalsRowShown="0">
+  <autoFilter ref="A1:U53"/>
+  <sortState ref="A2:U51">
+    <sortCondition ref="A1:A51"/>
+  </sortState>
   <tableColumns count="21">
     <tableColumn id="2" name="field"/>
     <tableColumn id="22" name="category"/>
@@ -1772,17 +1780,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U51"/>
+  <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A3" sqref="A3"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <pane xSplit="1" ySplit="15" topLeftCell="N16" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1938,10 +1940,10 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>366</v>
+        <v>341</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>252</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -1950,77 +1952,110 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>200</v>
       </c>
       <c r="F3" t="s">
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="G3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="I3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J3" t="s">
-        <v>240</v>
+        <v>41</v>
       </c>
       <c r="K3" t="s">
-        <v>82</v>
+        <v>211</v>
       </c>
       <c r="L3" t="s">
-        <v>41</v>
+        <v>175</v>
       </c>
       <c r="M3" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="N3" t="s">
-        <v>367</v>
+        <v>185</v>
       </c>
       <c r="O3" t="s">
         <v>41</v>
       </c>
       <c r="P3" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="Q3" t="s">
         <v>41</v>
       </c>
       <c r="R3" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="S3" t="s">
-        <v>6</v>
+        <v>350</v>
       </c>
       <c r="T3" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U3">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>248</v>
+        <v>351</v>
       </c>
       <c r="B4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>194</v>
+      </c>
+      <c r="F4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>177</v>
+      </c>
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" t="s">
+        <v>152</v>
+      </c>
+      <c r="L4" t="s">
+        <v>175</v>
+      </c>
+      <c r="M4" t="s">
+        <v>178</v>
+      </c>
+      <c r="N4" t="s">
+        <v>212</v>
+      </c>
+      <c r="O4" t="s">
+        <v>6</v>
       </c>
       <c r="P4" t="s">
-        <v>271</v>
+        <v>187</v>
+      </c>
+      <c r="S4" t="s">
+        <v>363</v>
       </c>
       <c r="T4" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2028,27 +2063,66 @@
       </c>
       <c r="U4">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>293</v>
+        <v>352</v>
       </c>
       <c r="B5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
+        <v>194</v>
+      </c>
+      <c r="F5" t="s">
+        <v>150</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" t="s">
+        <v>184</v>
+      </c>
+      <c r="N5" t="s">
+        <v>186</v>
+      </c>
+      <c r="O5" t="s">
         <v>41</v>
       </c>
       <c r="P5" t="s">
-        <v>41</v>
+        <v>229</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>41</v>
+      </c>
+      <c r="R5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S5" t="s">
+        <v>363</v>
       </c>
       <c r="T5" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2061,7 +2135,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B6" t="s">
         <v>253</v>
@@ -2089,7 +2163,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B7" t="s">
         <v>253</v>
@@ -2117,7 +2191,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B8" t="s">
         <v>253</v>
@@ -2131,41 +2205,8 @@
       <c r="E8" t="s">
         <v>41</v>
       </c>
-      <c r="F8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" t="s">
-        <v>279</v>
-      </c>
-      <c r="I8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" t="s">
-        <v>313</v>
-      </c>
-      <c r="K8" t="s">
-        <v>6</v>
-      </c>
-      <c r="L8" t="s">
-        <v>6</v>
-      </c>
-      <c r="M8" t="s">
-        <v>280</v>
-      </c>
-      <c r="N8" t="s">
-        <v>281</v>
-      </c>
-      <c r="O8" t="s">
-        <v>6</v>
-      </c>
       <c r="P8" t="s">
-        <v>275</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>41</v>
+        <v>271</v>
       </c>
       <c r="T8" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2173,12 +2214,12 @@
       </c>
       <c r="U8">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B9" t="s">
         <v>253</v>
@@ -2192,36 +2233,6 @@
       <c r="E9" t="s">
         <v>41</v>
       </c>
-      <c r="F9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" t="s">
-        <v>41</v>
-      </c>
-      <c r="J9" t="s">
-        <v>41</v>
-      </c>
-      <c r="K9" t="s">
-        <v>6</v>
-      </c>
-      <c r="L9" t="s">
-        <v>6</v>
-      </c>
-      <c r="M9" t="s">
-        <v>282</v>
-      </c>
-      <c r="N9" t="s">
-        <v>283</v>
-      </c>
-      <c r="O9" t="s">
-        <v>41</v>
-      </c>
       <c r="P9" t="s">
         <v>41</v>
       </c>
@@ -2231,82 +2242,76 @@
       </c>
       <c r="U9">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>244</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>253</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
       </c>
       <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
         <v>3</v>
       </c>
-      <c r="E10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" t="s">
-        <v>150</v>
-      </c>
       <c r="G10" t="s">
         <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>73</v>
+        <v>279</v>
       </c>
       <c r="I10" t="s">
         <v>41</v>
       </c>
       <c r="J10" t="s">
-        <v>104</v>
+        <v>313</v>
       </c>
       <c r="K10" t="s">
-        <v>105</v>
+        <v>6</v>
       </c>
       <c r="L10" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="M10" t="s">
-        <v>106</v>
+        <v>280</v>
       </c>
       <c r="N10" t="s">
-        <v>107</v>
+        <v>281</v>
       </c>
       <c r="O10" t="s">
-        <v>83</v>
+        <v>6</v>
       </c>
       <c r="P10" t="s">
-        <v>108</v>
+        <v>275</v>
       </c>
       <c r="Q10" t="s">
         <v>41</v>
       </c>
-      <c r="R10" t="s">
-        <v>109</v>
-      </c>
-      <c r="S10" t="s">
-        <v>6</v>
-      </c>
-      <c r="T10">
+      <c r="T10" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>0</v>
       </c>
       <c r="U10">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>263</v>
+        <v>291</v>
       </c>
       <c r="B11" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -2317,8 +2322,38 @@
       <c r="E11" t="s">
         <v>41</v>
       </c>
+      <c r="F11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" t="s">
+        <v>41</v>
+      </c>
+      <c r="K11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" t="s">
+        <v>6</v>
+      </c>
+      <c r="M11" t="s">
+        <v>282</v>
+      </c>
+      <c r="N11" t="s">
+        <v>283</v>
+      </c>
+      <c r="O11" t="s">
+        <v>41</v>
+      </c>
       <c r="P11" t="s">
-        <v>269</v>
+        <v>41</v>
       </c>
       <c r="T11" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2326,43 +2361,82 @@
       </c>
       <c r="U11">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>265</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>261</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E12" t="s">
         <v>41</v>
       </c>
+      <c r="F12" t="s">
+        <v>150</v>
+      </c>
+      <c r="G12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>73</v>
+      </c>
+      <c r="I12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J12" t="s">
+        <v>104</v>
+      </c>
+      <c r="K12" t="s">
+        <v>105</v>
+      </c>
+      <c r="L12" t="s">
+        <v>41</v>
+      </c>
+      <c r="M12" t="s">
+        <v>106</v>
+      </c>
+      <c r="N12" t="s">
+        <v>107</v>
+      </c>
+      <c r="O12" t="s">
+        <v>83</v>
+      </c>
       <c r="P12" t="s">
-        <v>41</v>
-      </c>
-      <c r="T12" s="8">
+        <v>108</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>41</v>
+      </c>
+      <c r="R12" t="s">
+        <v>109</v>
+      </c>
+      <c r="S12" t="s">
+        <v>6</v>
+      </c>
+      <c r="T12">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>0</v>
       </c>
       <c r="U12">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>246</v>
+        <v>263</v>
       </c>
       <c r="B13" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
@@ -2373,44 +2447,8 @@
       <c r="E13" t="s">
         <v>41</v>
       </c>
-      <c r="F13" t="s">
-        <v>162</v>
-      </c>
-      <c r="G13" t="s">
-        <v>3</v>
-      </c>
-      <c r="H13" t="s">
-        <v>279</v>
-      </c>
-      <c r="I13" t="s">
-        <v>3</v>
-      </c>
-      <c r="J13" t="s">
-        <v>313</v>
-      </c>
-      <c r="K13" t="s">
-        <v>6</v>
-      </c>
-      <c r="L13" t="s">
-        <v>6</v>
-      </c>
-      <c r="M13" t="s">
-        <v>299</v>
-      </c>
-      <c r="N13" t="s">
-        <v>300</v>
-      </c>
-      <c r="O13" t="s">
-        <v>306</v>
-      </c>
       <c r="P13" t="s">
-        <v>272</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>304</v>
-      </c>
-      <c r="R13" t="s">
-        <v>6</v>
+        <v>269</v>
       </c>
       <c r="T13" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2418,15 +2456,15 @@
       </c>
       <c r="U13">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B14" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
@@ -2438,7 +2476,7 @@
         <v>41</v>
       </c>
       <c r="P14" t="s">
-        <v>273</v>
+        <v>41</v>
       </c>
       <c r="T14" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2451,7 +2489,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B15" t="s">
         <v>253</v>
@@ -2466,7 +2504,7 @@
         <v>41</v>
       </c>
       <c r="F15" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="G15" t="s">
         <v>3</v>
@@ -2481,25 +2519,25 @@
         <v>313</v>
       </c>
       <c r="K15" t="s">
-        <v>301</v>
+        <v>6</v>
       </c>
       <c r="L15" t="s">
         <v>6</v>
       </c>
       <c r="M15" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="N15" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="O15" t="s">
         <v>306</v>
       </c>
       <c r="P15" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="Q15" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="R15" t="s">
         <v>6</v>
@@ -2510,66 +2548,27 @@
       </c>
       <c r="U15">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>341</v>
+        <v>264</v>
       </c>
       <c r="B16" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>200</v>
-      </c>
-      <c r="F16" t="s">
-        <v>150</v>
-      </c>
-      <c r="G16" t="s">
-        <v>2</v>
-      </c>
-      <c r="H16" t="s">
-        <v>41</v>
-      </c>
-      <c r="I16" t="s">
-        <v>6</v>
-      </c>
-      <c r="J16" t="s">
-        <v>41</v>
-      </c>
-      <c r="K16" t="s">
-        <v>211</v>
-      </c>
-      <c r="L16" t="s">
-        <v>175</v>
-      </c>
-      <c r="M16" t="s">
-        <v>221</v>
-      </c>
-      <c r="N16" t="s">
-        <v>185</v>
-      </c>
-      <c r="O16" t="s">
         <v>41</v>
       </c>
       <c r="P16" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>41</v>
-      </c>
-      <c r="R16" t="s">
-        <v>6</v>
-      </c>
-      <c r="S16" t="s">
-        <v>350</v>
+        <v>273</v>
       </c>
       <c r="T16" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2577,15 +2576,15 @@
       </c>
       <c r="U16">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>342</v>
+        <v>353</v>
       </c>
       <c r="B17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -2594,10 +2593,10 @@
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="F17" t="s">
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="G17" t="s">
         <v>2</v>
@@ -2606,37 +2605,37 @@
         <v>41</v>
       </c>
       <c r="I17" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="J17" t="s">
         <v>41</v>
       </c>
       <c r="K17" t="s">
-        <v>211</v>
+        <v>152</v>
       </c>
       <c r="L17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M17" t="s">
-        <v>347</v>
+        <v>153</v>
       </c>
       <c r="N17" t="s">
-        <v>215</v>
+        <v>154</v>
       </c>
       <c r="O17" t="s">
         <v>41</v>
       </c>
       <c r="P17" t="s">
-        <v>216</v>
+        <v>155</v>
       </c>
       <c r="Q17" t="s">
-        <v>41</v>
+        <v>361</v>
       </c>
       <c r="R17" t="s">
-        <v>349</v>
+        <v>156</v>
       </c>
       <c r="S17" t="s">
-        <v>350</v>
+        <v>363</v>
       </c>
       <c r="T17" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2649,61 +2648,58 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>343</v>
+        <v>247</v>
       </c>
       <c r="B18" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
       </c>
       <c r="D18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" t="s">
+        <v>150</v>
+      </c>
+      <c r="G18" t="s">
         <v>3</v>
       </c>
-      <c r="E18" t="s">
-        <v>200</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="H18" t="s">
+        <v>279</v>
+      </c>
+      <c r="I18" t="s">
         <v>3</v>
       </c>
-      <c r="G18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H18" t="s">
-        <v>41</v>
-      </c>
-      <c r="I18" t="s">
-        <v>6</v>
-      </c>
       <c r="J18" t="s">
-        <v>41</v>
+        <v>313</v>
       </c>
       <c r="K18" t="s">
-        <v>211</v>
+        <v>301</v>
       </c>
       <c r="L18" t="s">
-        <v>175</v>
+        <v>6</v>
       </c>
       <c r="M18" t="s">
-        <v>348</v>
+        <v>302</v>
       </c>
       <c r="N18" t="s">
-        <v>217</v>
+        <v>303</v>
       </c>
       <c r="O18" t="s">
-        <v>41</v>
+        <v>306</v>
       </c>
       <c r="P18" t="s">
-        <v>218</v>
+        <v>271</v>
       </c>
       <c r="Q18" t="s">
-        <v>41</v>
+        <v>305</v>
       </c>
       <c r="R18" t="s">
-        <v>349</v>
-      </c>
-      <c r="S18" t="s">
-        <v>350</v>
+        <v>6</v>
       </c>
       <c r="T18" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2711,66 +2707,27 @@
       </c>
       <c r="U18">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>346</v>
+        <v>259</v>
       </c>
       <c r="B19" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>200</v>
-      </c>
-      <c r="F19" t="s">
-        <v>162</v>
-      </c>
-      <c r="G19" t="s">
-        <v>3</v>
-      </c>
-      <c r="H19" t="s">
-        <v>41</v>
-      </c>
-      <c r="I19" t="s">
-        <v>3</v>
-      </c>
-      <c r="J19" t="s">
-        <v>41</v>
-      </c>
-      <c r="K19" t="s">
-        <v>211</v>
-      </c>
-      <c r="L19" t="s">
-        <v>175</v>
-      </c>
-      <c r="M19" t="s">
-        <v>224</v>
-      </c>
-      <c r="N19" t="s">
-        <v>225</v>
-      </c>
-      <c r="O19" t="s">
         <v>41</v>
       </c>
       <c r="P19" t="s">
-        <v>226</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>41</v>
-      </c>
-      <c r="R19" t="s">
-        <v>6</v>
-      </c>
-      <c r="S19" t="s">
-        <v>350</v>
+        <v>269</v>
       </c>
       <c r="T19" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2778,66 +2735,27 @@
       </c>
       <c r="U19">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>344</v>
+        <v>266</v>
       </c>
       <c r="B20" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>200</v>
-      </c>
-      <c r="F20" t="s">
-        <v>162</v>
-      </c>
-      <c r="G20" t="s">
-        <v>2</v>
-      </c>
-      <c r="H20" t="s">
-        <v>41</v>
-      </c>
-      <c r="I20" t="s">
-        <v>6</v>
-      </c>
-      <c r="J20" t="s">
-        <v>41</v>
-      </c>
-      <c r="K20" t="s">
-        <v>41</v>
-      </c>
-      <c r="L20" t="s">
-        <v>41</v>
-      </c>
-      <c r="M20" t="s">
-        <v>219</v>
-      </c>
-      <c r="N20" t="s">
-        <v>220</v>
-      </c>
-      <c r="O20" t="s">
         <v>41</v>
       </c>
       <c r="P20" t="s">
         <v>41</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>41</v>
-      </c>
-      <c r="R20" t="s">
-        <v>6</v>
-      </c>
-      <c r="S20" t="s">
-        <v>350</v>
       </c>
       <c r="T20" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2845,66 +2763,27 @@
       </c>
       <c r="U20">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>345</v>
+        <v>255</v>
       </c>
       <c r="B21" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>200</v>
-      </c>
-      <c r="F21" t="s">
-        <v>162</v>
-      </c>
-      <c r="G21" t="s">
-        <v>2</v>
-      </c>
-      <c r="H21" t="s">
-        <v>41</v>
-      </c>
-      <c r="I21" t="s">
-        <v>6</v>
-      </c>
-      <c r="J21" t="s">
-        <v>41</v>
-      </c>
-      <c r="K21" t="s">
-        <v>211</v>
-      </c>
-      <c r="L21" t="s">
-        <v>175</v>
-      </c>
-      <c r="M21" t="s">
-        <v>210</v>
-      </c>
-      <c r="N21" t="s">
-        <v>213</v>
-      </c>
-      <c r="O21" t="s">
         <v>41</v>
       </c>
       <c r="P21" t="s">
-        <v>214</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>41</v>
-      </c>
-      <c r="R21" t="s">
-        <v>6</v>
-      </c>
-      <c r="S21" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
       <c r="T21" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2912,27 +2791,66 @@
       </c>
       <c r="U21">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>259</v>
+        <v>194</v>
       </c>
       <c r="B22" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E22" t="s">
         <v>41</v>
       </c>
+      <c r="F22" t="s">
+        <v>150</v>
+      </c>
+      <c r="G22" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I22" t="s">
+        <v>3</v>
+      </c>
+      <c r="J22" t="s">
+        <v>41</v>
+      </c>
+      <c r="K22" t="s">
+        <v>152</v>
+      </c>
+      <c r="L22" t="s">
+        <v>41</v>
+      </c>
+      <c r="M22" t="s">
+        <v>370</v>
+      </c>
+      <c r="N22" t="s">
+        <v>6</v>
+      </c>
+      <c r="O22" t="s">
+        <v>41</v>
+      </c>
       <c r="P22" t="s">
-        <v>269</v>
+        <v>41</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>41</v>
+      </c>
+      <c r="R22" t="s">
+        <v>41</v>
+      </c>
+      <c r="S22" t="s">
+        <v>363</v>
       </c>
       <c r="T22" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2945,22 +2863,61 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>266</v>
+        <v>200</v>
       </c>
       <c r="B23" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E23" t="s">
         <v>41</v>
       </c>
+      <c r="F23" t="s">
+        <v>150</v>
+      </c>
+      <c r="G23" t="s">
+        <v>3</v>
+      </c>
+      <c r="H23" t="s">
+        <v>41</v>
+      </c>
+      <c r="I23" t="s">
+        <v>3</v>
+      </c>
+      <c r="J23" t="s">
+        <v>41</v>
+      </c>
+      <c r="K23" t="s">
+        <v>152</v>
+      </c>
+      <c r="L23" t="s">
+        <v>41</v>
+      </c>
+      <c r="M23" t="s">
+        <v>369</v>
+      </c>
+      <c r="N23" t="s">
+        <v>6</v>
+      </c>
+      <c r="O23" t="s">
+        <v>41</v>
+      </c>
       <c r="P23" t="s">
         <v>41</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>41</v>
+      </c>
+      <c r="R23" t="s">
+        <v>41</v>
+      </c>
+      <c r="S23" t="s">
+        <v>350</v>
       </c>
       <c r="T23" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2973,10 +2930,10 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>255</v>
+        <v>110</v>
       </c>
       <c r="B24" t="s">
-        <v>253</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
@@ -2987,10 +2944,49 @@
       <c r="E24" t="s">
         <v>41</v>
       </c>
+      <c r="F24" t="s">
+        <v>150</v>
+      </c>
+      <c r="G24" t="s">
+        <v>3</v>
+      </c>
+      <c r="H24" t="s">
+        <v>73</v>
+      </c>
+      <c r="I24" t="s">
+        <v>3</v>
+      </c>
+      <c r="J24" t="s">
+        <v>111</v>
+      </c>
+      <c r="K24" t="s">
+        <v>112</v>
+      </c>
+      <c r="L24" t="s">
+        <v>113</v>
+      </c>
+      <c r="M24" t="s">
+        <v>114</v>
+      </c>
+      <c r="N24" t="s">
+        <v>173</v>
+      </c>
+      <c r="O24" t="s">
+        <v>83</v>
+      </c>
       <c r="P24" t="s">
-        <v>271</v>
-      </c>
-      <c r="T24" s="8">
+        <v>111</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>41</v>
+      </c>
+      <c r="R24" t="s">
+        <v>190</v>
+      </c>
+      <c r="S24" t="s">
+        <v>6</v>
+      </c>
+      <c r="T24">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>0</v>
       </c>
@@ -3001,10 +2997,10 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="B25" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
@@ -3013,43 +3009,49 @@
         <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="F25" t="s">
-        <v>150</v>
+        <v>3</v>
       </c>
       <c r="G25" t="s">
         <v>2</v>
       </c>
       <c r="H25" t="s">
-        <v>177</v>
+        <v>41</v>
       </c>
       <c r="I25" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="J25" t="s">
         <v>41</v>
       </c>
       <c r="K25" t="s">
-        <v>152</v>
+        <v>211</v>
       </c>
       <c r="L25" t="s">
         <v>175</v>
       </c>
       <c r="M25" t="s">
-        <v>178</v>
+        <v>347</v>
       </c>
       <c r="N25" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="O25" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="P25" t="s">
-        <v>187</v>
+        <v>216</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>41</v>
+      </c>
+      <c r="R25" t="s">
+        <v>349</v>
       </c>
       <c r="S25" t="s">
-        <v>363</v>
+        <v>350</v>
       </c>
       <c r="T25" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3062,7 +3064,7 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B26" t="s">
         <v>251</v>
@@ -3077,7 +3079,7 @@
         <v>194</v>
       </c>
       <c r="F26" t="s">
-        <v>150</v>
+        <v>3</v>
       </c>
       <c r="G26" t="s">
         <v>2</v>
@@ -3092,28 +3094,28 @@
         <v>41</v>
       </c>
       <c r="K26" t="s">
-        <v>41</v>
+        <v>152</v>
       </c>
       <c r="L26" t="s">
-        <v>41</v>
+        <v>175</v>
       </c>
       <c r="M26" t="s">
-        <v>184</v>
+        <v>347</v>
       </c>
       <c r="N26" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="O26" t="s">
         <v>41</v>
       </c>
       <c r="P26" t="s">
-        <v>229</v>
+        <v>180</v>
       </c>
       <c r="Q26" t="s">
         <v>41</v>
       </c>
       <c r="R26" t="s">
-        <v>41</v>
+        <v>349</v>
       </c>
       <c r="S26" t="s">
         <v>363</v>
@@ -3124,15 +3126,15 @@
       </c>
       <c r="U26">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="B27" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
@@ -3141,10 +3143,10 @@
         <v>3</v>
       </c>
       <c r="E27" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="F27" t="s">
-        <v>150</v>
+        <v>3</v>
       </c>
       <c r="G27" t="s">
         <v>2</v>
@@ -3153,37 +3155,37 @@
         <v>41</v>
       </c>
       <c r="I27" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="J27" t="s">
         <v>41</v>
       </c>
       <c r="K27" t="s">
-        <v>152</v>
+        <v>211</v>
       </c>
       <c r="L27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M27" t="s">
-        <v>153</v>
+        <v>348</v>
       </c>
       <c r="N27" t="s">
-        <v>154</v>
+        <v>217</v>
       </c>
       <c r="O27" t="s">
         <v>41</v>
       </c>
       <c r="P27" t="s">
-        <v>155</v>
+        <v>218</v>
       </c>
       <c r="Q27" t="s">
-        <v>361</v>
+        <v>41</v>
       </c>
       <c r="R27" t="s">
-        <v>156</v>
+        <v>349</v>
       </c>
       <c r="S27" t="s">
-        <v>363</v>
+        <v>350</v>
       </c>
       <c r="T27" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3196,7 +3198,7 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B28" t="s">
         <v>251</v>
@@ -3232,16 +3234,16 @@
         <v>175</v>
       </c>
       <c r="M28" t="s">
-        <v>347</v>
+        <v>360</v>
       </c>
       <c r="N28" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="O28" t="s">
         <v>41</v>
       </c>
       <c r="P28" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="Q28" t="s">
         <v>41</v>
@@ -3263,10 +3265,10 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>355</v>
+        <v>366</v>
       </c>
       <c r="B29" t="s">
-        <v>251</v>
+        <v>6</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
@@ -3275,65 +3277,65 @@
         <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>194</v>
+        <v>41</v>
       </c>
       <c r="F29" t="s">
         <v>3</v>
       </c>
       <c r="G29" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H29" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="I29" t="s">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="J29" t="s">
-        <v>41</v>
+        <v>240</v>
       </c>
       <c r="K29" t="s">
-        <v>152</v>
+        <v>82</v>
       </c>
       <c r="L29" t="s">
-        <v>175</v>
+        <v>41</v>
       </c>
       <c r="M29" t="s">
-        <v>360</v>
+        <v>241</v>
       </c>
       <c r="N29" t="s">
-        <v>159</v>
+        <v>367</v>
       </c>
       <c r="O29" t="s">
         <v>41</v>
       </c>
       <c r="P29" t="s">
-        <v>160</v>
+        <v>240</v>
       </c>
       <c r="Q29" t="s">
         <v>41</v>
       </c>
       <c r="R29" t="s">
-        <v>349</v>
+        <v>41</v>
       </c>
       <c r="S29" t="s">
-        <v>363</v>
+        <v>6</v>
       </c>
       <c r="T29" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U29">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="B30" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
@@ -3342,7 +3344,7 @@
         <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="F30" t="s">
         <v>162</v>
@@ -3360,31 +3362,31 @@
         <v>41</v>
       </c>
       <c r="K30" t="s">
-        <v>152</v>
+        <v>211</v>
       </c>
       <c r="L30" t="s">
         <v>175</v>
       </c>
       <c r="M30" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="N30" t="s">
-        <v>163</v>
+        <v>225</v>
       </c>
       <c r="O30" t="s">
         <v>41</v>
       </c>
       <c r="P30" t="s">
-        <v>164</v>
+        <v>226</v>
       </c>
       <c r="Q30" t="s">
         <v>41</v>
       </c>
       <c r="R30" t="s">
-        <v>188</v>
+        <v>6</v>
       </c>
       <c r="S30" t="s">
-        <v>363</v>
+        <v>350</v>
       </c>
       <c r="T30" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3397,7 +3399,7 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B31" t="s">
         <v>251</v>
@@ -3415,40 +3417,40 @@
         <v>162</v>
       </c>
       <c r="G31" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H31" t="s">
         <v>41</v>
       </c>
       <c r="I31" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="J31" t="s">
         <v>41</v>
       </c>
       <c r="K31" t="s">
-        <v>2</v>
+        <v>152</v>
       </c>
       <c r="L31" t="s">
-        <v>41</v>
+        <v>175</v>
       </c>
       <c r="M31" t="s">
-        <v>148</v>
+        <v>223</v>
       </c>
       <c r="N31" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="O31" t="s">
         <v>41</v>
       </c>
       <c r="P31" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="Q31" t="s">
         <v>41</v>
       </c>
       <c r="R31" t="s">
-        <v>41</v>
+        <v>188</v>
       </c>
       <c r="S31" t="s">
         <v>363</v>
@@ -3464,61 +3466,22 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>358</v>
+        <v>249</v>
       </c>
       <c r="B32" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C32" t="s">
         <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>194</v>
-      </c>
-      <c r="F32" t="s">
-        <v>3</v>
-      </c>
-      <c r="G32" t="s">
-        <v>2</v>
-      </c>
-      <c r="H32" t="s">
-        <v>41</v>
-      </c>
-      <c r="I32" t="s">
-        <v>41</v>
-      </c>
-      <c r="J32" t="s">
-        <v>41</v>
-      </c>
-      <c r="K32" t="s">
-        <v>152</v>
-      </c>
-      <c r="L32" t="s">
-        <v>175</v>
-      </c>
-      <c r="M32" t="s">
-        <v>195</v>
-      </c>
-      <c r="N32" t="s">
-        <v>196</v>
-      </c>
-      <c r="O32" t="s">
         <v>41</v>
       </c>
       <c r="P32" t="s">
-        <v>197</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>41</v>
-      </c>
-      <c r="R32" t="s">
-        <v>362</v>
-      </c>
-      <c r="S32" t="s">
-        <v>363</v>
+        <v>271</v>
       </c>
       <c r="T32" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3526,70 +3489,31 @@
       </c>
       <c r="U32">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>359</v>
+        <v>294</v>
       </c>
       <c r="B33" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C33" t="s">
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E33" t="s">
-        <v>194</v>
-      </c>
-      <c r="F33" t="s">
-        <v>162</v>
-      </c>
-      <c r="G33" t="s">
-        <v>2</v>
-      </c>
-      <c r="H33" t="s">
-        <v>41</v>
-      </c>
-      <c r="I33" t="s">
-        <v>41</v>
-      </c>
-      <c r="J33" t="s">
-        <v>41</v>
-      </c>
-      <c r="K33" t="s">
-        <v>86</v>
-      </c>
-      <c r="L33" t="s">
-        <v>86</v>
-      </c>
-      <c r="M33" t="s">
-        <v>198</v>
-      </c>
-      <c r="N33" t="s">
-        <v>86</v>
-      </c>
-      <c r="O33" t="s">
         <v>41</v>
       </c>
       <c r="P33" t="s">
-        <v>199</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>41</v>
-      </c>
-      <c r="R33" t="s">
-        <v>6</v>
-      </c>
-      <c r="S33" t="s">
-        <v>363</v>
+        <v>41</v>
       </c>
       <c r="T33" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U33">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
@@ -3598,89 +3522,128 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>110</v>
+        <v>344</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>252</v>
       </c>
       <c r="C34" t="s">
         <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>41</v>
+        <v>200</v>
       </c>
       <c r="F34" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="G34" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H34" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="I34" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J34" t="s">
-        <v>111</v>
+        <v>41</v>
       </c>
       <c r="K34" t="s">
-        <v>112</v>
+        <v>41</v>
       </c>
       <c r="L34" t="s">
-        <v>113</v>
+        <v>41</v>
       </c>
       <c r="M34" t="s">
-        <v>114</v>
+        <v>219</v>
       </c>
       <c r="N34" t="s">
-        <v>173</v>
+        <v>220</v>
       </c>
       <c r="O34" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="P34" t="s">
-        <v>111</v>
+        <v>41</v>
       </c>
       <c r="Q34" t="s">
         <v>41</v>
       </c>
       <c r="R34" t="s">
-        <v>190</v>
+        <v>6</v>
       </c>
       <c r="S34" t="s">
-        <v>6</v>
-      </c>
-      <c r="T34">
+        <v>350</v>
+      </c>
+      <c r="T34" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>0</v>
       </c>
       <c r="U34">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>249</v>
+        <v>357</v>
       </c>
       <c r="B35" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E35" t="s">
+        <v>194</v>
+      </c>
+      <c r="F35" t="s">
+        <v>162</v>
+      </c>
+      <c r="G35" t="s">
+        <v>2</v>
+      </c>
+      <c r="H35" t="s">
+        <v>41</v>
+      </c>
+      <c r="I35" t="s">
+        <v>41</v>
+      </c>
+      <c r="J35" t="s">
+        <v>41</v>
+      </c>
+      <c r="K35" t="s">
+        <v>2</v>
+      </c>
+      <c r="L35" t="s">
+        <v>41</v>
+      </c>
+      <c r="M35" t="s">
+        <v>148</v>
+      </c>
+      <c r="N35" t="s">
+        <v>174</v>
+      </c>
+      <c r="O35" t="s">
         <v>41</v>
       </c>
       <c r="P35" t="s">
-        <v>271</v>
+        <v>149</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>41</v>
+      </c>
+      <c r="R35" t="s">
+        <v>41</v>
+      </c>
+      <c r="S35" t="s">
+        <v>363</v>
       </c>
       <c r="T35" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3688,15 +3651,15 @@
       </c>
       <c r="U35">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>294</v>
+        <v>260</v>
       </c>
       <c r="B36" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
@@ -3708,7 +3671,7 @@
         <v>41</v>
       </c>
       <c r="P36" t="s">
-        <v>41</v>
+        <v>269</v>
       </c>
       <c r="T36" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3721,7 +3684,7 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="B37" t="s">
         <v>261</v>
@@ -3736,7 +3699,7 @@
         <v>41</v>
       </c>
       <c r="P37" t="s">
-        <v>269</v>
+        <v>41</v>
       </c>
       <c r="T37" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3749,10 +3712,10 @@
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="B38" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C38" t="s">
         <v>2</v>
@@ -3764,7 +3727,7 @@
         <v>41</v>
       </c>
       <c r="P38" t="s">
-        <v>41</v>
+        <v>271</v>
       </c>
       <c r="T38" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3777,26 +3740,65 @@
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>256</v>
+        <v>201</v>
       </c>
       <c r="B39" t="s">
-        <v>253</v>
+        <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D39" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E39" t="s">
         <v>41</v>
       </c>
+      <c r="F39" t="s">
+        <v>162</v>
+      </c>
+      <c r="G39" t="s">
+        <v>3</v>
+      </c>
+      <c r="H39" t="s">
+        <v>202</v>
+      </c>
+      <c r="I39" t="s">
+        <v>2</v>
+      </c>
+      <c r="J39" t="s">
+        <v>41</v>
+      </c>
+      <c r="K39" t="s">
+        <v>203</v>
+      </c>
+      <c r="L39" t="s">
+        <v>6</v>
+      </c>
+      <c r="M39" t="s">
+        <v>204</v>
+      </c>
+      <c r="N39" t="s">
+        <v>205</v>
+      </c>
+      <c r="O39" t="s">
+        <v>41</v>
+      </c>
       <c r="P39" t="s">
-        <v>271</v>
+        <v>206</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>207</v>
+      </c>
+      <c r="R39" t="s">
+        <v>208</v>
+      </c>
+      <c r="S39" t="s">
+        <v>6</v>
       </c>
       <c r="T39" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U39">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
@@ -3805,69 +3807,69 @@
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>201</v>
+        <v>358</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>251</v>
       </c>
       <c r="C40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D40" t="s">
         <v>3</v>
       </c>
       <c r="E40" t="s">
-        <v>41</v>
+        <v>194</v>
       </c>
       <c r="F40" t="s">
-        <v>162</v>
+        <v>3</v>
       </c>
       <c r="G40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H40" t="s">
-        <v>202</v>
+        <v>41</v>
       </c>
       <c r="I40" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="J40" t="s">
         <v>41</v>
       </c>
       <c r="K40" t="s">
-        <v>203</v>
+        <v>152</v>
       </c>
       <c r="L40" t="s">
-        <v>6</v>
+        <v>175</v>
       </c>
       <c r="M40" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="N40" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="O40" t="s">
         <v>41</v>
       </c>
       <c r="P40" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="Q40" t="s">
-        <v>207</v>
+        <v>41</v>
       </c>
       <c r="R40" t="s">
-        <v>208</v>
+        <v>362</v>
       </c>
       <c r="S40" t="s">
-        <v>6</v>
+        <v>363</v>
       </c>
       <c r="T40" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U40">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
@@ -4338,22 +4340,61 @@
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>262</v>
+        <v>345</v>
       </c>
       <c r="B48" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E48" t="s">
+        <v>200</v>
+      </c>
+      <c r="F48" t="s">
+        <v>162</v>
+      </c>
+      <c r="G48" t="s">
+        <v>2</v>
+      </c>
+      <c r="H48" t="s">
+        <v>41</v>
+      </c>
+      <c r="I48" t="s">
+        <v>6</v>
+      </c>
+      <c r="J48" t="s">
+        <v>41</v>
+      </c>
+      <c r="K48" t="s">
+        <v>211</v>
+      </c>
+      <c r="L48" t="s">
+        <v>175</v>
+      </c>
+      <c r="M48" t="s">
+        <v>210</v>
+      </c>
+      <c r="N48" t="s">
+        <v>213</v>
+      </c>
+      <c r="O48" t="s">
         <v>41</v>
       </c>
       <c r="P48" t="s">
-        <v>276</v>
+        <v>214</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>41</v>
+      </c>
+      <c r="R48" t="s">
+        <v>6</v>
+      </c>
+      <c r="S48" t="s">
+        <v>350</v>
       </c>
       <c r="T48" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -4361,15 +4402,15 @@
       </c>
       <c r="U48">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="B49" t="s">
-        <v>253</v>
+        <v>268</v>
       </c>
       <c r="C49" t="s">
         <v>2</v>
@@ -4381,7 +4422,7 @@
         <v>41</v>
       </c>
       <c r="P49" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="T49" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -4394,10 +4435,10 @@
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>277</v>
+        <v>257</v>
       </c>
       <c r="B50" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="C50" t="s">
         <v>2</v>
@@ -4408,47 +4449,8 @@
       <c r="E50" t="s">
         <v>41</v>
       </c>
-      <c r="F50" t="s">
-        <v>3</v>
-      </c>
-      <c r="G50" t="s">
-        <v>2</v>
-      </c>
-      <c r="H50" t="s">
-        <v>268</v>
-      </c>
-      <c r="I50" t="s">
-        <v>41</v>
-      </c>
-      <c r="J50" t="s">
-        <v>41</v>
-      </c>
-      <c r="K50" t="s">
-        <v>6</v>
-      </c>
-      <c r="L50" t="s">
-        <v>6</v>
-      </c>
-      <c r="M50" t="s">
-        <v>307</v>
-      </c>
-      <c r="N50" t="s">
-        <v>308</v>
-      </c>
-      <c r="O50" t="s">
-        <v>309</v>
-      </c>
       <c r="P50" t="s">
-        <v>310</v>
-      </c>
-      <c r="Q50" t="s">
-        <v>311</v>
-      </c>
-      <c r="R50" t="s">
-        <v>6</v>
-      </c>
-      <c r="S50" t="s">
-        <v>6</v>
+        <v>270</v>
       </c>
       <c r="T50" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -4456,33 +4458,167 @@
       </c>
       <c r="U50">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>258</v>
+        <v>359</v>
       </c>
       <c r="B51" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="C51" t="s">
         <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E51" t="s">
+        <v>194</v>
+      </c>
+      <c r="F51" t="s">
+        <v>162</v>
+      </c>
+      <c r="G51" t="s">
+        <v>2</v>
+      </c>
+      <c r="H51" t="s">
+        <v>41</v>
+      </c>
+      <c r="I51" t="s">
+        <v>41</v>
+      </c>
+      <c r="J51" t="s">
+        <v>41</v>
+      </c>
+      <c r="K51" t="s">
+        <v>86</v>
+      </c>
+      <c r="L51" t="s">
+        <v>86</v>
+      </c>
+      <c r="M51" t="s">
+        <v>198</v>
+      </c>
+      <c r="N51" t="s">
+        <v>86</v>
+      </c>
+      <c r="O51" t="s">
         <v>41</v>
       </c>
       <c r="P51" t="s">
-        <v>278</v>
+        <v>199</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>41</v>
+      </c>
+      <c r="R51" t="s">
+        <v>6</v>
+      </c>
+      <c r="S51" t="s">
+        <v>363</v>
       </c>
       <c r="T51" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U51">
+        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>277</v>
+      </c>
+      <c r="B52" t="s">
+        <v>268</v>
+      </c>
+      <c r="C52" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" t="s">
+        <v>2</v>
+      </c>
+      <c r="E52" t="s">
+        <v>41</v>
+      </c>
+      <c r="F52" t="s">
+        <v>3</v>
+      </c>
+      <c r="G52" t="s">
+        <v>2</v>
+      </c>
+      <c r="H52" t="s">
+        <v>268</v>
+      </c>
+      <c r="I52" t="s">
+        <v>41</v>
+      </c>
+      <c r="J52" t="s">
+        <v>41</v>
+      </c>
+      <c r="K52" t="s">
+        <v>6</v>
+      </c>
+      <c r="L52" t="s">
+        <v>6</v>
+      </c>
+      <c r="M52" t="s">
+        <v>307</v>
+      </c>
+      <c r="N52" t="s">
+        <v>308</v>
+      </c>
+      <c r="O52" t="s">
+        <v>309</v>
+      </c>
+      <c r="P52" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>311</v>
+      </c>
+      <c r="R52" t="s">
+        <v>6</v>
+      </c>
+      <c r="S52" t="s">
+        <v>6</v>
+      </c>
+      <c r="T52" s="8">
+        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U52">
+        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>258</v>
+      </c>
+      <c r="B53" t="s">
+        <v>261</v>
+      </c>
+      <c r="C53" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" t="s">
+        <v>2</v>
+      </c>
+      <c r="E53" t="s">
+        <v>41</v>
+      </c>
+      <c r="P53" t="s">
+        <v>278</v>
+      </c>
+      <c r="T53" s="8">
+        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U53">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
         <v>0</v>
       </c>
@@ -4502,7 +4638,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4676,7 +4811,6 @@
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A41" sqref="A41"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9590,7 +9724,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
add location facet helper spreadsheet
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -1418,10 +1418,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="fields" displayName="fields" ref="A1:U53" totalsRowShown="0">
-  <autoFilter ref="A1:U53"/>
-  <sortState ref="A2:U51">
-    <sortCondition ref="A1:A51"/>
-  </sortState>
+  <autoFilter ref="A1:U53">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="holdings data"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="21">
     <tableColumn id="2" name="field"/>
     <tableColumn id="22" name="category"/>
@@ -1783,8 +1786,8 @@
   <dimension ref="A1:U53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U23" sqref="U23"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1871,7 +1874,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>254</v>
       </c>
@@ -2005,7 +2008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>351</v>
       </c>
@@ -2066,7 +2069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>352</v>
       </c>
@@ -2133,7 +2136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>248</v>
       </c>
@@ -2161,7 +2164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>293</v>
       </c>
@@ -2189,7 +2192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>245</v>
       </c>
@@ -2217,7 +2220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>292</v>
       </c>
@@ -2245,7 +2248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>244</v>
       </c>
@@ -2306,7 +2309,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>291</v>
       </c>
@@ -2364,7 +2367,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -2431,7 +2434,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>263</v>
       </c>
@@ -2459,7 +2462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>265</v>
       </c>
@@ -2487,7 +2490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>246</v>
       </c>
@@ -2551,7 +2554,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>264</v>
       </c>
@@ -2579,7 +2582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>353</v>
       </c>
@@ -2646,7 +2649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>247</v>
       </c>
@@ -2710,7 +2713,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>259</v>
       </c>
@@ -2738,7 +2741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>266</v>
       </c>
@@ -2766,7 +2769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>255</v>
       </c>
@@ -2794,7 +2797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>194</v>
       </c>
@@ -2928,7 +2931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>110</v>
       </c>
@@ -3062,7 +3065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>354</v>
       </c>
@@ -3196,7 +3199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>355</v>
       </c>
@@ -3263,7 +3266,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>366</v>
       </c>
@@ -3397,7 +3400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>356</v>
       </c>
@@ -3464,7 +3467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>249</v>
       </c>
@@ -3492,7 +3495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>294</v>
       </c>
@@ -3587,7 +3590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>357</v>
       </c>
@@ -3654,7 +3657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>260</v>
       </c>
@@ -3682,7 +3685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>267</v>
       </c>
@@ -3710,7 +3713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>256</v>
       </c>
@@ -3738,7 +3741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>201</v>
       </c>
@@ -3805,7 +3808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>358</v>
       </c>
@@ -3872,7 +3875,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -3939,7 +3942,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -4006,7 +4009,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -4073,7 +4076,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>123</v>
       </c>
@@ -4137,7 +4140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>38</v>
       </c>
@@ -4204,7 +4207,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>115</v>
       </c>
@@ -4271,7 +4274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>120</v>
       </c>
@@ -4405,7 +4408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>262</v>
       </c>
@@ -4433,7 +4436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>257</v>
       </c>
@@ -4461,7 +4464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>359</v>
       </c>
@@ -4528,7 +4531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>277</v>
       </c>
@@ -4595,7 +4598,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>258</v>
       </c>

</xml_diff>

<commit_message>
update item/holdings rec_id subelement names
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1747" uniqueCount="369">
   <si>
     <t>subject_chronological_facet</t>
   </si>
@@ -1061,9 +1061,6 @@
     <t>loc_n (holdings)</t>
   </si>
   <si>
-    <t>rec_id (holdings)</t>
-  </si>
-  <si>
     <t>summary (holdings)</t>
   </si>
   <si>
@@ -1100,9 +1097,6 @@
     <t>notes (items)</t>
   </si>
   <si>
-    <t>rec_id (items)</t>
-  </si>
-  <si>
     <t>status (items)</t>
   </si>
   <si>
@@ -1121,12 +1115,6 @@
     <t>https://github.com/trln/data-documentation/blob/master/argot/examples/items.md</t>
   </si>
   <si>
-    <t>Currently defined as single value. Have asked Adam if it is ever multivalued for NCSU -- 2017-10-25</t>
-  </si>
-  <si>
-    <t>Slack DM</t>
-  </si>
-  <si>
     <t>location_facet</t>
   </si>
   <si>
@@ -1140,6 +1128,12 @@
   </si>
   <si>
     <t>Array of item elements, each representing an item record attached to the bib. Each item element is an an escaped JSON string</t>
+  </si>
+  <si>
+    <t>holdings_id</t>
+  </si>
+  <si>
+    <t>item_id</t>
   </si>
 </sst>
 </file>
@@ -1244,7 +1238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1259,7 +1253,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -1418,13 +1411,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="fields" displayName="fields" ref="A1:U53" totalsRowShown="0">
-  <autoFilter ref="A1:U53">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="holdings data"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:U53"/>
   <tableColumns count="21">
     <tableColumn id="2" name="field"/>
     <tableColumn id="22" name="category"/>
@@ -1457,8 +1444,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="issuesfield" displayName="issuesfield" ref="A1:D11" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:D11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="issuesfield" displayName="issuesfield" ref="A1:D10" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:D10"/>
   <tableColumns count="4">
     <tableColumn id="1" name="field" dataDxfId="10"/>
     <tableColumn id="3" name="desc" dataDxfId="9"/>
@@ -1787,7 +1774,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D3" sqref="D3"/>
+      <selection pane="topRight" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1874,7 +1861,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>254</v>
       </c>
@@ -1997,7 +1984,7 @@
         <v>6</v>
       </c>
       <c r="S3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="T3" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2008,9 +1995,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B4" t="s">
         <v>251</v>
@@ -2058,7 +2045,7 @@
         <v>187</v>
       </c>
       <c r="S4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="T4" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2069,9 +2056,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B5" t="s">
         <v>251</v>
@@ -2125,7 +2112,7 @@
         <v>41</v>
       </c>
       <c r="S5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="T5" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2136,7 +2123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>248</v>
       </c>
@@ -2164,7 +2151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>293</v>
       </c>
@@ -2192,7 +2179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>245</v>
       </c>
@@ -2220,7 +2207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>292</v>
       </c>
@@ -2248,7 +2235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>244</v>
       </c>
@@ -2309,7 +2296,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>291</v>
       </c>
@@ -2367,7 +2354,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -2434,7 +2421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>263</v>
       </c>
@@ -2462,7 +2449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>265</v>
       </c>
@@ -2490,7 +2477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>246</v>
       </c>
@@ -2554,7 +2541,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>264</v>
       </c>
@@ -2582,9 +2569,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B17" t="s">
         <v>251</v>
@@ -2632,13 +2619,13 @@
         <v>155</v>
       </c>
       <c r="Q17" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="R17" t="s">
         <v>156</v>
       </c>
       <c r="S17" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="T17" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2649,7 +2636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>247</v>
       </c>
@@ -2713,7 +2700,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>259</v>
       </c>
@@ -2741,7 +2728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>266</v>
       </c>
@@ -2769,7 +2756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>255</v>
       </c>
@@ -2797,7 +2784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>194</v>
       </c>
@@ -2835,7 +2822,7 @@
         <v>41</v>
       </c>
       <c r="M22" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="N22" t="s">
         <v>6</v>
@@ -2853,7 +2840,7 @@
         <v>41</v>
       </c>
       <c r="S22" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="T22" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2902,7 +2889,7 @@
         <v>41</v>
       </c>
       <c r="M23" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="N23" t="s">
         <v>6</v>
@@ -2920,7 +2907,7 @@
         <v>41</v>
       </c>
       <c r="S23" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="T23" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2931,7 +2918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>110</v>
       </c>
@@ -3036,7 +3023,7 @@
         <v>175</v>
       </c>
       <c r="M25" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="N25" t="s">
         <v>215</v>
@@ -3051,10 +3038,10 @@
         <v>41</v>
       </c>
       <c r="R25" t="s">
+        <v>348</v>
+      </c>
+      <c r="S25" t="s">
         <v>349</v>
-      </c>
-      <c r="S25" t="s">
-        <v>350</v>
       </c>
       <c r="T25" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3065,9 +3052,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B26" t="s">
         <v>251</v>
@@ -3103,7 +3090,7 @@
         <v>175</v>
       </c>
       <c r="M26" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="N26" t="s">
         <v>179</v>
@@ -3118,10 +3105,10 @@
         <v>41</v>
       </c>
       <c r="R26" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="S26" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="T26" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3170,7 +3157,7 @@
         <v>175</v>
       </c>
       <c r="M27" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="N27" t="s">
         <v>217</v>
@@ -3185,10 +3172,10 @@
         <v>41</v>
       </c>
       <c r="R27" t="s">
+        <v>348</v>
+      </c>
+      <c r="S27" t="s">
         <v>349</v>
-      </c>
-      <c r="S27" t="s">
-        <v>350</v>
       </c>
       <c r="T27" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3199,9 +3186,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B28" t="s">
         <v>251</v>
@@ -3237,7 +3224,7 @@
         <v>175</v>
       </c>
       <c r="M28" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="N28" t="s">
         <v>159</v>
@@ -3252,10 +3239,10 @@
         <v>41</v>
       </c>
       <c r="R28" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="S28" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="T28" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3266,9 +3253,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
@@ -3307,7 +3294,7 @@
         <v>241</v>
       </c>
       <c r="N29" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="O29" t="s">
         <v>41</v>
@@ -3335,7 +3322,7 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B30" t="s">
         <v>252</v>
@@ -3389,7 +3376,7 @@
         <v>6</v>
       </c>
       <c r="S30" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="T30" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3400,9 +3387,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B31" t="s">
         <v>251</v>
@@ -3456,7 +3443,7 @@
         <v>188</v>
       </c>
       <c r="S31" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="T31" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3467,7 +3454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>249</v>
       </c>
@@ -3495,7 +3482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>294</v>
       </c>
@@ -3525,7 +3512,7 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>344</v>
+        <v>367</v>
       </c>
       <c r="B34" t="s">
         <v>252</v>
@@ -3579,7 +3566,7 @@
         <v>6</v>
       </c>
       <c r="S34" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="T34" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3590,9 +3577,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>357</v>
+        <v>368</v>
       </c>
       <c r="B35" t="s">
         <v>251</v>
@@ -3646,7 +3633,7 @@
         <v>41</v>
       </c>
       <c r="S35" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="T35" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3657,7 +3644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>260</v>
       </c>
@@ -3685,7 +3672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>267</v>
       </c>
@@ -3713,7 +3700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>256</v>
       </c>
@@ -3741,7 +3728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>201</v>
       </c>
@@ -3808,9 +3795,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B40" t="s">
         <v>251</v>
@@ -3861,10 +3848,10 @@
         <v>41</v>
       </c>
       <c r="R40" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="S40" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="T40" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3875,7 +3862,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -3942,7 +3929,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -4009,7 +3996,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -4076,7 +4063,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>123</v>
       </c>
@@ -4140,7 +4127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>38</v>
       </c>
@@ -4207,7 +4194,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="46" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>115</v>
       </c>
@@ -4274,7 +4261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>120</v>
       </c>
@@ -4343,7 +4330,7 @@
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B48" t="s">
         <v>252</v>
@@ -4397,7 +4384,7 @@
         <v>6</v>
       </c>
       <c r="S48" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="T48" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -4408,7 +4395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>262</v>
       </c>
@@ -4436,7 +4423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>257</v>
       </c>
@@ -4464,9 +4451,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B51" t="s">
         <v>251</v>
@@ -4520,18 +4507,18 @@
         <v>6</v>
       </c>
       <c r="S51" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="T51" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U51">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>277</v>
       </c>
@@ -4598,7 +4585,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>258</v>
       </c>
@@ -4636,10 +4623,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4761,42 +4748,28 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>359</v>
-      </c>
-      <c r="B9" s="12" t="s">
+      <c r="A9" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>362</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>364</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>366</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>368</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4812,7 +4785,7 @@
   <dimension ref="A1:N102"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6062,7 +6035,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B27" t="s">
         <v>53</v>
@@ -6110,7 +6083,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>344</v>
+        <v>367</v>
       </c>
       <c r="B28" t="s">
         <v>53</v>
@@ -6141,7 +6114,7 @@
       </c>
       <c r="K28" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>rec_id (holdings)UNC999a(i1=9 AND i2=2) AND $c &gt; 0</v>
+        <v>holdings_idUNC999a(i1=9 AND i2=2) AND $c &gt; 0</v>
       </c>
       <c r="L28" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6158,7 +6131,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B29" t="s">
         <v>53</v>
@@ -6206,7 +6179,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B30" t="s">
         <v>53</v>
@@ -6254,7 +6227,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B31" t="s">
         <v>53</v>
@@ -6302,7 +6275,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B32" t="s">
         <v>53</v>
@@ -6350,7 +6323,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B33" t="s">
         <v>53</v>
@@ -6398,7 +6371,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B34" t="s">
         <v>53</v>
@@ -6446,7 +6419,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B35" t="s">
         <v>53</v>
@@ -6494,7 +6467,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B36" t="s">
         <v>53</v>
@@ -6542,7 +6515,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>357</v>
+        <v>368</v>
       </c>
       <c r="B37" t="s">
         <v>53</v>
@@ -6573,7 +6546,7 @@
       </c>
       <c r="K37" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>rec_id (items)UNC999ii1=9 AND i2=1</v>
+        <v>item_idUNC999ii1=9 AND i2=1</v>
       </c>
       <c r="L37" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -6590,7 +6563,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B38" t="s">
         <v>53</v>
@@ -6638,7 +6611,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B39" t="s">
         <v>53</v>
@@ -6686,7 +6659,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B40" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
remove coden as its own field
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="5910"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="5910" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2163" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2136" uniqueCount="437">
   <si>
     <t>subject_chronological_facet</t>
   </si>
@@ -1269,15 +1269,6 @@
   </si>
   <si>
     <t>Digits only. Strip off ocn/ocm/on prefixes. If coming from 035z, remove (OCoLC)</t>
-  </si>
-  <si>
-    <t>coden</t>
-  </si>
-  <si>
-    <t>CODEN:</t>
-  </si>
-  <si>
-    <t>A specific unique ID assigned to journals and used in some communities</t>
   </si>
   <si>
     <t>sersol_number</t>
@@ -1631,8 +1622,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="fields" displayName="fields" ref="A1:W65" totalsRowShown="0">
-  <autoFilter ref="A1:W65"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="fields" displayName="fields" ref="A1:W64" totalsRowShown="0">
+  <autoFilter ref="A1:W64"/>
   <tableColumns count="23">
     <tableColumn id="2" name="field"/>
     <tableColumn id="22" name="category"/>
@@ -1680,8 +1671,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="mappings" displayName="mappings" ref="A1:P110" totalsRowShown="0">
-  <autoFilter ref="A1:P110"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="mappings" displayName="mappings" ref="A1:P109" totalsRowShown="0">
+  <autoFilter ref="A1:P109"/>
   <sortState ref="A2:N104">
     <sortCondition ref="A1:A104"/>
   </sortState>
@@ -1991,11 +1982,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W65"/>
+  <dimension ref="A1:W64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A61" sqref="A61"/>
+      <selection pane="topRight" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2352,60 +2343,57 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>414</v>
+        <v>384</v>
       </c>
       <c r="B6" t="s">
-        <v>404</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" t="s">
         <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="G6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H6" t="s">
-        <v>405</v>
+        <v>41</v>
       </c>
       <c r="I6" t="s">
         <v>41</v>
       </c>
       <c r="J6" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="K6" t="s">
-        <v>123</v>
+        <v>85</v>
       </c>
       <c r="L6" t="s">
-        <v>415</v>
+        <v>85</v>
       </c>
       <c r="M6" t="s">
-        <v>416</v>
+        <v>385</v>
       </c>
       <c r="N6" t="s">
-        <v>6</v>
+        <v>386</v>
       </c>
       <c r="O6" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="P6" t="s">
         <v>41</v>
       </c>
       <c r="Q6" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="R6" t="s">
-        <v>6</v>
-      </c>
-      <c r="S6" t="s">
         <v>6</v>
       </c>
       <c r="T6" s="8">
@@ -2414,63 +2402,27 @@
       </c>
       <c r="U6">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>384</v>
+        <v>246</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>251</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
         <v>41</v>
       </c>
-      <c r="F7" t="s">
-        <v>161</v>
-      </c>
-      <c r="G7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J7" t="s">
-        <v>85</v>
-      </c>
-      <c r="K7" t="s">
-        <v>85</v>
-      </c>
-      <c r="L7" t="s">
-        <v>85</v>
-      </c>
-      <c r="M7" t="s">
-        <v>385</v>
-      </c>
-      <c r="N7" t="s">
-        <v>386</v>
-      </c>
-      <c r="O7" t="s">
-        <v>41</v>
-      </c>
       <c r="P7" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>41</v>
-      </c>
-      <c r="R7" t="s">
-        <v>6</v>
+        <v>269</v>
       </c>
       <c r="T7" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2483,7 +2435,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>246</v>
+        <v>291</v>
       </c>
       <c r="B8" t="s">
         <v>251</v>
@@ -2498,7 +2450,7 @@
         <v>41</v>
       </c>
       <c r="P8" t="s">
-        <v>269</v>
+        <v>41</v>
       </c>
       <c r="T8" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2511,22 +2463,61 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>291</v>
+        <v>366</v>
       </c>
       <c r="B9" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9" t="s">
+        <v>193</v>
+      </c>
+      <c r="F9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" t="s">
+        <v>151</v>
+      </c>
+      <c r="L9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M9" t="s">
+        <v>370</v>
+      </c>
+      <c r="N9" t="s">
+        <v>371</v>
+      </c>
+      <c r="O9" t="s">
         <v>41</v>
       </c>
       <c r="P9" t="s">
         <v>41</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>41</v>
+      </c>
+      <c r="R9" t="s">
+        <v>6</v>
+      </c>
+      <c r="S9" t="s">
+        <v>358</v>
       </c>
       <c r="T9" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2534,66 +2525,27 @@
       </c>
       <c r="U9">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>366</v>
+        <v>243</v>
       </c>
       <c r="B10" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>193</v>
-      </c>
-      <c r="F10" t="s">
-        <v>149</v>
-      </c>
-      <c r="G10" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I10" t="s">
-        <v>41</v>
-      </c>
-      <c r="J10" t="s">
-        <v>41</v>
-      </c>
-      <c r="K10" t="s">
-        <v>151</v>
-      </c>
-      <c r="L10" t="s">
-        <v>6</v>
-      </c>
-      <c r="M10" t="s">
-        <v>370</v>
-      </c>
-      <c r="N10" t="s">
-        <v>371</v>
-      </c>
-      <c r="O10" t="s">
         <v>41</v>
       </c>
       <c r="P10" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>41</v>
-      </c>
-      <c r="R10" t="s">
-        <v>6</v>
-      </c>
-      <c r="S10" t="s">
-        <v>358</v>
+        <v>269</v>
       </c>
       <c r="T10" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2601,12 +2553,12 @@
       </c>
       <c r="U10">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>243</v>
+        <v>290</v>
       </c>
       <c r="B11" t="s">
         <v>251</v>
@@ -2621,7 +2573,7 @@
         <v>41</v>
       </c>
       <c r="P11" t="s">
-        <v>269</v>
+        <v>41</v>
       </c>
       <c r="T11" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2634,7 +2586,7 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>290</v>
+        <v>242</v>
       </c>
       <c r="B12" t="s">
         <v>251</v>
@@ -2648,7 +2600,40 @@
       <c r="E12" t="s">
         <v>41</v>
       </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>277</v>
+      </c>
+      <c r="I12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J12" t="s">
+        <v>310</v>
+      </c>
+      <c r="K12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M12" t="s">
+        <v>278</v>
+      </c>
+      <c r="N12" t="s">
+        <v>279</v>
+      </c>
+      <c r="O12" t="s">
+        <v>6</v>
+      </c>
       <c r="P12" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q12" t="s">
         <v>41</v>
       </c>
       <c r="T12" s="8">
@@ -2657,12 +2642,12 @@
       </c>
       <c r="U12">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>242</v>
+        <v>289</v>
       </c>
       <c r="B13" t="s">
         <v>251</v>
@@ -2683,13 +2668,13 @@
         <v>2</v>
       </c>
       <c r="H13" t="s">
-        <v>277</v>
+        <v>41</v>
       </c>
       <c r="I13" t="s">
         <v>41</v>
       </c>
       <c r="J13" t="s">
-        <v>310</v>
+        <v>41</v>
       </c>
       <c r="K13" t="s">
         <v>6</v>
@@ -2698,18 +2683,15 @@
         <v>6</v>
       </c>
       <c r="M13" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="N13" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="O13" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="P13" t="s">
-        <v>273</v>
-      </c>
-      <c r="Q13" t="s">
         <v>41</v>
       </c>
       <c r="T13" s="8">
@@ -2723,132 +2705,102 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>289</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>251</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14" t="s">
         <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>3</v>
+        <v>149</v>
       </c>
       <c r="G14" t="s">
         <v>2</v>
       </c>
       <c r="H14" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="I14" t="s">
         <v>41</v>
       </c>
       <c r="J14" t="s">
-        <v>41</v>
+        <v>103</v>
       </c>
       <c r="K14" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="L14" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="M14" t="s">
-        <v>280</v>
+        <v>105</v>
       </c>
       <c r="N14" t="s">
-        <v>281</v>
+        <v>106</v>
       </c>
       <c r="O14" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="P14" t="s">
-        <v>41</v>
-      </c>
-      <c r="T14" s="8">
+        <v>107</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>41</v>
+      </c>
+      <c r="R14" t="s">
+        <v>108</v>
+      </c>
+      <c r="S14" t="s">
+        <v>6</v>
+      </c>
+      <c r="T14">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>0</v>
       </c>
       <c r="U14">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>261</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>259</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E15" t="s">
         <v>41</v>
       </c>
-      <c r="F15" t="s">
-        <v>149</v>
-      </c>
-      <c r="G15" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" t="s">
-        <v>72</v>
-      </c>
-      <c r="I15" t="s">
-        <v>41</v>
-      </c>
-      <c r="J15" t="s">
-        <v>103</v>
-      </c>
-      <c r="K15" t="s">
-        <v>104</v>
-      </c>
-      <c r="L15" t="s">
-        <v>41</v>
-      </c>
-      <c r="M15" t="s">
-        <v>105</v>
-      </c>
-      <c r="N15" t="s">
-        <v>106</v>
-      </c>
-      <c r="O15" t="s">
-        <v>82</v>
-      </c>
       <c r="P15" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>41</v>
-      </c>
-      <c r="R15" t="s">
-        <v>108</v>
-      </c>
-      <c r="S15" t="s">
-        <v>6</v>
-      </c>
-      <c r="T15">
+        <v>267</v>
+      </c>
+      <c r="T15" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>0</v>
       </c>
       <c r="U15">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B16" t="s">
         <v>259</v>
@@ -2863,7 +2815,7 @@
         <v>41</v>
       </c>
       <c r="P16" t="s">
-        <v>267</v>
+        <v>41</v>
       </c>
       <c r="T16" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2876,10 +2828,10 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>263</v>
+        <v>244</v>
       </c>
       <c r="B17" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -2890,8 +2842,44 @@
       <c r="E17" t="s">
         <v>41</v>
       </c>
+      <c r="F17" t="s">
+        <v>161</v>
+      </c>
+      <c r="G17" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" t="s">
+        <v>277</v>
+      </c>
+      <c r="I17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" t="s">
+        <v>310</v>
+      </c>
+      <c r="K17" t="s">
+        <v>6</v>
+      </c>
+      <c r="L17" t="s">
+        <v>6</v>
+      </c>
+      <c r="M17" t="s">
+        <v>297</v>
+      </c>
+      <c r="N17" t="s">
+        <v>298</v>
+      </c>
+      <c r="O17" t="s">
+        <v>304</v>
+      </c>
       <c r="P17" t="s">
-        <v>41</v>
+        <v>270</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>302</v>
+      </c>
+      <c r="R17" t="s">
+        <v>6</v>
       </c>
       <c r="T17" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2899,12 +2887,12 @@
       </c>
       <c r="U17">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>244</v>
+        <v>262</v>
       </c>
       <c r="B18" t="s">
         <v>251</v>
@@ -2918,44 +2906,8 @@
       <c r="E18" t="s">
         <v>41</v>
       </c>
-      <c r="F18" t="s">
-        <v>161</v>
-      </c>
-      <c r="G18" t="s">
-        <v>3</v>
-      </c>
-      <c r="H18" t="s">
-        <v>277</v>
-      </c>
-      <c r="I18" t="s">
-        <v>3</v>
-      </c>
-      <c r="J18" t="s">
-        <v>310</v>
-      </c>
-      <c r="K18" t="s">
-        <v>6</v>
-      </c>
-      <c r="L18" t="s">
-        <v>6</v>
-      </c>
-      <c r="M18" t="s">
-        <v>297</v>
-      </c>
-      <c r="N18" t="s">
-        <v>298</v>
-      </c>
-      <c r="O18" t="s">
-        <v>304</v>
-      </c>
       <c r="P18" t="s">
-        <v>270</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>302</v>
-      </c>
-      <c r="R18" t="s">
-        <v>6</v>
+        <v>271</v>
       </c>
       <c r="T18" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2963,27 +2915,66 @@
       </c>
       <c r="U18">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>262</v>
+        <v>349</v>
       </c>
       <c r="B19" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E19" t="s">
+        <v>193</v>
+      </c>
+      <c r="F19" t="s">
+        <v>149</v>
+      </c>
+      <c r="G19" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" t="s">
+        <v>41</v>
+      </c>
+      <c r="I19" t="s">
+        <v>41</v>
+      </c>
+      <c r="J19" t="s">
+        <v>41</v>
+      </c>
+      <c r="K19" t="s">
+        <v>151</v>
+      </c>
+      <c r="L19" t="s">
+        <v>175</v>
+      </c>
+      <c r="M19" t="s">
+        <v>152</v>
+      </c>
+      <c r="N19" t="s">
+        <v>153</v>
+      </c>
+      <c r="O19" t="s">
         <v>41</v>
       </c>
       <c r="P19" t="s">
-        <v>271</v>
+        <v>154</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>356</v>
+      </c>
+      <c r="R19" t="s">
+        <v>155</v>
+      </c>
+      <c r="S19" t="s">
+        <v>358</v>
       </c>
       <c r="T19" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -2991,66 +2982,63 @@
       </c>
       <c r="U19">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>349</v>
+        <v>245</v>
       </c>
       <c r="B20" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>193</v>
+        <v>41</v>
       </c>
       <c r="F20" t="s">
         <v>149</v>
       </c>
       <c r="G20" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H20" t="s">
-        <v>41</v>
+        <v>277</v>
       </c>
       <c r="I20" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="J20" t="s">
-        <v>41</v>
+        <v>310</v>
       </c>
       <c r="K20" t="s">
-        <v>151</v>
+        <v>299</v>
       </c>
       <c r="L20" t="s">
-        <v>175</v>
+        <v>6</v>
       </c>
       <c r="M20" t="s">
-        <v>152</v>
+        <v>300</v>
       </c>
       <c r="N20" t="s">
-        <v>153</v>
+        <v>301</v>
       </c>
       <c r="O20" t="s">
-        <v>41</v>
+        <v>304</v>
       </c>
       <c r="P20" t="s">
-        <v>154</v>
+        <v>269</v>
       </c>
       <c r="Q20" t="s">
-        <v>356</v>
+        <v>303</v>
       </c>
       <c r="R20" t="s">
-        <v>155</v>
-      </c>
-      <c r="S20" t="s">
-        <v>358</v>
+        <v>6</v>
       </c>
       <c r="T20" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3058,21 +3046,21 @@
       </c>
       <c r="U20">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>245</v>
+        <v>199</v>
       </c>
       <c r="B21" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E21" t="s">
         <v>41</v>
@@ -3084,37 +3072,40 @@
         <v>3</v>
       </c>
       <c r="H21" t="s">
-        <v>277</v>
+        <v>41</v>
       </c>
       <c r="I21" t="s">
         <v>3</v>
       </c>
       <c r="J21" t="s">
-        <v>310</v>
+        <v>41</v>
       </c>
       <c r="K21" t="s">
-        <v>299</v>
+        <v>151</v>
       </c>
       <c r="L21" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="M21" t="s">
-        <v>300</v>
+        <v>362</v>
       </c>
       <c r="N21" t="s">
-        <v>301</v>
+        <v>6</v>
       </c>
       <c r="O21" t="s">
-        <v>304</v>
+        <v>41</v>
       </c>
       <c r="P21" t="s">
-        <v>269</v>
+        <v>41</v>
       </c>
       <c r="Q21" t="s">
-        <v>303</v>
+        <v>41</v>
       </c>
       <c r="R21" t="s">
-        <v>6</v>
+        <v>41</v>
+      </c>
+      <c r="S21" t="s">
+        <v>346</v>
       </c>
       <c r="T21" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3122,12 +3113,12 @@
       </c>
       <c r="U21">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>199</v>
+        <v>364</v>
       </c>
       <c r="B22" t="s">
         <v>250</v>
@@ -3139,34 +3130,34 @@
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>41</v>
+        <v>199</v>
       </c>
       <c r="F22" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="G22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H22" t="s">
         <v>41</v>
       </c>
       <c r="I22" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J22" t="s">
         <v>41</v>
       </c>
       <c r="K22" t="s">
-        <v>151</v>
+        <v>41</v>
       </c>
       <c r="L22" t="s">
         <v>41</v>
       </c>
       <c r="M22" t="s">
-        <v>362</v>
+        <v>218</v>
       </c>
       <c r="N22" t="s">
-        <v>6</v>
+        <v>219</v>
       </c>
       <c r="O22" t="s">
         <v>41</v>
@@ -3178,7 +3169,7 @@
         <v>41</v>
       </c>
       <c r="R22" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="S22" t="s">
         <v>346</v>
@@ -3189,66 +3180,27 @@
       </c>
       <c r="U22">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>364</v>
+        <v>257</v>
       </c>
       <c r="B23" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>199</v>
-      </c>
-      <c r="F23" t="s">
-        <v>161</v>
-      </c>
-      <c r="G23" t="s">
-        <v>2</v>
-      </c>
-      <c r="H23" t="s">
-        <v>41</v>
-      </c>
-      <c r="I23" t="s">
-        <v>6</v>
-      </c>
-      <c r="J23" t="s">
-        <v>41</v>
-      </c>
-      <c r="K23" t="s">
-        <v>41</v>
-      </c>
-      <c r="L23" t="s">
-        <v>41</v>
-      </c>
-      <c r="M23" t="s">
-        <v>218</v>
-      </c>
-      <c r="N23" t="s">
-        <v>219</v>
-      </c>
-      <c r="O23" t="s">
         <v>41</v>
       </c>
       <c r="P23" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>41</v>
-      </c>
-      <c r="R23" t="s">
-        <v>6</v>
-      </c>
-      <c r="S23" t="s">
-        <v>346</v>
+        <v>267</v>
       </c>
       <c r="T23" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3256,12 +3208,12 @@
       </c>
       <c r="U23">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="B24" t="s">
         <v>259</v>
@@ -3276,7 +3228,7 @@
         <v>41</v>
       </c>
       <c r="P24" t="s">
-        <v>267</v>
+        <v>41</v>
       </c>
       <c r="T24" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3289,10 +3241,10 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B25" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
@@ -3304,7 +3256,7 @@
         <v>41</v>
       </c>
       <c r="P25" t="s">
-        <v>41</v>
+        <v>269</v>
       </c>
       <c r="T25" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3317,22 +3269,61 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>253</v>
+        <v>365</v>
       </c>
       <c r="B26" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C26" t="s">
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E26" t="s">
+        <v>193</v>
+      </c>
+      <c r="F26" t="s">
+        <v>161</v>
+      </c>
+      <c r="G26" t="s">
+        <v>2</v>
+      </c>
+      <c r="H26" t="s">
+        <v>41</v>
+      </c>
+      <c r="I26" t="s">
+        <v>41</v>
+      </c>
+      <c r="J26" t="s">
+        <v>41</v>
+      </c>
+      <c r="K26" t="s">
+        <v>2</v>
+      </c>
+      <c r="L26" t="s">
+        <v>41</v>
+      </c>
+      <c r="M26" t="s">
+        <v>147</v>
+      </c>
+      <c r="N26" t="s">
+        <v>173</v>
+      </c>
+      <c r="O26" t="s">
         <v>41</v>
       </c>
       <c r="P26" t="s">
-        <v>269</v>
+        <v>148</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>41</v>
+      </c>
+      <c r="R26" t="s">
+        <v>41</v>
+      </c>
+      <c r="S26" t="s">
+        <v>358</v>
       </c>
       <c r="T26" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3340,12 +3331,12 @@
       </c>
       <c r="U26">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>365</v>
+        <v>193</v>
       </c>
       <c r="B27" t="s">
         <v>249</v>
@@ -3357,40 +3348,40 @@
         <v>3</v>
       </c>
       <c r="E27" t="s">
-        <v>193</v>
+        <v>41</v>
       </c>
       <c r="F27" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="G27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H27" t="s">
         <v>41</v>
       </c>
       <c r="I27" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="J27" t="s">
         <v>41</v>
       </c>
       <c r="K27" t="s">
-        <v>2</v>
+        <v>151</v>
       </c>
       <c r="L27" t="s">
         <v>41</v>
       </c>
       <c r="M27" t="s">
-        <v>147</v>
+        <v>363</v>
       </c>
       <c r="N27" t="s">
-        <v>173</v>
+        <v>6</v>
       </c>
       <c r="O27" t="s">
         <v>41</v>
       </c>
       <c r="P27" t="s">
-        <v>148</v>
+        <v>41</v>
       </c>
       <c r="Q27" t="s">
         <v>41</v>
@@ -3407,21 +3398,21 @@
       </c>
       <c r="U27">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>193</v>
+        <v>109</v>
       </c>
       <c r="B28" t="s">
-        <v>249</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E28" t="s">
         <v>41</v>
@@ -3433,42 +3424,42 @@
         <v>3</v>
       </c>
       <c r="H28" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="I28" t="s">
         <v>3</v>
       </c>
       <c r="J28" t="s">
-        <v>41</v>
+        <v>110</v>
       </c>
       <c r="K28" t="s">
-        <v>151</v>
+        <v>111</v>
       </c>
       <c r="L28" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="M28" t="s">
-        <v>363</v>
+        <v>113</v>
       </c>
       <c r="N28" t="s">
-        <v>6</v>
+        <v>172</v>
       </c>
       <c r="O28" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="P28" t="s">
-        <v>41</v>
+        <v>110</v>
       </c>
       <c r="Q28" t="s">
         <v>41</v>
       </c>
       <c r="R28" t="s">
-        <v>41</v>
+        <v>189</v>
       </c>
       <c r="S28" t="s">
-        <v>358</v>
-      </c>
-      <c r="T28" s="8">
+        <v>6</v>
+      </c>
+      <c r="T28">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>0</v>
       </c>
@@ -3479,77 +3470,77 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>109</v>
+        <v>339</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>250</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>41</v>
+        <v>199</v>
       </c>
       <c r="F29" t="s">
-        <v>149</v>
+        <v>3</v>
       </c>
       <c r="G29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H29" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="I29" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J29" t="s">
-        <v>110</v>
+        <v>41</v>
       </c>
       <c r="K29" t="s">
-        <v>111</v>
+        <v>210</v>
       </c>
       <c r="L29" t="s">
-        <v>112</v>
+        <v>174</v>
       </c>
       <c r="M29" t="s">
-        <v>113</v>
+        <v>343</v>
       </c>
       <c r="N29" t="s">
-        <v>172</v>
+        <v>214</v>
       </c>
       <c r="O29" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="P29" t="s">
-        <v>110</v>
+        <v>215</v>
       </c>
       <c r="Q29" t="s">
         <v>41</v>
       </c>
       <c r="R29" t="s">
-        <v>189</v>
+        <v>345</v>
       </c>
       <c r="S29" t="s">
-        <v>6</v>
-      </c>
-      <c r="T29">
+        <v>346</v>
+      </c>
+      <c r="T29" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>0</v>
       </c>
       <c r="U29">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>339</v>
+        <v>350</v>
       </c>
       <c r="B30" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
@@ -3558,7 +3549,7 @@
         <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="F30" t="s">
         <v>3</v>
@@ -3570,13 +3561,13 @@
         <v>41</v>
       </c>
       <c r="I30" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="J30" t="s">
         <v>41</v>
       </c>
       <c r="K30" t="s">
-        <v>210</v>
+        <v>151</v>
       </c>
       <c r="L30" t="s">
         <v>174</v>
@@ -3585,13 +3576,13 @@
         <v>343</v>
       </c>
       <c r="N30" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
       <c r="O30" t="s">
         <v>41</v>
       </c>
       <c r="P30" t="s">
-        <v>215</v>
+        <v>179</v>
       </c>
       <c r="Q30" t="s">
         <v>41</v>
@@ -3600,7 +3591,7 @@
         <v>345</v>
       </c>
       <c r="S30" t="s">
-        <v>346</v>
+        <v>358</v>
       </c>
       <c r="T30" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3608,15 +3599,15 @@
       </c>
       <c r="U30">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="B31" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C31" t="s">
         <v>2</v>
@@ -3625,7 +3616,7 @@
         <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="F31" t="s">
         <v>3</v>
@@ -3637,28 +3628,28 @@
         <v>41</v>
       </c>
       <c r="I31" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="J31" t="s">
         <v>41</v>
       </c>
       <c r="K31" t="s">
-        <v>151</v>
+        <v>210</v>
       </c>
       <c r="L31" t="s">
         <v>174</v>
       </c>
       <c r="M31" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="N31" t="s">
-        <v>178</v>
+        <v>216</v>
       </c>
       <c r="O31" t="s">
         <v>41</v>
       </c>
       <c r="P31" t="s">
-        <v>179</v>
+        <v>217</v>
       </c>
       <c r="Q31" t="s">
         <v>41</v>
@@ -3667,7 +3658,7 @@
         <v>345</v>
       </c>
       <c r="S31" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="T31" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3675,15 +3666,15 @@
       </c>
       <c r="U31">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>340</v>
+        <v>351</v>
       </c>
       <c r="B32" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C32" t="s">
         <v>2</v>
@@ -3692,7 +3683,7 @@
         <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="F32" t="s">
         <v>3</v>
@@ -3704,28 +3695,28 @@
         <v>41</v>
       </c>
       <c r="I32" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="J32" t="s">
         <v>41</v>
       </c>
       <c r="K32" t="s">
-        <v>210</v>
+        <v>151</v>
       </c>
       <c r="L32" t="s">
         <v>174</v>
       </c>
       <c r="M32" t="s">
-        <v>344</v>
+        <v>355</v>
       </c>
       <c r="N32" t="s">
-        <v>216</v>
+        <v>158</v>
       </c>
       <c r="O32" t="s">
         <v>41</v>
       </c>
       <c r="P32" t="s">
-        <v>217</v>
+        <v>159</v>
       </c>
       <c r="Q32" t="s">
         <v>41</v>
@@ -3734,7 +3725,7 @@
         <v>345</v>
       </c>
       <c r="S32" t="s">
-        <v>346</v>
+        <v>358</v>
       </c>
       <c r="T32" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3742,15 +3733,15 @@
       </c>
       <c r="U32">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>351</v>
+        <v>379</v>
       </c>
       <c r="B33" t="s">
-        <v>249</v>
+        <v>6</v>
       </c>
       <c r="C33" t="s">
         <v>2</v>
@@ -3759,49 +3750,49 @@
         <v>3</v>
       </c>
       <c r="E33" t="s">
-        <v>193</v>
+        <v>41</v>
       </c>
       <c r="F33" t="s">
         <v>3</v>
       </c>
       <c r="G33" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H33" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="I33" t="s">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="J33" t="s">
-        <v>41</v>
+        <v>238</v>
       </c>
       <c r="K33" t="s">
-        <v>151</v>
+        <v>81</v>
       </c>
       <c r="L33" t="s">
-        <v>174</v>
+        <v>41</v>
       </c>
       <c r="M33" t="s">
-        <v>355</v>
+        <v>239</v>
       </c>
       <c r="N33" t="s">
-        <v>158</v>
+        <v>360</v>
       </c>
       <c r="O33" t="s">
         <v>41</v>
       </c>
       <c r="P33" t="s">
-        <v>159</v>
+        <v>238</v>
       </c>
       <c r="Q33" t="s">
         <v>41</v>
       </c>
       <c r="R33" t="s">
-        <v>345</v>
+        <v>41</v>
       </c>
       <c r="S33" t="s">
-        <v>358</v>
+        <v>6</v>
       </c>
       <c r="T33" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3809,15 +3800,15 @@
       </c>
       <c r="U33">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>379</v>
+        <v>342</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>250</v>
       </c>
       <c r="C34" t="s">
         <v>2</v>
@@ -3826,49 +3817,49 @@
         <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>41</v>
+        <v>199</v>
       </c>
       <c r="F34" t="s">
-        <v>3</v>
+        <v>161</v>
       </c>
       <c r="G34" t="s">
         <v>3</v>
       </c>
       <c r="H34" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="I34" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J34" t="s">
-        <v>238</v>
+        <v>41</v>
       </c>
       <c r="K34" t="s">
-        <v>81</v>
+        <v>210</v>
       </c>
       <c r="L34" t="s">
-        <v>41</v>
+        <v>174</v>
       </c>
       <c r="M34" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="N34" t="s">
-        <v>360</v>
+        <v>224</v>
       </c>
       <c r="O34" t="s">
         <v>41</v>
       </c>
       <c r="P34" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="Q34" t="s">
         <v>41</v>
       </c>
       <c r="R34" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="S34" t="s">
-        <v>6</v>
+        <v>346</v>
       </c>
       <c r="T34" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3881,10 +3872,10 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="B35" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
@@ -3893,7 +3884,7 @@
         <v>3</v>
       </c>
       <c r="E35" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="F35" t="s">
         <v>161</v>
@@ -3911,31 +3902,31 @@
         <v>41</v>
       </c>
       <c r="K35" t="s">
-        <v>210</v>
+        <v>151</v>
       </c>
       <c r="L35" t="s">
         <v>174</v>
       </c>
       <c r="M35" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N35" t="s">
-        <v>224</v>
+        <v>162</v>
       </c>
       <c r="O35" t="s">
         <v>41</v>
       </c>
       <c r="P35" t="s">
-        <v>225</v>
+        <v>163</v>
       </c>
       <c r="Q35" t="s">
         <v>41</v>
       </c>
       <c r="R35" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="S35" t="s">
-        <v>346</v>
+        <v>358</v>
       </c>
       <c r="T35" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -3948,10 +3939,10 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>352</v>
+        <v>403</v>
       </c>
       <c r="B36" t="s">
-        <v>249</v>
+        <v>404</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
@@ -3960,49 +3951,49 @@
         <v>3</v>
       </c>
       <c r="E36" t="s">
-        <v>193</v>
+        <v>41</v>
       </c>
       <c r="F36" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="G36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H36" t="s">
-        <v>41</v>
+        <v>405</v>
       </c>
       <c r="I36" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="J36" t="s">
         <v>41</v>
       </c>
       <c r="K36" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="L36" t="s">
-        <v>174</v>
+        <v>6</v>
       </c>
       <c r="M36" t="s">
-        <v>222</v>
+        <v>406</v>
       </c>
       <c r="N36" t="s">
-        <v>162</v>
+        <v>6</v>
       </c>
       <c r="O36" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="P36" t="s">
-        <v>163</v>
+        <v>407</v>
       </c>
       <c r="Q36" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="R36" t="s">
-        <v>187</v>
+        <v>408</v>
       </c>
       <c r="S36" t="s">
-        <v>358</v>
+        <v>6</v>
       </c>
       <c r="T36" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -4010,12 +4001,12 @@
       </c>
       <c r="U36">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="B37" t="s">
         <v>404</v>
@@ -4033,7 +4024,7 @@
         <v>149</v>
       </c>
       <c r="G37" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H37" t="s">
         <v>405</v>
@@ -4045,28 +4036,28 @@
         <v>41</v>
       </c>
       <c r="K37" t="s">
-        <v>123</v>
+        <v>410</v>
       </c>
       <c r="L37" t="s">
         <v>6</v>
       </c>
       <c r="M37" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="N37" t="s">
-        <v>6</v>
+        <v>412</v>
       </c>
       <c r="O37" t="s">
         <v>6</v>
       </c>
       <c r="P37" t="s">
-        <v>407</v>
+        <v>41</v>
       </c>
       <c r="Q37" t="s">
         <v>6</v>
       </c>
       <c r="R37" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="S37" t="s">
         <v>6</v>
@@ -4077,66 +4068,27 @@
       </c>
       <c r="U37">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>409</v>
+        <v>247</v>
       </c>
       <c r="B38" t="s">
-        <v>404</v>
+        <v>251</v>
       </c>
       <c r="C38" t="s">
         <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E38" t="s">
         <v>41</v>
       </c>
-      <c r="F38" t="s">
-        <v>149</v>
-      </c>
-      <c r="G38" t="s">
-        <v>3</v>
-      </c>
-      <c r="H38" t="s">
-        <v>405</v>
-      </c>
-      <c r="I38" t="s">
-        <v>41</v>
-      </c>
-      <c r="J38" t="s">
-        <v>41</v>
-      </c>
-      <c r="K38" t="s">
-        <v>410</v>
-      </c>
-      <c r="L38" t="s">
-        <v>6</v>
-      </c>
-      <c r="M38" t="s">
-        <v>411</v>
-      </c>
-      <c r="N38" t="s">
-        <v>412</v>
-      </c>
-      <c r="O38" t="s">
-        <v>6</v>
-      </c>
       <c r="P38" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>6</v>
-      </c>
-      <c r="R38" t="s">
-        <v>413</v>
-      </c>
-      <c r="S38" t="s">
-        <v>6</v>
+        <v>269</v>
       </c>
       <c r="T38" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -4149,7 +4101,7 @@
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>247</v>
+        <v>292</v>
       </c>
       <c r="B39" t="s">
         <v>251</v>
@@ -4164,7 +4116,7 @@
         <v>41</v>
       </c>
       <c r="P39" t="s">
-        <v>269</v>
+        <v>41</v>
       </c>
       <c r="T39" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -4177,10 +4129,10 @@
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
       <c r="B40" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="C40" t="s">
         <v>2</v>
@@ -4192,7 +4144,7 @@
         <v>41</v>
       </c>
       <c r="P40" t="s">
-        <v>41</v>
+        <v>267</v>
       </c>
       <c r="T40" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -4205,7 +4157,7 @@
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="B41" t="s">
         <v>259</v>
@@ -4220,7 +4172,7 @@
         <v>41</v>
       </c>
       <c r="P41" t="s">
-        <v>267</v>
+        <v>41</v>
       </c>
       <c r="T41" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -4233,10 +4185,10 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B42" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C42" t="s">
         <v>2</v>
@@ -4248,7 +4200,7 @@
         <v>41</v>
       </c>
       <c r="P42" t="s">
-        <v>41</v>
+        <v>269</v>
       </c>
       <c r="T42" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -4261,26 +4213,65 @@
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>254</v>
+        <v>200</v>
       </c>
       <c r="B43" t="s">
-        <v>251</v>
+        <v>6</v>
       </c>
       <c r="C43" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D43" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E43" t="s">
         <v>41</v>
       </c>
+      <c r="F43" t="s">
+        <v>161</v>
+      </c>
+      <c r="G43" t="s">
+        <v>3</v>
+      </c>
+      <c r="H43" t="s">
+        <v>201</v>
+      </c>
+      <c r="I43" t="s">
+        <v>2</v>
+      </c>
+      <c r="J43" t="s">
+        <v>41</v>
+      </c>
+      <c r="K43" t="s">
+        <v>202</v>
+      </c>
+      <c r="L43" t="s">
+        <v>6</v>
+      </c>
+      <c r="M43" t="s">
+        <v>203</v>
+      </c>
+      <c r="N43" t="s">
+        <v>204</v>
+      </c>
+      <c r="O43" t="s">
+        <v>41</v>
+      </c>
       <c r="P43" t="s">
-        <v>269</v>
+        <v>205</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>206</v>
+      </c>
+      <c r="R43" t="s">
+        <v>207</v>
+      </c>
+      <c r="S43" t="s">
+        <v>6</v>
       </c>
       <c r="T43" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U43">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
@@ -4289,13 +4280,13 @@
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>200</v>
+        <v>414</v>
       </c>
       <c r="B44" t="s">
-        <v>6</v>
+        <v>404</v>
       </c>
       <c r="C44" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D44" t="s">
         <v>3</v>
@@ -4304,50 +4295,50 @@
         <v>41</v>
       </c>
       <c r="F44" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="G44" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H44" t="s">
-        <v>201</v>
+        <v>405</v>
       </c>
       <c r="I44" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="J44" t="s">
         <v>41</v>
       </c>
       <c r="K44" t="s">
-        <v>202</v>
+        <v>123</v>
       </c>
       <c r="L44" t="s">
-        <v>6</v>
+        <v>415</v>
       </c>
       <c r="M44" t="s">
-        <v>203</v>
+        <v>416</v>
       </c>
       <c r="N44" t="s">
-        <v>204</v>
+        <v>417</v>
       </c>
       <c r="O44" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="P44" t="s">
-        <v>205</v>
+        <v>41</v>
       </c>
       <c r="Q44" t="s">
-        <v>206</v>
+        <v>6</v>
       </c>
       <c r="R44" t="s">
-        <v>207</v>
+        <v>6</v>
       </c>
       <c r="S44" t="s">
         <v>6</v>
       </c>
       <c r="T44" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U44">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
@@ -4356,10 +4347,10 @@
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>417</v>
+        <v>353</v>
       </c>
       <c r="B45" t="s">
-        <v>404</v>
+        <v>249</v>
       </c>
       <c r="C45" t="s">
         <v>2</v>
@@ -4368,16 +4359,16 @@
         <v>3</v>
       </c>
       <c r="E45" t="s">
-        <v>41</v>
+        <v>193</v>
       </c>
       <c r="F45" t="s">
-        <v>149</v>
+        <v>3</v>
       </c>
       <c r="G45" t="s">
         <v>2</v>
       </c>
       <c r="H45" t="s">
-        <v>405</v>
+        <v>41</v>
       </c>
       <c r="I45" t="s">
         <v>41</v>
@@ -4386,31 +4377,31 @@
         <v>41</v>
       </c>
       <c r="K45" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
       <c r="L45" t="s">
-        <v>418</v>
+        <v>174</v>
       </c>
       <c r="M45" t="s">
-        <v>419</v>
+        <v>194</v>
       </c>
       <c r="N45" t="s">
-        <v>420</v>
+        <v>195</v>
       </c>
       <c r="O45" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="P45" t="s">
-        <v>41</v>
+        <v>196</v>
       </c>
       <c r="Q45" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="R45" t="s">
-        <v>6</v>
+        <v>357</v>
       </c>
       <c r="S45" t="s">
-        <v>6</v>
+        <v>358</v>
       </c>
       <c r="T45" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -4418,79 +4409,79 @@
       </c>
       <c r="U45">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>353</v>
+        <v>0</v>
       </c>
       <c r="B46" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C46" t="s">
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E46" t="s">
-        <v>193</v>
+        <v>41</v>
       </c>
       <c r="F46" t="s">
-        <v>3</v>
+        <v>149</v>
       </c>
       <c r="G46" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H46" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="I46" t="s">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="J46" t="s">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="K46" t="s">
-        <v>151</v>
+        <v>81</v>
       </c>
       <c r="L46" t="s">
-        <v>174</v>
+        <v>41</v>
       </c>
       <c r="M46" t="s">
-        <v>194</v>
+        <v>95</v>
       </c>
       <c r="N46" t="s">
-        <v>195</v>
+        <v>96</v>
       </c>
       <c r="O46" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="P46" t="s">
-        <v>196</v>
+        <v>97</v>
       </c>
       <c r="Q46" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
       <c r="R46" t="s">
-        <v>357</v>
+        <v>190</v>
       </c>
       <c r="S46" t="s">
-        <v>358</v>
-      </c>
-      <c r="T46" s="8">
+        <v>6</v>
+      </c>
+      <c r="T46">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U46">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B47" t="s">
         <v>248</v>
@@ -4517,7 +4508,7 @@
         <v>2</v>
       </c>
       <c r="J47" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="K47" t="s">
         <v>81</v>
@@ -4526,19 +4517,19 @@
         <v>41</v>
       </c>
       <c r="M47" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="N47" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="O47" t="s">
         <v>85</v>
       </c>
       <c r="P47" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="Q47" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="R47" t="s">
         <v>190</v>
@@ -4548,16 +4539,16 @@
       </c>
       <c r="T47">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U47">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B48" t="s">
         <v>248</v>
@@ -4584,7 +4575,7 @@
         <v>2</v>
       </c>
       <c r="J48" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="K48" t="s">
         <v>81</v>
@@ -4593,19 +4584,19 @@
         <v>41</v>
       </c>
       <c r="M48" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="N48" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="O48" t="s">
         <v>85</v>
       </c>
       <c r="P48" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="Q48" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R48" t="s">
         <v>190</v>
@@ -4615,16 +4606,16 @@
       </c>
       <c r="T48">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U48">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>36</v>
+        <v>122</v>
       </c>
       <c r="B49" t="s">
         <v>248</v>
@@ -4645,53 +4636,50 @@
         <v>3</v>
       </c>
       <c r="H49" t="s">
-        <v>72</v>
+        <v>182</v>
       </c>
       <c r="I49" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J49" t="s">
-        <v>99</v>
+        <v>41</v>
       </c>
       <c r="K49" t="s">
-        <v>81</v>
+        <v>123</v>
       </c>
       <c r="L49" t="s">
-        <v>41</v>
+        <v>124</v>
       </c>
       <c r="M49" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="N49" t="s">
-        <v>101</v>
-      </c>
-      <c r="O49" t="s">
-        <v>85</v>
+        <v>181</v>
       </c>
       <c r="P49" t="s">
-        <v>102</v>
+        <v>180</v>
       </c>
       <c r="Q49" t="s">
-        <v>98</v>
+        <v>6</v>
       </c>
       <c r="R49" t="s">
-        <v>190</v>
+        <v>6</v>
       </c>
       <c r="S49" t="s">
         <v>6</v>
       </c>
       <c r="T49">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U49">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>122</v>
+        <v>38</v>
       </c>
       <c r="B50" t="s">
         <v>248</v>
@@ -4712,56 +4700,59 @@
         <v>3</v>
       </c>
       <c r="H50" t="s">
-        <v>182</v>
+        <v>72</v>
       </c>
       <c r="I50" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J50" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="K50" t="s">
-        <v>123</v>
+        <v>81</v>
       </c>
       <c r="L50" t="s">
-        <v>124</v>
+        <v>41</v>
       </c>
       <c r="M50" t="s">
-        <v>125</v>
+        <v>83</v>
       </c>
       <c r="N50" t="s">
-        <v>181</v>
+        <v>84</v>
+      </c>
+      <c r="O50" t="s">
+        <v>85</v>
       </c>
       <c r="P50" t="s">
-        <v>180</v>
+        <v>86</v>
       </c>
       <c r="Q50" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="R50" t="s">
-        <v>6</v>
+        <v>190</v>
       </c>
       <c r="S50" t="s">
         <v>6</v>
       </c>
       <c r="T50">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U50">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>38</v>
+        <v>114</v>
       </c>
       <c r="B51" t="s">
         <v>248</v>
       </c>
       <c r="C51" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D51" t="s">
         <v>2</v>
@@ -4782,7 +4773,7 @@
         <v>2</v>
       </c>
       <c r="J51" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="K51" t="s">
         <v>81</v>
@@ -4791,22 +4782,22 @@
         <v>41</v>
       </c>
       <c r="M51" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="N51" t="s">
-        <v>84</v>
+        <v>117</v>
       </c>
       <c r="O51" t="s">
         <v>85</v>
       </c>
       <c r="P51" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="Q51" t="s">
-        <v>87</v>
+        <v>41</v>
       </c>
       <c r="R51" t="s">
-        <v>190</v>
+        <v>6</v>
       </c>
       <c r="S51" t="s">
         <v>6</v>
@@ -4817,12 +4808,12 @@
       </c>
       <c r="U51">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B52" t="s">
         <v>248</v>
@@ -4849,7 +4840,7 @@
         <v>2</v>
       </c>
       <c r="J52" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="K52" t="s">
         <v>81</v>
@@ -4858,16 +4849,16 @@
         <v>41</v>
       </c>
       <c r="M52" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="N52" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O52" t="s">
         <v>85</v>
       </c>
       <c r="P52" t="s">
-        <v>118</v>
+        <v>86</v>
       </c>
       <c r="Q52" t="s">
         <v>41</v>
@@ -4889,52 +4880,52 @@
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>119</v>
+        <v>341</v>
       </c>
       <c r="B53" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C53" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E53" t="s">
-        <v>41</v>
+        <v>199</v>
       </c>
       <c r="F53" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="G53" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H53" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="I53" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J53" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="K53" t="s">
-        <v>81</v>
+        <v>210</v>
       </c>
       <c r="L53" t="s">
-        <v>41</v>
+        <v>174</v>
       </c>
       <c r="M53" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="N53" t="s">
-        <v>121</v>
+        <v>212</v>
       </c>
       <c r="O53" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="P53" t="s">
-        <v>86</v>
+        <v>213</v>
       </c>
       <c r="Q53" t="s">
         <v>41</v>
@@ -4943,41 +4934,41 @@
         <v>6</v>
       </c>
       <c r="S53" t="s">
-        <v>6</v>
-      </c>
-      <c r="T53">
+        <v>346</v>
+      </c>
+      <c r="T53" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U53">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>341</v>
+        <v>387</v>
       </c>
       <c r="B54" t="s">
-        <v>250</v>
+        <v>266</v>
       </c>
       <c r="C54" t="s">
         <v>2</v>
       </c>
       <c r="D54" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E54" t="s">
-        <v>199</v>
+        <v>41</v>
       </c>
       <c r="F54" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="G54" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H54" t="s">
-        <v>41</v>
+        <v>388</v>
       </c>
       <c r="I54" t="s">
         <v>6</v>
@@ -4986,31 +4977,31 @@
         <v>41</v>
       </c>
       <c r="K54" t="s">
-        <v>210</v>
+        <v>2</v>
       </c>
       <c r="L54" t="s">
-        <v>174</v>
+        <v>41</v>
       </c>
       <c r="M54" t="s">
-        <v>209</v>
+        <v>389</v>
       </c>
       <c r="N54" t="s">
-        <v>212</v>
+        <v>390</v>
       </c>
       <c r="O54" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="P54" t="s">
-        <v>213</v>
+        <v>391</v>
       </c>
       <c r="Q54" t="s">
         <v>41</v>
       </c>
       <c r="R54" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="S54" t="s">
-        <v>346</v>
+        <v>41</v>
       </c>
       <c r="T54" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -5023,7 +5014,7 @@
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>387</v>
+        <v>260</v>
       </c>
       <c r="B55" t="s">
         <v>266</v>
@@ -5037,47 +5028,8 @@
       <c r="E55" t="s">
         <v>41</v>
       </c>
-      <c r="F55" t="s">
-        <v>149</v>
-      </c>
-      <c r="G55" t="s">
-        <v>3</v>
-      </c>
-      <c r="H55" t="s">
-        <v>388</v>
-      </c>
-      <c r="I55" t="s">
-        <v>6</v>
-      </c>
-      <c r="J55" t="s">
-        <v>41</v>
-      </c>
-      <c r="K55" t="s">
-        <v>2</v>
-      </c>
-      <c r="L55" t="s">
-        <v>41</v>
-      </c>
-      <c r="M55" t="s">
-        <v>389</v>
-      </c>
-      <c r="N55" t="s">
-        <v>390</v>
-      </c>
-      <c r="O55" t="s">
-        <v>6</v>
-      </c>
       <c r="P55" t="s">
-        <v>391</v>
-      </c>
-      <c r="Q55" t="s">
-        <v>41</v>
-      </c>
-      <c r="R55" t="s">
-        <v>41</v>
-      </c>
-      <c r="S55" t="s">
-        <v>41</v>
+        <v>274</v>
       </c>
       <c r="T55" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -5085,15 +5037,15 @@
       </c>
       <c r="U55">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B56" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="C56" t="s">
         <v>2</v>
@@ -5105,7 +5057,7 @@
         <v>41</v>
       </c>
       <c r="P56" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="T56" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -5118,22 +5070,61 @@
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>255</v>
+        <v>354</v>
       </c>
       <c r="B57" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C57" t="s">
         <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E57" t="s">
+        <v>193</v>
+      </c>
+      <c r="F57" t="s">
+        <v>161</v>
+      </c>
+      <c r="G57" t="s">
+        <v>2</v>
+      </c>
+      <c r="H57" t="s">
+        <v>41</v>
+      </c>
+      <c r="I57" t="s">
+        <v>41</v>
+      </c>
+      <c r="J57" t="s">
+        <v>41</v>
+      </c>
+      <c r="K57" t="s">
+        <v>85</v>
+      </c>
+      <c r="L57" t="s">
+        <v>85</v>
+      </c>
+      <c r="M57" t="s">
+        <v>197</v>
+      </c>
+      <c r="N57" t="s">
+        <v>85</v>
+      </c>
+      <c r="O57" t="s">
         <v>41</v>
       </c>
       <c r="P57" t="s">
-        <v>268</v>
+        <v>198</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>41</v>
+      </c>
+      <c r="R57" t="s">
+        <v>6</v>
+      </c>
+      <c r="S57" t="s">
+        <v>358</v>
       </c>
       <c r="T57" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -5146,28 +5137,28 @@
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>354</v>
+        <v>275</v>
       </c>
       <c r="B58" t="s">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="C58" t="s">
         <v>2</v>
       </c>
       <c r="D58" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E58" t="s">
-        <v>193</v>
+        <v>41</v>
       </c>
       <c r="F58" t="s">
-        <v>161</v>
+        <v>3</v>
       </c>
       <c r="G58" t="s">
         <v>2</v>
       </c>
       <c r="H58" t="s">
-        <v>41</v>
+        <v>266</v>
       </c>
       <c r="I58" t="s">
         <v>41</v>
@@ -5176,31 +5167,31 @@
         <v>41</v>
       </c>
       <c r="K58" t="s">
-        <v>85</v>
+        <v>6</v>
       </c>
       <c r="L58" t="s">
-        <v>85</v>
+        <v>6</v>
       </c>
       <c r="M58" t="s">
-        <v>197</v>
+        <v>305</v>
       </c>
       <c r="N58" t="s">
-        <v>85</v>
+        <v>306</v>
       </c>
       <c r="O58" t="s">
-        <v>41</v>
+        <v>307</v>
       </c>
       <c r="P58" t="s">
-        <v>198</v>
+        <v>308</v>
       </c>
       <c r="Q58" t="s">
-        <v>41</v>
+        <v>309</v>
       </c>
       <c r="R58" t="s">
         <v>6</v>
       </c>
       <c r="S58" t="s">
-        <v>358</v>
+        <v>6</v>
       </c>
       <c r="T58" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -5208,33 +5199,33 @@
       </c>
       <c r="U58">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>275</v>
+        <v>418</v>
       </c>
       <c r="B59" t="s">
-        <v>266</v>
+        <v>404</v>
       </c>
       <c r="C59" t="s">
         <v>2</v>
       </c>
       <c r="D59" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E59" t="s">
         <v>41</v>
       </c>
       <c r="F59" t="s">
-        <v>3</v>
+        <v>161</v>
       </c>
       <c r="G59" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H59" t="s">
-        <v>266</v>
+        <v>405</v>
       </c>
       <c r="I59" t="s">
         <v>41</v>
@@ -5243,25 +5234,25 @@
         <v>41</v>
       </c>
       <c r="K59" t="s">
-        <v>6</v>
+        <v>123</v>
       </c>
       <c r="L59" t="s">
-        <v>6</v>
+        <v>419</v>
       </c>
       <c r="M59" t="s">
-        <v>305</v>
+        <v>420</v>
       </c>
       <c r="N59" t="s">
-        <v>306</v>
+        <v>421</v>
       </c>
       <c r="O59" t="s">
-        <v>307</v>
+        <v>6</v>
       </c>
       <c r="P59" t="s">
-        <v>308</v>
+        <v>41</v>
       </c>
       <c r="Q59" t="s">
-        <v>309</v>
+        <v>6</v>
       </c>
       <c r="R59" t="s">
         <v>6</v>
@@ -5275,15 +5266,15 @@
       </c>
       <c r="U59">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>421</v>
+        <v>367</v>
       </c>
       <c r="B60" t="s">
-        <v>404</v>
+        <v>249</v>
       </c>
       <c r="C60" t="s">
         <v>2</v>
@@ -5292,16 +5283,16 @@
         <v>3</v>
       </c>
       <c r="E60" t="s">
-        <v>41</v>
+        <v>193</v>
       </c>
       <c r="F60" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="G60" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H60" t="s">
-        <v>405</v>
+        <v>41</v>
       </c>
       <c r="I60" t="s">
         <v>41</v>
@@ -5310,31 +5301,31 @@
         <v>41</v>
       </c>
       <c r="K60" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
       <c r="L60" t="s">
-        <v>422</v>
+        <v>6</v>
       </c>
       <c r="M60" t="s">
-        <v>423</v>
+        <v>368</v>
       </c>
       <c r="N60" t="s">
-        <v>424</v>
+        <v>369</v>
       </c>
       <c r="O60" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="P60" t="s">
         <v>41</v>
       </c>
       <c r="Q60" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="R60" t="s">
         <v>6</v>
       </c>
       <c r="S60" t="s">
-        <v>6</v>
+        <v>358</v>
       </c>
       <c r="T60" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -5342,66 +5333,27 @@
       </c>
       <c r="U60">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>367</v>
+        <v>256</v>
       </c>
       <c r="B61" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="C61" t="s">
         <v>2</v>
       </c>
       <c r="D61" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E61" t="s">
-        <v>193</v>
-      </c>
-      <c r="F61" t="s">
-        <v>149</v>
-      </c>
-      <c r="G61" t="s">
-        <v>2</v>
-      </c>
-      <c r="H61" t="s">
-        <v>41</v>
-      </c>
-      <c r="I61" t="s">
-        <v>41</v>
-      </c>
-      <c r="J61" t="s">
-        <v>41</v>
-      </c>
-      <c r="K61" t="s">
-        <v>151</v>
-      </c>
-      <c r="L61" t="s">
-        <v>6</v>
-      </c>
-      <c r="M61" t="s">
-        <v>368</v>
-      </c>
-      <c r="N61" t="s">
-        <v>369</v>
-      </c>
-      <c r="O61" t="s">
         <v>41</v>
       </c>
       <c r="P61" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q61" t="s">
-        <v>41</v>
-      </c>
-      <c r="R61" t="s">
-        <v>6</v>
-      </c>
-      <c r="S61" t="s">
-        <v>358</v>
+        <v>276</v>
       </c>
       <c r="T61" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -5409,15 +5361,15 @@
       </c>
       <c r="U61">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>256</v>
+        <v>424</v>
       </c>
       <c r="B62" t="s">
-        <v>259</v>
+        <v>404</v>
       </c>
       <c r="C62" t="s">
         <v>2</v>
@@ -5428,8 +5380,38 @@
       <c r="E62" t="s">
         <v>41</v>
       </c>
+      <c r="F62" t="s">
+        <v>149</v>
+      </c>
+      <c r="G62" t="s">
+        <v>3</v>
+      </c>
+      <c r="H62" t="s">
+        <v>405</v>
+      </c>
+      <c r="I62" t="s">
+        <v>3</v>
+      </c>
+      <c r="J62" t="s">
+        <v>41</v>
+      </c>
+      <c r="K62" t="s">
+        <v>123</v>
+      </c>
+      <c r="L62" s="14" t="s">
+        <v>433</v>
+      </c>
+      <c r="M62" t="s">
+        <v>428</v>
+      </c>
+      <c r="N62" t="s">
+        <v>429</v>
+      </c>
+      <c r="O62" t="s">
+        <v>41</v>
+      </c>
       <c r="P62" t="s">
-        <v>276</v>
+        <v>430</v>
       </c>
       <c r="T62" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -5442,10 +5424,10 @@
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="B63" t="s">
-        <v>404</v>
+        <v>432</v>
       </c>
       <c r="C63" t="s">
         <v>2</v>
@@ -5463,7 +5445,7 @@
         <v>3</v>
       </c>
       <c r="H63" t="s">
-        <v>405</v>
+        <v>41</v>
       </c>
       <c r="I63" t="s">
         <v>3</v>
@@ -5475,19 +5457,28 @@
         <v>123</v>
       </c>
       <c r="L63" s="14" t="s">
+        <v>433</v>
+      </c>
+      <c r="M63" t="s">
+        <v>434</v>
+      </c>
+      <c r="N63" t="s">
+        <v>435</v>
+      </c>
+      <c r="O63" t="s">
+        <v>41</v>
+      </c>
+      <c r="P63" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>41</v>
+      </c>
+      <c r="R63" t="s">
         <v>436</v>
       </c>
-      <c r="M63" t="s">
-        <v>431</v>
-      </c>
-      <c r="N63" t="s">
-        <v>432</v>
-      </c>
-      <c r="O63" t="s">
-        <v>41</v>
-      </c>
-      <c r="P63" t="s">
-        <v>433</v>
+      <c r="S63" t="s">
+        <v>6</v>
       </c>
       <c r="T63" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -5500,46 +5491,46 @@
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="B64" t="s">
-        <v>435</v>
+        <v>6</v>
       </c>
       <c r="C64" t="s">
         <v>2</v>
       </c>
       <c r="D64" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E64" t="s">
         <v>41</v>
       </c>
       <c r="F64" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="G64" t="s">
         <v>3</v>
       </c>
       <c r="H64" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="I64" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="J64" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="K64" t="s">
-        <v>123</v>
-      </c>
-      <c r="L64" s="14" t="s">
-        <v>436</v>
+        <v>41</v>
+      </c>
+      <c r="L64" t="s">
+        <v>41</v>
       </c>
       <c r="M64" t="s">
-        <v>437</v>
+        <v>426</v>
       </c>
       <c r="N64" t="s">
-        <v>438</v>
+        <v>427</v>
       </c>
       <c r="O64" t="s">
         <v>41</v>
@@ -5551,83 +5542,16 @@
         <v>41</v>
       </c>
       <c r="R64" t="s">
-        <v>439</v>
+        <v>41</v>
       </c>
       <c r="S64" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="T64" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>0</v>
       </c>
       <c r="U64">
-        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>428</v>
-      </c>
-      <c r="B65" t="s">
-        <v>6</v>
-      </c>
-      <c r="C65" t="s">
-        <v>2</v>
-      </c>
-      <c r="D65" t="s">
-        <v>3</v>
-      </c>
-      <c r="E65" t="s">
-        <v>41</v>
-      </c>
-      <c r="F65" t="s">
-        <v>161</v>
-      </c>
-      <c r="G65" t="s">
-        <v>3</v>
-      </c>
-      <c r="H65" t="s">
-        <v>6</v>
-      </c>
-      <c r="I65" t="s">
-        <v>41</v>
-      </c>
-      <c r="J65" t="s">
-        <v>6</v>
-      </c>
-      <c r="K65" t="s">
-        <v>41</v>
-      </c>
-      <c r="L65" t="s">
-        <v>41</v>
-      </c>
-      <c r="M65" t="s">
-        <v>429</v>
-      </c>
-      <c r="N65" t="s">
-        <v>430</v>
-      </c>
-      <c r="O65" t="s">
-        <v>41</v>
-      </c>
-      <c r="P65" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q65" t="s">
-        <v>41</v>
-      </c>
-      <c r="R65" t="s">
-        <v>41</v>
-      </c>
-      <c r="S65" t="s">
-        <v>41</v>
-      </c>
-      <c r="T65" s="8">
-        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="U65">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
         <v>0</v>
       </c>
@@ -5801,10 +5725,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P110"/>
+  <dimension ref="A1:P109"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="G110" sqref="G110:J110"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107:XFD107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11309,7 +11233,7 @@
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>414</v>
+        <v>403</v>
       </c>
       <c r="B107" t="s">
         <v>1</v>
@@ -11318,26 +11242,29 @@
         <v>2</v>
       </c>
       <c r="D107" t="s">
-        <v>138</v>
+        <v>54</v>
       </c>
       <c r="E107" s="1">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="F107" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="G107" t="s">
+        <v>422</v>
       </c>
       <c r="H107" t="s">
-        <v>5</v>
+        <v>422</v>
       </c>
       <c r="I107" t="s">
-        <v>6</v>
-      </c>
-      <c r="J107" t="s">
-        <v>6</v>
+        <v>422</v>
+      </c>
+      <c r="J107" s="10" t="s">
+        <v>423</v>
       </c>
       <c r="K107" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>codenGEN30a</v>
+        <v>oclc_numberUNC1.see notes</v>
       </c>
       <c r="L107" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -11368,26 +11295,26 @@
         <v>54</v>
       </c>
       <c r="E108" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F108" t="s">
         <v>6</v>
       </c>
       <c r="G108" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="H108" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="I108" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="J108" s="10" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="K108" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>oclc_numberUNC1.see notes</v>
+        <v>oclc_numberUNC3.see notes</v>
       </c>
       <c r="L108" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -11418,26 +11345,26 @@
         <v>54</v>
       </c>
       <c r="E109" s="1">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="F109" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G109" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="H109" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="I109" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="J109" s="10" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="K109" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>oclc_numberUNC3.see notes</v>
+        <v>oclc_numberUNC35asee notes</v>
       </c>
       <c r="L109" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -11453,65 +11380,15 @@
       </c>
       <c r="O109" s="8"/>
       <c r="P109" s="8"/>
-    </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>403</v>
-      </c>
-      <c r="B110" t="s">
-        <v>1</v>
-      </c>
-      <c r="C110" t="s">
-        <v>2</v>
-      </c>
-      <c r="D110" t="s">
-        <v>54</v>
-      </c>
-      <c r="E110" s="1">
-        <v>35</v>
-      </c>
-      <c r="F110" t="s">
-        <v>7</v>
-      </c>
-      <c r="G110" t="s">
-        <v>425</v>
-      </c>
-      <c r="H110" t="s">
-        <v>425</v>
-      </c>
-      <c r="I110" t="s">
-        <v>425</v>
-      </c>
-      <c r="J110" s="10" t="s">
-        <v>426</v>
-      </c>
-      <c r="K110" s="8" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>oclc_numberUNC35asee notes</v>
-      </c>
-      <c r="L110" s="8">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M110" s="8">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="N110" s="8" t="str">
-        <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
-        <v>y</v>
-      </c>
-      <c r="O110" s="8"/>
-      <c r="P110" s="8"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K3:K65">
     <cfRule type="duplicateValues" dxfId="1" priority="8"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J108" r:id="rId1"/>
-    <hyperlink ref="J109" r:id="rId2"/>
-    <hyperlink ref="J110" r:id="rId3"/>
+    <hyperlink ref="J107" r:id="rId1"/>
+    <hyperlink ref="J108" r:id="rId2"/>
+    <hyperlink ref="J109" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId4"/>

</xml_diff>

<commit_message>
misc_ids << lccn, nucmc
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="5910"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="5910" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2152" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2170" uniqueCount="455">
   <si>
     <t>subject_chronological_facet</t>
   </si>
@@ -1386,6 +1386,12 @@
   </si>
   <si>
     <t>Staff search, possibly of use for rolling up e-resources or other format records, if institutions use the same MARC record source</t>
+  </si>
+  <si>
+    <t>qual MUST = "";;;type = "LCCN";;;Do NOT trim leading/trailing spaces</t>
+  </si>
+  <si>
+    <t>qual MUST = "";;;type = "NUCMC";;;Do NOT trim leading/trailing spaces</t>
   </si>
 </sst>
 </file>
@@ -1672,6 +1678,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="fields" displayName="fields" ref="A1:V60" totalsRowShown="0">
   <autoFilter ref="A1:V60"/>
+  <sortState ref="A2:V60">
+    <sortCondition ref="A1:A60"/>
+  </sortState>
   <tableColumns count="22">
     <tableColumn id="2" name="field"/>
     <tableColumn id="22" name="category"/>
@@ -1718,11 +1727,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="mappings" displayName="mappings" ref="A1:P109" totalsRowShown="0">
-  <autoFilter ref="A1:P109"/>
-  <sortState ref="A2:P109">
-    <sortCondition ref="A1:A109"/>
-  </sortState>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="mappings" displayName="mappings" ref="A1:P111" totalsRowShown="0">
+  <autoFilter ref="A1:P111"/>
   <tableColumns count="16">
     <tableColumn id="1" name="field"/>
     <tableColumn id="2" name="source data format"/>
@@ -2031,9 +2037,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H34" sqref="H34"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A34" sqref="A34:A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4013,7 +4019,7 @@
       </c>
       <c r="T34">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
@@ -5421,10 +5427,10 @@
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>421</v>
+        <v>450</v>
       </c>
       <c r="B58" t="s">
-        <v>6</v>
+        <v>385</v>
       </c>
       <c r="C58" t="s">
         <v>2</v>
@@ -5439,25 +5445,25 @@
         <v>440</v>
       </c>
       <c r="G58" t="s">
-        <v>6</v>
+        <v>386</v>
       </c>
       <c r="H58" t="s">
         <v>41</v>
       </c>
       <c r="I58" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="J58" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="K58" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="L58" t="s">
-        <v>401</v>
+        <v>451</v>
       </c>
       <c r="M58" t="s">
-        <v>402</v>
+        <v>452</v>
       </c>
       <c r="N58" t="s">
         <v>41</v>
@@ -5485,10 +5491,10 @@
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>348</v>
+        <v>421</v>
       </c>
       <c r="B59" t="s">
-        <v>245</v>
+        <v>6</v>
       </c>
       <c r="C59" t="s">
         <v>2</v>
@@ -5497,31 +5503,31 @@
         <v>3</v>
       </c>
       <c r="E59" t="s">
-        <v>190</v>
+        <v>41</v>
       </c>
       <c r="F59" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="G59" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="H59" t="s">
         <v>41</v>
       </c>
       <c r="I59" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="J59" t="s">
-        <v>150</v>
+        <v>41</v>
       </c>
       <c r="K59" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="L59" t="s">
-        <v>349</v>
+        <v>401</v>
       </c>
       <c r="M59" t="s">
-        <v>350</v>
+        <v>402</v>
       </c>
       <c r="N59" t="s">
         <v>41</v>
@@ -5533,10 +5539,10 @@
         <v>41</v>
       </c>
       <c r="Q59" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="R59" t="s">
-        <v>339</v>
+        <v>41</v>
       </c>
       <c r="S59" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -5544,15 +5550,15 @@
       </c>
       <c r="T59">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>450</v>
+        <v>348</v>
       </c>
       <c r="B60" t="s">
-        <v>385</v>
+        <v>245</v>
       </c>
       <c r="C60" t="s">
         <v>2</v>
@@ -5561,13 +5567,13 @@
         <v>3</v>
       </c>
       <c r="E60" t="s">
-        <v>41</v>
+        <v>190</v>
       </c>
       <c r="F60" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="G60" t="s">
-        <v>386</v>
+        <v>41</v>
       </c>
       <c r="H60" t="s">
         <v>41</v>
@@ -5576,16 +5582,16 @@
         <v>41</v>
       </c>
       <c r="J60" t="s">
-        <v>84</v>
+        <v>150</v>
       </c>
       <c r="K60" t="s">
         <v>6</v>
       </c>
       <c r="L60" t="s">
-        <v>451</v>
+        <v>349</v>
       </c>
       <c r="M60" t="s">
-        <v>452</v>
+        <v>350</v>
       </c>
       <c r="N60" t="s">
         <v>41</v>
@@ -5597,10 +5603,10 @@
         <v>41</v>
       </c>
       <c r="Q60" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="R60" t="s">
-        <v>41</v>
+        <v>339</v>
       </c>
       <c r="S60" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -5608,7 +5614,7 @@
       </c>
       <c r="T60">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5780,9 +5786,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P109"/>
+  <dimension ref="A1:P111"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="I112" sqref="I112"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11433,6 +11441,106 @@
       <c r="P109" s="8" t="s">
         <v>3</v>
       </c>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>422</v>
+      </c>
+      <c r="B110" t="s">
+        <v>1</v>
+      </c>
+      <c r="C110" t="s">
+        <v>2</v>
+      </c>
+      <c r="D110" t="s">
+        <v>137</v>
+      </c>
+      <c r="E110" s="1">
+        <v>10</v>
+      </c>
+      <c r="F110" t="s">
+        <v>7</v>
+      </c>
+      <c r="G110" t="s">
+        <v>6</v>
+      </c>
+      <c r="H110" t="s">
+        <v>5</v>
+      </c>
+      <c r="I110" t="s">
+        <v>453</v>
+      </c>
+      <c r="J110" t="s">
+        <v>41</v>
+      </c>
+      <c r="K110" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>misc_idGEN10a.</v>
+      </c>
+      <c r="L110" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M110" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N110" s="8" t="str">
+        <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
+        <v>y</v>
+      </c>
+      <c r="O110" s="8"/>
+      <c r="P110" s="8"/>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>422</v>
+      </c>
+      <c r="B111" t="s">
+        <v>1</v>
+      </c>
+      <c r="C111" t="s">
+        <v>2</v>
+      </c>
+      <c r="D111" t="s">
+        <v>137</v>
+      </c>
+      <c r="E111" s="1">
+        <v>10</v>
+      </c>
+      <c r="F111" t="s">
+        <v>163</v>
+      </c>
+      <c r="G111" t="s">
+        <v>6</v>
+      </c>
+      <c r="H111" t="s">
+        <v>5</v>
+      </c>
+      <c r="I111" t="s">
+        <v>454</v>
+      </c>
+      <c r="J111" t="s">
+        <v>41</v>
+      </c>
+      <c r="K111" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>misc_idGEN10b.</v>
+      </c>
+      <c r="L111" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M111" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N111" s="8" t="str">
+        <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
+        <v>y</v>
+      </c>
+      <c r="O111" s="8"/>
+      <c r="P111" s="8"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K3:K65">

</xml_diff>

<commit_message>
misc_id << natl biblio num
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2170" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2196" uniqueCount="459">
   <si>
     <t>subject_chronological_facet</t>
   </si>
@@ -1392,6 +1392,18 @@
   </si>
   <si>
     <t>qual MUST = "";;;type = "NUCMC";;;Do NOT trim leading/trailing spaces</t>
+  </si>
+  <si>
+    <t>if subfield includes parentheses, split into 'id' and 'qual';;;if subfield contains no parentheses, 'id' = whole subfield value</t>
+  </si>
+  <si>
+    <t>qual = subfield valuewith parentheses removed</t>
+  </si>
+  <si>
+    <t>type = "National Bibliography Number" if there is no $2; otherwise, map $2 using https://github.com/trln/marc-to-argot/blob/master/lib/translation_maps/shared/national_bibliography_codes.yaml</t>
+  </si>
+  <si>
+    <t>Mapping is from: https://www.loc.gov/standards/sourcelist/national-bibliography.html</t>
   </si>
 </sst>
 </file>
@@ -1727,8 +1739,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="mappings" displayName="mappings" ref="A1:P111" totalsRowShown="0">
-  <autoFilter ref="A1:P111"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="mappings" displayName="mappings" ref="A1:P114" totalsRowShown="0">
+  <autoFilter ref="A1:P114"/>
   <tableColumns count="16">
     <tableColumn id="1" name="field"/>
     <tableColumn id="2" name="source data format"/>
@@ -4019,7 +4031,7 @@
       </c>
       <c r="T34">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
@@ -5786,10 +5798,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P111"/>
+  <dimension ref="A1:P114"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="I112" sqref="I112"/>
+      <selection activeCell="K114" sqref="K114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11541,6 +11553,156 @@
       </c>
       <c r="O111" s="8"/>
       <c r="P111" s="8"/>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>422</v>
+      </c>
+      <c r="B112" t="s">
+        <v>1</v>
+      </c>
+      <c r="C112" t="s">
+        <v>2</v>
+      </c>
+      <c r="D112" t="s">
+        <v>137</v>
+      </c>
+      <c r="E112" s="1">
+        <v>15</v>
+      </c>
+      <c r="F112" t="s">
+        <v>7</v>
+      </c>
+      <c r="G112" t="s">
+        <v>6</v>
+      </c>
+      <c r="H112" t="s">
+        <v>5</v>
+      </c>
+      <c r="I112" t="s">
+        <v>455</v>
+      </c>
+      <c r="J112" t="s">
+        <v>41</v>
+      </c>
+      <c r="K112" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>misc_idGEN15a.</v>
+      </c>
+      <c r="L112" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M112" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N112" s="8" t="str">
+        <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
+        <v>y</v>
+      </c>
+      <c r="O112" s="8"/>
+      <c r="P112" s="8"/>
+    </row>
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>422</v>
+      </c>
+      <c r="B113" t="s">
+        <v>1</v>
+      </c>
+      <c r="C113" t="s">
+        <v>2</v>
+      </c>
+      <c r="D113" t="s">
+        <v>137</v>
+      </c>
+      <c r="E113" s="1">
+        <v>15</v>
+      </c>
+      <c r="F113" t="s">
+        <v>356</v>
+      </c>
+      <c r="G113" t="s">
+        <v>6</v>
+      </c>
+      <c r="H113" t="s">
+        <v>5</v>
+      </c>
+      <c r="I113" t="s">
+        <v>456</v>
+      </c>
+      <c r="J113" t="s">
+        <v>41</v>
+      </c>
+      <c r="K113" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>misc_idGEN15q.</v>
+      </c>
+      <c r="L113" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M113" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N113" s="8" t="str">
+        <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
+        <v>y</v>
+      </c>
+      <c r="O113" s="8"/>
+      <c r="P113" s="8"/>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>422</v>
+      </c>
+      <c r="B114" t="s">
+        <v>1</v>
+      </c>
+      <c r="C114" t="s">
+        <v>2</v>
+      </c>
+      <c r="D114" t="s">
+        <v>137</v>
+      </c>
+      <c r="E114" s="1">
+        <v>15</v>
+      </c>
+      <c r="F114">
+        <v>2</v>
+      </c>
+      <c r="G114" t="s">
+        <v>6</v>
+      </c>
+      <c r="H114" t="s">
+        <v>228</v>
+      </c>
+      <c r="I114" t="s">
+        <v>457</v>
+      </c>
+      <c r="J114" t="s">
+        <v>458</v>
+      </c>
+      <c r="K114" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>misc_idGEN152.</v>
+      </c>
+      <c r="L114" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M114" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N114" s="8" t="str">
+        <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
+        <v>y</v>
+      </c>
+      <c r="O114" s="8"/>
+      <c r="P114" s="8"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K3:K65">

</xml_diff>

<commit_message>
add record_data_source field and mapping
At this point mapping assumes all records sent through MARC-to-Argot
will MARC records from institutional ILSs. Mapping specifies that value
should = 'ILSMARC'
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="5910" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="5910"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2243" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2281" uniqueCount="477">
   <si>
     <t>subject_chronological_facet</t>
   </si>
@@ -1434,6 +1434,30 @@
   </si>
   <si>
     <t>Prefix with OCLC</t>
+  </si>
+  <si>
+    <t>record_data_source</t>
+  </si>
+  <si>
+    <t>value = 'ILSMARC'</t>
+  </si>
+  <si>
+    <t>{1,n}</t>
+  </si>
+  <si>
+    <t>(admin/reference implementation only): Data source</t>
+  </si>
+  <si>
+    <t>Data source(s) for record</t>
+  </si>
+  <si>
+    <t>Invaluable for doing data work/troubleshooting.</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Values: ILSMARC, DC, EAD, ICE, Shared:#{Name/code of shared record set};;;Multiple values required because a final record in the system may mainly come from ILSMARC, but also be Shared, or have data merged in from EAD or ICE. </t>
   </si>
 </sst>
 </file>
@@ -1720,8 +1744,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="fields" displayName="fields" ref="A1:V61" totalsRowShown="0">
-  <autoFilter ref="A1:V61"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="fields" displayName="fields" ref="A1:V62" totalsRowShown="0">
+  <autoFilter ref="A1:V62"/>
   <sortState ref="A2:V60">
     <sortCondition ref="A1:A60"/>
   </sortState>
@@ -1771,8 +1795,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="mappings" displayName="mappings" ref="A1:P116" totalsRowShown="0">
-  <autoFilter ref="A1:P116"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="mappings" displayName="mappings" ref="A1:P117" totalsRowShown="0">
+  <autoFilter ref="A1:P117"/>
   <sortState ref="A2:P116">
     <sortCondition ref="A1:A116"/>
   </sortState>
@@ -2082,11 +2106,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V61"/>
+  <dimension ref="A1:V62"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S41" sqref="S41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4455,71 +4479,71 @@
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>459</v>
+        <v>469</v>
       </c>
       <c r="B41" t="s">
-        <v>385</v>
+        <v>6</v>
       </c>
       <c r="C41" t="s">
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E41" t="s">
         <v>41</v>
       </c>
       <c r="F41" t="s">
-        <v>443</v>
+        <v>471</v>
       </c>
       <c r="G41" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="H41" t="s">
         <v>41</v>
       </c>
       <c r="I41" t="s">
-        <v>41</v>
+        <v>472</v>
       </c>
       <c r="J41" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="K41" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="L41" t="s">
-        <v>460</v>
+        <v>473</v>
       </c>
       <c r="M41" t="s">
-        <v>461</v>
+        <v>474</v>
       </c>
       <c r="N41" t="s">
         <v>41</v>
       </c>
       <c r="O41" t="s">
-        <v>462</v>
+        <v>475</v>
       </c>
       <c r="P41" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="Q41" t="s">
-        <v>6</v>
+        <v>476</v>
       </c>
       <c r="R41" t="s">
         <v>6</v>
       </c>
       <c r="S41" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T41">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>394</v>
+        <v>459</v>
       </c>
       <c r="B42" t="s">
         <v>385</v>
@@ -4537,7 +4561,7 @@
         <v>443</v>
       </c>
       <c r="G42" t="s">
-        <v>386</v>
+        <v>41</v>
       </c>
       <c r="H42" t="s">
         <v>41</v>
@@ -4546,22 +4570,22 @@
         <v>41</v>
       </c>
       <c r="J42" t="s">
-        <v>122</v>
+        <v>41</v>
       </c>
       <c r="K42" t="s">
-        <v>395</v>
+        <v>41</v>
       </c>
       <c r="L42" t="s">
-        <v>396</v>
+        <v>460</v>
       </c>
       <c r="M42" t="s">
-        <v>397</v>
+        <v>461</v>
       </c>
       <c r="N42" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="O42" t="s">
-        <v>41</v>
+        <v>462</v>
       </c>
       <c r="P42" t="s">
         <v>6</v>
@@ -4574,25 +4598,25 @@
       </c>
       <c r="S42" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T42">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>445</v>
+        <v>394</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>385</v>
       </c>
       <c r="C43" t="s">
         <v>2</v>
       </c>
       <c r="D43" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E43" t="s">
         <v>41</v>
@@ -4601,13 +4625,40 @@
         <v>443</v>
       </c>
       <c r="G43" t="s">
-        <v>447</v>
+        <v>386</v>
       </c>
       <c r="H43" t="s">
         <v>41</v>
       </c>
+      <c r="I43" t="s">
+        <v>41</v>
+      </c>
+      <c r="J43" t="s">
+        <v>122</v>
+      </c>
+      <c r="K43" t="s">
+        <v>395</v>
+      </c>
+      <c r="L43" t="s">
+        <v>396</v>
+      </c>
+      <c r="M43" t="s">
+        <v>397</v>
+      </c>
+      <c r="N43" t="s">
+        <v>6</v>
+      </c>
       <c r="O43" t="s">
-        <v>463</v>
+        <v>41</v>
+      </c>
+      <c r="P43" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>6</v>
+      </c>
+      <c r="R43" t="s">
+        <v>6</v>
       </c>
       <c r="S43" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -4620,58 +4671,31 @@
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>334</v>
+        <v>445</v>
       </c>
       <c r="B44" t="s">
-        <v>245</v>
+        <v>6</v>
       </c>
       <c r="C44" t="s">
         <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E44" t="s">
-        <v>190</v>
+        <v>41</v>
       </c>
       <c r="F44" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="G44" t="s">
-        <v>41</v>
+        <v>447</v>
       </c>
       <c r="H44" t="s">
         <v>41</v>
       </c>
-      <c r="I44" t="s">
-        <v>41</v>
-      </c>
-      <c r="J44" t="s">
-        <v>150</v>
-      </c>
-      <c r="K44" t="s">
-        <v>171</v>
-      </c>
-      <c r="L44" t="s">
-        <v>191</v>
-      </c>
-      <c r="M44" t="s">
-        <v>192</v>
-      </c>
-      <c r="N44" t="s">
-        <v>41</v>
-      </c>
       <c r="O44" t="s">
-        <v>193</v>
-      </c>
-      <c r="P44" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q44" t="s">
-        <v>338</v>
-      </c>
-      <c r="R44" t="s">
-        <v>339</v>
+        <v>463</v>
       </c>
       <c r="S44" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -4679,76 +4703,76 @@
       </c>
       <c r="T44">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>0</v>
+        <v>334</v>
       </c>
       <c r="B45" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C45" t="s">
         <v>2</v>
       </c>
       <c r="D45" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E45" t="s">
-        <v>41</v>
+        <v>190</v>
       </c>
       <c r="F45" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="G45" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="H45" t="s">
         <v>41</v>
       </c>
       <c r="I45" t="s">
-        <v>93</v>
+        <v>41</v>
       </c>
       <c r="J45" t="s">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="K45" t="s">
-        <v>41</v>
+        <v>171</v>
       </c>
       <c r="L45" t="s">
-        <v>94</v>
+        <v>191</v>
       </c>
       <c r="M45" t="s">
-        <v>95</v>
+        <v>192</v>
       </c>
       <c r="N45" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="O45" t="s">
-        <v>96</v>
+        <v>193</v>
       </c>
       <c r="P45" t="s">
-        <v>97</v>
+        <v>41</v>
       </c>
       <c r="Q45" t="s">
-        <v>187</v>
+        <v>338</v>
       </c>
       <c r="R45" t="s">
-        <v>6</v>
-      </c>
-      <c r="S45">
+        <v>339</v>
+      </c>
+      <c r="S45" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T45">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B46" t="s">
         <v>244</v>
@@ -4772,7 +4796,7 @@
         <v>41</v>
       </c>
       <c r="I46" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="J46" t="s">
         <v>80</v>
@@ -4781,19 +4805,19 @@
         <v>41</v>
       </c>
       <c r="L46" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="M46" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="N46" t="s">
         <v>84</v>
       </c>
       <c r="O46" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="P46" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="Q46" t="s">
         <v>187</v>
@@ -4803,16 +4827,16 @@
       </c>
       <c r="S46">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T46">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B47" t="s">
         <v>244</v>
@@ -4836,7 +4860,7 @@
         <v>41</v>
       </c>
       <c r="I47" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="J47" t="s">
         <v>80</v>
@@ -4845,19 +4869,19 @@
         <v>41</v>
       </c>
       <c r="L47" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="M47" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="N47" t="s">
         <v>84</v>
       </c>
       <c r="O47" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="P47" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="Q47" t="s">
         <v>187</v>
@@ -4867,16 +4891,16 @@
       </c>
       <c r="S47">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T47">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>121</v>
+        <v>36</v>
       </c>
       <c r="B48" t="s">
         <v>244</v>
@@ -4894,50 +4918,53 @@
         <v>440</v>
       </c>
       <c r="G48" t="s">
-        <v>179</v>
+        <v>71</v>
       </c>
       <c r="H48" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="I48" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
       <c r="J48" t="s">
-        <v>122</v>
+        <v>80</v>
       </c>
       <c r="K48" t="s">
-        <v>123</v>
+        <v>41</v>
       </c>
       <c r="L48" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="M48" t="s">
-        <v>178</v>
+        <v>100</v>
+      </c>
+      <c r="N48" t="s">
+        <v>84</v>
       </c>
       <c r="O48" t="s">
-        <v>177</v>
+        <v>101</v>
       </c>
       <c r="P48" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="Q48" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="R48" t="s">
         <v>6</v>
       </c>
       <c r="S48">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T48">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>38</v>
+        <v>121</v>
       </c>
       <c r="B49" t="s">
         <v>244</v>
@@ -4955,59 +4982,56 @@
         <v>440</v>
       </c>
       <c r="G49" t="s">
-        <v>71</v>
+        <v>179</v>
       </c>
       <c r="H49" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="I49" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="J49" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="K49" t="s">
-        <v>41</v>
+        <v>123</v>
       </c>
       <c r="L49" t="s">
-        <v>82</v>
+        <v>124</v>
       </c>
       <c r="M49" t="s">
-        <v>83</v>
-      </c>
-      <c r="N49" t="s">
-        <v>84</v>
+        <v>178</v>
       </c>
       <c r="O49" t="s">
-        <v>85</v>
+        <v>177</v>
       </c>
       <c r="P49" t="s">
-        <v>86</v>
+        <v>6</v>
       </c>
       <c r="Q49" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="R49" t="s">
         <v>6</v>
       </c>
       <c r="S49">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T49">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>113</v>
+        <v>38</v>
       </c>
       <c r="B50" t="s">
         <v>244</v>
       </c>
       <c r="C50" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D50" t="s">
         <v>2</v>
@@ -5025,7 +5049,7 @@
         <v>41</v>
       </c>
       <c r="I50" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="J50" t="s">
         <v>80</v>
@@ -5034,22 +5058,22 @@
         <v>41</v>
       </c>
       <c r="L50" t="s">
-        <v>115</v>
+        <v>82</v>
       </c>
       <c r="M50" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
       <c r="N50" t="s">
         <v>84</v>
       </c>
       <c r="O50" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="P50" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="Q50" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="R50" t="s">
         <v>6</v>
@@ -5060,12 +5084,12 @@
       </c>
       <c r="T50">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B51" t="s">
         <v>244</v>
@@ -5089,7 +5113,7 @@
         <v>41</v>
       </c>
       <c r="I51" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="J51" t="s">
         <v>80</v>
@@ -5098,16 +5122,16 @@
         <v>41</v>
       </c>
       <c r="L51" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="M51" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="N51" t="s">
         <v>84</v>
       </c>
       <c r="O51" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="P51" t="s">
         <v>41</v>
@@ -5129,89 +5153,89 @@
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>322</v>
+        <v>118</v>
       </c>
       <c r="B52" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C52" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D52" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E52" t="s">
-        <v>196</v>
+        <v>41</v>
       </c>
       <c r="F52" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="G52" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="H52" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="I52" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="J52" t="s">
-        <v>207</v>
+        <v>80</v>
       </c>
       <c r="K52" t="s">
-        <v>171</v>
+        <v>41</v>
       </c>
       <c r="L52" t="s">
-        <v>206</v>
+        <v>119</v>
       </c>
       <c r="M52" t="s">
-        <v>209</v>
+        <v>120</v>
       </c>
       <c r="N52" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="O52" t="s">
-        <v>210</v>
+        <v>85</v>
       </c>
       <c r="P52" t="s">
         <v>41</v>
       </c>
       <c r="Q52" t="s">
-        <v>446</v>
+        <v>6</v>
       </c>
       <c r="R52" t="s">
-        <v>327</v>
-      </c>
-      <c r="S52" s="8">
+        <v>6</v>
+      </c>
+      <c r="S52">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T52">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>368</v>
+        <v>322</v>
       </c>
       <c r="B53" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C53" t="s">
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E53" t="s">
-        <v>41</v>
+        <v>196</v>
       </c>
       <c r="F53" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="G53" t="s">
-        <v>369</v>
+        <v>41</v>
       </c>
       <c r="H53" t="s">
         <v>3</v>
@@ -5220,31 +5244,31 @@
         <v>41</v>
       </c>
       <c r="J53" t="s">
-        <v>2</v>
+        <v>207</v>
       </c>
       <c r="K53" t="s">
-        <v>41</v>
+        <v>171</v>
       </c>
       <c r="L53" t="s">
-        <v>370</v>
+        <v>206</v>
       </c>
       <c r="M53" t="s">
-        <v>371</v>
+        <v>209</v>
       </c>
       <c r="N53" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="O53" t="s">
-        <v>372</v>
+        <v>210</v>
       </c>
       <c r="P53" t="s">
         <v>41</v>
       </c>
       <c r="Q53" t="s">
-        <v>41</v>
+        <v>446</v>
       </c>
       <c r="R53" t="s">
-        <v>41</v>
+        <v>327</v>
       </c>
       <c r="S53" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -5257,7 +5281,7 @@
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>249</v>
+        <v>368</v>
       </c>
       <c r="B54" t="s">
         <v>251</v>
@@ -5272,16 +5296,43 @@
         <v>41</v>
       </c>
       <c r="F54" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="G54" t="s">
-        <v>448</v>
+        <v>369</v>
       </c>
       <c r="H54" t="s">
-        <v>41</v>
+        <v>3</v>
+      </c>
+      <c r="I54" t="s">
+        <v>41</v>
+      </c>
+      <c r="J54" t="s">
+        <v>2</v>
+      </c>
+      <c r="K54" t="s">
+        <v>41</v>
+      </c>
+      <c r="L54" t="s">
+        <v>370</v>
+      </c>
+      <c r="M54" t="s">
+        <v>371</v>
+      </c>
+      <c r="N54" t="s">
+        <v>6</v>
       </c>
       <c r="O54" t="s">
-        <v>257</v>
+        <v>372</v>
+      </c>
+      <c r="P54" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>41</v>
+      </c>
+      <c r="R54" t="s">
+        <v>41</v>
       </c>
       <c r="S54" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -5289,63 +5340,36 @@
       </c>
       <c r="T54">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>335</v>
+        <v>249</v>
       </c>
       <c r="B55" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="C55" t="s">
         <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E55" t="s">
-        <v>190</v>
+        <v>41</v>
       </c>
       <c r="F55" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="G55" t="s">
-        <v>41</v>
+        <v>448</v>
       </c>
       <c r="H55" t="s">
         <v>41</v>
       </c>
-      <c r="I55" t="s">
-        <v>41</v>
-      </c>
-      <c r="J55" t="s">
-        <v>84</v>
-      </c>
-      <c r="K55" t="s">
-        <v>84</v>
-      </c>
-      <c r="L55" t="s">
-        <v>194</v>
-      </c>
-      <c r="M55" t="s">
-        <v>84</v>
-      </c>
-      <c r="N55" t="s">
-        <v>41</v>
-      </c>
       <c r="O55" t="s">
-        <v>195</v>
-      </c>
-      <c r="P55" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q55" t="s">
-        <v>6</v>
-      </c>
-      <c r="R55" t="s">
-        <v>339</v>
+        <v>257</v>
       </c>
       <c r="S55" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -5358,25 +5382,25 @@
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>258</v>
+        <v>335</v>
       </c>
       <c r="B56" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C56" t="s">
         <v>2</v>
       </c>
       <c r="D56" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E56" t="s">
-        <v>41</v>
+        <v>190</v>
       </c>
       <c r="F56" t="s">
         <v>443</v>
       </c>
       <c r="G56" t="s">
-        <v>251</v>
+        <v>41</v>
       </c>
       <c r="H56" t="s">
         <v>41</v>
@@ -5385,31 +5409,31 @@
         <v>41</v>
       </c>
       <c r="J56" t="s">
-        <v>6</v>
+        <v>84</v>
       </c>
       <c r="K56" t="s">
-        <v>6</v>
+        <v>84</v>
       </c>
       <c r="L56" t="s">
-        <v>286</v>
+        <v>194</v>
       </c>
       <c r="M56" t="s">
-        <v>287</v>
+        <v>84</v>
       </c>
       <c r="N56" t="s">
-        <v>288</v>
+        <v>41</v>
       </c>
       <c r="O56" t="s">
-        <v>289</v>
+        <v>195</v>
       </c>
       <c r="P56" t="s">
-        <v>290</v>
+        <v>41</v>
       </c>
       <c r="Q56" t="s">
         <v>6</v>
       </c>
       <c r="R56" t="s">
-        <v>6</v>
+        <v>339</v>
       </c>
       <c r="S56" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -5417,15 +5441,15 @@
       </c>
       <c r="T56">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>400</v>
+        <v>258</v>
       </c>
       <c r="B57" t="s">
-        <v>385</v>
+        <v>251</v>
       </c>
       <c r="C57" t="s">
         <v>2</v>
@@ -5437,34 +5461,43 @@
         <v>41</v>
       </c>
       <c r="F57" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="G57" t="s">
-        <v>386</v>
+        <v>251</v>
       </c>
       <c r="H57" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="I57" t="s">
         <v>41</v>
       </c>
       <c r="J57" t="s">
-        <v>122</v>
-      </c>
-      <c r="K57" s="14" t="s">
-        <v>408</v>
+        <v>6</v>
+      </c>
+      <c r="K57" t="s">
+        <v>6</v>
       </c>
       <c r="L57" t="s">
-        <v>403</v>
+        <v>286</v>
       </c>
       <c r="M57" t="s">
-        <v>404</v>
+        <v>287</v>
       </c>
       <c r="N57" t="s">
-        <v>41</v>
+        <v>288</v>
       </c>
       <c r="O57" t="s">
-        <v>405</v>
+        <v>289</v>
+      </c>
+      <c r="P57" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>6</v>
+      </c>
+      <c r="R57" t="s">
+        <v>6</v>
       </c>
       <c r="S57" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -5472,15 +5505,15 @@
       </c>
       <c r="T57">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="B58" t="s">
-        <v>407</v>
+        <v>385</v>
       </c>
       <c r="C58" t="s">
         <v>2</v>
@@ -5495,7 +5528,7 @@
         <v>440</v>
       </c>
       <c r="G58" t="s">
-        <v>41</v>
+        <v>386</v>
       </c>
       <c r="H58" t="s">
         <v>3</v>
@@ -5510,25 +5543,16 @@
         <v>408</v>
       </c>
       <c r="L58" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="M58" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="N58" t="s">
         <v>41</v>
       </c>
       <c r="O58" t="s">
-        <v>41</v>
-      </c>
-      <c r="P58" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q58" t="s">
-        <v>411</v>
-      </c>
-      <c r="R58" t="s">
-        <v>6</v>
+        <v>405</v>
       </c>
       <c r="S58" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -5541,16 +5565,16 @@
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>450</v>
+        <v>406</v>
       </c>
       <c r="B59" t="s">
-        <v>385</v>
+        <v>407</v>
       </c>
       <c r="C59" t="s">
         <v>2</v>
       </c>
       <c r="D59" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E59" t="s">
         <v>41</v>
@@ -5559,25 +5583,25 @@
         <v>440</v>
       </c>
       <c r="G59" t="s">
-        <v>386</v>
+        <v>41</v>
       </c>
       <c r="H59" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="I59" t="s">
         <v>41</v>
       </c>
       <c r="J59" t="s">
-        <v>84</v>
-      </c>
-      <c r="K59" t="s">
-        <v>6</v>
+        <v>122</v>
+      </c>
+      <c r="K59" s="14" t="s">
+        <v>408</v>
       </c>
       <c r="L59" t="s">
-        <v>451</v>
+        <v>409</v>
       </c>
       <c r="M59" t="s">
-        <v>452</v>
+        <v>410</v>
       </c>
       <c r="N59" t="s">
         <v>41</v>
@@ -5589,10 +5613,10 @@
         <v>41</v>
       </c>
       <c r="Q59" t="s">
-        <v>41</v>
+        <v>411</v>
       </c>
       <c r="R59" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="S59" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -5605,10 +5629,10 @@
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>421</v>
+        <v>450</v>
       </c>
       <c r="B60" t="s">
-        <v>6</v>
+        <v>385</v>
       </c>
       <c r="C60" t="s">
         <v>2</v>
@@ -5623,25 +5647,25 @@
         <v>440</v>
       </c>
       <c r="G60" t="s">
-        <v>6</v>
+        <v>386</v>
       </c>
       <c r="H60" t="s">
         <v>41</v>
       </c>
       <c r="I60" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="J60" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="K60" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="L60" t="s">
-        <v>401</v>
+        <v>451</v>
       </c>
       <c r="M60" t="s">
-        <v>402</v>
+        <v>452</v>
       </c>
       <c r="N60" t="s">
         <v>41</v>
@@ -5669,10 +5693,10 @@
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>348</v>
+        <v>421</v>
       </c>
       <c r="B61" t="s">
-        <v>245</v>
+        <v>6</v>
       </c>
       <c r="C61" t="s">
         <v>2</v>
@@ -5681,31 +5705,31 @@
         <v>3</v>
       </c>
       <c r="E61" t="s">
-        <v>190</v>
+        <v>41</v>
       </c>
       <c r="F61" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="G61" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="H61" t="s">
         <v>41</v>
       </c>
       <c r="I61" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="J61" t="s">
-        <v>150</v>
+        <v>41</v>
       </c>
       <c r="K61" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="L61" t="s">
-        <v>349</v>
+        <v>401</v>
       </c>
       <c r="M61" t="s">
-        <v>350</v>
+        <v>402</v>
       </c>
       <c r="N61" t="s">
         <v>41</v>
@@ -5717,16 +5741,80 @@
         <v>41</v>
       </c>
       <c r="Q61" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="R61" t="s">
-        <v>339</v>
+        <v>41</v>
       </c>
       <c r="S61" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>0</v>
       </c>
       <c r="T61">
+        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>348</v>
+      </c>
+      <c r="B62" t="s">
+        <v>245</v>
+      </c>
+      <c r="C62" t="s">
+        <v>2</v>
+      </c>
+      <c r="D62" t="s">
+        <v>3</v>
+      </c>
+      <c r="E62" t="s">
+        <v>190</v>
+      </c>
+      <c r="F62" t="s">
+        <v>443</v>
+      </c>
+      <c r="G62" t="s">
+        <v>41</v>
+      </c>
+      <c r="H62" t="s">
+        <v>41</v>
+      </c>
+      <c r="I62" t="s">
+        <v>41</v>
+      </c>
+      <c r="J62" t="s">
+        <v>150</v>
+      </c>
+      <c r="K62" t="s">
+        <v>6</v>
+      </c>
+      <c r="L62" t="s">
+        <v>349</v>
+      </c>
+      <c r="M62" t="s">
+        <v>350</v>
+      </c>
+      <c r="N62" t="s">
+        <v>41</v>
+      </c>
+      <c r="O62" t="s">
+        <v>41</v>
+      </c>
+      <c r="P62" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>6</v>
+      </c>
+      <c r="R62" t="s">
+        <v>339</v>
+      </c>
+      <c r="S62" s="8">
+        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T62">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
         <v>1</v>
       </c>
@@ -5932,10 +6020,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P116"/>
+  <dimension ref="A1:P117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7846,8 +7934,12 @@
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
         <v>y</v>
       </c>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
+      <c r="O37" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="P37" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -7896,8 +7988,12 @@
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
         <v>y</v>
       </c>
-      <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
+      <c r="O38" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="P38" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -7946,8 +8042,12 @@
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
         <v>y</v>
       </c>
-      <c r="O39" s="8"/>
-      <c r="P39" s="8"/>
+      <c r="O39" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="P39" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -7996,8 +8096,12 @@
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
         <v>y</v>
       </c>
-      <c r="O40" s="8"/>
-      <c r="P40" s="8"/>
+      <c r="O40" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="P40" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -8046,8 +8150,12 @@
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
         <v>y</v>
       </c>
-      <c r="O41" s="8"/>
-      <c r="P41" s="8"/>
+      <c r="O41" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="P41" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -8309,7 +8417,7 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>459</v>
+        <v>469</v>
       </c>
       <c r="B47" t="s">
         <v>361</v>
@@ -8318,29 +8426,29 @@
         <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>54</v>
-      </c>
-      <c r="E47" s="1">
-        <v>1</v>
+        <v>137</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="F47" t="s">
         <v>6</v>
       </c>
       <c r="G47" t="s">
-        <v>465</v>
+        <v>41</v>
       </c>
       <c r="H47" t="s">
-        <v>228</v>
+        <v>359</v>
       </c>
       <c r="I47" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="J47" t="s">
         <v>41</v>
       </c>
       <c r="K47" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>rollup_idUNC1.Is OCLC number or SerialsSolutions number</v>
+        <v>record_data_sourceGEN..x</v>
       </c>
       <c r="L47" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8348,7 +8456,7 @@
       </c>
       <c r="M47" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N47" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -8371,26 +8479,26 @@
         <v>54</v>
       </c>
       <c r="E48" s="1">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F48" t="s">
         <v>6</v>
       </c>
       <c r="G48" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H48" t="s">
         <v>228</v>
       </c>
       <c r="I48" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="J48" t="s">
         <v>41</v>
       </c>
       <c r="K48" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>rollup_idUNC19.If oclc_number is not set, and 019 has at least 1 $a</v>
+        <v>rollup_idUNC1.Is OCLC number or SerialsSolutions number</v>
       </c>
       <c r="L48" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8409,10 +8517,10 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>334</v>
+        <v>459</v>
       </c>
       <c r="B49" t="s">
-        <v>53</v>
+        <v>361</v>
       </c>
       <c r="C49" t="s">
         <v>2</v>
@@ -8421,26 +8529,26 @@
         <v>54</v>
       </c>
       <c r="E49" s="1">
-        <v>999</v>
+        <v>19</v>
       </c>
       <c r="F49" t="s">
-        <v>168</v>
+        <v>6</v>
       </c>
       <c r="G49" t="s">
-        <v>229</v>
+        <v>467</v>
       </c>
       <c r="H49" t="s">
         <v>228</v>
       </c>
       <c r="I49" t="s">
-        <v>230</v>
+        <v>468</v>
       </c>
       <c r="J49" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="K49" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>status (items)UNC999si1=9 AND i2=1 and $d IS blank</v>
+        <v>rollup_idUNC19.If oclc_number is not set, and 019 has at least 1 $a</v>
       </c>
       <c r="L49" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8448,18 +8556,14 @@
       </c>
       <c r="M49" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N49" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
         <v>y</v>
       </c>
-      <c r="O49" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="P49" s="8" t="s">
-        <v>3</v>
-      </c>
+      <c r="O49" s="8"/>
+      <c r="P49" s="8"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
@@ -8478,23 +8582,23 @@
         <v>999</v>
       </c>
       <c r="F50" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="G50" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="H50" t="s">
-        <v>359</v>
+        <v>228</v>
       </c>
       <c r="I50" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="J50" t="s">
         <v>6</v>
       </c>
       <c r="K50" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>status (items)UNC999di1=9 AND i2=1 and $d IS NOT blank</v>
+        <v>status (items)UNC999si1=9 AND i2=1 and $d IS blank</v>
       </c>
       <c r="L50" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8532,27 +8636,27 @@
         <v>999</v>
       </c>
       <c r="F51" t="s">
-        <v>7</v>
+        <v>155</v>
       </c>
       <c r="G51" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="H51" t="s">
         <v>359</v>
       </c>
       <c r="I51" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="J51" t="s">
-        <v>233</v>
+        <v>6</v>
       </c>
       <c r="K51" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>status (items)UNC999ai1=9 AND i2=4 AND NOT EXIST (tag=999 AND i1=9 and i2=1)</v>
+        <v>status (items)UNC999di1=9 AND i2=1 and $d IS NOT blank</v>
       </c>
       <c r="L51" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M51" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
@@ -8562,59 +8666,61 @@
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
         <v>y</v>
       </c>
-      <c r="O51" s="8"/>
-      <c r="P51" s="8"/>
+      <c r="O51" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="P51" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>0</v>
+        <v>334</v>
       </c>
       <c r="B52" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C52" t="s">
         <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>137</v>
+        <v>54</v>
       </c>
       <c r="E52" s="1">
-        <v>600</v>
+        <v>999</v>
       </c>
       <c r="F52" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G52" t="s">
-        <v>4</v>
+        <v>231</v>
       </c>
       <c r="H52" t="s">
-        <v>5</v>
+        <v>359</v>
       </c>
       <c r="I52" t="s">
-        <v>6</v>
+        <v>232</v>
       </c>
       <c r="J52" t="s">
-        <v>6</v>
-      </c>
-      <c r="K52" t="str">
+        <v>233</v>
+      </c>
+      <c r="K52" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN600yi2=0 OR (i2=7 AND $2=lcsh)</v>
-      </c>
-      <c r="L52">
+        <v>status (items)UNC999ai1=9 AND i2=4 AND NOT EXIST (tag=999 AND i1=9 and i2=1)</v>
+      </c>
+      <c r="L52" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M52">
+        <v>1</v>
+      </c>
+      <c r="M52" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N52" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
         <v>y</v>
       </c>
-      <c r="O52" s="8" t="s">
-        <v>3</v>
-      </c>
+      <c r="O52" s="8"/>
       <c r="P52" s="8"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
@@ -8631,7 +8737,7 @@
         <v>137</v>
       </c>
       <c r="E53" s="1">
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="F53" t="s">
         <v>3</v>
@@ -8650,7 +8756,7 @@
       </c>
       <c r="K53" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN610yi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_chronological_facetGEN600yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L53">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8683,7 +8789,7 @@
         <v>137</v>
       </c>
       <c r="E54" s="1">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F54" t="s">
         <v>3</v>
@@ -8702,7 +8808,7 @@
       </c>
       <c r="K54" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN611yi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_chronological_facetGEN610yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L54">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8735,7 +8841,7 @@
         <v>137</v>
       </c>
       <c r="E55" s="1">
-        <v>630</v>
+        <v>611</v>
       </c>
       <c r="F55" t="s">
         <v>3</v>
@@ -8754,7 +8860,7 @@
       </c>
       <c r="K55" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN630yi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_chronological_facetGEN611yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L55">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8787,7 +8893,7 @@
         <v>137</v>
       </c>
       <c r="E56" s="1">
-        <v>650</v>
+        <v>630</v>
       </c>
       <c r="F56" t="s">
         <v>3</v>
@@ -8806,7 +8912,7 @@
       </c>
       <c r="K56" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN650yi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_chronological_facetGEN630yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L56">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8839,7 +8945,7 @@
         <v>137</v>
       </c>
       <c r="E57" s="1">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="F57" t="s">
         <v>3</v>
@@ -8858,7 +8964,7 @@
       </c>
       <c r="K57" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN651yi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_chronological_facetGEN650yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L57">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8891,7 +8997,7 @@
         <v>137</v>
       </c>
       <c r="E58" s="1">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="F58" t="s">
         <v>3</v>
@@ -8910,7 +9016,7 @@
       </c>
       <c r="K58" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN655yi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_chronological_facetGEN651yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L58">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8937,19 +9043,19 @@
         <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D59" t="s">
         <v>137</v>
       </c>
       <c r="E59" s="1">
-        <v>648</v>
+        <v>655</v>
       </c>
       <c r="F59" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G59" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H59" t="s">
         <v>5</v>
@@ -8958,11 +9064,11 @@
         <v>6</v>
       </c>
       <c r="J59" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K59" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronological_facetGEN648ai2=0 OR (i2=7 AND $2=~/lcsh|fast/)</v>
+        <v>subject_chronological_facetGEN655yi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L59">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -8983,7 +9089,7 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B60" t="s">
         <v>1</v>
@@ -8995,26 +9101,26 @@
         <v>137</v>
       </c>
       <c r="E60" s="1">
-        <v>655</v>
+        <v>648</v>
       </c>
       <c r="F60" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="G60" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H60" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I60" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="J60" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="K60" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655axi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_chronological_facetGEN648ai2=0 OR (i2=7 AND $2=~/lcsh|fast/)</v>
       </c>
       <c r="L60">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9022,7 +9128,7 @@
       </c>
       <c r="M60">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N60" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -9053,7 +9159,7 @@
         <v>19</v>
       </c>
       <c r="G61" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="H61" t="s">
         <v>20</v>
@@ -9062,11 +9168,11 @@
         <v>21</v>
       </c>
       <c r="J61" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K61" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655axi2=7 AND $2=lcgft</v>
+        <v>subject_genre_facetGEN655axi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L61">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9105,7 +9211,7 @@
         <v>19</v>
       </c>
       <c r="G62" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H62" t="s">
         <v>20</v>
@@ -9114,11 +9220,11 @@
         <v>21</v>
       </c>
       <c r="J62" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K62" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655axi2=7 AND $2=rbbin</v>
+        <v>subject_genre_facetGEN655axi2=7 AND $2=lcgft</v>
       </c>
       <c r="L62">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9157,7 +9263,7 @@
         <v>19</v>
       </c>
       <c r="G63" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H63" t="s">
         <v>20</v>
@@ -9166,11 +9272,11 @@
         <v>21</v>
       </c>
       <c r="J63" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K63" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655axi2=7 AND $2=rbgenr</v>
+        <v>subject_genre_facetGEN655axi2=7 AND $2=rbbin</v>
       </c>
       <c r="L63">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9209,20 +9315,20 @@
         <v>19</v>
       </c>
       <c r="G64" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H64" t="s">
         <v>20</v>
       </c>
       <c r="I64" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="J64" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K64" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655axi2=7 AND $2=rbprov</v>
+        <v>subject_genre_facetGEN655axi2=7 AND $2=rbgenr</v>
       </c>
       <c r="L64">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9249,32 +9355,32 @@
         <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D65" t="s">
         <v>137</v>
       </c>
       <c r="E65" s="1">
-        <v>6</v>
-      </c>
-      <c r="F65">
-        <v>16</v>
+        <v>655</v>
+      </c>
+      <c r="F65" t="s">
+        <v>19</v>
       </c>
       <c r="G65" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="H65" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I65" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="J65" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="K65" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN616LDR/06 = a AND LDR/07 =~ [acdm] AND 006/00 =~ [at]</v>
+        <v>subject_genre_facetGEN655axi2=7 AND $2=rbprov</v>
       </c>
       <c r="L65">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9310,7 +9416,7 @@
         <v>6</v>
       </c>
       <c r="F66">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G66" t="s">
         <v>11</v>
@@ -9319,14 +9425,14 @@
         <v>5</v>
       </c>
       <c r="I66" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J66" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="K66" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN617LDR/06 = a AND LDR/07 =~ [acdm] AND 006/00 =~ [at]</v>
+        <v>subject_genre_facetGEN616LDR/06 = a AND LDR/07 =~ [acdm] AND 006/00 =~ [at]</v>
       </c>
       <c r="L66">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9359,26 +9465,26 @@
         <v>137</v>
       </c>
       <c r="E67" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F67">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="G67" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H67" t="s">
         <v>5</v>
       </c>
       <c r="I67" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J67" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="K67" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN833LDR/06 = a AND LDR/07 =~ [acdm]</v>
+        <v>subject_genre_facetGEN617LDR/06 = a AND LDR/07 =~ [acdm] AND 006/00 =~ [at]</v>
       </c>
       <c r="L67">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9414,7 +9520,7 @@
         <v>8</v>
       </c>
       <c r="F68">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G68" t="s">
         <v>15</v>
@@ -9423,14 +9529,14 @@
         <v>5</v>
       </c>
       <c r="I68" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J68" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="K68" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN834LDR/06 = a AND LDR/07 =~ [acdm]</v>
+        <v>subject_genre_facetGEN833LDR/06 = a AND LDR/07 =~ [acdm]</v>
       </c>
       <c r="L68">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9463,26 +9569,26 @@
         <v>137</v>
       </c>
       <c r="E69" s="1">
-        <v>600</v>
-      </c>
-      <c r="F69" t="s">
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="F69">
+        <v>34</v>
       </c>
       <c r="G69" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="H69" t="s">
         <v>5</v>
       </c>
       <c r="I69" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="J69" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="K69" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN600vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN834LDR/06 = a AND LDR/07 =~ [acdm]</v>
       </c>
       <c r="L69">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9515,7 +9621,7 @@
         <v>137</v>
       </c>
       <c r="E70" s="1">
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="F70" t="s">
         <v>16</v>
@@ -9534,7 +9640,7 @@
       </c>
       <c r="K70" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN610vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN600vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L70">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9567,7 +9673,7 @@
         <v>137</v>
       </c>
       <c r="E71" s="1">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F71" t="s">
         <v>16</v>
@@ -9586,7 +9692,7 @@
       </c>
       <c r="K71" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN611vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN610vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L71">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9619,7 +9725,7 @@
         <v>137</v>
       </c>
       <c r="E72" s="1">
-        <v>630</v>
+        <v>611</v>
       </c>
       <c r="F72" t="s">
         <v>16</v>
@@ -9638,7 +9744,7 @@
       </c>
       <c r="K72" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN630vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN611vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L72">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9671,7 +9777,7 @@
         <v>137</v>
       </c>
       <c r="E73" s="1">
-        <v>650</v>
+        <v>630</v>
       </c>
       <c r="F73" t="s">
         <v>16</v>
@@ -9690,7 +9796,7 @@
       </c>
       <c r="K73" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN650vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN630vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L73">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9723,7 +9829,7 @@
         <v>137</v>
       </c>
       <c r="E74" s="1">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="F74" t="s">
         <v>16</v>
@@ -9742,7 +9848,7 @@
       </c>
       <c r="K74" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN651vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN650vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L74">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9775,7 +9881,7 @@
         <v>137</v>
       </c>
       <c r="E75" s="1">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="F75" t="s">
         <v>16</v>
@@ -9794,7 +9900,7 @@
       </c>
       <c r="K75" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN651vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L75">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9821,13 +9927,13 @@
         <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D76" t="s">
         <v>137</v>
       </c>
       <c r="E76" s="1">
-        <v>647</v>
+        <v>655</v>
       </c>
       <c r="F76" t="s">
         <v>16</v>
@@ -9842,11 +9948,11 @@
         <v>6</v>
       </c>
       <c r="J76" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="K76" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN647vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN655vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L76">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9879,7 +9985,7 @@
         <v>137</v>
       </c>
       <c r="E77" s="1">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F77" t="s">
         <v>16</v>
@@ -9894,11 +10000,11 @@
         <v>6</v>
       </c>
       <c r="J77" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K77" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN648vi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN647vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L77">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9931,13 +10037,13 @@
         <v>137</v>
       </c>
       <c r="E78" s="1">
-        <v>655</v>
+        <v>648</v>
       </c>
       <c r="F78" t="s">
         <v>16</v>
       </c>
       <c r="G78" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="H78" t="s">
         <v>5</v>
@@ -9946,11 +10052,11 @@
         <v>6</v>
       </c>
       <c r="J78" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="K78" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655vi2=7 AND $2=lcgft</v>
+        <v>subject_genre_facetGEN648vi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L78">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -9989,7 +10095,7 @@
         <v>16</v>
       </c>
       <c r="G79" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H79" t="s">
         <v>5</v>
@@ -9998,11 +10104,11 @@
         <v>6</v>
       </c>
       <c r="J79" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K79" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655vi2=7 AND $2=rbbin</v>
+        <v>subject_genre_facetGEN655vi2=7 AND $2=lcgft</v>
       </c>
       <c r="L79">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -10041,7 +10147,7 @@
         <v>16</v>
       </c>
       <c r="G80" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H80" t="s">
         <v>5</v>
@@ -10050,11 +10156,11 @@
         <v>6</v>
       </c>
       <c r="J80" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K80" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655vi2=7 AND $2=rbgenr</v>
+        <v>subject_genre_facetGEN655vi2=7 AND $2=rbbin</v>
       </c>
       <c r="L80">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -10093,7 +10199,7 @@
         <v>16</v>
       </c>
       <c r="G81" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H81" t="s">
         <v>5</v>
@@ -10102,11 +10208,11 @@
         <v>6</v>
       </c>
       <c r="J81" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K81" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN655vi2=7 AND $2=rbprov</v>
+        <v>subject_genre_facetGEN655vi2=7 AND $2=rbgenr</v>
       </c>
       <c r="L81">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -10139,13 +10245,13 @@
         <v>137</v>
       </c>
       <c r="E82" s="1">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="F82" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="G82" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H82" t="s">
         <v>5</v>
@@ -10154,11 +10260,11 @@
         <v>6</v>
       </c>
       <c r="J82" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K82" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN656kvi2=7 AND $2=lcsh</v>
+        <v>subject_genre_facetGEN655vi2=7 AND $2=rbprov</v>
       </c>
       <c r="L82">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -10191,10 +10297,10 @@
         <v>137</v>
       </c>
       <c r="E83" s="1">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F83" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="G83" t="s">
         <v>34</v>
@@ -10210,7 +10316,7 @@
       </c>
       <c r="K83" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genre_facetGEN657vi2=7 AND $2=lcsh</v>
+        <v>subject_genre_facetGEN656kvi2=7 AND $2=lcsh</v>
       </c>
       <c r="L83">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -10231,25 +10337,25 @@
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B84" t="s">
         <v>1</v>
       </c>
       <c r="C84" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D84" t="s">
         <v>137</v>
       </c>
       <c r="E84" s="1">
-        <v>600</v>
+        <v>657</v>
       </c>
       <c r="F84" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="G84" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="H84" t="s">
         <v>5</v>
@@ -10258,11 +10364,11 @@
         <v>6</v>
       </c>
       <c r="J84" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="K84" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN600zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_genre_facetGEN657vi2=7 AND $2=lcsh</v>
       </c>
       <c r="L84">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -10270,7 +10376,7 @@
       </c>
       <c r="M84">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N84" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -10295,7 +10401,7 @@
         <v>137</v>
       </c>
       <c r="E85" s="1">
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="F85" t="s">
         <v>37</v>
@@ -10314,7 +10420,7 @@
       </c>
       <c r="K85" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN610zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN600zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L85">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -10347,7 +10453,7 @@
         <v>137</v>
       </c>
       <c r="E86" s="1">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F86" t="s">
         <v>37</v>
@@ -10366,7 +10472,7 @@
       </c>
       <c r="K86" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN611zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN610zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L86">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -10399,7 +10505,7 @@
         <v>137</v>
       </c>
       <c r="E87" s="1">
-        <v>630</v>
+        <v>611</v>
       </c>
       <c r="F87" t="s">
         <v>37</v>
@@ -10418,7 +10524,7 @@
       </c>
       <c r="K87" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN630zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN611zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L87">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -10451,7 +10557,7 @@
         <v>137</v>
       </c>
       <c r="E88" s="1">
-        <v>650</v>
+        <v>630</v>
       </c>
       <c r="F88" t="s">
         <v>37</v>
@@ -10470,7 +10576,7 @@
       </c>
       <c r="K88" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN650zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN630zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L88">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -10503,7 +10609,7 @@
         <v>137</v>
       </c>
       <c r="E89" s="1">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="F89" t="s">
         <v>37</v>
@@ -10522,7 +10628,7 @@
       </c>
       <c r="K89" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN651zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN650zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L89">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -10555,7 +10661,7 @@
         <v>137</v>
       </c>
       <c r="E90" s="1">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="F90" t="s">
         <v>37</v>
@@ -10574,7 +10680,7 @@
       </c>
       <c r="K90" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN655zi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN651zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L90">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -10601,19 +10707,19 @@
         <v>1</v>
       </c>
       <c r="C91" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D91" t="s">
         <v>137</v>
       </c>
       <c r="E91" s="1">
-        <v>648</v>
+        <v>655</v>
       </c>
       <c r="F91" t="s">
         <v>37</v>
       </c>
       <c r="G91" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H91" t="s">
         <v>5</v>
@@ -10622,11 +10728,11 @@
         <v>6</v>
       </c>
       <c r="J91" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="K91" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographic_facetGEN648zi2=0 OR (i2=7 AND $2=~/lcsh|fast/)</v>
+        <v>subject_geographic_facetGEN655zi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L91">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -10647,38 +10753,38 @@
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B92" t="s">
         <v>1</v>
       </c>
       <c r="C92" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D92" t="s">
         <v>137</v>
       </c>
       <c r="E92" s="1">
-        <v>600</v>
+        <v>648</v>
       </c>
       <c r="F92" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G92" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H92" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I92" t="s">
         <v>6</v>
       </c>
       <c r="J92" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="K92" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN600abcdfghjklmnopqrstui2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_geographic_facetGEN648zi2=0 OR (i2=7 AND $2=~/lcsh|fast/)</v>
       </c>
       <c r="L92">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -10711,10 +10817,10 @@
         <v>137</v>
       </c>
       <c r="E93" s="1">
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="F93" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G93" t="s">
         <v>4</v>
@@ -10726,11 +10832,11 @@
         <v>6</v>
       </c>
       <c r="J93" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="K93" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN610abcdfghklmnoprstui2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN600abcdfghjklmnopqrstui2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L93">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -10763,10 +10869,10 @@
         <v>137</v>
       </c>
       <c r="E94" s="1">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F94" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G94" t="s">
         <v>4</v>
@@ -10778,11 +10884,11 @@
         <v>6</v>
       </c>
       <c r="J94" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K94" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN611acdefghklnpqstui2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN610abcdfghklmnoprstui2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L94">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -10815,10 +10921,10 @@
         <v>137</v>
       </c>
       <c r="E95" s="1">
-        <v>630</v>
+        <v>611</v>
       </c>
       <c r="F95" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G95" t="s">
         <v>4</v>
@@ -10830,11 +10936,11 @@
         <v>6</v>
       </c>
       <c r="J95" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K95" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN630adfghklmnoprsti2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN611acdefghklnpqstui2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L95">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -10867,10 +10973,10 @@
         <v>137</v>
       </c>
       <c r="E96" s="1">
-        <v>650</v>
+        <v>630</v>
       </c>
       <c r="F96" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G96" t="s">
         <v>4</v>
@@ -10882,11 +10988,11 @@
         <v>6</v>
       </c>
       <c r="J96" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="K96" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN650abcdgi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN630adfghklmnoprsti2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L96">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -10913,16 +11019,16 @@
         <v>1</v>
       </c>
       <c r="C97" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D97" t="s">
         <v>137</v>
       </c>
       <c r="E97" s="1">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="F97" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G97" t="s">
         <v>4</v>
@@ -10934,11 +11040,11 @@
         <v>6</v>
       </c>
       <c r="J97" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="K97" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN647acdgi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN650abcdgi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L97">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -10965,32 +11071,32 @@
         <v>1</v>
       </c>
       <c r="C98" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D98" t="s">
         <v>137</v>
       </c>
       <c r="E98" s="1">
-        <v>600</v>
+        <v>647</v>
       </c>
       <c r="F98" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G98" t="s">
         <v>4</v>
       </c>
       <c r="H98" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I98" t="s">
         <v>6</v>
       </c>
       <c r="J98" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="K98" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN600xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN647acdgi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L98">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -11023,7 +11129,7 @@
         <v>137</v>
       </c>
       <c r="E99" s="1">
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="F99" t="s">
         <v>41</v>
@@ -11042,7 +11148,7 @@
       </c>
       <c r="K99" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN610xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN600xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L99">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -11075,7 +11181,7 @@
         <v>137</v>
       </c>
       <c r="E100" s="1">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F100" t="s">
         <v>41</v>
@@ -11094,7 +11200,7 @@
       </c>
       <c r="K100" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN611xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN610xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L100">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -11127,7 +11233,7 @@
         <v>137</v>
       </c>
       <c r="E101" s="1">
-        <v>630</v>
+        <v>611</v>
       </c>
       <c r="F101" t="s">
         <v>41</v>
@@ -11146,7 +11252,7 @@
       </c>
       <c r="K101" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN630xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN611xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L101">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -11179,7 +11285,7 @@
         <v>137</v>
       </c>
       <c r="E102" s="1">
-        <v>650</v>
+        <v>630</v>
       </c>
       <c r="F102" t="s">
         <v>41</v>
@@ -11198,7 +11304,7 @@
       </c>
       <c r="K102" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN650xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN630xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L102">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -11231,7 +11337,7 @@
         <v>137</v>
       </c>
       <c r="E103" s="1">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="F103" t="s">
         <v>41</v>
@@ -11250,7 +11356,7 @@
       </c>
       <c r="K103" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN651xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN650xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L103">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -11277,13 +11383,13 @@
         <v>1</v>
       </c>
       <c r="C104" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D104" t="s">
         <v>137</v>
       </c>
       <c r="E104" s="1">
-        <v>647</v>
+        <v>651</v>
       </c>
       <c r="F104" t="s">
         <v>41</v>
@@ -11298,11 +11404,11 @@
         <v>6</v>
       </c>
       <c r="J104" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="K104" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN647xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN651xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L104">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -11335,7 +11441,7 @@
         <v>137</v>
       </c>
       <c r="E105" s="1">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F105" t="s">
         <v>41</v>
@@ -11350,11 +11456,11 @@
         <v>6</v>
       </c>
       <c r="J105" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K105" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN648xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN647xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L105">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -11387,7 +11493,7 @@
         <v>137</v>
       </c>
       <c r="E106" s="1">
-        <v>655</v>
+        <v>648</v>
       </c>
       <c r="F106" t="s">
         <v>41</v>
@@ -11402,15 +11508,15 @@
         <v>6</v>
       </c>
       <c r="J106" t="s">
-        <v>6</v>
-      </c>
-      <c r="K106" s="8" t="str">
+        <v>18</v>
+      </c>
+      <c r="K106" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN655xi2=0 OR (i2=7 AND $2=lcsh)</v>
+        <v>subject_topic_lcsh_facetGEN648xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L106">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M106">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
@@ -11439,13 +11545,13 @@
         <v>137</v>
       </c>
       <c r="E107" s="1">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="F107" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="G107" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="H107" t="s">
         <v>5</v>
@@ -11454,15 +11560,15 @@
         <v>6</v>
       </c>
       <c r="J107" t="s">
-        <v>50</v>
-      </c>
-      <c r="K107" t="str">
+        <v>6</v>
+      </c>
+      <c r="K107" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN656ai2=7 AND $2=lcsh</v>
+        <v>subject_topic_lcsh_facetGEN655xi2=0 OR (i2=7 AND $2=lcsh)</v>
       </c>
       <c r="L107">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M107">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
@@ -11494,7 +11600,7 @@
         <v>656</v>
       </c>
       <c r="F108" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="G108" t="s">
         <v>34</v>
@@ -11506,11 +11612,11 @@
         <v>6</v>
       </c>
       <c r="J108" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="K108" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN656xi2=7 AND $2=lcsh</v>
+        <v>subject_topic_lcsh_facetGEN656ai2=7 AND $2=lcsh</v>
       </c>
       <c r="L108">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -11543,10 +11649,10 @@
         <v>137</v>
       </c>
       <c r="E109" s="1">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F109" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="G109" t="s">
         <v>34</v>
@@ -11558,11 +11664,11 @@
         <v>6</v>
       </c>
       <c r="J109" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="K109" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN657ai2=7 AND $2=lcsh</v>
+        <v>subject_topic_lcsh_facetGEN656xi2=7 AND $2=lcsh</v>
       </c>
       <c r="L109">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -11598,7 +11704,7 @@
         <v>657</v>
       </c>
       <c r="F110" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="G110" t="s">
         <v>34</v>
@@ -11614,7 +11720,7 @@
       </c>
       <c r="K110" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_topic_lcsh_facetGEN657xi2=7 AND $2=lcsh</v>
+        <v>subject_topic_lcsh_facetGEN657ai2=7 AND $2=lcsh</v>
       </c>
       <c r="L110">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -11635,46 +11741,46 @@
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>322</v>
+        <v>38</v>
       </c>
       <c r="B111" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="C111" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D111" t="s">
-        <v>54</v>
+        <v>137</v>
       </c>
       <c r="E111" s="1">
-        <v>999</v>
+        <v>657</v>
       </c>
       <c r="F111" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="G111" t="s">
-        <v>296</v>
+        <v>34</v>
       </c>
       <c r="H111" t="s">
         <v>5</v>
       </c>
       <c r="I111" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="J111" t="s">
-        <v>41</v>
-      </c>
-      <c r="K111" s="8" t="str">
+        <v>51</v>
+      </c>
+      <c r="K111" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>summary (holdings)UNC999ai1=9 AND i2=3 AND $0=#{holdings_record_id} AND $2='866'</v>
-      </c>
-      <c r="L111" s="8">
+        <v>subject_topic_lcsh_facetGEN657xi2=7 AND $2=lcsh</v>
+      </c>
+      <c r="L111">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>1</v>
-      </c>
-      <c r="M111" s="8">
+        <v>0</v>
+      </c>
+      <c r="M111">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N111" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
@@ -11683,45 +11789,46 @@
       <c r="O111" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="P111" s="8" t="s">
-        <v>3</v>
-      </c>
+      <c r="P111" s="8"/>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>368</v>
+        <v>322</v>
       </c>
       <c r="B112" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C112" t="s">
         <v>2</v>
       </c>
       <c r="D112" t="s">
-        <v>137</v>
+        <v>54</v>
       </c>
       <c r="E112" s="1">
-        <v>210</v>
+        <v>999</v>
       </c>
       <c r="F112" t="s">
-        <v>373</v>
+        <v>7</v>
       </c>
       <c r="G112" t="s">
-        <v>374</v>
+        <v>296</v>
       </c>
       <c r="H112" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I112" t="s">
-        <v>6</v>
+        <v>41</v>
+      </c>
+      <c r="J112" t="s">
+        <v>41</v>
       </c>
       <c r="K112" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>title_abbreviatedGEN210abi1=1</v>
+        <v>summary (holdings)UNC999ai1=9 AND i2=3 AND $0=#{holdings_record_id} AND $2='866'</v>
       </c>
       <c r="L112" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M112" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
@@ -11731,12 +11838,16 @@
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
         <v>y</v>
       </c>
-      <c r="O112" s="8"/>
-      <c r="P112" s="8"/>
+      <c r="O112" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="P112" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>258</v>
+        <v>368</v>
       </c>
       <c r="B113" t="s">
         <v>1</v>
@@ -11748,26 +11859,23 @@
         <v>137</v>
       </c>
       <c r="E113" s="1">
-        <v>100</v>
+        <v>210</v>
       </c>
       <c r="F113" t="s">
-        <v>266</v>
+        <v>373</v>
       </c>
       <c r="G113" t="s">
-        <v>6</v>
+        <v>374</v>
       </c>
       <c r="H113" t="s">
         <v>20</v>
       </c>
       <c r="I113" t="s">
-        <v>315</v>
-      </c>
-      <c r="J113" t="s">
-        <v>264</v>
+        <v>6</v>
       </c>
       <c r="K113" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>uniform_titleGEN100f(g)klnpt.</v>
+        <v>title_abbreviatedGEN210abi1=1</v>
       </c>
       <c r="L113" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -11798,10 +11906,10 @@
         <v>137</v>
       </c>
       <c r="E114" s="1">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F114" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G114" t="s">
         <v>6</v>
@@ -11810,14 +11918,14 @@
         <v>20</v>
       </c>
       <c r="I114" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J114" t="s">
         <v>264</v>
       </c>
       <c r="K114" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>uniform_titleGEN110f(g)kl(n)pt.</v>
+        <v>uniform_titleGEN100f(g)klnpt.</v>
       </c>
       <c r="L114" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -11848,7 +11956,7 @@
         <v>137</v>
       </c>
       <c r="E115" s="1">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F115" t="s">
         <v>268</v>
@@ -11867,7 +11975,7 @@
       </c>
       <c r="K115" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>uniform_titleGEN111f(g)kl(n)pt.</v>
+        <v>uniform_titleGEN110f(g)kl(n)pt.</v>
       </c>
       <c r="L115" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -11886,38 +11994,38 @@
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>348</v>
+        <v>258</v>
       </c>
       <c r="B116" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="C116" t="s">
         <v>2</v>
       </c>
       <c r="D116" t="s">
-        <v>54</v>
+        <v>137</v>
       </c>
       <c r="E116" s="1">
-        <v>999</v>
+        <v>111</v>
       </c>
       <c r="F116" t="s">
-        <v>16</v>
+        <v>268</v>
       </c>
       <c r="G116" t="s">
-        <v>149</v>
+        <v>6</v>
       </c>
       <c r="H116" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I116" t="s">
-        <v>6</v>
+        <v>316</v>
       </c>
       <c r="J116" t="s">
-        <v>6</v>
+        <v>264</v>
       </c>
       <c r="K116" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>vol (items)UNC999vi1=9 AND i2=1</v>
+        <v>uniform_titleGEN111f(g)kl(n)pt.</v>
       </c>
       <c r="L116" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -11931,15 +12039,65 @@
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
         <v>y</v>
       </c>
-      <c r="O116" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="P116" s="8" t="s">
+      <c r="O116" s="8"/>
+      <c r="P116" s="8"/>
+    </row>
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>348</v>
+      </c>
+      <c r="B117" t="s">
+        <v>53</v>
+      </c>
+      <c r="C117" t="s">
+        <v>2</v>
+      </c>
+      <c r="D117" t="s">
+        <v>54</v>
+      </c>
+      <c r="E117" s="1">
+        <v>999</v>
+      </c>
+      <c r="F117" t="s">
+        <v>16</v>
+      </c>
+      <c r="G117" t="s">
+        <v>149</v>
+      </c>
+      <c r="H117" t="s">
+        <v>5</v>
+      </c>
+      <c r="I117" t="s">
+        <v>6</v>
+      </c>
+      <c r="J117" t="s">
+        <v>6</v>
+      </c>
+      <c r="K117" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>vol (items)UNC999vi1=9 AND i2=1</v>
+      </c>
+      <c r="L117" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M117" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N117" s="8" t="str">
+        <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
+        <v>y</v>
+      </c>
+      <c r="O117" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="P117" s="8" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K3:K65">
+  <conditionalFormatting sqref="K3:K66">
     <cfRule type="duplicateValues" dxfId="1" priority="8"/>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>

<commit_message>
Detailed note mappings begin...
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3175" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3333" uniqueCount="619">
   <si>
     <t>subject_chronological_facet</t>
   </si>
@@ -1849,6 +1849,42 @@
   </si>
   <si>
     <t>$3 label; prepend ISBN to $z value</t>
+  </si>
+  <si>
+    <t>note_display</t>
+  </si>
+  <si>
+    <t>note_index</t>
+  </si>
+  <si>
+    <t>All displayed notes, kept in catalog record order, with labels provided</t>
+  </si>
+  <si>
+    <t>https://github.com/trln/data-documentation/blob/master/argot/spec_docs/notes_fields.adoc</t>
+  </si>
+  <si>
+    <t>Indexed note data</t>
+  </si>
+  <si>
+    <t>note_display[label]</t>
+  </si>
+  <si>
+    <t>note_display[value]</t>
+  </si>
+  <si>
+    <t>Intial label portion of note</t>
+  </si>
+  <si>
+    <t>Displayed note value</t>
+  </si>
+  <si>
+    <t>abcdefhno3</t>
+  </si>
+  <si>
+    <t>DO NOT use $3 to create label</t>
+  </si>
+  <si>
+    <t>ind1 != 0</t>
   </si>
 </sst>
 </file>
@@ -2230,8 +2266,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="fields" displayName="fields" ref="A1:V106" totalsRowShown="0">
-  <autoFilter ref="A1:V106"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="fields" displayName="fields" ref="A1:V110" totalsRowShown="0">
+  <autoFilter ref="A1:V110"/>
   <sortState ref="A2:V106">
     <sortCondition ref="A1:A106"/>
   </sortState>
@@ -2281,8 +2317,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="mappings" displayName="mappings" ref="A1:P148" totalsRowShown="0">
-  <autoFilter ref="A1:P148"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="mappings" displayName="mappings" ref="A1:P156" totalsRowShown="0">
+  <autoFilter ref="A1:P156"/>
   <sortState ref="A2:P140">
     <sortCondition ref="A1:A140"/>
   </sortState>
@@ -2592,11 +2628,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V106"/>
+  <dimension ref="A1:V110"/>
   <sheetViews>
     <sheetView topLeftCell="A61" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A77" sqref="A77"/>
+      <selection pane="topRight" activeCell="A67" sqref="A67:A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5943,11 +5979,59 @@
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>474</v>
+        <v>607</v>
       </c>
       <c r="B66" t="s">
         <v>64</v>
       </c>
+      <c r="C66" t="s">
+        <v>2</v>
+      </c>
+      <c r="D66" t="s">
+        <v>2</v>
+      </c>
+      <c r="E66" t="s">
+        <v>2</v>
+      </c>
+      <c r="F66" t="s">
+        <v>422</v>
+      </c>
+      <c r="G66" t="s">
+        <v>41</v>
+      </c>
+      <c r="H66" t="s">
+        <v>3</v>
+      </c>
+      <c r="I66" t="s">
+        <v>41</v>
+      </c>
+      <c r="J66" t="s">
+        <v>121</v>
+      </c>
+      <c r="K66" t="s">
+        <v>41</v>
+      </c>
+      <c r="L66" t="s">
+        <v>609</v>
+      </c>
+      <c r="M66" t="s">
+        <v>41</v>
+      </c>
+      <c r="N66" t="s">
+        <v>41</v>
+      </c>
+      <c r="O66" t="s">
+        <v>599</v>
+      </c>
+      <c r="P66" t="s">
+        <v>498</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>498</v>
+      </c>
+      <c r="R66" t="s">
+        <v>610</v>
+      </c>
       <c r="S66" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>0</v>
@@ -5959,24 +6043,122 @@
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>589</v>
+        <v>612</v>
       </c>
       <c r="B67" t="s">
-        <v>482</v>
-      </c>
-      <c r="R67" s="10"/>
+        <v>64</v>
+      </c>
+      <c r="C67" t="s">
+        <v>2</v>
+      </c>
+      <c r="D67" t="s">
+        <v>2</v>
+      </c>
+      <c r="E67" t="s">
+        <v>607</v>
+      </c>
+      <c r="F67" t="s">
+        <v>425</v>
+      </c>
+      <c r="G67" t="s">
+        <v>41</v>
+      </c>
+      <c r="H67" t="s">
+        <v>3</v>
+      </c>
+      <c r="I67" t="s">
+        <v>41</v>
+      </c>
+      <c r="J67" t="s">
+        <v>121</v>
+      </c>
+      <c r="K67" t="s">
+        <v>41</v>
+      </c>
+      <c r="L67" t="s">
+        <v>614</v>
+      </c>
+      <c r="M67" t="s">
+        <v>41</v>
+      </c>
+      <c r="N67" t="s">
+        <v>41</v>
+      </c>
+      <c r="O67" t="s">
+        <v>599</v>
+      </c>
+      <c r="P67" t="s">
+        <v>498</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>498</v>
+      </c>
+      <c r="R67" t="s">
+        <v>610</v>
+      </c>
       <c r="S67" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>0</v>
       </c>
       <c r="T67">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>476</v>
+        <v>613</v>
+      </c>
+      <c r="B68" t="s">
+        <v>64</v>
+      </c>
+      <c r="C68" t="s">
+        <v>2</v>
+      </c>
+      <c r="D68" t="s">
+        <v>2</v>
+      </c>
+      <c r="E68" t="s">
+        <v>607</v>
+      </c>
+      <c r="F68" t="s">
+        <v>426</v>
+      </c>
+      <c r="G68" t="s">
+        <v>41</v>
+      </c>
+      <c r="H68" t="s">
+        <v>3</v>
+      </c>
+      <c r="I68" t="s">
+        <v>41</v>
+      </c>
+      <c r="J68" t="s">
+        <v>121</v>
+      </c>
+      <c r="K68" t="s">
+        <v>41</v>
+      </c>
+      <c r="L68" t="s">
+        <v>615</v>
+      </c>
+      <c r="M68" t="s">
+        <v>41</v>
+      </c>
+      <c r="N68" t="s">
+        <v>41</v>
+      </c>
+      <c r="O68" t="s">
+        <v>599</v>
+      </c>
+      <c r="P68" t="s">
+        <v>498</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>498</v>
+      </c>
+      <c r="R68" t="s">
+        <v>610</v>
       </c>
       <c r="S68" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -5984,12 +6166,63 @@
       </c>
       <c r="T68">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>475</v>
+        <v>608</v>
+      </c>
+      <c r="B69" t="s">
+        <v>64</v>
+      </c>
+      <c r="C69" t="s">
+        <v>2</v>
+      </c>
+      <c r="D69" t="s">
+        <v>2</v>
+      </c>
+      <c r="E69" t="s">
+        <v>41</v>
+      </c>
+      <c r="F69" t="s">
+        <v>422</v>
+      </c>
+      <c r="G69" t="s">
+        <v>598</v>
+      </c>
+      <c r="H69" t="s">
+        <v>41</v>
+      </c>
+      <c r="I69" t="s">
+        <v>41</v>
+      </c>
+      <c r="J69" t="s">
+        <v>41</v>
+      </c>
+      <c r="K69" t="s">
+        <v>41</v>
+      </c>
+      <c r="L69" t="s">
+        <v>611</v>
+      </c>
+      <c r="M69" t="s">
+        <v>41</v>
+      </c>
+      <c r="N69" t="s">
+        <v>6</v>
+      </c>
+      <c r="O69" t="s">
+        <v>605</v>
+      </c>
+      <c r="P69" t="s">
+        <v>498</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>498</v>
+      </c>
+      <c r="R69" t="s">
+        <v>610</v>
       </c>
       <c r="S69" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -5997,63 +6230,15 @@
       </c>
       <c r="T69">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>315</v>
+        <v>474</v>
       </c>
       <c r="B70" t="s">
-        <v>241</v>
-      </c>
-      <c r="C70" t="s">
-        <v>2</v>
-      </c>
-      <c r="D70" t="s">
-        <v>3</v>
-      </c>
-      <c r="E70" t="s">
-        <v>193</v>
-      </c>
-      <c r="F70" t="s">
-        <v>422</v>
-      </c>
-      <c r="G70" t="s">
-        <v>41</v>
-      </c>
-      <c r="H70" t="s">
-        <v>3</v>
-      </c>
-      <c r="I70" t="s">
-        <v>41</v>
-      </c>
-      <c r="J70" t="s">
-        <v>204</v>
-      </c>
-      <c r="K70" t="s">
-        <v>169</v>
-      </c>
-      <c r="L70" t="s">
-        <v>217</v>
-      </c>
-      <c r="M70" t="s">
-        <v>218</v>
-      </c>
-      <c r="N70" t="s">
-        <v>41</v>
-      </c>
-      <c r="O70" t="s">
-        <v>219</v>
-      </c>
-      <c r="P70" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q70" t="s">
-        <v>6</v>
-      </c>
-      <c r="R70" t="s">
-        <v>319</v>
+        <v>64</v>
       </c>
       <c r="S70" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -6061,127 +6246,29 @@
       </c>
       <c r="T70">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>325</v>
+        <v>589</v>
       </c>
       <c r="B71" t="s">
-        <v>240</v>
-      </c>
-      <c r="C71" t="s">
-        <v>2</v>
-      </c>
-      <c r="D71" t="s">
-        <v>3</v>
-      </c>
-      <c r="E71" t="s">
-        <v>187</v>
-      </c>
-      <c r="F71" t="s">
-        <v>422</v>
-      </c>
-      <c r="G71" t="s">
-        <v>41</v>
-      </c>
-      <c r="H71" t="s">
-        <v>3</v>
-      </c>
-      <c r="I71" t="s">
-        <v>41</v>
-      </c>
-      <c r="J71" t="s">
-        <v>148</v>
-      </c>
-      <c r="K71" t="s">
-        <v>169</v>
-      </c>
-      <c r="L71" t="s">
-        <v>216</v>
-      </c>
-      <c r="M71" t="s">
-        <v>158</v>
-      </c>
-      <c r="N71" t="s">
-        <v>41</v>
-      </c>
-      <c r="O71" t="s">
-        <v>159</v>
-      </c>
-      <c r="P71" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q71" t="s">
-        <v>181</v>
-      </c>
-      <c r="R71" t="s">
-        <v>331</v>
-      </c>
+        <v>482</v>
+      </c>
+      <c r="R71" s="10"/>
       <c r="S71" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
         <v>0</v>
       </c>
       <c r="T71">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>376</v>
-      </c>
-      <c r="B72" t="s">
-        <v>377</v>
-      </c>
-      <c r="C72" t="s">
-        <v>2</v>
-      </c>
-      <c r="D72" t="s">
-        <v>3</v>
-      </c>
-      <c r="E72" t="s">
-        <v>41</v>
-      </c>
-      <c r="F72" t="s">
-        <v>425</v>
-      </c>
-      <c r="G72" t="s">
-        <v>41</v>
-      </c>
-      <c r="H72" t="s">
-        <v>41</v>
-      </c>
-      <c r="I72" t="s">
-        <v>41</v>
-      </c>
-      <c r="J72" t="s">
-        <v>41</v>
-      </c>
-      <c r="K72" t="s">
-        <v>41</v>
-      </c>
-      <c r="L72" t="s">
-        <v>459</v>
-      </c>
-      <c r="M72" t="s">
-        <v>6</v>
-      </c>
-      <c r="N72" t="s">
-        <v>41</v>
-      </c>
-      <c r="O72" t="s">
-        <v>41</v>
-      </c>
-      <c r="P72" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q72" t="s">
-        <v>41</v>
-      </c>
-      <c r="R72" t="s">
-        <v>6</v>
+        <v>476</v>
       </c>
       <c r="S72" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -6194,58 +6281,7 @@
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>458</v>
-      </c>
-      <c r="B73" t="s">
-        <v>377</v>
-      </c>
-      <c r="C73" t="s">
-        <v>2</v>
-      </c>
-      <c r="D73" t="s">
-        <v>3</v>
-      </c>
-      <c r="E73" t="s">
-        <v>376</v>
-      </c>
-      <c r="F73" t="s">
-        <v>422</v>
-      </c>
-      <c r="G73" t="s">
-        <v>378</v>
-      </c>
-      <c r="H73" t="s">
-        <v>41</v>
-      </c>
-      <c r="I73" t="s">
-        <v>41</v>
-      </c>
-      <c r="J73" t="s">
-        <v>382</v>
-      </c>
-      <c r="K73" t="s">
-        <v>6</v>
-      </c>
-      <c r="L73" t="s">
-        <v>383</v>
-      </c>
-      <c r="M73" t="s">
-        <v>384</v>
-      </c>
-      <c r="N73" t="s">
-        <v>6</v>
-      </c>
-      <c r="O73" t="s">
-        <v>41</v>
-      </c>
-      <c r="P73" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q73" t="s">
-        <v>385</v>
-      </c>
-      <c r="R73" t="s">
-        <v>6</v>
+        <v>475</v>
       </c>
       <c r="S73" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -6253,15 +6289,63 @@
       </c>
       <c r="T73">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>590</v>
+        <v>315</v>
       </c>
       <c r="B74" t="s">
-        <v>592</v>
+        <v>241</v>
+      </c>
+      <c r="C74" t="s">
+        <v>2</v>
+      </c>
+      <c r="D74" t="s">
+        <v>3</v>
+      </c>
+      <c r="E74" t="s">
+        <v>193</v>
+      </c>
+      <c r="F74" t="s">
+        <v>422</v>
+      </c>
+      <c r="G74" t="s">
+        <v>41</v>
+      </c>
+      <c r="H74" t="s">
+        <v>3</v>
+      </c>
+      <c r="I74" t="s">
+        <v>41</v>
+      </c>
+      <c r="J74" t="s">
+        <v>204</v>
+      </c>
+      <c r="K74" t="s">
+        <v>169</v>
+      </c>
+      <c r="L74" t="s">
+        <v>217</v>
+      </c>
+      <c r="M74" t="s">
+        <v>218</v>
+      </c>
+      <c r="N74" t="s">
+        <v>41</v>
+      </c>
+      <c r="O74" t="s">
+        <v>219</v>
+      </c>
+      <c r="P74" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>6</v>
+      </c>
+      <c r="R74" t="s">
+        <v>319</v>
       </c>
       <c r="S74" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -6269,63 +6353,63 @@
       </c>
       <c r="T74">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>483</v>
+        <v>325</v>
       </c>
       <c r="B75" t="s">
-        <v>482</v>
+        <v>240</v>
       </c>
       <c r="C75" t="s">
         <v>2</v>
       </c>
       <c r="D75" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E75" t="s">
-        <v>41</v>
+        <v>187</v>
       </c>
       <c r="F75" t="s">
         <v>422</v>
       </c>
       <c r="G75" t="s">
-        <v>488</v>
+        <v>41</v>
       </c>
       <c r="H75" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="I75" t="s">
         <v>41</v>
       </c>
       <c r="J75" t="s">
-        <v>41</v>
+        <v>148</v>
       </c>
       <c r="K75" t="s">
-        <v>41</v>
+        <v>169</v>
       </c>
       <c r="L75" t="s">
-        <v>489</v>
+        <v>216</v>
       </c>
       <c r="M75" t="s">
-        <v>41</v>
+        <v>158</v>
       </c>
       <c r="N75" t="s">
         <v>41</v>
       </c>
       <c r="O75" t="s">
-        <v>505</v>
+        <v>159</v>
       </c>
       <c r="P75" t="s">
         <v>41</v>
       </c>
       <c r="Q75" t="s">
-        <v>41</v>
-      </c>
-      <c r="R75" s="10" t="s">
-        <v>490</v>
+        <v>181</v>
+      </c>
+      <c r="R75" t="s">
+        <v>331</v>
       </c>
       <c r="S75" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -6333,60 +6417,60 @@
       </c>
       <c r="T75">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>449</v>
+        <v>376</v>
       </c>
       <c r="B76" t="s">
-        <v>6</v>
+        <v>377</v>
       </c>
       <c r="C76" t="s">
         <v>2</v>
       </c>
       <c r="D76" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E76" t="s">
         <v>41</v>
       </c>
       <c r="F76" t="s">
-        <v>451</v>
+        <v>425</v>
       </c>
       <c r="G76" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="H76" t="s">
         <v>41</v>
       </c>
       <c r="I76" t="s">
-        <v>452</v>
+        <v>41</v>
       </c>
       <c r="J76" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="K76" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="L76" t="s">
-        <v>453</v>
+        <v>459</v>
       </c>
       <c r="M76" t="s">
-        <v>454</v>
+        <v>6</v>
       </c>
       <c r="N76" t="s">
         <v>41</v>
       </c>
       <c r="O76" t="s">
-        <v>455</v>
+        <v>41</v>
       </c>
       <c r="P76" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="Q76" t="s">
-        <v>456</v>
+        <v>41</v>
       </c>
       <c r="R76" t="s">
         <v>6</v>
@@ -6397,60 +6481,60 @@
       </c>
       <c r="T76">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>603</v>
+        <v>458</v>
       </c>
       <c r="B77" t="s">
-        <v>597</v>
+        <v>377</v>
       </c>
       <c r="C77" t="s">
         <v>2</v>
       </c>
       <c r="D77" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E77" t="s">
-        <v>41</v>
+        <v>376</v>
       </c>
       <c r="F77" t="s">
         <v>422</v>
       </c>
       <c r="G77" t="s">
-        <v>598</v>
+        <v>378</v>
       </c>
       <c r="H77" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="I77" t="s">
         <v>41</v>
       </c>
       <c r="J77" t="s">
-        <v>602</v>
+        <v>382</v>
       </c>
       <c r="K77" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="L77" t="s">
-        <v>604</v>
+        <v>383</v>
       </c>
       <c r="M77" t="s">
-        <v>6</v>
+        <v>384</v>
       </c>
       <c r="N77" t="s">
         <v>6</v>
       </c>
       <c r="O77" t="s">
-        <v>605</v>
+        <v>41</v>
       </c>
       <c r="P77" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="Q77" t="s">
-        <v>6</v>
+        <v>385</v>
       </c>
       <c r="R77" t="s">
         <v>6</v>
@@ -6466,58 +6550,10 @@
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="B78" t="s">
-        <v>597</v>
-      </c>
-      <c r="C78" t="s">
-        <v>2</v>
-      </c>
-      <c r="D78" t="s">
-        <v>2</v>
-      </c>
-      <c r="E78" t="s">
-        <v>41</v>
-      </c>
-      <c r="F78" t="s">
-        <v>422</v>
-      </c>
-      <c r="G78" t="s">
-        <v>41</v>
-      </c>
-      <c r="H78" t="s">
-        <v>3</v>
-      </c>
-      <c r="I78" t="s">
-        <v>41</v>
-      </c>
-      <c r="J78" t="s">
-        <v>602</v>
-      </c>
-      <c r="K78" t="s">
-        <v>41</v>
-      </c>
-      <c r="L78" t="s">
-        <v>600</v>
-      </c>
-      <c r="M78" t="s">
-        <v>6</v>
-      </c>
-      <c r="N78" t="s">
-        <v>6</v>
-      </c>
-      <c r="O78" t="s">
-        <v>599</v>
-      </c>
-      <c r="P78" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q78" t="s">
-        <v>6</v>
-      </c>
-      <c r="R78" t="s">
-        <v>6</v>
+        <v>592</v>
       </c>
       <c r="S78" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -6525,30 +6561,30 @@
       </c>
       <c r="T78">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>439</v>
+        <v>483</v>
       </c>
       <c r="B79" t="s">
-        <v>377</v>
+        <v>482</v>
       </c>
       <c r="C79" t="s">
         <v>2</v>
       </c>
       <c r="D79" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E79" t="s">
         <v>41</v>
       </c>
       <c r="F79" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G79" t="s">
-        <v>41</v>
+        <v>488</v>
       </c>
       <c r="H79" t="s">
         <v>41</v>
@@ -6563,29 +6599,29 @@
         <v>41</v>
       </c>
       <c r="L79" t="s">
-        <v>440</v>
+        <v>489</v>
       </c>
       <c r="M79" t="s">
-        <v>441</v>
+        <v>41</v>
       </c>
       <c r="N79" t="s">
         <v>41</v>
       </c>
       <c r="O79" t="s">
-        <v>442</v>
+        <v>505</v>
       </c>
       <c r="P79" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="Q79" t="s">
-        <v>6</v>
-      </c>
-      <c r="R79" t="s">
-        <v>6</v>
+        <v>41</v>
+      </c>
+      <c r="R79" s="10" t="s">
+        <v>490</v>
       </c>
       <c r="S79" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T79">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
@@ -6594,55 +6630,55 @@
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>386</v>
+        <v>449</v>
       </c>
       <c r="B80" t="s">
-        <v>377</v>
+        <v>6</v>
       </c>
       <c r="C80" t="s">
         <v>2</v>
       </c>
       <c r="D80" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E80" t="s">
         <v>41</v>
       </c>
       <c r="F80" t="s">
-        <v>425</v>
+        <v>451</v>
       </c>
       <c r="G80" t="s">
-        <v>378</v>
+        <v>71</v>
       </c>
       <c r="H80" t="s">
         <v>41</v>
       </c>
       <c r="I80" t="s">
-        <v>41</v>
+        <v>452</v>
       </c>
       <c r="J80" t="s">
-        <v>121</v>
+        <v>6</v>
       </c>
       <c r="K80" t="s">
-        <v>387</v>
+        <v>6</v>
       </c>
       <c r="L80" t="s">
-        <v>388</v>
+        <v>453</v>
       </c>
       <c r="M80" t="s">
-        <v>389</v>
+        <v>454</v>
       </c>
       <c r="N80" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="O80" t="s">
-        <v>41</v>
+        <v>455</v>
       </c>
       <c r="P80" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="Q80" t="s">
-        <v>6</v>
+        <v>456</v>
       </c>
       <c r="R80" t="s">
         <v>6</v>
@@ -6653,15 +6689,15 @@
       </c>
       <c r="T80">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>427</v>
+        <v>603</v>
       </c>
       <c r="B81" t="s">
-        <v>6</v>
+        <v>597</v>
       </c>
       <c r="C81" t="s">
         <v>2</v>
@@ -6673,16 +6709,43 @@
         <v>41</v>
       </c>
       <c r="F81" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G81" t="s">
-        <v>429</v>
+        <v>598</v>
       </c>
       <c r="H81" t="s">
-        <v>41</v>
+        <v>3</v>
+      </c>
+      <c r="I81" t="s">
+        <v>41</v>
+      </c>
+      <c r="J81" t="s">
+        <v>602</v>
+      </c>
+      <c r="K81" t="s">
+        <v>41</v>
+      </c>
+      <c r="L81" t="s">
+        <v>604</v>
+      </c>
+      <c r="M81" t="s">
+        <v>6</v>
+      </c>
+      <c r="N81" t="s">
+        <v>6</v>
       </c>
       <c r="O81" t="s">
-        <v>443</v>
+        <v>605</v>
+      </c>
+      <c r="P81" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>6</v>
+      </c>
+      <c r="R81" t="s">
+        <v>6</v>
       </c>
       <c r="S81" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -6690,63 +6753,63 @@
       </c>
       <c r="T81">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>326</v>
+        <v>596</v>
       </c>
       <c r="B82" t="s">
-        <v>240</v>
+        <v>597</v>
       </c>
       <c r="C82" t="s">
         <v>2</v>
       </c>
       <c r="D82" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E82" t="s">
-        <v>187</v>
+        <v>41</v>
       </c>
       <c r="F82" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="G82" t="s">
         <v>41</v>
       </c>
       <c r="H82" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="I82" t="s">
         <v>41</v>
       </c>
       <c r="J82" t="s">
-        <v>148</v>
+        <v>602</v>
       </c>
       <c r="K82" t="s">
-        <v>169</v>
+        <v>41</v>
       </c>
       <c r="L82" t="s">
-        <v>188</v>
+        <v>600</v>
       </c>
       <c r="M82" t="s">
-        <v>189</v>
+        <v>6</v>
       </c>
       <c r="N82" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="O82" t="s">
-        <v>190</v>
+        <v>599</v>
       </c>
       <c r="P82" t="s">
         <v>41</v>
       </c>
       <c r="Q82" t="s">
-        <v>330</v>
+        <v>6</v>
       </c>
       <c r="R82" t="s">
-        <v>331</v>
+        <v>6</v>
       </c>
       <c r="S82" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -6754,143 +6817,143 @@
       </c>
       <c r="T82">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>0</v>
+        <v>439</v>
       </c>
       <c r="B83" t="s">
-        <v>239</v>
+        <v>377</v>
       </c>
       <c r="C83" t="s">
         <v>2</v>
       </c>
       <c r="D83" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E83" t="s">
         <v>41</v>
       </c>
       <c r="F83" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="G83" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="H83" t="s">
         <v>41</v>
       </c>
       <c r="I83" t="s">
-        <v>93</v>
+        <v>41</v>
       </c>
       <c r="J83" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="K83" t="s">
         <v>41</v>
       </c>
       <c r="L83" t="s">
-        <v>94</v>
+        <v>440</v>
       </c>
       <c r="M83" t="s">
-        <v>95</v>
+        <v>441</v>
       </c>
       <c r="N83" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="O83" t="s">
-        <v>96</v>
+        <v>442</v>
       </c>
       <c r="P83" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="Q83" t="s">
-        <v>184</v>
+        <v>6</v>
       </c>
       <c r="R83" t="s">
         <v>6</v>
       </c>
-      <c r="S83">
+      <c r="S83" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T83">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>10</v>
+        <v>386</v>
       </c>
       <c r="B84" t="s">
-        <v>239</v>
+        <v>377</v>
       </c>
       <c r="C84" t="s">
         <v>2</v>
       </c>
       <c r="D84" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E84" t="s">
         <v>41</v>
       </c>
       <c r="F84" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="G84" t="s">
-        <v>71</v>
+        <v>378</v>
       </c>
       <c r="H84" t="s">
         <v>41</v>
       </c>
       <c r="I84" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="J84" t="s">
-        <v>80</v>
+        <v>121</v>
       </c>
       <c r="K84" t="s">
-        <v>41</v>
+        <v>387</v>
       </c>
       <c r="L84" t="s">
-        <v>89</v>
+        <v>388</v>
       </c>
       <c r="M84" t="s">
-        <v>90</v>
+        <v>389</v>
       </c>
       <c r="N84" t="s">
-        <v>84</v>
+        <v>6</v>
       </c>
       <c r="O84" t="s">
-        <v>91</v>
+        <v>41</v>
       </c>
       <c r="P84" t="s">
-        <v>92</v>
+        <v>6</v>
       </c>
       <c r="Q84" t="s">
-        <v>184</v>
+        <v>6</v>
       </c>
       <c r="R84" t="s">
         <v>6</v>
       </c>
-      <c r="S84">
+      <c r="S84" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T84">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>36</v>
+        <v>427</v>
       </c>
       <c r="B85" t="s">
-        <v>239</v>
+        <v>6</v>
       </c>
       <c r="C85" t="s">
         <v>2</v>
@@ -6902,126 +6965,99 @@
         <v>41</v>
       </c>
       <c r="F85" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="G85" t="s">
-        <v>71</v>
+        <v>429</v>
       </c>
       <c r="H85" t="s">
         <v>41</v>
       </c>
-      <c r="I85" t="s">
-        <v>98</v>
-      </c>
-      <c r="J85" t="s">
-        <v>80</v>
-      </c>
-      <c r="K85" t="s">
-        <v>41</v>
-      </c>
-      <c r="L85" t="s">
-        <v>99</v>
-      </c>
-      <c r="M85" t="s">
-        <v>100</v>
-      </c>
-      <c r="N85" t="s">
-        <v>84</v>
-      </c>
       <c r="O85" t="s">
-        <v>101</v>
-      </c>
-      <c r="P85" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q85" t="s">
-        <v>184</v>
-      </c>
-      <c r="R85" t="s">
-        <v>6</v>
-      </c>
-      <c r="S85">
+        <v>443</v>
+      </c>
+      <c r="S85" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T85">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>38</v>
+        <v>326</v>
       </c>
       <c r="B86" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C86" t="s">
         <v>2</v>
       </c>
       <c r="D86" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E86" t="s">
-        <v>41</v>
+        <v>187</v>
       </c>
       <c r="F86" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="G86" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="H86" t="s">
         <v>41</v>
       </c>
       <c r="I86" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="J86" t="s">
-        <v>80</v>
+        <v>148</v>
       </c>
       <c r="K86" t="s">
-        <v>41</v>
+        <v>169</v>
       </c>
       <c r="L86" t="s">
-        <v>82</v>
+        <v>188</v>
       </c>
       <c r="M86" t="s">
-        <v>83</v>
+        <v>189</v>
       </c>
       <c r="N86" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="O86" t="s">
-        <v>85</v>
+        <v>190</v>
       </c>
       <c r="P86" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="Q86" t="s">
-        <v>184</v>
+        <v>330</v>
       </c>
       <c r="R86" t="s">
-        <v>6</v>
-      </c>
-      <c r="S86">
+        <v>331</v>
+      </c>
+      <c r="S86" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T86">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>113</v>
+        <v>0</v>
       </c>
       <c r="B87" t="s">
         <v>239</v>
       </c>
       <c r="C87" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D87" t="s">
         <v>2</v>
@@ -7039,7 +7075,7 @@
         <v>41</v>
       </c>
       <c r="I87" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="J87" t="s">
         <v>80</v>
@@ -7048,22 +7084,22 @@
         <v>41</v>
       </c>
       <c r="L87" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="M87" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="N87" t="s">
         <v>84</v>
       </c>
       <c r="O87" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="P87" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="Q87" t="s">
-        <v>6</v>
+        <v>184</v>
       </c>
       <c r="R87" t="s">
         <v>6</v>
@@ -7074,18 +7110,18 @@
       </c>
       <c r="T87">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>118</v>
+        <v>10</v>
       </c>
       <c r="B88" t="s">
         <v>239</v>
       </c>
       <c r="C88" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D88" t="s">
         <v>2</v>
@@ -7103,7 +7139,7 @@
         <v>41</v>
       </c>
       <c r="I88" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="J88" t="s">
         <v>80</v>
@@ -7112,38 +7148,38 @@
         <v>41</v>
       </c>
       <c r="L88" t="s">
-        <v>119</v>
+        <v>89</v>
       </c>
       <c r="M88" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="N88" t="s">
         <v>84</v>
       </c>
       <c r="O88" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="P88" t="s">
-        <v>41</v>
+        <v>92</v>
       </c>
       <c r="Q88" t="s">
-        <v>6</v>
+        <v>184</v>
       </c>
       <c r="R88" t="s">
         <v>6</v>
       </c>
       <c r="S88">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T88">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>544</v>
+        <v>36</v>
       </c>
       <c r="B89" t="s">
         <v>239</v>
@@ -7161,120 +7197,123 @@
         <v>422</v>
       </c>
       <c r="G89" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="H89" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="I89" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
       <c r="J89" t="s">
-        <v>121</v>
+        <v>80</v>
       </c>
       <c r="K89" t="s">
-        <v>545</v>
+        <v>41</v>
       </c>
       <c r="L89" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="M89" t="s">
-        <v>176</v>
+        <v>100</v>
+      </c>
+      <c r="N89" t="s">
+        <v>84</v>
       </c>
       <c r="O89" t="s">
-        <v>175</v>
+        <v>101</v>
       </c>
       <c r="P89" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="Q89" t="s">
-        <v>41</v>
+        <v>184</v>
       </c>
       <c r="R89" t="s">
-        <v>41</v>
-      </c>
-      <c r="S89" s="8">
+        <v>6</v>
+      </c>
+      <c r="S89">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T89">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>314</v>
+        <v>38</v>
       </c>
       <c r="B90" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C90" t="s">
         <v>2</v>
       </c>
       <c r="D90" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E90" t="s">
-        <v>193</v>
+        <v>41</v>
       </c>
       <c r="F90" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G90" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="H90" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="I90" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="J90" t="s">
-        <v>204</v>
+        <v>80</v>
       </c>
       <c r="K90" t="s">
-        <v>169</v>
+        <v>41</v>
       </c>
       <c r="L90" t="s">
-        <v>203</v>
+        <v>82</v>
       </c>
       <c r="M90" t="s">
-        <v>206</v>
+        <v>83</v>
       </c>
       <c r="N90" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="O90" t="s">
-        <v>207</v>
+        <v>85</v>
       </c>
       <c r="P90" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="Q90" t="s">
-        <v>428</v>
+        <v>184</v>
       </c>
       <c r="R90" t="s">
-        <v>319</v>
-      </c>
-      <c r="S90" s="8">
+        <v>6</v>
+      </c>
+      <c r="S90">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T90">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>360</v>
+        <v>113</v>
       </c>
       <c r="B91" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="C91" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D91" t="s">
         <v>2</v>
@@ -7286,60 +7325,108 @@
         <v>422</v>
       </c>
       <c r="G91" t="s">
-        <v>361</v>
+        <v>71</v>
       </c>
       <c r="H91" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="I91" t="s">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="J91" t="s">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="K91" t="s">
         <v>41</v>
       </c>
       <c r="L91" t="s">
-        <v>362</v>
+        <v>115</v>
       </c>
       <c r="M91" t="s">
-        <v>363</v>
+        <v>116</v>
       </c>
       <c r="N91" t="s">
-        <v>6</v>
+        <v>84</v>
       </c>
       <c r="O91" t="s">
-        <v>364</v>
+        <v>117</v>
       </c>
       <c r="P91" t="s">
         <v>41</v>
       </c>
       <c r="Q91" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="R91" t="s">
-        <v>41</v>
-      </c>
-      <c r="S91" s="8">
+        <v>6</v>
+      </c>
+      <c r="S91">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T91">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>588</v>
+        <v>118</v>
       </c>
       <c r="B92" t="s">
-        <v>246</v>
-      </c>
-      <c r="S92" s="8">
+        <v>239</v>
+      </c>
+      <c r="C92" t="s">
+        <v>3</v>
+      </c>
+      <c r="D92" t="s">
+        <v>2</v>
+      </c>
+      <c r="E92" t="s">
+        <v>41</v>
+      </c>
+      <c r="F92" t="s">
+        <v>422</v>
+      </c>
+      <c r="G92" t="s">
+        <v>71</v>
+      </c>
+      <c r="H92" t="s">
+        <v>41</v>
+      </c>
+      <c r="I92" t="s">
+        <v>79</v>
+      </c>
+      <c r="J92" t="s">
+        <v>80</v>
+      </c>
+      <c r="K92" t="s">
+        <v>41</v>
+      </c>
+      <c r="L92" t="s">
+        <v>119</v>
+      </c>
+      <c r="M92" t="s">
+        <v>120</v>
+      </c>
+      <c r="N92" t="s">
+        <v>84</v>
+      </c>
+      <c r="O92" t="s">
+        <v>85</v>
+      </c>
+      <c r="P92" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>6</v>
+      </c>
+      <c r="R92" t="s">
+        <v>6</v>
+      </c>
+      <c r="S92">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T92">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
@@ -7348,10 +7435,10 @@
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>244</v>
+        <v>544</v>
       </c>
       <c r="B93" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="C93" t="s">
         <v>2</v>
@@ -7363,16 +7450,40 @@
         <v>41</v>
       </c>
       <c r="F93" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="G93" t="s">
-        <v>430</v>
+        <v>3</v>
       </c>
       <c r="H93" t="s">
-        <v>41</v>
+        <v>3</v>
+      </c>
+      <c r="I93" t="s">
+        <v>41</v>
+      </c>
+      <c r="J93" t="s">
+        <v>121</v>
+      </c>
+      <c r="K93" t="s">
+        <v>545</v>
+      </c>
+      <c r="L93" t="s">
+        <v>122</v>
+      </c>
+      <c r="M93" t="s">
+        <v>176</v>
       </c>
       <c r="O93" t="s">
-        <v>252</v>
+        <v>175</v>
+      </c>
+      <c r="P93" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q93" t="s">
+        <v>41</v>
+      </c>
+      <c r="R93" t="s">
+        <v>41</v>
       </c>
       <c r="S93" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -7385,10 +7496,10 @@
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
       <c r="B94" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C94" t="s">
         <v>2</v>
@@ -7397,7 +7508,7 @@
         <v>3</v>
       </c>
       <c r="E94" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="F94" t="s">
         <v>425</v>
@@ -7406,37 +7517,37 @@
         <v>41</v>
       </c>
       <c r="H94" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="I94" t="s">
         <v>41</v>
       </c>
       <c r="J94" t="s">
-        <v>84</v>
+        <v>204</v>
       </c>
       <c r="K94" t="s">
-        <v>84</v>
+        <v>169</v>
       </c>
       <c r="L94" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="M94" t="s">
-        <v>84</v>
+        <v>206</v>
       </c>
       <c r="N94" t="s">
         <v>41</v>
       </c>
       <c r="O94" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
       <c r="P94" t="s">
         <v>41</v>
       </c>
       <c r="Q94" t="s">
-        <v>6</v>
+        <v>428</v>
       </c>
       <c r="R94" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="S94" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -7444,12 +7555,12 @@
       </c>
       <c r="T94">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>253</v>
+        <v>360</v>
       </c>
       <c r="B95" t="s">
         <v>246</v>
@@ -7464,43 +7575,43 @@
         <v>41</v>
       </c>
       <c r="F95" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G95" t="s">
-        <v>246</v>
+        <v>361</v>
       </c>
       <c r="H95" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="I95" t="s">
         <v>41</v>
       </c>
       <c r="J95" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K95" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="L95" t="s">
-        <v>278</v>
+        <v>362</v>
       </c>
       <c r="M95" t="s">
-        <v>279</v>
+        <v>363</v>
       </c>
       <c r="N95" t="s">
-        <v>280</v>
+        <v>6</v>
       </c>
       <c r="O95" t="s">
-        <v>281</v>
+        <v>364</v>
       </c>
       <c r="P95" t="s">
-        <v>282</v>
+        <v>41</v>
       </c>
       <c r="Q95" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="R95" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="S95" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -7508,54 +7619,15 @@
       </c>
       <c r="T95">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>392</v>
+        <v>588</v>
       </c>
       <c r="B96" t="s">
-        <v>377</v>
-      </c>
-      <c r="C96" t="s">
-        <v>2</v>
-      </c>
-      <c r="D96" t="s">
-        <v>2</v>
-      </c>
-      <c r="E96" t="s">
-        <v>41</v>
-      </c>
-      <c r="F96" t="s">
-        <v>422</v>
-      </c>
-      <c r="G96" t="s">
-        <v>378</v>
-      </c>
-      <c r="H96" t="s">
-        <v>3</v>
-      </c>
-      <c r="I96" t="s">
-        <v>41</v>
-      </c>
-      <c r="J96" t="s">
-        <v>121</v>
-      </c>
-      <c r="K96" s="14" t="s">
-        <v>400</v>
-      </c>
-      <c r="L96" t="s">
-        <v>395</v>
-      </c>
-      <c r="M96" t="s">
-        <v>396</v>
-      </c>
-      <c r="N96" t="s">
-        <v>41</v>
-      </c>
-      <c r="O96" t="s">
-        <v>397</v>
+        <v>246</v>
       </c>
       <c r="S96" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -7568,10 +7640,10 @@
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>398</v>
+        <v>244</v>
       </c>
       <c r="B97" t="s">
-        <v>399</v>
+        <v>246</v>
       </c>
       <c r="C97" t="s">
         <v>2</v>
@@ -7583,43 +7655,16 @@
         <v>41</v>
       </c>
       <c r="F97" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="G97" t="s">
-        <v>41</v>
+        <v>430</v>
       </c>
       <c r="H97" t="s">
-        <v>3</v>
-      </c>
-      <c r="I97" t="s">
-        <v>41</v>
-      </c>
-      <c r="J97" t="s">
-        <v>121</v>
-      </c>
-      <c r="K97" s="14" t="s">
-        <v>400</v>
-      </c>
-      <c r="L97" t="s">
-        <v>401</v>
-      </c>
-      <c r="M97" t="s">
-        <v>402</v>
-      </c>
-      <c r="N97" t="s">
         <v>41</v>
       </c>
       <c r="O97" t="s">
-        <v>41</v>
-      </c>
-      <c r="P97" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q97" t="s">
-        <v>403</v>
-      </c>
-      <c r="R97" t="s">
-        <v>6</v>
+        <v>252</v>
       </c>
       <c r="S97" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -7632,10 +7677,10 @@
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>464</v>
+        <v>327</v>
       </c>
       <c r="B98" t="s">
-        <v>464</v>
+        <v>240</v>
       </c>
       <c r="C98" t="s">
         <v>2</v>
@@ -7644,37 +7689,37 @@
         <v>3</v>
       </c>
       <c r="E98" t="s">
-        <v>41</v>
+        <v>187</v>
       </c>
       <c r="F98" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="G98" t="s">
         <v>41</v>
       </c>
       <c r="H98" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="I98" t="s">
         <v>41</v>
       </c>
       <c r="J98" t="s">
-        <v>6</v>
+        <v>84</v>
       </c>
       <c r="K98" t="s">
-        <v>6</v>
+        <v>84</v>
       </c>
       <c r="L98" t="s">
-        <v>6</v>
+        <v>191</v>
       </c>
       <c r="M98" t="s">
-        <v>6</v>
+        <v>84</v>
       </c>
       <c r="N98" t="s">
         <v>41</v>
       </c>
       <c r="O98" t="s">
-        <v>465</v>
+        <v>192</v>
       </c>
       <c r="P98" t="s">
         <v>41</v>
@@ -7683,7 +7728,7 @@
         <v>6</v>
       </c>
       <c r="R98" t="s">
-        <v>6</v>
+        <v>331</v>
       </c>
       <c r="S98" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -7696,25 +7741,25 @@
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>463</v>
+        <v>253</v>
       </c>
       <c r="B99" t="s">
-        <v>464</v>
+        <v>246</v>
       </c>
       <c r="C99" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D99" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E99" t="s">
-        <v>464</v>
+        <v>41</v>
       </c>
       <c r="F99" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G99" t="s">
-        <v>41</v>
+        <v>246</v>
       </c>
       <c r="H99" t="s">
         <v>41</v>
@@ -7723,25 +7768,25 @@
         <v>41</v>
       </c>
       <c r="J99" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="K99" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="L99" t="s">
-        <v>472</v>
+        <v>278</v>
       </c>
       <c r="M99" t="s">
-        <v>473</v>
+        <v>279</v>
       </c>
       <c r="N99" t="s">
-        <v>41</v>
+        <v>280</v>
       </c>
       <c r="O99" t="s">
-        <v>41</v>
+        <v>281</v>
       </c>
       <c r="P99" t="s">
-        <v>41</v>
+        <v>282</v>
       </c>
       <c r="Q99" t="s">
         <v>6</v>
@@ -7755,63 +7800,54 @@
       </c>
       <c r="T99">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>461</v>
+        <v>392</v>
       </c>
       <c r="B100" t="s">
-        <v>464</v>
+        <v>377</v>
       </c>
       <c r="C100" t="s">
         <v>2</v>
       </c>
       <c r="D100" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E100" t="s">
-        <v>464</v>
+        <v>41</v>
       </c>
       <c r="F100" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="G100" t="s">
-        <v>41</v>
+        <v>378</v>
       </c>
       <c r="H100" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="I100" t="s">
         <v>41</v>
       </c>
       <c r="J100" t="s">
-        <v>41</v>
-      </c>
-      <c r="K100" t="s">
-        <v>41</v>
+        <v>121</v>
+      </c>
+      <c r="K100" s="14" t="s">
+        <v>400</v>
       </c>
       <c r="L100" t="s">
-        <v>468</v>
+        <v>395</v>
       </c>
       <c r="M100" t="s">
-        <v>469</v>
+        <v>396</v>
       </c>
       <c r="N100" t="s">
         <v>41</v>
       </c>
       <c r="O100" t="s">
-        <v>41</v>
-      </c>
-      <c r="P100" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q100" t="s">
-        <v>6</v>
-      </c>
-      <c r="R100" t="s">
-        <v>6</v>
+        <v>397</v>
       </c>
       <c r="S100" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -7824,43 +7860,43 @@
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>460</v>
+        <v>398</v>
       </c>
       <c r="B101" t="s">
-        <v>464</v>
+        <v>399</v>
       </c>
       <c r="C101" t="s">
         <v>2</v>
       </c>
       <c r="D101" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E101" t="s">
-        <v>464</v>
+        <v>41</v>
       </c>
       <c r="F101" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="G101" t="s">
         <v>41</v>
       </c>
       <c r="H101" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="I101" t="s">
         <v>41</v>
       </c>
       <c r="J101" t="s">
-        <v>41</v>
-      </c>
-      <c r="K101" t="s">
-        <v>41</v>
+        <v>121</v>
+      </c>
+      <c r="K101" s="14" t="s">
+        <v>400</v>
       </c>
       <c r="L101" t="s">
-        <v>466</v>
+        <v>401</v>
       </c>
       <c r="M101" t="s">
-        <v>467</v>
+        <v>402</v>
       </c>
       <c r="N101" t="s">
         <v>41</v>
@@ -7872,7 +7908,7 @@
         <v>41</v>
       </c>
       <c r="Q101" t="s">
-        <v>6</v>
+        <v>403</v>
       </c>
       <c r="R101" t="s">
         <v>6</v>
@@ -7888,7 +7924,7 @@
     </row>
     <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="B102" t="s">
         <v>464</v>
@@ -7900,37 +7936,37 @@
         <v>3</v>
       </c>
       <c r="E102" t="s">
-        <v>464</v>
+        <v>41</v>
       </c>
       <c r="F102" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="G102" t="s">
         <v>41</v>
       </c>
       <c r="H102" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="I102" t="s">
         <v>41</v>
       </c>
       <c r="J102" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="K102" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="L102" t="s">
-        <v>470</v>
+        <v>6</v>
       </c>
       <c r="M102" t="s">
-        <v>471</v>
+        <v>6</v>
       </c>
       <c r="N102" t="s">
         <v>41</v>
       </c>
       <c r="O102" t="s">
-        <v>41</v>
+        <v>465</v>
       </c>
       <c r="P102" t="s">
         <v>41</v>
@@ -7952,25 +7988,25 @@
     </row>
     <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>457</v>
+        <v>463</v>
       </c>
       <c r="B103" t="s">
-        <v>377</v>
+        <v>464</v>
       </c>
       <c r="C103" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D103" t="s">
         <v>3</v>
       </c>
       <c r="E103" t="s">
-        <v>376</v>
+        <v>464</v>
       </c>
       <c r="F103" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="G103" t="s">
-        <v>378</v>
+        <v>41</v>
       </c>
       <c r="H103" t="s">
         <v>41</v>
@@ -7979,28 +8015,28 @@
         <v>41</v>
       </c>
       <c r="J103" t="s">
-        <v>121</v>
+        <v>41</v>
       </c>
       <c r="K103" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="L103" t="s">
-        <v>379</v>
+        <v>472</v>
       </c>
       <c r="M103" t="s">
-        <v>6</v>
+        <v>473</v>
       </c>
       <c r="N103" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="O103" t="s">
-        <v>380</v>
+        <v>41</v>
       </c>
       <c r="P103" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="Q103" t="s">
-        <v>381</v>
+        <v>6</v>
       </c>
       <c r="R103" t="s">
         <v>6</v>
@@ -8011,15 +8047,15 @@
       </c>
       <c r="T103">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>432</v>
+        <v>461</v>
       </c>
       <c r="B104" t="s">
-        <v>377</v>
+        <v>464</v>
       </c>
       <c r="C104" t="s">
         <v>2</v>
@@ -8028,13 +8064,13 @@
         <v>3</v>
       </c>
       <c r="E104" t="s">
-        <v>41</v>
+        <v>464</v>
       </c>
       <c r="F104" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="G104" t="s">
-        <v>378</v>
+        <v>41</v>
       </c>
       <c r="H104" t="s">
         <v>41</v>
@@ -8043,16 +8079,16 @@
         <v>41</v>
       </c>
       <c r="J104" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="K104" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="L104" t="s">
-        <v>433</v>
+        <v>468</v>
       </c>
       <c r="M104" t="s">
-        <v>434</v>
+        <v>469</v>
       </c>
       <c r="N104" t="s">
         <v>41</v>
@@ -8064,10 +8100,10 @@
         <v>41</v>
       </c>
       <c r="Q104" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="R104" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="S104" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -8080,10 +8116,10 @@
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>411</v>
+        <v>460</v>
       </c>
       <c r="B105" t="s">
-        <v>484</v>
+        <v>464</v>
       </c>
       <c r="C105" t="s">
         <v>2</v>
@@ -8092,19 +8128,19 @@
         <v>3</v>
       </c>
       <c r="E105" t="s">
-        <v>41</v>
+        <v>464</v>
       </c>
       <c r="F105" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="G105" t="s">
-        <v>485</v>
+        <v>41</v>
       </c>
       <c r="H105" t="s">
         <v>41</v>
       </c>
       <c r="I105" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="J105" t="s">
         <v>41</v>
@@ -8113,10 +8149,10 @@
         <v>41</v>
       </c>
       <c r="L105" t="s">
-        <v>393</v>
+        <v>466</v>
       </c>
       <c r="M105" t="s">
-        <v>394</v>
+        <v>467</v>
       </c>
       <c r="N105" t="s">
         <v>41</v>
@@ -8128,10 +8164,10 @@
         <v>41</v>
       </c>
       <c r="Q105" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="R105" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="S105" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -8139,15 +8175,15 @@
       </c>
       <c r="T105">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>340</v>
+        <v>462</v>
       </c>
       <c r="B106" t="s">
-        <v>240</v>
+        <v>464</v>
       </c>
       <c r="C106" t="s">
         <v>2</v>
@@ -8156,10 +8192,10 @@
         <v>3</v>
       </c>
       <c r="E106" t="s">
-        <v>187</v>
+        <v>464</v>
       </c>
       <c r="F106" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="G106" t="s">
         <v>41</v>
@@ -8171,16 +8207,16 @@
         <v>41</v>
       </c>
       <c r="J106" t="s">
-        <v>148</v>
+        <v>41</v>
       </c>
       <c r="K106" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="L106" t="s">
-        <v>341</v>
+        <v>470</v>
       </c>
       <c r="M106" t="s">
-        <v>342</v>
+        <v>471</v>
       </c>
       <c r="N106" t="s">
         <v>41</v>
@@ -8195,7 +8231,7 @@
         <v>6</v>
       </c>
       <c r="R106" t="s">
-        <v>331</v>
+        <v>6</v>
       </c>
       <c r="S106" s="8">
         <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
@@ -8203,12 +8239,268 @@
       </c>
       <c r="T106">
         <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>457</v>
+      </c>
+      <c r="B107" t="s">
+        <v>377</v>
+      </c>
+      <c r="C107" t="s">
+        <v>2</v>
+      </c>
+      <c r="D107" t="s">
+        <v>3</v>
+      </c>
+      <c r="E107" t="s">
+        <v>376</v>
+      </c>
+      <c r="F107" t="s">
+        <v>425</v>
+      </c>
+      <c r="G107" t="s">
+        <v>378</v>
+      </c>
+      <c r="H107" t="s">
+        <v>41</v>
+      </c>
+      <c r="I107" t="s">
+        <v>41</v>
+      </c>
+      <c r="J107" t="s">
+        <v>121</v>
+      </c>
+      <c r="K107" t="s">
+        <v>6</v>
+      </c>
+      <c r="L107" t="s">
+        <v>379</v>
+      </c>
+      <c r="M107" t="s">
+        <v>6</v>
+      </c>
+      <c r="N107" t="s">
+        <v>6</v>
+      </c>
+      <c r="O107" t="s">
+        <v>380</v>
+      </c>
+      <c r="P107" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q107" t="s">
+        <v>381</v>
+      </c>
+      <c r="R107" t="s">
+        <v>6</v>
+      </c>
+      <c r="S107" s="8">
+        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T107">
+        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>432</v>
+      </c>
+      <c r="B108" t="s">
+        <v>377</v>
+      </c>
+      <c r="C108" t="s">
+        <v>2</v>
+      </c>
+      <c r="D108" t="s">
+        <v>3</v>
+      </c>
+      <c r="E108" t="s">
+        <v>41</v>
+      </c>
+      <c r="F108" t="s">
+        <v>422</v>
+      </c>
+      <c r="G108" t="s">
+        <v>378</v>
+      </c>
+      <c r="H108" t="s">
+        <v>41</v>
+      </c>
+      <c r="I108" t="s">
+        <v>41</v>
+      </c>
+      <c r="J108" t="s">
+        <v>84</v>
+      </c>
+      <c r="K108" t="s">
+        <v>6</v>
+      </c>
+      <c r="L108" t="s">
+        <v>433</v>
+      </c>
+      <c r="M108" t="s">
+        <v>434</v>
+      </c>
+      <c r="N108" t="s">
+        <v>41</v>
+      </c>
+      <c r="O108" t="s">
+        <v>41</v>
+      </c>
+      <c r="P108" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q108" t="s">
+        <v>41</v>
+      </c>
+      <c r="R108" t="s">
+        <v>41</v>
+      </c>
+      <c r="S108" s="8">
+        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T108">
+        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>411</v>
+      </c>
+      <c r="B109" t="s">
+        <v>484</v>
+      </c>
+      <c r="C109" t="s">
+        <v>2</v>
+      </c>
+      <c r="D109" t="s">
+        <v>3</v>
+      </c>
+      <c r="E109" t="s">
+        <v>41</v>
+      </c>
+      <c r="F109" t="s">
+        <v>422</v>
+      </c>
+      <c r="G109" t="s">
+        <v>485</v>
+      </c>
+      <c r="H109" t="s">
+        <v>41</v>
+      </c>
+      <c r="I109" t="s">
+        <v>6</v>
+      </c>
+      <c r="J109" t="s">
+        <v>41</v>
+      </c>
+      <c r="K109" t="s">
+        <v>41</v>
+      </c>
+      <c r="L109" t="s">
+        <v>393</v>
+      </c>
+      <c r="M109" t="s">
+        <v>394</v>
+      </c>
+      <c r="N109" t="s">
+        <v>41</v>
+      </c>
+      <c r="O109" t="s">
+        <v>41</v>
+      </c>
+      <c r="P109" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q109" t="s">
+        <v>41</v>
+      </c>
+      <c r="R109" t="s">
+        <v>41</v>
+      </c>
+      <c r="S109" s="8">
+        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T109">
+        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>340</v>
+      </c>
+      <c r="B110" t="s">
+        <v>240</v>
+      </c>
+      <c r="C110" t="s">
+        <v>2</v>
+      </c>
+      <c r="D110" t="s">
+        <v>3</v>
+      </c>
+      <c r="E110" t="s">
+        <v>187</v>
+      </c>
+      <c r="F110" t="s">
+        <v>425</v>
+      </c>
+      <c r="G110" t="s">
+        <v>41</v>
+      </c>
+      <c r="H110" t="s">
+        <v>41</v>
+      </c>
+      <c r="I110" t="s">
+        <v>41</v>
+      </c>
+      <c r="J110" t="s">
+        <v>148</v>
+      </c>
+      <c r="K110" t="s">
+        <v>6</v>
+      </c>
+      <c r="L110" t="s">
+        <v>341</v>
+      </c>
+      <c r="M110" t="s">
+        <v>342</v>
+      </c>
+      <c r="N110" t="s">
+        <v>41</v>
+      </c>
+      <c r="O110" t="s">
+        <v>41</v>
+      </c>
+      <c r="P110" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q110" t="s">
+        <v>6</v>
+      </c>
+      <c r="R110" t="s">
+        <v>331</v>
+      </c>
+      <c r="S110" s="8">
+        <f>IF(ISNUMBER(MATCH(fields[field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T110">
+        <f>IF(ISNUMBER(MATCH(fields[field],mappings[field],0)),COUNTIF(mappings[field],fields[field]),0)</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="R75" r:id="rId1"/>
+    <hyperlink ref="R79" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -8410,10 +8702,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P148"/>
+  <dimension ref="A1:P156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G109" workbookViewId="0">
-      <selection activeCell="L148" sqref="L148"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="A152" sqref="A152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16380,6 +16672,438 @@
       </c>
       <c r="O148" s="8"/>
       <c r="P148" s="8"/>
+    </row>
+    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>612</v>
+      </c>
+      <c r="B149" t="s">
+        <v>1</v>
+      </c>
+      <c r="C149" t="s">
+        <v>2</v>
+      </c>
+      <c r="D149" t="s">
+        <v>135</v>
+      </c>
+      <c r="E149" s="1">
+        <v>500</v>
+      </c>
+      <c r="F149">
+        <v>3</v>
+      </c>
+      <c r="G149" t="s">
+        <v>6</v>
+      </c>
+      <c r="H149" t="s">
+        <v>5</v>
+      </c>
+      <c r="I149" t="s">
+        <v>6</v>
+      </c>
+      <c r="J149" t="s">
+        <v>6</v>
+      </c>
+      <c r="K149" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>note_display[label]GEN5003.</v>
+      </c>
+      <c r="L149" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M149" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N149" s="8" t="str">
+        <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
+        <v>y</v>
+      </c>
+      <c r="O149" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="P149" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>613</v>
+      </c>
+      <c r="B150" t="s">
+        <v>1</v>
+      </c>
+      <c r="C150" t="s">
+        <v>2</v>
+      </c>
+      <c r="D150" t="s">
+        <v>135</v>
+      </c>
+      <c r="E150" s="1">
+        <v>500</v>
+      </c>
+      <c r="F150" t="s">
+        <v>7</v>
+      </c>
+      <c r="G150" t="s">
+        <v>6</v>
+      </c>
+      <c r="H150" t="s">
+        <v>5</v>
+      </c>
+      <c r="I150" t="s">
+        <v>6</v>
+      </c>
+      <c r="J150" t="s">
+        <v>6</v>
+      </c>
+      <c r="K150" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>note_display[value]GEN500a.</v>
+      </c>
+      <c r="L150" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M150" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N150" s="8" t="str">
+        <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
+        <v>y</v>
+      </c>
+      <c r="O150" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="P150" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>608</v>
+      </c>
+      <c r="B151" t="s">
+        <v>1</v>
+      </c>
+      <c r="C151" t="s">
+        <v>2</v>
+      </c>
+      <c r="D151" t="s">
+        <v>135</v>
+      </c>
+      <c r="E151" s="1">
+        <v>500</v>
+      </c>
+      <c r="F151" t="s">
+        <v>7</v>
+      </c>
+      <c r="G151" t="s">
+        <v>6</v>
+      </c>
+      <c r="H151" t="s">
+        <v>5</v>
+      </c>
+      <c r="I151" t="s">
+        <v>6</v>
+      </c>
+      <c r="J151" t="s">
+        <v>6</v>
+      </c>
+      <c r="K151" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>note_indexGEN500a.</v>
+      </c>
+      <c r="L151" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M151" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N151" s="8" t="str">
+        <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
+        <v>y</v>
+      </c>
+      <c r="O151" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="P151" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>613</v>
+      </c>
+      <c r="B152" t="s">
+        <v>1</v>
+      </c>
+      <c r="C152" t="s">
+        <v>2</v>
+      </c>
+      <c r="D152" t="s">
+        <v>135</v>
+      </c>
+      <c r="E152" s="1">
+        <v>541</v>
+      </c>
+      <c r="F152" t="s">
+        <v>616</v>
+      </c>
+      <c r="G152" t="s">
+        <v>6</v>
+      </c>
+      <c r="H152" t="s">
+        <v>20</v>
+      </c>
+      <c r="I152" t="s">
+        <v>617</v>
+      </c>
+      <c r="J152" t="s">
+        <v>6</v>
+      </c>
+      <c r="K152" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>note_display[value]GEN541abcdefhno3.</v>
+      </c>
+      <c r="L152" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M152" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N152" s="8" t="str">
+        <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
+        <v>y</v>
+      </c>
+      <c r="O152" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="P152" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>608</v>
+      </c>
+      <c r="B153" t="s">
+        <v>1</v>
+      </c>
+      <c r="C153" t="s">
+        <v>2</v>
+      </c>
+      <c r="D153" t="s">
+        <v>135</v>
+      </c>
+      <c r="E153" s="1">
+        <v>541</v>
+      </c>
+      <c r="F153" t="s">
+        <v>7</v>
+      </c>
+      <c r="G153" t="s">
+        <v>6</v>
+      </c>
+      <c r="H153" t="s">
+        <v>5</v>
+      </c>
+      <c r="I153" t="s">
+        <v>6</v>
+      </c>
+      <c r="J153" t="s">
+        <v>6</v>
+      </c>
+      <c r="K153" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>note_indexGEN541a.</v>
+      </c>
+      <c r="L153" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M153" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N153" s="8" t="str">
+        <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
+        <v>y</v>
+      </c>
+      <c r="O153" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="P153" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>612</v>
+      </c>
+      <c r="B154" t="s">
+        <v>1</v>
+      </c>
+      <c r="C154" t="s">
+        <v>2</v>
+      </c>
+      <c r="D154" t="s">
+        <v>135</v>
+      </c>
+      <c r="E154" s="1">
+        <v>561</v>
+      </c>
+      <c r="F154">
+        <v>3</v>
+      </c>
+      <c r="G154" t="s">
+        <v>618</v>
+      </c>
+      <c r="H154" t="s">
+        <v>5</v>
+      </c>
+      <c r="I154" t="s">
+        <v>6</v>
+      </c>
+      <c r="J154" t="s">
+        <v>6</v>
+      </c>
+      <c r="K154" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>note_display[label]GEN5613ind1 != 0</v>
+      </c>
+      <c r="L154" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M154" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N154" s="8" t="str">
+        <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
+        <v>y</v>
+      </c>
+      <c r="O154" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="P154" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>613</v>
+      </c>
+      <c r="B155" t="s">
+        <v>1</v>
+      </c>
+      <c r="C155" t="s">
+        <v>2</v>
+      </c>
+      <c r="D155" t="s">
+        <v>135</v>
+      </c>
+      <c r="E155" s="1">
+        <v>561</v>
+      </c>
+      <c r="F155" t="s">
+        <v>7</v>
+      </c>
+      <c r="G155" t="s">
+        <v>618</v>
+      </c>
+      <c r="H155" t="s">
+        <v>5</v>
+      </c>
+      <c r="I155" t="s">
+        <v>6</v>
+      </c>
+      <c r="J155" t="s">
+        <v>6</v>
+      </c>
+      <c r="K155" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>note_display[value]GEN561aind1 != 0</v>
+      </c>
+      <c r="L155" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M155" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N155" s="8" t="str">
+        <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
+        <v>y</v>
+      </c>
+      <c r="O155" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="P155" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>608</v>
+      </c>
+      <c r="B156" t="s">
+        <v>1</v>
+      </c>
+      <c r="C156" t="s">
+        <v>2</v>
+      </c>
+      <c r="D156" t="s">
+        <v>135</v>
+      </c>
+      <c r="E156" s="1">
+        <v>561</v>
+      </c>
+      <c r="F156" t="s">
+        <v>7</v>
+      </c>
+      <c r="G156" t="s">
+        <v>618</v>
+      </c>
+      <c r="H156" t="s">
+        <v>5</v>
+      </c>
+      <c r="I156" t="s">
+        <v>6</v>
+      </c>
+      <c r="J156" t="s">
+        <v>6</v>
+      </c>
+      <c r="K156" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>note_indexGEN561aind1 != 0</v>
+      </c>
+      <c r="L156" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M156" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N156" s="8" t="str">
+        <f>IF(ISNUMBER(MATCH(mappings[field],fields[field],0)),"y","n")</f>
+        <v>y</v>
+      </c>
+      <c r="O156" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="P156" s="8" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K3:K67">

</xml_diff>

<commit_message>
074 -> misc_ids mappings in spreadsheet
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8841" uniqueCount="1274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8877" uniqueCount="1276">
   <si>
     <t>subject_chronological_facet</t>
   </si>
@@ -3849,6 +3849,12 @@
   </si>
   <si>
     <t>"type":"CODEN designation (canceled or invalid)"</t>
+  </si>
+  <si>
+    <t>"type":"GPO Item Number"</t>
+  </si>
+  <si>
+    <t>"type":"GPO Item Number (canceled or invalid)"</t>
   </si>
 </sst>
 </file>
@@ -4303,12 +4309,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="mappings" displayName="mappings" ref="A1:Q359" totalsRowShown="0">
-  <autoFilter ref="A1:Q359"/>
-  <sortState ref="A2:Q359">
-    <sortCondition ref="A2:A359"/>
-    <sortCondition ref="F2:F359"/>
-    <sortCondition ref="B2:B359"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="mappings" displayName="mappings" ref="A1:Q362" totalsRowShown="0">
+  <autoFilter ref="A1:Q362">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="misc_id"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState ref="A84:Q362">
+    <sortCondition ref="A2:A362"/>
+    <sortCondition ref="F2:F362"/>
+    <sortCondition ref="B2:B362"/>
   </sortState>
   <tableColumns count="17">
     <tableColumn id="17" name="parentfield"/>
@@ -11524,7 +11536,7 @@
       </c>
       <c r="Y82">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="Z82" t="s">
         <v>6</v>
@@ -11609,7 +11621,7 @@
       </c>
       <c r="Y83">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Z83" t="s">
         <v>6</v>
@@ -20476,9 +20488,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q359"/>
+  <dimension ref="A1:Q362"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D105" workbookViewId="0">
+      <selection activeCell="J362" sqref="A1:Q362"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -20542,7 +20556,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>213</v>
       </c>
@@ -20599,7 +20613,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>213</v>
       </c>
@@ -20656,7 +20670,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>213</v>
       </c>
@@ -20713,7 +20727,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>213</v>
       </c>
@@ -20770,7 +20784,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>213</v>
       </c>
@@ -20827,7 +20841,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>213</v>
       </c>
@@ -20884,7 +20898,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>213</v>
       </c>
@@ -20941,7 +20955,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>458</v>
       </c>
@@ -20998,7 +21012,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>458</v>
       </c>
@@ -21055,7 +21069,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>458</v>
       </c>
@@ -21112,7 +21126,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>458</v>
       </c>
@@ -21169,7 +21183,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>458</v>
       </c>
@@ -21226,7 +21240,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>458</v>
       </c>
@@ -21283,7 +21297,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>490</v>
       </c>
@@ -21336,7 +21350,7 @@
       <c r="P15" s="8"/>
       <c r="Q15" s="20"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -21393,7 +21407,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -21450,7 +21464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -21507,7 +21521,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -21564,7 +21578,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>502</v>
       </c>
@@ -21617,7 +21631,7 @@
       <c r="P20" s="8"/>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1040</v>
       </c>
@@ -21664,7 +21678,7 @@
       <c r="P21" s="8"/>
       <c r="Q21" s="8"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>1041</v>
       </c>
@@ -21711,7 +21725,7 @@
       <c r="P22" s="8"/>
       <c r="Q22" s="8"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1042</v>
       </c>
@@ -21758,7 +21772,7 @@
       <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1043</v>
       </c>
@@ -21805,7 +21819,7 @@
       <c r="P24" s="8"/>
       <c r="Q24" s="8"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>207</v>
       </c>
@@ -21862,7 +21876,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>207</v>
       </c>
@@ -21919,7 +21933,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>207</v>
       </c>
@@ -21976,7 +21990,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>842</v>
       </c>
@@ -22029,7 +22043,7 @@
       <c r="P28" s="8"/>
       <c r="Q28" s="8"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>208</v>
       </c>
@@ -22086,7 +22100,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>208</v>
       </c>
@@ -22143,7 +22157,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>392</v>
       </c>
@@ -22200,7 +22214,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>392</v>
       </c>
@@ -22257,7 +22271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>455</v>
       </c>
@@ -22295,7 +22309,7 @@
       <c r="P33" s="8"/>
       <c r="Q33" s="8"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>455</v>
       </c>
@@ -22352,7 +22366,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>173</v>
       </c>
@@ -22409,7 +22423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>173</v>
       </c>
@@ -22466,7 +22480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>173</v>
       </c>
@@ -22523,7 +22537,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>173</v>
       </c>
@@ -22577,7 +22591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>173</v>
       </c>
@@ -22634,7 +22648,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>173</v>
       </c>
@@ -22691,7 +22705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>395</v>
       </c>
@@ -22748,7 +22762,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>395</v>
       </c>
@@ -22805,7 +22819,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>395</v>
       </c>
@@ -22862,7 +22876,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>395</v>
       </c>
@@ -22919,7 +22933,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>395</v>
       </c>
@@ -22976,7 +22990,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>395</v>
       </c>
@@ -23033,7 +23047,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>395</v>
       </c>
@@ -23090,7 +23104,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>395</v>
       </c>
@@ -23147,7 +23161,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>395</v>
       </c>
@@ -23204,7 +23218,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>396</v>
       </c>
@@ -23261,7 +23275,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>396</v>
       </c>
@@ -23318,7 +23332,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>396</v>
       </c>
@@ -23375,7 +23389,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>396</v>
       </c>
@@ -23432,7 +23446,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>396</v>
       </c>
@@ -23489,7 +23503,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>396</v>
       </c>
@@ -23546,7 +23560,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>396</v>
       </c>
@@ -23603,7 +23617,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>396</v>
       </c>
@@ -23660,7 +23674,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>396</v>
       </c>
@@ -23717,7 +23731,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>396</v>
       </c>
@@ -23774,7 +23788,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>329</v>
       </c>
@@ -23824,7 +23838,7 @@
       <c r="P60" s="8"/>
       <c r="Q60" s="8"/>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>329</v>
       </c>
@@ -23877,7 +23891,7 @@
       <c r="P61" s="8"/>
       <c r="Q61" s="8"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>329</v>
       </c>
@@ -23930,7 +23944,7 @@
       <c r="P62" s="8"/>
       <c r="Q62" s="8"/>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>1165</v>
       </c>
@@ -23983,7 +23997,7 @@
       <c r="P63" s="8"/>
       <c r="Q63" s="8"/>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>871</v>
       </c>
@@ -24040,7 +24054,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>871</v>
       </c>
@@ -24097,7 +24111,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>871</v>
       </c>
@@ -24154,7 +24168,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>871</v>
       </c>
@@ -24211,7 +24225,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>871</v>
       </c>
@@ -24268,7 +24282,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>1168</v>
       </c>
@@ -24321,7 +24335,7 @@
       <c r="P69" s="8"/>
       <c r="Q69" s="8"/>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>167</v>
       </c>
@@ -24378,7 +24392,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>167</v>
       </c>
@@ -24435,7 +24449,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>167</v>
       </c>
@@ -24492,7 +24506,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>167</v>
       </c>
@@ -24549,7 +24563,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>167</v>
       </c>
@@ -24606,7 +24620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>167</v>
       </c>
@@ -24663,7 +24677,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>167</v>
       </c>
@@ -24720,7 +24734,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>167</v>
       </c>
@@ -24777,7 +24791,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>167</v>
       </c>
@@ -24834,7 +24848,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>167</v>
       </c>
@@ -24891,7 +24905,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>167</v>
       </c>
@@ -24948,7 +24962,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>167</v>
       </c>
@@ -25005,7 +25019,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>167</v>
       </c>
@@ -25062,7 +25076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>290</v>
       </c>
@@ -27335,7 +27349,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>1044</v>
       </c>
@@ -27392,7 +27406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>514</v>
       </c>
@@ -27449,7 +27463,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>726</v>
       </c>
@@ -27502,7 +27516,7 @@
       <c r="P125" s="8"/>
       <c r="Q125" s="8"/>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>1107</v>
       </c>
@@ -27555,7 +27569,7 @@
       <c r="P126" s="8"/>
       <c r="Q126" s="8"/>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>1107</v>
       </c>
@@ -27608,7 +27622,7 @@
       <c r="P127" s="8"/>
       <c r="Q127" s="8"/>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>389</v>
       </c>
@@ -27661,7 +27675,7 @@
       <c r="P128" s="8"/>
       <c r="Q128" s="8"/>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>1113</v>
       </c>
@@ -27714,7 +27728,7 @@
       <c r="P129" s="8"/>
       <c r="Q129" s="8"/>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>1065</v>
       </c>
@@ -27771,7 +27785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>1148</v>
       </c>
@@ -27828,7 +27842,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>1148</v>
       </c>
@@ -27885,7 +27899,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>1148</v>
       </c>
@@ -27942,7 +27956,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>1148</v>
       </c>
@@ -27999,7 +28013,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>978</v>
       </c>
@@ -28056,7 +28070,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>1103</v>
       </c>
@@ -28109,7 +28123,7 @@
       <c r="P136" s="8"/>
       <c r="Q136" s="8"/>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>1179</v>
       </c>
@@ -28162,7 +28176,7 @@
       <c r="P137" s="8"/>
       <c r="Q137" s="8"/>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>954</v>
       </c>
@@ -28219,7 +28233,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>954</v>
       </c>
@@ -28276,7 +28290,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>954</v>
       </c>
@@ -28333,7 +28347,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>954</v>
       </c>
@@ -28390,7 +28404,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>954</v>
       </c>
@@ -28443,7 +28457,7 @@
       <c r="P142" s="8"/>
       <c r="Q142" s="8"/>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>954</v>
       </c>
@@ -28496,7 +28510,7 @@
       <c r="P143" s="8"/>
       <c r="Q143" s="8"/>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>954</v>
       </c>
@@ -28549,7 +28563,7 @@
       <c r="P144" s="8"/>
       <c r="Q144" s="8"/>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>954</v>
       </c>
@@ -28602,7 +28616,7 @@
       <c r="P145" s="8"/>
       <c r="Q145" s="8"/>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>954</v>
       </c>
@@ -28655,7 +28669,7 @@
       <c r="P146" s="8"/>
       <c r="Q146" s="8"/>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>954</v>
       </c>
@@ -28708,7 +28722,7 @@
       <c r="P147" s="8"/>
       <c r="Q147" s="8"/>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>954</v>
       </c>
@@ -28761,7 +28775,7 @@
       <c r="P148" s="8"/>
       <c r="Q148" s="8"/>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>954</v>
       </c>
@@ -28814,7 +28828,7 @@
       <c r="P149" s="8"/>
       <c r="Q149" s="8"/>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>954</v>
       </c>
@@ -28867,7 +28881,7 @@
       <c r="P150" s="8"/>
       <c r="Q150" s="8"/>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>954</v>
       </c>
@@ -28920,7 +28934,7 @@
       <c r="P151" s="8"/>
       <c r="Q151" s="8"/>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>954</v>
       </c>
@@ -28973,7 +28987,7 @@
       <c r="P152" s="8"/>
       <c r="Q152" s="8"/>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>954</v>
       </c>
@@ -29026,7 +29040,7 @@
       <c r="P153" s="8"/>
       <c r="Q153" s="8"/>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>954</v>
       </c>
@@ -29079,7 +29093,7 @@
       <c r="P154" s="8"/>
       <c r="Q154" s="8"/>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>954</v>
       </c>
@@ -29132,7 +29146,7 @@
       <c r="P155" s="8"/>
       <c r="Q155" s="8"/>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>954</v>
       </c>
@@ -29185,7 +29199,7 @@
       <c r="P156" s="8"/>
       <c r="Q156" s="8"/>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>954</v>
       </c>
@@ -29238,7 +29252,7 @@
       <c r="P157" s="8"/>
       <c r="Q157" s="8"/>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>954</v>
       </c>
@@ -29291,7 +29305,7 @@
       <c r="P158" s="8"/>
       <c r="Q158" s="8"/>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>954</v>
       </c>
@@ -29344,7 +29358,7 @@
       <c r="P159" s="8"/>
       <c r="Q159" s="8"/>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>954</v>
       </c>
@@ -29397,7 +29411,7 @@
       <c r="P160" s="8"/>
       <c r="Q160" s="8"/>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>954</v>
       </c>
@@ -29450,7 +29464,7 @@
       <c r="P161" s="8"/>
       <c r="Q161" s="8"/>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>954</v>
       </c>
@@ -29503,7 +29517,7 @@
       <c r="P162" s="8"/>
       <c r="Q162" s="8"/>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>954</v>
       </c>
@@ -29556,7 +29570,7 @@
       <c r="P163" s="8"/>
       <c r="Q163" s="8"/>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>954</v>
       </c>
@@ -29603,7 +29617,7 @@
       <c r="P164" s="8"/>
       <c r="Q164" s="8"/>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>954</v>
       </c>
@@ -29656,7 +29670,7 @@
       <c r="P165" s="8"/>
       <c r="Q165" s="8"/>
     </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>954</v>
       </c>
@@ -29709,7 +29723,7 @@
       <c r="P166" s="8"/>
       <c r="Q166" s="8"/>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>954</v>
       </c>
@@ -29762,7 +29776,7 @@
       <c r="P167" s="8"/>
       <c r="Q167" s="8"/>
     </row>
-    <row r="168" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>954</v>
       </c>
@@ -29815,7 +29829,7 @@
       <c r="P168" s="8"/>
       <c r="Q168" s="8"/>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>506</v>
       </c>
@@ -29872,7 +29886,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>506</v>
       </c>
@@ -29925,7 +29939,7 @@
       <c r="P170" s="8"/>
       <c r="Q170" s="8"/>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>506</v>
       </c>
@@ -29982,7 +29996,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>506</v>
       </c>
@@ -30039,7 +30053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>495</v>
       </c>
@@ -30092,7 +30106,7 @@
       <c r="P173" s="8"/>
       <c r="Q173" s="8"/>
     </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>1006</v>
       </c>
@@ -30149,7 +30163,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>1006</v>
       </c>
@@ -30206,7 +30220,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>1006</v>
       </c>
@@ -30263,7 +30277,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>1006</v>
       </c>
@@ -30316,7 +30330,7 @@
       <c r="P177" s="8"/>
       <c r="Q177" s="8"/>
     </row>
-    <row r="178" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>1006</v>
       </c>
@@ -30373,7 +30387,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="179" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>1006</v>
       </c>
@@ -30426,7 +30440,7 @@
       <c r="P179" s="8"/>
       <c r="Q179" s="8"/>
     </row>
-    <row r="180" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>1006</v>
       </c>
@@ -30476,7 +30490,7 @@
       <c r="P180" s="8"/>
       <c r="Q180" s="8"/>
     </row>
-    <row r="181" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>1006</v>
       </c>
@@ -30533,7 +30547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="182" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>1006</v>
       </c>
@@ -30590,7 +30604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="183" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>1171</v>
       </c>
@@ -30643,7 +30657,7 @@
       <c r="P183" s="8"/>
       <c r="Q183" s="8"/>
     </row>
-    <row r="184" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>1068</v>
       </c>
@@ -30700,7 +30714,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="185" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>1033</v>
       </c>
@@ -30757,7 +30771,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="186" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>982</v>
       </c>
@@ -30814,7 +30828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>982</v>
       </c>
@@ -30871,7 +30885,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>993</v>
       </c>
@@ -30928,7 +30942,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>1071</v>
       </c>
@@ -30981,7 +30995,7 @@
       <c r="P189" s="8"/>
       <c r="Q189" s="8"/>
     </row>
-    <row r="190" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>1071</v>
       </c>
@@ -31034,7 +31048,7 @@
       <c r="P190" s="8"/>
       <c r="Q190" s="8"/>
     </row>
-    <row r="191" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>1071</v>
       </c>
@@ -31087,7 +31101,7 @@
       <c r="P191" s="8"/>
       <c r="Q191" s="8"/>
     </row>
-    <row r="192" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>1071</v>
       </c>
@@ -31140,7 +31154,7 @@
       <c r="P192" s="8"/>
       <c r="Q192" s="8"/>
     </row>
-    <row r="193" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>1071</v>
       </c>
@@ -31193,7 +31207,7 @@
       <c r="P193" s="8"/>
       <c r="Q193" s="8"/>
     </row>
-    <row r="194" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>1071</v>
       </c>
@@ -31246,7 +31260,7 @@
       <c r="P194" s="8"/>
       <c r="Q194" s="8"/>
     </row>
-    <row r="195" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>1071</v>
       </c>
@@ -31299,7 +31313,7 @@
       <c r="P195" s="8"/>
       <c r="Q195" s="8"/>
     </row>
-    <row r="196" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>1071</v>
       </c>
@@ -31352,7 +31366,7 @@
       <c r="P196" s="8"/>
       <c r="Q196" s="8"/>
     </row>
-    <row r="197" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>1071</v>
       </c>
@@ -31405,7 +31419,7 @@
       <c r="P197" s="8"/>
       <c r="Q197" s="8"/>
     </row>
-    <row r="198" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>1071</v>
       </c>
@@ -31458,7 +31472,7 @@
       <c r="P198" s="8"/>
       <c r="Q198" s="8"/>
     </row>
-    <row r="199" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>1071</v>
       </c>
@@ -31511,7 +31525,7 @@
       <c r="P199" s="8"/>
       <c r="Q199" s="8"/>
     </row>
-    <row r="200" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>1071</v>
       </c>
@@ -31564,7 +31578,7 @@
       <c r="P200" s="8"/>
       <c r="Q200" s="8"/>
     </row>
-    <row r="201" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>1071</v>
       </c>
@@ -31617,7 +31631,7 @@
       <c r="P201" s="8"/>
       <c r="Q201" s="8"/>
     </row>
-    <row r="202" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>1071</v>
       </c>
@@ -31670,7 +31684,7 @@
       <c r="P202" s="8"/>
       <c r="Q202" s="8"/>
     </row>
-    <row r="203" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>1071</v>
       </c>
@@ -31723,7 +31737,7 @@
       <c r="P203" s="8"/>
       <c r="Q203" s="8"/>
     </row>
-    <row r="204" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>1071</v>
       </c>
@@ -31776,7 +31790,7 @@
       <c r="P204" s="8"/>
       <c r="Q204" s="8"/>
     </row>
-    <row r="205" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>1001</v>
       </c>
@@ -31833,7 +31847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="206" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>998</v>
       </c>
@@ -31890,7 +31904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="207" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>1127</v>
       </c>
@@ -31943,7 +31957,7 @@
       <c r="P207" s="8"/>
       <c r="Q207" s="8"/>
     </row>
-    <row r="208" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>1127</v>
       </c>
@@ -31996,7 +32010,7 @@
       <c r="P208" s="8"/>
       <c r="Q208" s="8"/>
     </row>
-    <row r="209" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>1127</v>
       </c>
@@ -32049,7 +32063,7 @@
       <c r="P209" s="8"/>
       <c r="Q209" s="8"/>
     </row>
-    <row r="210" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>1127</v>
       </c>
@@ -32102,7 +32116,7 @@
       <c r="P210" s="8"/>
       <c r="Q210" s="8"/>
     </row>
-    <row r="211" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>1127</v>
       </c>
@@ -32155,7 +32169,7 @@
       <c r="P211" s="8"/>
       <c r="Q211" s="8"/>
     </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>1127</v>
       </c>
@@ -32208,7 +32222,7 @@
       <c r="P212" s="8"/>
       <c r="Q212" s="8"/>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>1127</v>
       </c>
@@ -32261,7 +32275,7 @@
       <c r="P213" s="8"/>
       <c r="Q213" s="8"/>
     </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>1127</v>
       </c>
@@ -32314,7 +32328,7 @@
       <c r="P214" s="8"/>
       <c r="Q214" s="8"/>
     </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>1127</v>
       </c>
@@ -32367,7 +32381,7 @@
       <c r="P215" s="8"/>
       <c r="Q215" s="8"/>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>1127</v>
       </c>
@@ -32420,7 +32434,7 @@
       <c r="P216" s="8"/>
       <c r="Q216" s="8"/>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>1127</v>
       </c>
@@ -32473,7 +32487,7 @@
       <c r="P217" s="8"/>
       <c r="Q217" s="8"/>
     </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>1127</v>
       </c>
@@ -32526,7 +32540,7 @@
       <c r="P218" s="8"/>
       <c r="Q218" s="8"/>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>987</v>
       </c>
@@ -32583,7 +32597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="220" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>987</v>
       </c>
@@ -32640,7 +32654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="221" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>391</v>
       </c>
@@ -32697,7 +32711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="222" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>1124</v>
       </c>
@@ -32750,7 +32764,7 @@
       <c r="P222" s="8"/>
       <c r="Q222" s="8"/>
     </row>
-    <row r="223" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>890</v>
       </c>
@@ -32803,7 +32817,7 @@
       <c r="P223" s="8"/>
       <c r="Q223" s="8"/>
     </row>
-    <row r="224" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>390</v>
       </c>
@@ -32860,7 +32874,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="225" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>976</v>
       </c>
@@ -32917,7 +32931,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="226" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>309</v>
       </c>
@@ -32974,7 +32988,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="227" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>309</v>
       </c>
@@ -33031,7 +33045,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="228" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>309</v>
       </c>
@@ -33088,7 +33102,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="229" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>309</v>
       </c>
@@ -33145,7 +33159,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="230" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>496</v>
       </c>
@@ -33198,7 +33212,7 @@
       <c r="P230" s="8"/>
       <c r="Q230" s="8"/>
     </row>
-    <row r="231" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>398</v>
       </c>
@@ -33255,7 +33269,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="232" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>398</v>
       </c>
@@ -33312,7 +33326,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="233" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>368</v>
       </c>
@@ -33369,7 +33383,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="234" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>815</v>
       </c>
@@ -33423,7 +33437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="235" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>815</v>
       </c>
@@ -33477,7 +33491,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="236" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>815</v>
       </c>
@@ -33531,7 +33545,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="237" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>815</v>
       </c>
@@ -33585,7 +33599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="238" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>815</v>
       </c>
@@ -33639,7 +33653,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="239" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>815</v>
       </c>
@@ -33693,7 +33707,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="240" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>815</v>
       </c>
@@ -33747,7 +33761,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="241" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>815</v>
       </c>
@@ -33801,7 +33815,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="242" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>815</v>
       </c>
@@ -33855,7 +33869,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="243" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>815</v>
       </c>
@@ -33909,7 +33923,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="244" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>815</v>
       </c>
@@ -33963,7 +33977,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="245" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>815</v>
       </c>
@@ -34017,7 +34031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="246" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>815</v>
       </c>
@@ -34074,7 +34088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="247" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>815</v>
       </c>
@@ -34131,7 +34145,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="248" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>815</v>
       </c>
@@ -34188,7 +34202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="249" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>815</v>
       </c>
@@ -34245,7 +34259,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="250" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>815</v>
       </c>
@@ -34302,7 +34316,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="251" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>815</v>
       </c>
@@ -34359,7 +34373,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="252" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>815</v>
       </c>
@@ -34416,7 +34430,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="253" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>815</v>
       </c>
@@ -34473,7 +34487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="254" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>815</v>
       </c>
@@ -34530,7 +34544,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="255" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>358</v>
       </c>
@@ -34587,7 +34601,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="256" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>358</v>
       </c>
@@ -34644,7 +34658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="257" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>795</v>
       </c>
@@ -34701,7 +34715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="258" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>931</v>
       </c>
@@ -34758,7 +34772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="259" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>632</v>
       </c>
@@ -34811,7 +34825,7 @@
       <c r="P259" s="8"/>
       <c r="Q259" s="8"/>
     </row>
-    <row r="260" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>350</v>
       </c>
@@ -34866,7 +34880,7 @@
       </c>
       <c r="Q260" s="8"/>
     </row>
-    <row r="261" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>595</v>
       </c>
@@ -34923,7 +34937,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="262" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>595</v>
       </c>
@@ -34980,7 +34994,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="263" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>595</v>
       </c>
@@ -35037,7 +35051,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="264" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>595</v>
       </c>
@@ -35094,7 +35108,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="265" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>595</v>
       </c>
@@ -35151,7 +35165,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="266" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>595</v>
       </c>
@@ -35208,7 +35222,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="267" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>595</v>
       </c>
@@ -35265,7 +35279,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="268" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>595</v>
       </c>
@@ -35322,7 +35336,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="269" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>594</v>
       </c>
@@ -35379,7 +35393,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="270" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>594</v>
       </c>
@@ -35436,7 +35450,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="271" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>594</v>
       </c>
@@ -35493,7 +35507,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="272" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>594</v>
       </c>
@@ -35550,7 +35564,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="273" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>594</v>
       </c>
@@ -35588,7 +35602,7 @@
       <c r="P273" s="8"/>
       <c r="Q273" s="8"/>
     </row>
-    <row r="274" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>594</v>
       </c>
@@ -35645,7 +35659,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="275" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>594</v>
       </c>
@@ -35702,7 +35716,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="276" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>594</v>
       </c>
@@ -35759,7 +35773,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="277" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>594</v>
       </c>
@@ -35816,7 +35830,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="278" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>594</v>
       </c>
@@ -35873,7 +35887,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="279" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>594</v>
       </c>
@@ -35930,7 +35944,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="280" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>594</v>
       </c>
@@ -35987,7 +36001,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="281" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>594</v>
       </c>
@@ -36044,7 +36058,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="282" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>594</v>
       </c>
@@ -36101,7 +36115,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="283" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>594</v>
       </c>
@@ -36158,7 +36172,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="284" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>594</v>
       </c>
@@ -36215,7 +36229,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="285" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>594</v>
       </c>
@@ -36272,7 +36286,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="286" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>594</v>
       </c>
@@ -36329,7 +36343,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="287" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>594</v>
       </c>
@@ -36386,7 +36400,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="288" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>594</v>
       </c>
@@ -36443,7 +36457,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="289" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>594</v>
       </c>
@@ -36500,7 +36514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="290" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>594</v>
       </c>
@@ -36557,7 +36571,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="291" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>594</v>
       </c>
@@ -36614,7 +36628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="292" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>594</v>
       </c>
@@ -36671,7 +36685,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="293" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>594</v>
       </c>
@@ -36728,7 +36742,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="294" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>594</v>
       </c>
@@ -36785,7 +36799,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="295" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>596</v>
       </c>
@@ -36842,7 +36856,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="296" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>596</v>
       </c>
@@ -36899,7 +36913,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="297" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>596</v>
       </c>
@@ -36956,7 +36970,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="298" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>596</v>
       </c>
@@ -37013,7 +37027,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="299" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>596</v>
       </c>
@@ -37070,7 +37084,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="300" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>596</v>
       </c>
@@ -37127,7 +37141,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="301" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>596</v>
       </c>
@@ -37184,7 +37198,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="302" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>596</v>
       </c>
@@ -37241,7 +37255,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="303" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>593</v>
       </c>
@@ -37298,7 +37312,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="304" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>593</v>
       </c>
@@ -37355,7 +37369,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="305" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>593</v>
       </c>
@@ -37412,7 +37426,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="306" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>593</v>
       </c>
@@ -37469,7 +37483,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="307" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>593</v>
       </c>
@@ -37526,7 +37540,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="308" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>593</v>
       </c>
@@ -37583,7 +37597,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="309" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>593</v>
       </c>
@@ -37640,7 +37654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="310" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>593</v>
       </c>
@@ -37697,7 +37711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="311" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>593</v>
       </c>
@@ -37754,7 +37768,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="312" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>593</v>
       </c>
@@ -37811,7 +37825,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="313" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>593</v>
       </c>
@@ -37868,7 +37882,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="314" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>593</v>
       </c>
@@ -37925,7 +37939,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="315" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>593</v>
       </c>
@@ -37982,7 +37996,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="316" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>593</v>
       </c>
@@ -38039,7 +38053,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="317" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>593</v>
       </c>
@@ -38096,7 +38110,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="318" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>593</v>
       </c>
@@ -38153,7 +38167,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="319" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>593</v>
       </c>
@@ -38210,7 +38224,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="320" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>593</v>
       </c>
@@ -38267,7 +38281,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="321" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>593</v>
       </c>
@@ -38324,7 +38338,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="322" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>901</v>
       </c>
@@ -38366,7 +38380,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="323" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>797</v>
       </c>
@@ -38413,7 +38427,7 @@
       <c r="P323" s="8"/>
       <c r="Q323" s="8"/>
     </row>
-    <row r="324" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>797</v>
       </c>
@@ -38460,7 +38474,7 @@
       <c r="P324" s="8"/>
       <c r="Q324" s="8"/>
     </row>
-    <row r="325" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>797</v>
       </c>
@@ -38507,7 +38521,7 @@
       <c r="P325" s="8"/>
       <c r="Q325" s="8"/>
     </row>
-    <row r="326" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>797</v>
       </c>
@@ -38554,7 +38568,7 @@
       <c r="P326" s="8"/>
       <c r="Q326" s="8"/>
     </row>
-    <row r="327" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>797</v>
       </c>
@@ -38601,7 +38615,7 @@
       <c r="P327" s="8"/>
       <c r="Q327" s="8"/>
     </row>
-    <row r="328" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>797</v>
       </c>
@@ -38648,7 +38662,7 @@
       <c r="P328" s="8"/>
       <c r="Q328" s="8"/>
     </row>
-    <row r="329" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>900</v>
       </c>
@@ -38690,7 +38704,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="330" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>214</v>
       </c>
@@ -38743,7 +38757,7 @@
       <c r="P330" s="8"/>
       <c r="Q330" s="8"/>
     </row>
-    <row r="331" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>214</v>
       </c>
@@ -38796,7 +38810,7 @@
       <c r="P331" s="8"/>
       <c r="Q331" s="8"/>
     </row>
-    <row r="332" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>1183</v>
       </c>
@@ -38853,7 +38867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="333" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>1183</v>
       </c>
@@ -38910,7 +38924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="334" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>1183</v>
       </c>
@@ -38967,7 +38981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="335" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>1183</v>
       </c>
@@ -39024,7 +39038,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="336" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>1183</v>
       </c>
@@ -39081,7 +39095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="337" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>1183</v>
       </c>
@@ -39138,7 +39152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="338" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>1183</v>
       </c>
@@ -39195,7 +39209,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="339" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>1183</v>
       </c>
@@ -39252,7 +39266,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="340" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>1183</v>
       </c>
@@ -39309,7 +39323,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="341" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>1183</v>
       </c>
@@ -39366,7 +39380,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="342" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>1183</v>
       </c>
@@ -39423,7 +39437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="343" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>1183</v>
       </c>
@@ -39480,7 +39494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="344" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>1183</v>
       </c>
@@ -39537,7 +39551,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="345" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>1183</v>
       </c>
@@ -39594,7 +39608,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="346" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>1183</v>
       </c>
@@ -39651,7 +39665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="347" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>1183</v>
       </c>
@@ -39708,7 +39722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="348" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>1183</v>
       </c>
@@ -39765,7 +39779,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="349" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>1183</v>
       </c>
@@ -39822,7 +39836,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="350" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>1183</v>
       </c>
@@ -39879,7 +39893,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="351" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>1183</v>
       </c>
@@ -39936,7 +39950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="352" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>322</v>
       </c>
@@ -39989,7 +40003,7 @@
       <c r="P352" s="8"/>
       <c r="Q352" s="8"/>
     </row>
-    <row r="353" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>322</v>
       </c>
@@ -40042,7 +40056,7 @@
       <c r="P353" s="8"/>
       <c r="Q353" s="8"/>
     </row>
-    <row r="354" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>322</v>
       </c>
@@ -40095,7 +40109,7 @@
       <c r="P354" s="8"/>
       <c r="Q354" s="8"/>
     </row>
-    <row r="355" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>336</v>
       </c>
@@ -40152,7 +40166,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="356" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>946</v>
       </c>
@@ -40209,7 +40223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="357" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>946</v>
       </c>
@@ -40266,7 +40280,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="358" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>946</v>
       </c>
@@ -40323,7 +40337,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="359" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>946</v>
       </c>
@@ -40377,6 +40391,177 @@
         <v>2</v>
       </c>
       <c r="Q359" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="360" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>337</v>
+      </c>
+      <c r="B360" t="s">
+        <v>447</v>
+      </c>
+      <c r="C360" t="s">
+        <v>1</v>
+      </c>
+      <c r="D360" t="s">
+        <v>2</v>
+      </c>
+      <c r="E360" t="s">
+        <v>118</v>
+      </c>
+      <c r="F360" s="1">
+        <v>74</v>
+      </c>
+      <c r="G360" t="s">
+        <v>1078</v>
+      </c>
+      <c r="H360" t="s">
+        <v>1253</v>
+      </c>
+      <c r="I360" t="s">
+        <v>289</v>
+      </c>
+      <c r="J360" t="s">
+        <v>1274</v>
+      </c>
+      <c r="K360" s="10" t="s">
+        <v>714</v>
+      </c>
+      <c r="L360" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>misc_id[type]GEN74{na}value is from $a</v>
+      </c>
+      <c r="M360" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N360" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O360" s="8" t="str">
+        <f>IF(ISNUMBER(MATCH(mappings[field],fields[argot_field],0)),"y","n")</f>
+        <v>y</v>
+      </c>
+      <c r="P360" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q360" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="361" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>337</v>
+      </c>
+      <c r="B361" t="s">
+        <v>447</v>
+      </c>
+      <c r="C361" t="s">
+        <v>1</v>
+      </c>
+      <c r="D361" t="s">
+        <v>2</v>
+      </c>
+      <c r="E361" t="s">
+        <v>118</v>
+      </c>
+      <c r="F361" s="1">
+        <v>74</v>
+      </c>
+      <c r="G361" t="s">
+        <v>1078</v>
+      </c>
+      <c r="H361" t="s">
+        <v>1254</v>
+      </c>
+      <c r="I361" t="s">
+        <v>289</v>
+      </c>
+      <c r="J361" t="s">
+        <v>1275</v>
+      </c>
+      <c r="K361" s="10" t="s">
+        <v>714</v>
+      </c>
+      <c r="L361" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>misc_id[type]GEN74{na}value is from $z</v>
+      </c>
+      <c r="M361" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N361" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O361" s="8" t="str">
+        <f>IF(ISNUMBER(MATCH(mappings[field],fields[argot_field],0)),"y","n")</f>
+        <v>y</v>
+      </c>
+      <c r="P361" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q361" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="362" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>337</v>
+      </c>
+      <c r="B362" t="s">
+        <v>448</v>
+      </c>
+      <c r="C362" t="s">
+        <v>1</v>
+      </c>
+      <c r="D362" t="s">
+        <v>2</v>
+      </c>
+      <c r="E362" t="s">
+        <v>118</v>
+      </c>
+      <c r="F362" s="1">
+        <v>74</v>
+      </c>
+      <c r="G362" t="s">
+        <v>488</v>
+      </c>
+      <c r="H362" t="s">
+        <v>670</v>
+      </c>
+      <c r="I362" t="s">
+        <v>5</v>
+      </c>
+      <c r="J362" t="s">
+        <v>40</v>
+      </c>
+      <c r="K362" s="10" t="s">
+        <v>714</v>
+      </c>
+      <c r="L362" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>misc_id[value]GEN74aznone</v>
+      </c>
+      <c r="M362" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N362" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O362" s="8" t="str">
+        <f>IF(ISNUMBER(MATCH(mappings[field],fields[argot_field],0)),"y","n")</f>
+        <v>y</v>
+      </c>
+      <c r="P362" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q362" s="8" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
clarify aspects of 247->title_variant
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="5910" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="5910"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9072" uniqueCount="1305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9109" uniqueCount="1308">
   <si>
     <t>subject_chronological_facet</t>
   </si>
@@ -3942,6 +3942,15 @@
   </si>
   <si>
     <t>$g included if it follows $t and/or $k</t>
+  </si>
+  <si>
+    <t>title_variant[issn]</t>
+  </si>
+  <si>
+    <t>When displayed, prepend ". ISSN:"</t>
+  </si>
+  <si>
+    <t>ISSN for former title</t>
   </si>
 </sst>
 </file>
@@ -4356,8 +4365,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="fields" displayName="fields" ref="A1:AA195" totalsRowShown="0">
-  <autoFilter ref="A1:AA195"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="fields" displayName="fields" ref="A1:AA196" totalsRowShown="0">
+  <autoFilter ref="A1:AA196"/>
+  <sortState ref="A2:AA196">
+    <sortCondition ref="A1:A196"/>
+  </sortState>
   <tableColumns count="27">
     <tableColumn id="2" name="argot_field"/>
     <tableColumn id="9" name="argot-marc processor"/>
@@ -4396,8 +4408,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="mappings" displayName="mappings" ref="A1:Q371" totalsRowShown="0">
-  <autoFilter ref="A1:Q371"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="mappings" displayName="mappings" ref="A1:Q372" totalsRowShown="0">
+  <autoFilter ref="A1:Q372"/>
   <sortState ref="A2:Q371">
     <sortCondition ref="A2:A371"/>
     <sortCondition ref="F2:F371"/>
@@ -4723,11 +4735,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA195"/>
+  <dimension ref="A1:AA196"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A59" sqref="A55:A59"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9285,7 +9297,7 @@
     </row>
     <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>1281</v>
+        <v>1283</v>
       </c>
       <c r="B55" t="s">
         <v>1280</v>
@@ -9309,10 +9321,10 @@
         <v>858</v>
       </c>
       <c r="I55" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J55" t="s">
-        <v>40</v>
+        <v>1294</v>
       </c>
       <c r="K55" t="s">
         <v>40</v>
@@ -9324,22 +9336,22 @@
         <v>40</v>
       </c>
       <c r="N55" t="s">
-        <v>40</v>
+        <v>861</v>
       </c>
       <c r="O55" t="s">
-        <v>6</v>
+        <v>1289</v>
       </c>
       <c r="P55" t="s">
-        <v>1287</v>
+        <v>1290</v>
       </c>
       <c r="Q55" t="s">
-        <v>1288</v>
+        <v>40</v>
       </c>
       <c r="R55" t="s">
         <v>40</v>
       </c>
       <c r="S55" s="9" t="s">
-        <v>40</v>
+        <v>217</v>
       </c>
       <c r="T55" t="s">
         <v>40</v>
@@ -9358,7 +9370,7 @@
     </row>
     <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
-        <v>1282</v>
+        <v>1285</v>
       </c>
       <c r="B56" t="s">
         <v>1280</v>
@@ -9403,7 +9415,7 @@
         <v>6</v>
       </c>
       <c r="P56" t="s">
-        <v>1194</v>
+        <v>1296</v>
       </c>
       <c r="Q56" t="s">
         <v>40</v>
@@ -9431,7 +9443,7 @@
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="B57" t="s">
         <v>1280</v>
@@ -9458,7 +9470,7 @@
         <v>348</v>
       </c>
       <c r="J57" t="s">
-        <v>1294</v>
+        <v>40</v>
       </c>
       <c r="K57" t="s">
         <v>40</v>
@@ -9473,10 +9485,10 @@
         <v>861</v>
       </c>
       <c r="O57" t="s">
-        <v>1289</v>
+        <v>6</v>
       </c>
       <c r="P57" t="s">
-        <v>1290</v>
+        <v>1194</v>
       </c>
       <c r="Q57" t="s">
         <v>40</v>
@@ -9485,7 +9497,7 @@
         <v>40</v>
       </c>
       <c r="S57" s="9" t="s">
-        <v>217</v>
+        <v>40</v>
       </c>
       <c r="T57" t="s">
         <v>40</v>
@@ -9577,7 +9589,7 @@
     </row>
     <row r="59" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
-        <v>1285</v>
+        <v>1281</v>
       </c>
       <c r="B59" t="s">
         <v>1280</v>
@@ -9601,7 +9613,7 @@
         <v>858</v>
       </c>
       <c r="I59" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="J59" t="s">
         <v>40</v>
@@ -9616,16 +9628,16 @@
         <v>40</v>
       </c>
       <c r="N59" t="s">
-        <v>861</v>
+        <v>40</v>
       </c>
       <c r="O59" t="s">
         <v>6</v>
       </c>
       <c r="P59" t="s">
-        <v>1296</v>
+        <v>1287</v>
       </c>
       <c r="Q59" t="s">
-        <v>40</v>
+        <v>1288</v>
       </c>
       <c r="R59" t="s">
         <v>40</v>
@@ -11823,7 +11835,7 @@
     </row>
     <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>446</v>
+        <v>1256</v>
       </c>
       <c r="B86" t="s">
         <v>6</v>
@@ -11862,16 +11874,16 @@
         <v>40</v>
       </c>
       <c r="N86" t="s">
-        <v>715</v>
+        <v>40</v>
       </c>
       <c r="O86" t="s">
-        <v>717</v>
+        <v>6</v>
       </c>
       <c r="P86" t="s">
-        <v>450</v>
+        <v>1257</v>
       </c>
       <c r="Q86" t="s">
-        <v>339</v>
+        <v>40</v>
       </c>
       <c r="R86" t="s">
         <v>40</v>
@@ -11897,7 +11909,7 @@
       </c>
       <c r="Y86">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="Z86" t="s">
         <v>6</v>
@@ -11908,7 +11920,7 @@
     </row>
     <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B87" t="s">
         <v>6</v>
@@ -11932,7 +11944,7 @@
         <v>337</v>
       </c>
       <c r="I87" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J87" t="s">
         <v>40</v>
@@ -11950,13 +11962,13 @@
         <v>715</v>
       </c>
       <c r="O87" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="P87" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Q87" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="R87" t="s">
         <v>40</v>
@@ -11982,7 +11994,7 @@
       </c>
       <c r="Y87">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="Z87" t="s">
         <v>6</v>
@@ -11993,7 +12005,7 @@
     </row>
     <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B88" t="s">
         <v>6</v>
@@ -12020,7 +12032,7 @@
         <v>349</v>
       </c>
       <c r="J88" t="s">
-        <v>526</v>
+        <v>40</v>
       </c>
       <c r="K88" t="s">
         <v>40</v>
@@ -12035,13 +12047,13 @@
         <v>715</v>
       </c>
       <c r="O88" t="s">
-        <v>6</v>
+        <v>718</v>
       </c>
       <c r="P88" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="Q88" t="s">
-        <v>40</v>
+        <v>340</v>
       </c>
       <c r="R88" t="s">
         <v>40</v>
@@ -12067,7 +12079,7 @@
       </c>
       <c r="Y88">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="Z88" t="s">
         <v>6</v>
@@ -12078,7 +12090,7 @@
     </row>
     <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>1256</v>
+        <v>448</v>
       </c>
       <c r="B89" t="s">
         <v>6</v>
@@ -12102,10 +12114,10 @@
         <v>337</v>
       </c>
       <c r="I89" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="J89" t="s">
-        <v>40</v>
+        <v>526</v>
       </c>
       <c r="K89" t="s">
         <v>40</v>
@@ -12117,13 +12129,13 @@
         <v>40</v>
       </c>
       <c r="N89" t="s">
-        <v>40</v>
+        <v>715</v>
       </c>
       <c r="O89" t="s">
         <v>6</v>
       </c>
       <c r="P89" t="s">
-        <v>1257</v>
+        <v>452</v>
       </c>
       <c r="Q89" t="s">
         <v>40</v>
@@ -12152,7 +12164,7 @@
       </c>
       <c r="Y89">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="Z89" t="s">
         <v>6</v>
@@ -19333,7 +19345,7 @@
     </row>
     <row r="177" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>1183</v>
+        <v>1187</v>
       </c>
       <c r="B177" t="s">
         <v>6</v>
@@ -19375,13 +19387,13 @@
         <v>40</v>
       </c>
       <c r="O177" t="s">
-        <v>1192</v>
+        <v>6</v>
       </c>
       <c r="P177" t="s">
-        <v>1193</v>
+        <v>1198</v>
       </c>
       <c r="Q177" t="s">
-        <v>6</v>
+        <v>1199</v>
       </c>
       <c r="R177" t="s">
         <v>40</v>
@@ -19418,7 +19430,7 @@
     </row>
     <row r="178" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>1184</v>
+        <v>1186</v>
       </c>
       <c r="B178" t="s">
         <v>6</v>
@@ -19445,7 +19457,7 @@
         <v>348</v>
       </c>
       <c r="J178" t="s">
-        <v>40</v>
+        <v>525</v>
       </c>
       <c r="K178" t="s">
         <v>40</v>
@@ -19457,19 +19469,19 @@
         <v>40</v>
       </c>
       <c r="N178" t="s">
-        <v>1188</v>
+        <v>40</v>
       </c>
       <c r="O178" t="s">
-        <v>1196</v>
+        <v>6</v>
       </c>
       <c r="P178" t="s">
-        <v>1194</v>
+        <v>1197</v>
       </c>
       <c r="Q178" t="s">
         <v>6</v>
       </c>
       <c r="R178" t="s">
-        <v>40</v>
+        <v>239</v>
       </c>
       <c r="S178" t="s">
         <v>40</v>
@@ -19492,7 +19504,7 @@
       </c>
       <c r="Y178">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Z178" t="s">
         <v>2</v>
@@ -19503,7 +19515,7 @@
     </row>
     <row r="179" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>1185</v>
+        <v>1305</v>
       </c>
       <c r="B179" t="s">
         <v>6</v>
@@ -19527,10 +19539,10 @@
         <v>1182</v>
       </c>
       <c r="I179" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J179" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="K179" t="s">
         <v>40</v>
@@ -19545,16 +19557,16 @@
         <v>1188</v>
       </c>
       <c r="O179" t="s">
-        <v>1196</v>
+        <v>1306</v>
       </c>
       <c r="P179" t="s">
-        <v>1195</v>
+        <v>1307</v>
       </c>
       <c r="Q179" t="s">
         <v>6</v>
       </c>
       <c r="R179" t="s">
-        <v>239</v>
+        <v>40</v>
       </c>
       <c r="S179" t="s">
         <v>40</v>
@@ -19577,7 +19589,7 @@
       </c>
       <c r="Y179">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="Z179" t="s">
         <v>2</v>
@@ -19588,7 +19600,7 @@
     </row>
     <row r="180" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="B180" t="s">
         <v>6</v>
@@ -19615,7 +19627,7 @@
         <v>348</v>
       </c>
       <c r="J180" t="s">
-        <v>525</v>
+        <v>40</v>
       </c>
       <c r="K180" t="s">
         <v>40</v>
@@ -19627,19 +19639,19 @@
         <v>40</v>
       </c>
       <c r="N180" t="s">
-        <v>40</v>
+        <v>1188</v>
       </c>
       <c r="O180" t="s">
-        <v>6</v>
+        <v>1196</v>
       </c>
       <c r="P180" t="s">
-        <v>1197</v>
+        <v>1194</v>
       </c>
       <c r="Q180" t="s">
         <v>6</v>
       </c>
       <c r="R180" t="s">
-        <v>239</v>
+        <v>40</v>
       </c>
       <c r="S180" t="s">
         <v>40</v>
@@ -19662,7 +19674,7 @@
       </c>
       <c r="Y180">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Z180" t="s">
         <v>2</v>
@@ -19673,7 +19685,7 @@
     </row>
     <row r="181" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>1187</v>
+        <v>1183</v>
       </c>
       <c r="B181" t="s">
         <v>6</v>
@@ -19715,13 +19727,13 @@
         <v>40</v>
       </c>
       <c r="O181" t="s">
-        <v>6</v>
+        <v>1192</v>
       </c>
       <c r="P181" t="s">
-        <v>1198</v>
+        <v>1193</v>
       </c>
       <c r="Q181" t="s">
-        <v>1199</v>
+        <v>6</v>
       </c>
       <c r="R181" t="s">
         <v>40</v>
@@ -19758,7 +19770,7 @@
     </row>
     <row r="182" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>322</v>
+        <v>1185</v>
       </c>
       <c r="B182" t="s">
         <v>6</v>
@@ -19770,7 +19782,7 @@
         <v>6</v>
       </c>
       <c r="E182" t="s">
-        <v>310</v>
+        <v>216</v>
       </c>
       <c r="F182" t="s">
         <v>2</v>
@@ -19779,16 +19791,16 @@
         <v>2</v>
       </c>
       <c r="H182" t="s">
-        <v>40</v>
+        <v>1182</v>
       </c>
       <c r="I182" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="J182" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="K182" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="L182" t="s">
         <v>40</v>
@@ -19797,34 +19809,34 @@
         <v>40</v>
       </c>
       <c r="N182" t="s">
-        <v>819</v>
+        <v>1188</v>
       </c>
       <c r="O182" t="s">
-        <v>6</v>
+        <v>1196</v>
       </c>
       <c r="P182" t="s">
-        <v>820</v>
+        <v>1195</v>
       </c>
       <c r="Q182" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="R182" t="s">
-        <v>40</v>
+        <v>239</v>
       </c>
       <c r="S182" t="s">
         <v>40</v>
       </c>
       <c r="T182" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="U182" t="s">
-        <v>6</v>
+        <v>411</v>
       </c>
       <c r="V182" t="s">
-        <v>648</v>
+        <v>1190</v>
       </c>
       <c r="W182" t="s">
-        <v>823</v>
+        <v>1191</v>
       </c>
       <c r="X182" s="8">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
@@ -19832,18 +19844,18 @@
       </c>
       <c r="Y182">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Z182" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AA182" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="183" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>818</v>
+        <v>322</v>
       </c>
       <c r="B183" t="s">
         <v>6</v>
@@ -19864,13 +19876,13 @@
         <v>2</v>
       </c>
       <c r="H183" t="s">
-        <v>322</v>
+        <v>40</v>
       </c>
       <c r="I183" t="s">
         <v>347</v>
       </c>
       <c r="J183" t="s">
-        <v>40</v>
+        <v>526</v>
       </c>
       <c r="K183" t="s">
         <v>3</v>
@@ -19888,10 +19900,10 @@
         <v>6</v>
       </c>
       <c r="P183" t="s">
-        <v>327</v>
+        <v>820</v>
       </c>
       <c r="Q183" t="s">
-        <v>822</v>
+        <v>40</v>
       </c>
       <c r="R183" t="s">
         <v>40</v>
@@ -19903,7 +19915,7 @@
         <v>6</v>
       </c>
       <c r="U183" t="s">
-        <v>328</v>
+        <v>6</v>
       </c>
       <c r="V183" t="s">
         <v>648</v>
@@ -19917,7 +19929,7 @@
       </c>
       <c r="Y183">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z183" t="s">
         <v>6</v>
@@ -19928,7 +19940,7 @@
     </row>
     <row r="184" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="B184" t="s">
         <v>6</v>
@@ -19955,7 +19967,7 @@
         <v>347</v>
       </c>
       <c r="J184" t="s">
-        <v>526</v>
+        <v>40</v>
       </c>
       <c r="K184" t="s">
         <v>3</v>
@@ -19973,22 +19985,22 @@
         <v>6</v>
       </c>
       <c r="P184" t="s">
-        <v>821</v>
+        <v>327</v>
       </c>
       <c r="Q184" t="s">
-        <v>325</v>
+        <v>822</v>
       </c>
       <c r="R184" t="s">
         <v>40</v>
       </c>
       <c r="S184" t="s">
-        <v>326</v>
+        <v>40</v>
       </c>
       <c r="T184" t="s">
         <v>6</v>
       </c>
       <c r="U184" t="s">
-        <v>40</v>
+        <v>328</v>
       </c>
       <c r="V184" t="s">
         <v>648</v>
@@ -20002,7 +20014,7 @@
       </c>
       <c r="Y184">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z184" t="s">
         <v>6</v>
@@ -20013,7 +20025,7 @@
     </row>
     <row r="185" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>379</v>
+        <v>817</v>
       </c>
       <c r="B185" t="s">
         <v>6</v>
@@ -20025,22 +20037,22 @@
         <v>6</v>
       </c>
       <c r="E185" t="s">
-        <v>379</v>
+        <v>310</v>
       </c>
       <c r="F185" t="s">
         <v>2</v>
       </c>
       <c r="G185" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H185" t="s">
-        <v>40</v>
+        <v>322</v>
       </c>
       <c r="I185" t="s">
         <v>347</v>
       </c>
       <c r="J185" t="s">
-        <v>40</v>
+        <v>526</v>
       </c>
       <c r="K185" t="s">
         <v>3</v>
@@ -20049,37 +20061,37 @@
         <v>40</v>
       </c>
       <c r="M185" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="N185" t="s">
-        <v>827</v>
+        <v>819</v>
       </c>
       <c r="O185" t="s">
         <v>6</v>
       </c>
       <c r="P185" t="s">
-        <v>6</v>
+        <v>821</v>
       </c>
       <c r="Q185" t="s">
-        <v>6</v>
+        <v>325</v>
       </c>
       <c r="R185" t="s">
         <v>40</v>
       </c>
       <c r="S185" t="s">
-        <v>380</v>
+        <v>326</v>
       </c>
       <c r="T185" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="U185" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="V185" t="s">
         <v>648</v>
       </c>
       <c r="W185" t="s">
-        <v>6</v>
+        <v>823</v>
       </c>
       <c r="X185" s="8">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
@@ -20087,7 +20099,7 @@
       </c>
       <c r="Y185">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z185" t="s">
         <v>6</v>
@@ -20098,7 +20110,7 @@
     </row>
     <row r="186" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B186" t="s">
         <v>6</v>
@@ -20113,46 +20125,46 @@
         <v>379</v>
       </c>
       <c r="F186" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G186" t="s">
         <v>3</v>
       </c>
       <c r="H186" t="s">
-        <v>379</v>
+        <v>40</v>
       </c>
       <c r="I186" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="J186" t="s">
         <v>40</v>
       </c>
       <c r="K186" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="L186" t="s">
         <v>40</v>
       </c>
       <c r="M186" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="N186" t="s">
-        <v>40</v>
+        <v>827</v>
       </c>
       <c r="O186" t="s">
         <v>6</v>
       </c>
       <c r="P186" t="s">
-        <v>387</v>
+        <v>6</v>
       </c>
       <c r="Q186" t="s">
-        <v>388</v>
+        <v>6</v>
       </c>
       <c r="R186" t="s">
         <v>40</v>
       </c>
       <c r="S186" t="s">
-        <v>40</v>
+        <v>380</v>
       </c>
       <c r="T186" t="s">
         <v>40</v>
@@ -20183,7 +20195,7 @@
     </row>
     <row r="187" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B187" t="s">
         <v>6</v>
@@ -20198,7 +20210,7 @@
         <v>379</v>
       </c>
       <c r="F187" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G187" t="s">
         <v>3</v>
@@ -20219,19 +20231,19 @@
         <v>40</v>
       </c>
       <c r="M187" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="N187" t="s">
-        <v>827</v>
+        <v>40</v>
       </c>
       <c r="O187" t="s">
         <v>6</v>
       </c>
       <c r="P187" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="Q187" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="R187" t="s">
         <v>40</v>
@@ -20268,7 +20280,7 @@
     </row>
     <row r="188" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B188" t="s">
         <v>6</v>
@@ -20304,19 +20316,19 @@
         <v>40</v>
       </c>
       <c r="M188" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="N188" t="s">
-        <v>40</v>
+        <v>827</v>
       </c>
       <c r="O188" t="s">
         <v>6</v>
       </c>
       <c r="P188" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="Q188" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="R188" t="s">
         <v>40</v>
@@ -20353,7 +20365,7 @@
     </row>
     <row r="189" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B189" t="s">
         <v>6</v>
@@ -20389,19 +20401,19 @@
         <v>40</v>
       </c>
       <c r="M189" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="N189" t="s">
-        <v>827</v>
+        <v>40</v>
       </c>
       <c r="O189" t="s">
         <v>6</v>
       </c>
       <c r="P189" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="Q189" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="R189" t="s">
         <v>40</v>
@@ -20438,7 +20450,7 @@
     </row>
     <row r="190" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>352</v>
+        <v>377</v>
       </c>
       <c r="B190" t="s">
         <v>6</v>
@@ -20450,7 +20462,7 @@
         <v>6</v>
       </c>
       <c r="E190" t="s">
-        <v>310</v>
+        <v>379</v>
       </c>
       <c r="F190" t="s">
         <v>2</v>
@@ -20459,13 +20471,13 @@
         <v>3</v>
       </c>
       <c r="H190" t="s">
-        <v>40</v>
+        <v>379</v>
       </c>
       <c r="I190" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="J190" t="s">
-        <v>526</v>
+        <v>40</v>
       </c>
       <c r="K190" t="s">
         <v>40</v>
@@ -20474,22 +20486,22 @@
         <v>40</v>
       </c>
       <c r="M190" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="N190" t="s">
-        <v>40</v>
+        <v>827</v>
       </c>
       <c r="O190" t="s">
-        <v>828</v>
+        <v>6</v>
       </c>
       <c r="P190" t="s">
-        <v>353</v>
+        <v>385</v>
       </c>
       <c r="Q190" t="s">
-        <v>354</v>
+        <v>386</v>
       </c>
       <c r="R190" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="S190" t="s">
         <v>40</v>
@@ -20498,7 +20510,7 @@
         <v>40</v>
       </c>
       <c r="U190" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="V190" t="s">
         <v>648</v>
@@ -20515,7 +20527,7 @@
         <v>0</v>
       </c>
       <c r="Z190" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AA190" t="s">
         <v>6</v>
@@ -20523,7 +20535,7 @@
     </row>
     <row r="191" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>336</v>
+        <v>352</v>
       </c>
       <c r="B191" t="s">
         <v>6</v>
@@ -20535,7 +20547,7 @@
         <v>6</v>
       </c>
       <c r="E191" t="s">
-        <v>399</v>
+        <v>310</v>
       </c>
       <c r="F191" t="s">
         <v>2</v>
@@ -20550,13 +20562,13 @@
         <v>347</v>
       </c>
       <c r="J191" t="s">
-        <v>400</v>
+        <v>526</v>
       </c>
       <c r="K191" t="s">
         <v>40</v>
       </c>
       <c r="L191" t="s">
-        <v>830</v>
+        <v>40</v>
       </c>
       <c r="M191" t="s">
         <v>40</v>
@@ -20565,16 +20577,16 @@
         <v>40</v>
       </c>
       <c r="O191" t="s">
-        <v>40</v>
+        <v>828</v>
       </c>
       <c r="P191" t="s">
-        <v>323</v>
+        <v>353</v>
       </c>
       <c r="Q191" t="s">
-        <v>324</v>
+        <v>354</v>
       </c>
       <c r="R191" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="S191" t="s">
         <v>40</v>
@@ -20589,7 +20601,7 @@
         <v>648</v>
       </c>
       <c r="W191" t="s">
-        <v>829</v>
+        <v>6</v>
       </c>
       <c r="X191" s="8">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
@@ -20597,18 +20609,18 @@
       </c>
       <c r="Y191">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z191" t="s">
         <v>3</v>
       </c>
       <c r="AA191" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="192" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>803</v>
+        <v>336</v>
       </c>
       <c r="B192" t="s">
         <v>6</v>
@@ -20620,61 +20632,61 @@
         <v>6</v>
       </c>
       <c r="E192" t="s">
-        <v>6</v>
+        <v>399</v>
       </c>
       <c r="F192" t="s">
         <v>2</v>
       </c>
       <c r="G192" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H192" t="s">
         <v>40</v>
       </c>
       <c r="I192" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="J192" t="s">
-        <v>946</v>
+        <v>400</v>
       </c>
       <c r="K192" t="s">
         <v>40</v>
       </c>
       <c r="L192" t="s">
-        <v>40</v>
+        <v>830</v>
       </c>
       <c r="M192" t="s">
         <v>40</v>
       </c>
       <c r="N192" t="s">
-        <v>804</v>
+        <v>40</v>
       </c>
       <c r="O192" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="P192" t="s">
-        <v>806</v>
+        <v>323</v>
       </c>
       <c r="Q192" t="s">
-        <v>805</v>
+        <v>324</v>
       </c>
       <c r="R192" t="s">
-        <v>239</v>
+        <v>40</v>
       </c>
       <c r="S192" t="s">
         <v>40</v>
       </c>
       <c r="T192" t="s">
-        <v>241</v>
+        <v>40</v>
       </c>
       <c r="U192" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="V192" t="s">
-        <v>6</v>
+        <v>648</v>
       </c>
       <c r="W192" t="s">
-        <v>6</v>
+        <v>829</v>
       </c>
       <c r="X192" s="8">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
@@ -20682,18 +20694,18 @@
       </c>
       <c r="Y192">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z192" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AA192" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="193" spans="1:25" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="193" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="B193" t="s">
         <v>6</v>
@@ -20705,22 +20717,22 @@
         <v>6</v>
       </c>
       <c r="E193" t="s">
-        <v>212</v>
+        <v>6</v>
       </c>
       <c r="F193" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G193" t="s">
         <v>2</v>
       </c>
       <c r="H193" t="s">
-        <v>803</v>
+        <v>40</v>
       </c>
       <c r="I193" t="s">
         <v>348</v>
       </c>
       <c r="J193" t="s">
-        <v>40</v>
+        <v>946</v>
       </c>
       <c r="K193" t="s">
         <v>40</v>
@@ -20738,28 +20750,28 @@
         <v>6</v>
       </c>
       <c r="P193" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="Q193" t="s">
-        <v>6</v>
+        <v>805</v>
       </c>
       <c r="R193" t="s">
-        <v>40</v>
+        <v>239</v>
       </c>
       <c r="S193" t="s">
         <v>40</v>
       </c>
       <c r="T193" t="s">
-        <v>811</v>
+        <v>241</v>
       </c>
       <c r="U193" t="s">
         <v>6</v>
       </c>
       <c r="V193" t="s">
-        <v>813</v>
+        <v>6</v>
       </c>
       <c r="W193" t="s">
-        <v>814</v>
+        <v>6</v>
       </c>
       <c r="X193" s="8">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
@@ -20769,10 +20781,16 @@
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="194" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z193" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA193" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="194" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B194" t="s">
         <v>6</v>
@@ -20784,7 +20802,7 @@
         <v>6</v>
       </c>
       <c r="E194" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F194" t="s">
         <v>3</v>
@@ -20796,10 +20814,10 @@
         <v>803</v>
       </c>
       <c r="I194" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J194" t="s">
-        <v>525</v>
+        <v>40</v>
       </c>
       <c r="K194" t="s">
         <v>40</v>
@@ -20813,23 +20831,32 @@
       <c r="N194" t="s">
         <v>804</v>
       </c>
+      <c r="O194" t="s">
+        <v>6</v>
+      </c>
       <c r="P194" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="Q194" t="s">
         <v>6</v>
       </c>
       <c r="R194" t="s">
-        <v>239</v>
+        <v>40</v>
       </c>
       <c r="S194" t="s">
-        <v>240</v>
+        <v>40</v>
       </c>
       <c r="T194" t="s">
-        <v>6</v>
+        <v>811</v>
       </c>
       <c r="U194" t="s">
         <v>6</v>
+      </c>
+      <c r="V194" t="s">
+        <v>813</v>
+      </c>
+      <c r="W194" t="s">
+        <v>814</v>
       </c>
       <c r="X194" s="8">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
@@ -20840,9 +20867,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>945</v>
+        <v>808</v>
       </c>
       <c r="B195" t="s">
         <v>6</v>
@@ -20854,7 +20881,7 @@
         <v>6</v>
       </c>
       <c r="E195" t="s">
-        <v>6</v>
+        <v>216</v>
       </c>
       <c r="F195" t="s">
         <v>3</v>
@@ -20863,13 +20890,13 @@
         <v>2</v>
       </c>
       <c r="H195" t="s">
-        <v>40</v>
+        <v>803</v>
       </c>
       <c r="I195" t="s">
         <v>349</v>
       </c>
       <c r="J195" t="s">
-        <v>946</v>
+        <v>525</v>
       </c>
       <c r="K195" t="s">
         <v>40</v>
@@ -20881,40 +20908,110 @@
         <v>40</v>
       </c>
       <c r="N195" t="s">
-        <v>40</v>
-      </c>
-      <c r="O195" t="s">
-        <v>6</v>
+        <v>804</v>
       </c>
       <c r="P195" t="s">
-        <v>947</v>
+        <v>812</v>
       </c>
       <c r="Q195" t="s">
-        <v>948</v>
+        <v>6</v>
       </c>
       <c r="R195" t="s">
         <v>239</v>
       </c>
       <c r="S195" t="s">
-        <v>40</v>
+        <v>240</v>
       </c>
       <c r="T195" t="s">
         <v>6</v>
       </c>
       <c r="U195" t="s">
         <v>6</v>
-      </c>
-      <c r="V195" t="s">
-        <v>813</v>
-      </c>
-      <c r="W195" t="s">
-        <v>949</v>
       </c>
       <c r="X195" s="8">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
         <v>0</v>
       </c>
       <c r="Y195">
+        <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>945</v>
+      </c>
+      <c r="B196" t="s">
+        <v>6</v>
+      </c>
+      <c r="C196" t="s">
+        <v>6</v>
+      </c>
+      <c r="D196" t="s">
+        <v>6</v>
+      </c>
+      <c r="E196" t="s">
+        <v>6</v>
+      </c>
+      <c r="F196" t="s">
+        <v>3</v>
+      </c>
+      <c r="G196" t="s">
+        <v>2</v>
+      </c>
+      <c r="H196" t="s">
+        <v>40</v>
+      </c>
+      <c r="I196" t="s">
+        <v>349</v>
+      </c>
+      <c r="J196" t="s">
+        <v>946</v>
+      </c>
+      <c r="K196" t="s">
+        <v>40</v>
+      </c>
+      <c r="L196" t="s">
+        <v>40</v>
+      </c>
+      <c r="M196" t="s">
+        <v>40</v>
+      </c>
+      <c r="N196" t="s">
+        <v>40</v>
+      </c>
+      <c r="O196" t="s">
+        <v>6</v>
+      </c>
+      <c r="P196" t="s">
+        <v>947</v>
+      </c>
+      <c r="Q196" t="s">
+        <v>948</v>
+      </c>
+      <c r="R196" t="s">
+        <v>239</v>
+      </c>
+      <c r="S196" t="s">
+        <v>40</v>
+      </c>
+      <c r="T196" t="s">
+        <v>6</v>
+      </c>
+      <c r="U196" t="s">
+        <v>6</v>
+      </c>
+      <c r="V196" t="s">
+        <v>813</v>
+      </c>
+      <c r="W196" t="s">
+        <v>949</v>
+      </c>
+      <c r="X196" s="8">
+        <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y196">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
         <v>4</v>
       </c>
@@ -20934,10 +21031,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q371"/>
+  <dimension ref="A1:Q372"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J352" workbookViewId="0">
-      <selection activeCell="Q371" sqref="A1:Q371"/>
+    <sheetView topLeftCell="A339" workbookViewId="0">
+      <selection activeCell="I359" sqref="I359"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40771,7 +40868,7 @@
         <v>1182</v>
       </c>
       <c r="B359" t="s">
-        <v>1184</v>
+        <v>1305</v>
       </c>
       <c r="C359" t="s">
         <v>1</v>
@@ -40786,10 +40883,10 @@
         <v>247</v>
       </c>
       <c r="G359" t="s">
-        <v>203</v>
+        <v>40</v>
       </c>
       <c r="H359" t="s">
-        <v>1203</v>
+        <v>670</v>
       </c>
       <c r="I359" t="s">
         <v>20</v>
@@ -40802,7 +40899,7 @@
       </c>
       <c r="L359" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>title_variant[label]GEN247f[display]!='false'</v>
+        <v>title_variant[issn]GEN247xnone</v>
       </c>
       <c r="M359" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -40843,13 +40940,13 @@
         <v>247</v>
       </c>
       <c r="G360" t="s">
-        <v>1077</v>
+        <v>203</v>
       </c>
       <c r="H360" t="s">
-        <v>1206</v>
+        <v>1203</v>
       </c>
       <c r="I360" t="s">
-        <v>1079</v>
+        <v>20</v>
       </c>
       <c r="J360" t="s">
         <v>411</v>
@@ -40859,7 +40956,7 @@
       </c>
       <c r="L360" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>title_variant[label]GEN247{na}[display]='false'</v>
+        <v>title_variant[label]GEN247f[display]!='false'</v>
       </c>
       <c r="M360" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -40885,7 +40982,7 @@
         <v>1182</v>
       </c>
       <c r="B361" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="C361" t="s">
         <v>1</v>
@@ -40903,20 +41000,20 @@
         <v>1077</v>
       </c>
       <c r="H361" t="s">
-        <v>670</v>
+        <v>1206</v>
       </c>
       <c r="I361" t="s">
-        <v>289</v>
+        <v>1079</v>
       </c>
       <c r="J361" t="s">
-        <v>1214</v>
+        <v>411</v>
       </c>
       <c r="K361" t="s">
         <v>1190</v>
       </c>
       <c r="L361" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>title_variant[type]GEN247{na}none</v>
+        <v>title_variant[label]GEN247{na}[display]='false'</v>
       </c>
       <c r="M361" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -40942,7 +41039,7 @@
         <v>1182</v>
       </c>
       <c r="B362" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="C362" t="s">
         <v>1</v>
@@ -40957,23 +41054,23 @@
         <v>247</v>
       </c>
       <c r="G362" t="s">
-        <v>1215</v>
+        <v>1077</v>
       </c>
       <c r="H362" t="s">
-        <v>1203</v>
+        <v>670</v>
       </c>
       <c r="I362" t="s">
-        <v>20</v>
+        <v>289</v>
       </c>
       <c r="J362" t="s">
-        <v>411</v>
+        <v>1214</v>
       </c>
       <c r="K362" t="s">
         <v>1190</v>
       </c>
       <c r="L362" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>title_variant[value]GEN247abghnp[display]!='false'</v>
+        <v>title_variant[type]GEN247{na}none</v>
       </c>
       <c r="M362" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -41014,10 +41111,10 @@
         <v>247</v>
       </c>
       <c r="G363" t="s">
-        <v>1204</v>
+        <v>1215</v>
       </c>
       <c r="H363" t="s">
-        <v>1206</v>
+        <v>1203</v>
       </c>
       <c r="I363" t="s">
         <v>20</v>
@@ -41030,7 +41127,7 @@
       </c>
       <c r="L363" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>title_variant[value]GEN247abnp[display]='false'</v>
+        <v>title_variant[value]GEN247abghnp[display]!='false'</v>
       </c>
       <c r="M363" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -41053,10 +41150,10 @@
     </row>
     <row r="364" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>322</v>
+        <v>1182</v>
       </c>
       <c r="B364" t="s">
-        <v>818</v>
+        <v>1185</v>
       </c>
       <c r="C364" t="s">
         <v>1</v>
@@ -41068,26 +41165,26 @@
         <v>118</v>
       </c>
       <c r="F364" s="1">
-        <v>24</v>
+        <v>247</v>
       </c>
       <c r="G364" t="s">
-        <v>7</v>
+        <v>1204</v>
       </c>
       <c r="H364" t="s">
-        <v>825</v>
+        <v>1206</v>
       </c>
       <c r="I364" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="J364" t="s">
-        <v>826</v>
+        <v>411</v>
       </c>
       <c r="K364" t="s">
-        <v>6</v>
+        <v>1190</v>
       </c>
       <c r="L364" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>upc[qualifying_info]GEN24ai1=1 and $a data includes parenthetical qualifying info</v>
+        <v>title_variant[value]GEN247abnp[display]='false'</v>
       </c>
       <c r="M364" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -41101,8 +41198,12 @@
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[argot_field],0)),"y","n")</f>
         <v>y</v>
       </c>
-      <c r="P364" s="8"/>
-      <c r="Q364" s="8"/>
+      <c r="P364" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q364" s="8" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="365" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
@@ -41124,23 +41225,23 @@
         <v>24</v>
       </c>
       <c r="G365" t="s">
-        <v>286</v>
+        <v>7</v>
       </c>
       <c r="H365" t="s">
-        <v>299</v>
+        <v>825</v>
       </c>
       <c r="I365" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="J365" t="s">
-        <v>487</v>
+        <v>826</v>
       </c>
       <c r="K365" t="s">
         <v>6</v>
       </c>
       <c r="L365" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>upc[qualifying_info]GEN24qi1=1</v>
+        <v>upc[qualifying_info]GEN24ai1=1 and $a data includes parenthetical qualifying info</v>
       </c>
       <c r="M365" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -41162,7 +41263,7 @@
         <v>322</v>
       </c>
       <c r="B366" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="C366" t="s">
         <v>1</v>
@@ -41177,23 +41278,23 @@
         <v>24</v>
       </c>
       <c r="G366" t="s">
-        <v>7</v>
+        <v>286</v>
       </c>
       <c r="H366" t="s">
         <v>299</v>
       </c>
       <c r="I366" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="J366" t="s">
-        <v>824</v>
+        <v>487</v>
       </c>
       <c r="K366" t="s">
         <v>6</v>
       </c>
       <c r="L366" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>upc[value]GEN24ai1=1</v>
+        <v>upc[qualifying_info]GEN24qi1=1</v>
       </c>
       <c r="M366" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -41212,41 +41313,41 @@
     </row>
     <row r="367" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
       <c r="B367" t="s">
-        <v>336</v>
+        <v>817</v>
       </c>
       <c r="C367" t="s">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="D367" t="s">
         <v>2</v>
       </c>
       <c r="E367" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="F367" s="1">
-        <v>919</v>
+        <v>24</v>
       </c>
       <c r="G367" t="s">
-        <v>401</v>
+        <v>7</v>
       </c>
       <c r="H367" t="s">
-        <v>6</v>
+        <v>299</v>
       </c>
       <c r="I367" t="s">
         <v>5</v>
       </c>
       <c r="J367" t="s">
-        <v>40</v>
+        <v>824</v>
       </c>
       <c r="K367" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="L367" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>virtual_collectionUNC919t.</v>
+        <v>upc[value]GEN24ai1=1</v>
       </c>
       <c r="M367" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -41260,50 +41361,46 @@
         <f>IF(ISNUMBER(MATCH(mappings[field],fields[argot_field],0)),"y","n")</f>
         <v>y</v>
       </c>
-      <c r="P367" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q367" s="8" t="s">
-        <v>2</v>
-      </c>
+      <c r="P367" s="8"/>
+      <c r="Q367" s="8"/>
     </row>
     <row r="368" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>945</v>
+        <v>336</v>
       </c>
       <c r="B368" t="s">
-        <v>945</v>
+        <v>336</v>
       </c>
       <c r="C368" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="D368" t="s">
         <v>2</v>
       </c>
       <c r="E368" t="s">
-        <v>118</v>
+        <v>53</v>
       </c>
       <c r="F368" s="1">
-        <v>100</v>
+        <v>919</v>
       </c>
       <c r="G368" t="s">
-        <v>226</v>
+        <v>401</v>
       </c>
       <c r="H368" t="s">
         <v>6</v>
       </c>
       <c r="I368" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="J368" t="s">
-        <v>263</v>
+        <v>40</v>
       </c>
       <c r="K368" t="s">
-        <v>950</v>
+        <v>40</v>
       </c>
       <c r="L368" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>work_citation_uncontrolledGEN100abcd(g)jqu.</v>
+        <v>virtual_collectionUNC919t.</v>
       </c>
       <c r="M368" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -41324,7 +41421,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="369" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>945</v>
       </c>
@@ -41341,10 +41438,10 @@
         <v>118</v>
       </c>
       <c r="F369" s="1">
-        <v>110</v>
-      </c>
-      <c r="G369" s="11" t="s">
-        <v>227</v>
+        <v>100</v>
+      </c>
+      <c r="G369" t="s">
+        <v>226</v>
       </c>
       <c r="H369" t="s">
         <v>6</v>
@@ -41360,7 +41457,7 @@
       </c>
       <c r="L369" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>work_citation_uncontrolledGEN110abcd(g)(n)u.</v>
+        <v>work_citation_uncontrolledGEN100abcd(g)jqu.</v>
       </c>
       <c r="M369" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -41381,7 +41478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="370" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>945</v>
       </c>
@@ -41398,10 +41495,10 @@
         <v>118</v>
       </c>
       <c r="F370" s="1">
-        <v>111</v>
-      </c>
-      <c r="G370" t="s">
-        <v>228</v>
+        <v>110</v>
+      </c>
+      <c r="G370" s="11" t="s">
+        <v>227</v>
       </c>
       <c r="H370" t="s">
         <v>6</v>
@@ -41410,14 +41507,14 @@
         <v>20</v>
       </c>
       <c r="J370" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K370" t="s">
         <v>950</v>
       </c>
       <c r="L370" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>work_citation_uncontrolledGEN111acde(g)(n)qu.</v>
+        <v>work_citation_uncontrolledGEN110abcd(g)(n)u.</v>
       </c>
       <c r="M370" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -41455,10 +41552,10 @@
         <v>118</v>
       </c>
       <c r="F371" s="1">
-        <v>245</v>
+        <v>111</v>
       </c>
       <c r="G371" t="s">
-        <v>951</v>
+        <v>228</v>
       </c>
       <c r="H371" t="s">
         <v>6</v>
@@ -41467,14 +41564,14 @@
         <v>20</v>
       </c>
       <c r="J371" t="s">
-        <v>952</v>
+        <v>264</v>
       </c>
       <c r="K371" t="s">
         <v>950</v>
       </c>
       <c r="L371" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>work_citation_uncontrolledGEN245anp.</v>
+        <v>work_citation_uncontrolledGEN111acde(g)(n)qu.</v>
       </c>
       <c r="M371" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -41492,6 +41589,63 @@
         <v>2</v>
       </c>
       <c r="Q371" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="372" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A372" t="s">
+        <v>945</v>
+      </c>
+      <c r="B372" t="s">
+        <v>945</v>
+      </c>
+      <c r="C372" t="s">
+        <v>1</v>
+      </c>
+      <c r="D372" t="s">
+        <v>2</v>
+      </c>
+      <c r="E372" t="s">
+        <v>118</v>
+      </c>
+      <c r="F372" s="1">
+        <v>245</v>
+      </c>
+      <c r="G372" t="s">
+        <v>951</v>
+      </c>
+      <c r="H372" t="s">
+        <v>6</v>
+      </c>
+      <c r="I372" t="s">
+        <v>20</v>
+      </c>
+      <c r="J372" t="s">
+        <v>952</v>
+      </c>
+      <c r="K372" t="s">
+        <v>950</v>
+      </c>
+      <c r="L372" s="8" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>work_citation_uncontrolledGEN245anp.</v>
+      </c>
+      <c r="M372" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N372" s="8">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O372" s="8" t="str">
+        <f>IF(ISNUMBER(MATCH(mappings[field],fields[argot_field],0)),"y","n")</f>
+        <v>y</v>
+      </c>
+      <c r="P372" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q372" s="8" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
clarify series constraints; fix 810 example
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12816" uniqueCount="1428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12816" uniqueCount="1430">
   <si>
     <t>subject_chronological_facet</t>
   </si>
@@ -4312,6 +4312,12 @@
   </si>
   <si>
     <t>"label":"Data set graphics details"</t>
+  </si>
+  <si>
+    <t>$t OR $k</t>
+  </si>
+  <si>
+    <t>($t OR $k) AND ($i OR $3)</t>
   </si>
 </sst>
 </file>
@@ -5006,11 +5012,6 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="mappings" displayName="mappings" ref="A1:Q653" totalsRowShown="0">
   <autoFilter ref="A1:Q653"/>
-  <sortState ref="A2:Q653">
-    <sortCondition ref="A2:A653"/>
-    <sortCondition ref="F2:F653"/>
-    <sortCondition ref="B2:B653"/>
-  </sortState>
   <tableColumns count="17">
     <tableColumn id="17" name="parentfield"/>
     <tableColumn id="1" name="field"/>
@@ -22568,8 +22569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q653"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A313" workbookViewId="0">
-      <selection activeCell="A333" sqref="A333"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H495" sqref="H495"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52074,7 +52075,7 @@
         <v>220</v>
       </c>
       <c r="H525" t="s">
-        <v>569</v>
+        <v>1428</v>
       </c>
       <c r="I525" t="s">
         <v>20</v>
@@ -52087,7 +52088,7 @@
       </c>
       <c r="L525" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>series_work[author]GEN800abcd(g)jqunone</v>
+        <v>series_work[author]GEN800abcd(g)jqu$t OR $k</v>
       </c>
       <c r="M525" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -52131,7 +52132,7 @@
         <v>40</v>
       </c>
       <c r="H526" t="s">
-        <v>569</v>
+        <v>1428</v>
       </c>
       <c r="I526" t="s">
         <v>20</v>
@@ -52144,7 +52145,7 @@
       </c>
       <c r="L526" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>series_work[issn]GEN800xnone</v>
+        <v>series_work[issn]GEN800x$t OR $k</v>
       </c>
       <c r="M526" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -52188,7 +52189,7 @@
         <v>1108</v>
       </c>
       <c r="H527" t="s">
-        <v>1214</v>
+        <v>1429</v>
       </c>
       <c r="I527" t="s">
         <v>20</v>
@@ -52201,7 +52202,7 @@
       </c>
       <c r="L527" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>series_work[label]GEN800i3$i OR $3</v>
+        <v>series_work[label]GEN800i3($t OR $k) AND ($i OR $3)</v>
       </c>
       <c r="M527" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -52245,7 +52246,7 @@
         <v>468</v>
       </c>
       <c r="H528" t="s">
-        <v>569</v>
+        <v>1428</v>
       </c>
       <c r="I528" t="s">
         <v>1272</v>
@@ -52258,7 +52259,7 @@
       </c>
       <c r="L528" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>series_work[title]GEN800f(g)hklmnoprstnone</v>
+        <v>series_work[title]GEN800f(g)hklmnoprst$t OR $k</v>
       </c>
       <c r="M528" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -52302,7 +52303,7 @@
         <v>889</v>
       </c>
       <c r="H529" t="s">
-        <v>569</v>
+        <v>1428</v>
       </c>
       <c r="I529" t="s">
         <v>254</v>
@@ -52315,7 +52316,7 @@
       </c>
       <c r="L529" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>series_work[type]GEN800{na}none</v>
+        <v>series_work[type]GEN800{na}$t OR $k</v>
       </c>
       <c r="M529" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -52359,7 +52360,7 @@
         <v>1115</v>
       </c>
       <c r="H530" t="s">
-        <v>569</v>
+        <v>1428</v>
       </c>
       <c r="I530" t="s">
         <v>20</v>
@@ -52372,7 +52373,7 @@
       </c>
       <c r="L530" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>series_work[author]GEN810abc(d)(g)(n)unone</v>
+        <v>series_work[author]GEN810abc(d)(g)(n)u$t OR $k</v>
       </c>
       <c r="M530" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -52416,7 +52417,7 @@
         <v>40</v>
       </c>
       <c r="H531" t="s">
-        <v>569</v>
+        <v>1428</v>
       </c>
       <c r="I531" t="s">
         <v>20</v>
@@ -52429,7 +52430,7 @@
       </c>
       <c r="L531" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>series_work[issn]GEN810xnone</v>
+        <v>series_work[issn]GEN810x$t OR $k</v>
       </c>
       <c r="M531" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -52472,8 +52473,8 @@
       <c r="G532" t="s">
         <v>1108</v>
       </c>
-      <c r="H532" s="30" t="s">
-        <v>1214</v>
+      <c r="H532" t="s">
+        <v>1429</v>
       </c>
       <c r="I532" t="s">
         <v>20</v>
@@ -52486,7 +52487,7 @@
       </c>
       <c r="L532" s="35" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>series_work[label]GEN810i3$i OR $3</v>
+        <v>series_work[label]GEN810i3($t OR $k) AND ($i OR $3)</v>
       </c>
       <c r="M532" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -52529,8 +52530,8 @@
       <c r="G533" t="s">
         <v>470</v>
       </c>
-      <c r="H533" s="30" t="s">
-        <v>569</v>
+      <c r="H533" t="s">
+        <v>1428</v>
       </c>
       <c r="I533" t="s">
         <v>1272</v>
@@ -52543,7 +52544,7 @@
       </c>
       <c r="L533" s="8" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>series_work[title]GEN810(d)f(g)hklm(n)oprstnone</v>
+        <v>series_work[title]GEN810(d)f(g)hklm(n)oprst$t OR $k</v>
       </c>
       <c r="M533" s="8">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -52586,8 +52587,8 @@
       <c r="G534" s="30" t="s">
         <v>889</v>
       </c>
-      <c r="H534" s="30" t="s">
-        <v>569</v>
+      <c r="H534" t="s">
+        <v>1428</v>
       </c>
       <c r="I534" t="s">
         <v>254</v>
@@ -52600,7 +52601,7 @@
       </c>
       <c r="L534" s="35" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>series_work[type]GEN810{na}none</v>
+        <v>series_work[type]GEN810{na}$t OR $k</v>
       </c>
       <c r="M534" s="35">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -52643,8 +52644,8 @@
       <c r="G535" s="31" t="s">
         <v>1120</v>
       </c>
-      <c r="H535" s="31" t="s">
-        <v>569</v>
+      <c r="H535" t="s">
+        <v>1428</v>
       </c>
       <c r="I535" t="s">
         <v>20</v>
@@ -52657,7 +52658,7 @@
       </c>
       <c r="L535" s="37" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>series_work[author]GEN811ac(d)e(g)(n)unone</v>
+        <v>series_work[author]GEN811ac(d)e(g)(n)u$t OR $k</v>
       </c>
       <c r="M535" s="37">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -52700,8 +52701,8 @@
       <c r="G536" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="H536" s="31" t="s">
-        <v>569</v>
+      <c r="H536" t="s">
+        <v>1428</v>
       </c>
       <c r="I536" s="31" t="s">
         <v>20</v>
@@ -52714,7 +52715,7 @@
       </c>
       <c r="L536" s="37" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>series_work[issn]GEN811xnone</v>
+        <v>series_work[issn]GEN811x$t OR $k</v>
       </c>
       <c r="M536" s="37">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -52757,8 +52758,8 @@
       <c r="G537" s="30" t="s">
         <v>1108</v>
       </c>
-      <c r="H537" s="30" t="s">
-        <v>1214</v>
+      <c r="H537" t="s">
+        <v>1429</v>
       </c>
       <c r="I537" s="30" t="s">
         <v>20</v>
@@ -52771,7 +52772,7 @@
       </c>
       <c r="L537" s="35" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>series_work[label]GEN811i3$i OR $3</v>
+        <v>series_work[label]GEN811i3($t OR $k) AND ($i OR $3)</v>
       </c>
       <c r="M537" s="35">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -52814,8 +52815,8 @@
       <c r="G538" s="30" t="s">
         <v>1188</v>
       </c>
-      <c r="H538" s="30" t="s">
-        <v>569</v>
+      <c r="H538" t="s">
+        <v>1428</v>
       </c>
       <c r="I538" s="16" t="s">
         <v>1272</v>
@@ -52828,7 +52829,7 @@
       </c>
       <c r="L538" s="35" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>series_work[title]GEN811(d)f(g)hklm(n)pstnone</v>
+        <v>series_work[title]GEN811(d)f(g)hklm(n)pst$t OR $k</v>
       </c>
       <c r="M538" s="35">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -52871,8 +52872,8 @@
       <c r="G539" s="31" t="s">
         <v>889</v>
       </c>
-      <c r="H539" s="31" t="s">
-        <v>569</v>
+      <c r="H539" t="s">
+        <v>1428</v>
       </c>
       <c r="I539" s="16" t="s">
         <v>254</v>
@@ -52885,7 +52886,7 @@
       </c>
       <c r="L539" s="37" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>series_work[type]GEN811{na}none</v>
+        <v>series_work[type]GEN811{na}$t OR $k</v>
       </c>
       <c r="M539" s="37">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>

</xml_diff>

<commit_message>
update specs for non-roman script handling in names
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="5910" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="5910"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13790" uniqueCount="1479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13790" uniqueCount="1480">
   <si>
     <t>subject_chronological_facet</t>
   </si>
@@ -4464,6 +4464,9 @@
   </si>
   <si>
     <t>Other details &gt; (notes cluster) &gt; Described by:</t>
+  </si>
+  <si>
+    <t>https://trlnmain.atlassian.net/browse/TD-705</t>
   </si>
 </sst>
 </file>
@@ -5536,13 +5539,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC214"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" topLeftCell="D44" workbookViewId="0">
+      <selection activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -12757,7 +12761,7 @@
         <v>1337</v>
       </c>
       <c r="Y79" t="s">
-        <v>1039</v>
+        <v>1479</v>
       </c>
       <c r="Z79" s="15">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
@@ -25200,7 +25204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q723"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G116" sqref="G116"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
spec non-roman subject and genre headings
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13790" uniqueCount="1480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13790" uniqueCount="1484">
   <si>
     <t>subject_chronological_facet</t>
   </si>
@@ -4467,6 +4467,18 @@
   </si>
   <si>
     <t>https://trlnmain.atlassian.net/browse/TD-705</t>
+  </si>
+  <si>
+    <t>implementation needed, institution-specific</t>
+  </si>
+  <si>
+    <t>https://trlnmain.atlassian.net/browse/TD-713</t>
+  </si>
+  <si>
+    <t>https://trlnmain.atlassian.net/browse/TD-738</t>
+  </si>
+  <si>
+    <t>https://trlnmain.atlassian.net/browse/TD-715</t>
   </si>
 </sst>
 </file>
@@ -5170,7 +5182,18 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fields" displayName="fields" ref="A1:AC214" totalsRowShown="0">
-  <autoFilter ref="A1:AC214"/>
+  <autoFilter ref="A1:AC214">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="genre_headings"/>
+        <filter val="genre_headings[lang]"/>
+        <filter val="genre_headings[value]"/>
+        <filter val="subject_headings"/>
+        <filter val="subject_headings[lang]"/>
+        <filter val="subject_headings[value]"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="29">
     <tableColumn id="2" name="argot_field"/>
     <tableColumn id="18" name="has parent"/>
@@ -5539,8 +5562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D44" workbookViewId="0">
-      <selection activeCell="K50" sqref="K50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A183" sqref="A183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5638,7 +5661,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>492</v>
       </c>
@@ -5725,7 +5748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>413</v>
       </c>
@@ -5818,7 +5841,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>244</v>
       </c>
@@ -5911,7 +5934,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -6004,7 +6027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>425</v>
       </c>
@@ -6097,7 +6120,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>198</v>
       </c>
@@ -6190,7 +6213,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1361</v>
       </c>
@@ -6205,7 +6228,7 @@
         <v>1466</v>
       </c>
       <c r="E8" t="s">
-        <v>770</v>
+        <v>1480</v>
       </c>
       <c r="F8" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
@@ -6263,7 +6286,7 @@
         <v>1364</v>
       </c>
       <c r="Y8" t="s">
-        <v>522</v>
+        <v>1481</v>
       </c>
       <c r="Z8" s="8">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
@@ -6274,7 +6297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1360</v>
       </c>
@@ -6289,7 +6312,7 @@
         <v>1467</v>
       </c>
       <c r="E9" t="s">
-        <v>1470</v>
+        <v>1480</v>
       </c>
       <c r="F9" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
@@ -6355,7 +6378,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>635</v>
       </c>
@@ -6448,7 +6471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1316</v>
       </c>
@@ -6538,7 +6561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1315</v>
       </c>
@@ -6628,7 +6651,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>337</v>
       </c>
@@ -6721,7 +6744,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>338</v>
       </c>
@@ -6814,7 +6837,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>339</v>
       </c>
@@ -7076,7 +7099,7 @@
         <v>1399</v>
       </c>
       <c r="Y17" t="s">
-        <v>530</v>
+        <v>1482</v>
       </c>
       <c r="Z17" s="8">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
@@ -7186,7 +7209,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>159</v>
       </c>
@@ -7279,7 +7302,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>480</v>
       </c>
@@ -7372,7 +7395,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>479</v>
       </c>
@@ -7465,7 +7488,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>481</v>
       </c>
@@ -7558,7 +7581,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>482</v>
       </c>
@@ -7651,7 +7674,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>483</v>
       </c>
@@ -7744,7 +7767,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>484</v>
       </c>
@@ -7837,7 +7860,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>292</v>
       </c>
@@ -7930,7 +7953,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>340</v>
       </c>
@@ -8023,7 +8046,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>366</v>
       </c>
@@ -8116,7 +8139,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>361</v>
       </c>
@@ -8209,7 +8232,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>371</v>
       </c>
@@ -8302,7 +8325,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>341</v>
       </c>
@@ -8395,7 +8418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>373</v>
       </c>
@@ -8488,7 +8511,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>372</v>
       </c>
@@ -8581,7 +8604,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>374</v>
       </c>
@@ -8674,7 +8697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>646</v>
       </c>
@@ -8767,7 +8790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>975</v>
       </c>
@@ -8856,7 +8879,7 @@
       <c r="AB36" s="9"/>
       <c r="AC36" s="9"/>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>977</v>
       </c>
@@ -8945,7 +8968,7 @@
       <c r="AB37" s="9"/>
       <c r="AC37" s="9"/>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>1015</v>
       </c>
@@ -9034,7 +9057,7 @@
       <c r="AB38" s="9"/>
       <c r="AC38" s="9"/>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>1013</v>
       </c>
@@ -9123,7 +9146,7 @@
       <c r="AB39" s="9"/>
       <c r="AC39" s="9"/>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>998</v>
       </c>
@@ -9212,7 +9235,7 @@
       <c r="AB40" s="9"/>
       <c r="AC40" s="9"/>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>974</v>
       </c>
@@ -9301,7 +9324,7 @@
       <c r="AB41" s="9"/>
       <c r="AC41" s="9"/>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>1334</v>
       </c>
@@ -9394,7 +9417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>1011</v>
       </c>
@@ -9483,7 +9506,7 @@
       <c r="AB43" s="9"/>
       <c r="AC43" s="9"/>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>976</v>
       </c>
@@ -9572,7 +9595,7 @@
       <c r="AB44" s="9"/>
       <c r="AC44" s="9"/>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>1002</v>
       </c>
@@ -9661,7 +9684,7 @@
       <c r="AB45" s="9"/>
       <c r="AC45" s="9"/>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>1005</v>
       </c>
@@ -9750,7 +9773,7 @@
       <c r="AB46" s="9"/>
       <c r="AC46" s="9"/>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>973</v>
       </c>
@@ -9839,7 +9862,7 @@
       <c r="AB47" s="9"/>
       <c r="AC47" s="9"/>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>44</v>
       </c>
@@ -9928,7 +9951,7 @@
       <c r="AB48" s="9"/>
       <c r="AC48" s="9"/>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>277</v>
       </c>
@@ -10021,7 +10044,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>402</v>
       </c>
@@ -10114,7 +10137,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>403</v>
       </c>
@@ -10207,7 +10230,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>856</v>
       </c>
@@ -10294,7 +10317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>653</v>
       </c>
@@ -10387,7 +10410,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>1415</v>
       </c>
@@ -10480,7 +10503,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>1414</v>
       </c>
@@ -10573,7 +10596,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>859</v>
       </c>
@@ -10660,7 +10683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>153</v>
       </c>
@@ -10753,7 +10776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>469</v>
       </c>
@@ -10846,7 +10869,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>470</v>
       </c>
@@ -10939,7 +10962,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>471</v>
       </c>
@@ -11032,7 +11055,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>472</v>
       </c>
@@ -11125,7 +11148,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>468</v>
       </c>
@@ -11218,7 +11241,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>473</v>
       </c>
@@ -11311,7 +11334,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>474</v>
       </c>
@@ -11404,7 +11427,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>475</v>
       </c>
@@ -11497,7 +11520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>476</v>
       </c>
@@ -11590,7 +11613,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>477</v>
       </c>
@@ -11683,7 +11706,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>478</v>
       </c>
@@ -11776,7 +11799,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>487</v>
       </c>
@@ -11869,7 +11892,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>750</v>
       </c>
@@ -11962,7 +11985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>751</v>
       </c>
@@ -12034,7 +12057,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>239</v>
       </c>
@@ -12127,7 +12150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>285</v>
       </c>
@@ -12220,7 +12243,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>948</v>
       </c>
@@ -12313,7 +12336,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>391</v>
       </c>
@@ -12406,7 +12429,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>392</v>
       </c>
@@ -12499,7 +12522,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>393</v>
       </c>
@@ -12592,7 +12615,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>196</v>
       </c>
@@ -12685,7 +12708,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>1343</v>
       </c>
@@ -12778,7 +12801,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>1133</v>
       </c>
@@ -12871,7 +12894,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>1134</v>
       </c>
@@ -12964,7 +12987,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>1135</v>
       </c>
@@ -13057,7 +13080,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>434</v>
       </c>
@@ -13150,7 +13173,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>574</v>
       </c>
@@ -13243,7 +13266,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>799</v>
       </c>
@@ -13336,7 +13359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>801</v>
       </c>
@@ -13423,7 +13446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>800</v>
       </c>
@@ -13510,7 +13533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>334</v>
       </c>
@@ -13603,7 +13626,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>1344</v>
       </c>
@@ -13696,7 +13719,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>805</v>
       </c>
@@ -13789,7 +13812,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>757</v>
       </c>
@@ -13882,7 +13905,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>1350</v>
       </c>
@@ -13975,7 +13998,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>690</v>
       </c>
@@ -14068,7 +14091,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>795</v>
       </c>
@@ -14161,7 +14184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>870</v>
       </c>
@@ -14254,7 +14277,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>666</v>
       </c>
@@ -14347,7 +14370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>670</v>
       </c>
@@ -14431,7 +14454,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>669</v>
       </c>
@@ -14524,7 +14547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>667</v>
       </c>
@@ -14617,7 +14640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>668</v>
       </c>
@@ -14710,7 +14733,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>418</v>
       </c>
@@ -14803,7 +14826,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>718</v>
       </c>
@@ -14896,7 +14919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>719</v>
       </c>
@@ -14989,7 +15012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>680</v>
       </c>
@@ -15082,7 +15105,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>677</v>
       </c>
@@ -15175,7 +15198,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>678</v>
       </c>
@@ -15268,7 +15291,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>862</v>
       </c>
@@ -15355,7 +15378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>760</v>
       </c>
@@ -15448,7 +15471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>740</v>
       </c>
@@ -15535,7 +15558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>694</v>
       </c>
@@ -15628,7 +15651,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>701</v>
       </c>
@@ -15721,7 +15744,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>697</v>
       </c>
@@ -15814,7 +15837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>705</v>
       </c>
@@ -15907,7 +15930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>763</v>
       </c>
@@ -15994,7 +16017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>777</v>
       </c>
@@ -16081,7 +16104,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>766</v>
       </c>
@@ -16168,7 +16191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>767</v>
       </c>
@@ -16255,7 +16278,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="118" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>764</v>
       </c>
@@ -16342,7 +16365,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>713</v>
       </c>
@@ -16435,7 +16458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>710</v>
       </c>
@@ -16528,7 +16551,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>819</v>
       </c>
@@ -16621,7 +16644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>820</v>
       </c>
@@ -16708,7 +16731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>821</v>
       </c>
@@ -16801,7 +16824,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>822</v>
       </c>
@@ -16894,7 +16917,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>823</v>
       </c>
@@ -16987,7 +17010,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>699</v>
       </c>
@@ -17080,7 +17103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>1191</v>
       </c>
@@ -17173,7 +17196,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>336</v>
       </c>
@@ -17266,7 +17289,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>816</v>
       </c>
@@ -17359,7 +17382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>658</v>
       </c>
@@ -17446,7 +17469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>335</v>
       </c>
@@ -17539,7 +17562,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>688</v>
       </c>
@@ -17632,7 +17655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>258</v>
       </c>
@@ -17725,7 +17748,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>485</v>
       </c>
@@ -17818,7 +17841,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>486</v>
       </c>
@@ -17911,7 +17934,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>419</v>
       </c>
@@ -18004,7 +18027,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="137" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>1198</v>
       </c>
@@ -18097,7 +18120,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>1199</v>
       </c>
@@ -18190,7 +18213,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>1204</v>
       </c>
@@ -18283,7 +18306,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="140" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>1205</v>
       </c>
@@ -18376,7 +18399,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="141" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>1206</v>
       </c>
@@ -18469,7 +18492,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="142" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>731</v>
       </c>
@@ -18556,7 +18579,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>343</v>
       </c>
@@ -18649,7 +18672,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="144" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>315</v>
       </c>
@@ -18742,7 +18765,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="145" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="9" t="s">
         <v>618</v>
       </c>
@@ -18835,7 +18858,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="9" t="s">
         <v>629</v>
       </c>
@@ -18924,7 +18947,7 @@
       <c r="AB146" s="9"/>
       <c r="AC146" s="9"/>
     </row>
-    <row r="147" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="9" t="s">
         <v>633</v>
       </c>
@@ -19013,7 +19036,7 @@
       <c r="AB147" s="9"/>
       <c r="AC147" s="9"/>
     </row>
-    <row r="148" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="9" t="s">
         <v>1036</v>
       </c>
@@ -19102,7 +19125,7 @@
       <c r="AB148" s="9"/>
       <c r="AC148" s="9"/>
     </row>
-    <row r="149" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="9" t="s">
         <v>634</v>
       </c>
@@ -19191,7 +19214,7 @@
       <c r="AB149" s="9"/>
       <c r="AC149" s="9"/>
     </row>
-    <row r="150" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="9" t="s">
         <v>630</v>
       </c>
@@ -19280,7 +19303,7 @@
       <c r="AB150" s="9"/>
       <c r="AC150" s="9"/>
     </row>
-    <row r="151" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="9" t="s">
         <v>631</v>
       </c>
@@ -19369,7 +19392,7 @@
       <c r="AB151" s="9"/>
       <c r="AC151" s="9"/>
     </row>
-    <row r="152" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="9" t="s">
         <v>1338</v>
       </c>
@@ -19462,7 +19485,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="153" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="9" t="s">
         <v>1037</v>
       </c>
@@ -19551,7 +19574,7 @@
       <c r="AB153" s="9"/>
       <c r="AC153" s="9"/>
     </row>
-    <row r="154" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="9" t="s">
         <v>632</v>
       </c>
@@ -19640,7 +19663,7 @@
       <c r="AB154" s="9"/>
       <c r="AC154" s="9"/>
     </row>
-    <row r="155" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="9" t="s">
         <v>1030</v>
       </c>
@@ -19729,7 +19752,7 @@
       <c r="AB155" s="9"/>
       <c r="AC155" s="9"/>
     </row>
-    <row r="156" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="9" t="s">
         <v>1032</v>
       </c>
@@ -19818,7 +19841,7 @@
       <c r="AB156" s="9"/>
       <c r="AC156" s="9"/>
     </row>
-    <row r="157" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="9" t="s">
         <v>1034</v>
       </c>
@@ -19907,7 +19930,7 @@
       <c r="AB157" s="9"/>
       <c r="AC157" s="9"/>
     </row>
-    <row r="158" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>160</v>
       </c>
@@ -19994,7 +20017,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>305</v>
       </c>
@@ -20087,7 +20110,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="160" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>1155</v>
       </c>
@@ -20180,7 +20203,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="161" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>1164</v>
       </c>
@@ -20273,7 +20296,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="162" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>1166</v>
       </c>
@@ -20366,7 +20389,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="163" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>1165</v>
       </c>
@@ -20459,7 +20482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="164" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>1163</v>
       </c>
@@ -20552,7 +20575,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="165" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="9" t="s">
         <v>1072</v>
       </c>
@@ -20645,7 +20668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="166" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="9" t="s">
         <v>1075</v>
       </c>
@@ -20738,7 +20761,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="167" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="9" t="s">
         <v>1077</v>
       </c>
@@ -20831,7 +20854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="168" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="9" t="s">
         <v>1079</v>
       </c>
@@ -20924,7 +20947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="169" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="9" t="s">
         <v>1081</v>
       </c>
@@ -21017,7 +21040,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="170" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="9" t="s">
         <v>1082</v>
       </c>
@@ -21110,7 +21133,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="171" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="9" t="s">
         <v>1339</v>
       </c>
@@ -21203,7 +21226,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="9" t="s">
         <v>1083</v>
       </c>
@@ -21296,7 +21319,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="173" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="9" t="s">
         <v>1085</v>
       </c>
@@ -21389,7 +21412,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="174" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="9" t="s">
         <v>1087</v>
       </c>
@@ -21482,7 +21505,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="175" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="9" t="s">
         <v>1089</v>
       </c>
@@ -21575,7 +21598,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="176" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="9" t="s">
         <v>1091</v>
       </c>
@@ -21668,7 +21691,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="177" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>266</v>
       </c>
@@ -21761,7 +21784,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="178" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>297</v>
       </c>
@@ -21854,7 +21877,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="179" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>490</v>
       </c>
@@ -21947,7 +21970,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="180" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>489</v>
       </c>
@@ -22040,7 +22063,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>491</v>
       </c>
@@ -22302,7 +22325,7 @@
         <v>1399</v>
       </c>
       <c r="Y183" t="s">
-        <v>5</v>
+        <v>1483</v>
       </c>
       <c r="Z183" s="8">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
@@ -22412,7 +22435,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="20" t="s">
         <v>1371</v>
       </c>
@@ -22505,7 +22528,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="9" t="s">
         <v>1102</v>
       </c>
@@ -22598,7 +22621,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="187" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="9" t="s">
         <v>1103</v>
       </c>
@@ -22689,7 +22712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="9" t="s">
         <v>1340</v>
       </c>
@@ -22782,7 +22805,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="189" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="9" t="s">
         <v>1104</v>
       </c>
@@ -22873,7 +22896,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="190" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="9" t="s">
         <v>1105</v>
       </c>
@@ -22964,7 +22987,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="191" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="9" t="s">
         <v>1106</v>
       </c>
@@ -23055,7 +23078,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="192" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="9" t="s">
         <v>1107</v>
       </c>
@@ -23146,7 +23169,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="193" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="9" t="s">
         <v>197</v>
       </c>
@@ -23239,7 +23262,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="194" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>1328</v>
       </c>
@@ -23329,7 +23352,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="195" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>611</v>
       </c>
@@ -23422,7 +23445,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="196" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>1323</v>
       </c>
@@ -23515,7 +23538,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="197" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>874</v>
       </c>
@@ -23608,7 +23631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="198" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>879</v>
       </c>
@@ -23701,7 +23724,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="199" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>878</v>
       </c>
@@ -23794,7 +23817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="200" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>992</v>
       </c>
@@ -23887,7 +23910,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="201" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>876</v>
       </c>
@@ -23980,7 +24003,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="202" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>875</v>
       </c>
@@ -24073,7 +24096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="203" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>877</v>
       </c>
@@ -24166,7 +24189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="204" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>271</v>
       </c>
@@ -24259,7 +24282,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="205" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>1179</v>
       </c>
@@ -24352,7 +24375,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="206" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>1180</v>
       </c>
@@ -24445,7 +24468,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="207" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>619</v>
       </c>
@@ -24538,7 +24561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="208" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>324</v>
       </c>
@@ -24631,7 +24654,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="209" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>323</v>
       </c>
@@ -24724,7 +24747,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="210" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>321</v>
       </c>
@@ -24817,7 +24840,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="211" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>322</v>
       </c>
@@ -24910,7 +24933,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="212" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>1422</v>
       </c>
@@ -25003,7 +25026,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="213" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>299</v>
       </c>
@@ -25096,7 +25119,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="214" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>284</v>
       </c>

</xml_diff>

<commit_message>
add lang element to statement_of_responsibility
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13815" uniqueCount="1488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13861" uniqueCount="1494">
   <si>
     <t>subject_chronological_facet</t>
   </si>
@@ -4491,6 +4491,24 @@
   </si>
   <si>
     <t>Access Facet</t>
+  </si>
+  <si>
+    <t>statement_of_responsibility[value]</t>
+  </si>
+  <si>
+    <t>statement_of_responsibility[lang]</t>
+  </si>
+  <si>
+    <t>The value of the statement of responsibility</t>
+  </si>
+  <si>
+    <t>Language code for non-Roman script data in field</t>
+  </si>
+  <si>
+    <t>https://trlnmain.atlassian.net/browse/TD-737</t>
+  </si>
+  <si>
+    <t>https://github.com/trln/data-documentation/blob/master/argot/spec_docs/other_argot_fields.adoc#code-statement_of_responsibility-code</t>
   </si>
 </sst>
 </file>
@@ -5193,8 +5211,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fields" displayName="fields" ref="A1:AC215" totalsRowShown="0">
-  <autoFilter ref="A1:AC215"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="fields" displayName="fields" ref="A1:AC217" totalsRowShown="0">
+  <autoFilter ref="A1:AC217"/>
   <tableColumns count="29">
     <tableColumn id="2" name="argot_field"/>
     <tableColumn id="18" name="has parent"/>
@@ -5561,16 +5579,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC215"/>
+  <dimension ref="A1:AC217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
-      <selection activeCell="A214" sqref="A214"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="A178" sqref="A178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.7109375" customWidth="1"/>
     <col min="5" max="5" width="31.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -21794,7 +21813,7 @@
       </c>
       <c r="C178" t="str">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
-        <v>n</v>
+        <v>y</v>
       </c>
       <c r="D178" t="s">
         <v>1467</v>
@@ -21804,13 +21823,13 @@
       </c>
       <c r="F178" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
-        <v>simple field</v>
+        <v>parent field</v>
       </c>
       <c r="G178" t="s">
-        <v>5</v>
+        <v>1358</v>
       </c>
       <c r="H178" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I178" t="s">
         <v>2</v>
@@ -21822,7 +21841,7 @@
         <v>295</v>
       </c>
       <c r="L178" t="s">
-        <v>442</v>
+        <v>501</v>
       </c>
       <c r="M178" t="s">
         <v>27</v>
@@ -21834,7 +21853,7 @@
         <v>502</v>
       </c>
       <c r="P178" t="s">
-        <v>602</v>
+        <v>27</v>
       </c>
       <c r="Q178" t="s">
         <v>5</v>
@@ -21849,7 +21868,7 @@
         <v>5</v>
       </c>
       <c r="U178" t="s">
-        <v>309</v>
+        <v>27</v>
       </c>
       <c r="V178" t="s">
         <v>5</v>
@@ -21858,7 +21877,7 @@
         <v>5</v>
       </c>
       <c r="X178" t="s">
-        <v>519</v>
+        <v>1493</v>
       </c>
       <c r="Y178" t="s">
         <v>5</v>
@@ -21880,30 +21899,27 @@
     </row>
     <row r="179" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>490</v>
+        <v>1488</v>
       </c>
       <c r="B179" t="s">
-        <v>27</v>
-      </c>
-      <c r="C179" t="str">
+        <v>297</v>
+      </c>
+      <c r="C179" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
         <v>n</v>
       </c>
       <c r="D179" t="s">
-        <v>1465</v>
-      </c>
-      <c r="E179" t="s">
-        <v>1472</v>
-      </c>
-      <c r="F179" t="str">
+        <v>1467</v>
+      </c>
+      <c r="F179" s="8" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
-        <v>simple field</v>
+        <v>field element</v>
       </c>
       <c r="G179" t="s">
-        <v>5</v>
+        <v>1358</v>
       </c>
       <c r="H179" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="I179" t="s">
         <v>2</v>
@@ -21912,57 +21928,54 @@
         <v>1332</v>
       </c>
       <c r="K179" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="L179" t="s">
-        <v>605</v>
+        <v>442</v>
       </c>
       <c r="M179" t="s">
         <v>27</v>
       </c>
       <c r="N179" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="O179" t="s">
-        <v>27</v>
+        <v>502</v>
       </c>
       <c r="P179" t="s">
-        <v>27</v>
+        <v>602</v>
       </c>
       <c r="Q179" t="s">
         <v>5</v>
       </c>
       <c r="R179" t="s">
-        <v>77</v>
+        <v>1490</v>
       </c>
       <c r="S179" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="T179" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="U179" t="s">
-        <v>79</v>
+        <v>309</v>
       </c>
       <c r="V179" t="s">
-        <v>80</v>
-      </c>
-      <c r="W179" t="s">
-        <v>151</v>
+        <v>5</v>
       </c>
       <c r="X179" t="s">
-        <v>519</v>
+        <v>1493</v>
       </c>
       <c r="Y179" t="s">
         <v>5</v>
       </c>
-      <c r="Z179">
+      <c r="Z179" s="8">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA179">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="AB179" t="s">
         <v>5</v>
@@ -21973,30 +21986,27 @@
     </row>
     <row r="180" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>489</v>
+        <v>1489</v>
       </c>
       <c r="B180" t="s">
-        <v>27</v>
-      </c>
-      <c r="C180" t="str">
+        <v>297</v>
+      </c>
+      <c r="C180" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
         <v>n</v>
       </c>
       <c r="D180" t="s">
-        <v>1465</v>
-      </c>
-      <c r="E180" t="s">
-        <v>1472</v>
-      </c>
-      <c r="F180" t="str">
+        <v>1464</v>
+      </c>
+      <c r="F180" s="8" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
-        <v>simple field</v>
+        <v>field element</v>
       </c>
       <c r="G180" t="s">
-        <v>5</v>
+        <v>1358</v>
       </c>
       <c r="H180" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="I180" t="s">
         <v>2</v>
@@ -22005,19 +22015,19 @@
         <v>1332</v>
       </c>
       <c r="K180" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="L180" t="s">
-        <v>606</v>
+        <v>501</v>
       </c>
       <c r="M180" t="s">
         <v>27</v>
       </c>
       <c r="N180" t="s">
-        <v>71</v>
+        <v>27</v>
       </c>
       <c r="O180" t="s">
-        <v>27</v>
+        <v>502</v>
       </c>
       <c r="P180" t="s">
         <v>27</v>
@@ -22026,36 +22036,33 @@
         <v>5</v>
       </c>
       <c r="R180" t="s">
-        <v>72</v>
+        <v>1491</v>
       </c>
       <c r="S180" t="s">
-        <v>73</v>
+        <v>5</v>
       </c>
       <c r="T180" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="U180" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="V180" t="s">
-        <v>75</v>
-      </c>
-      <c r="W180" t="s">
-        <v>151</v>
+        <v>5</v>
       </c>
       <c r="X180" t="s">
-        <v>519</v>
-      </c>
-      <c r="Y180" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z180">
+        <v>1493</v>
+      </c>
+      <c r="Y180" s="9" t="s">
+        <v>1492</v>
+      </c>
+      <c r="Z180" s="8">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA180">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AB180" t="s">
         <v>5</v>
@@ -22066,7 +22073,7 @@
     </row>
     <row r="181" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B181" t="s">
         <v>27</v>
@@ -22101,13 +22108,13 @@
         <v>294</v>
       </c>
       <c r="L181" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="M181" t="s">
         <v>27</v>
       </c>
       <c r="N181" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="O181" t="s">
         <v>27</v>
@@ -22119,16 +22126,16 @@
         <v>5</v>
       </c>
       <c r="R181" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="S181" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="T181" t="s">
         <v>27</v>
       </c>
       <c r="U181" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="V181" t="s">
         <v>80</v>
@@ -22148,7 +22155,7 @@
       </c>
       <c r="AA181">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AB181" t="s">
         <v>5</v>
@@ -22159,27 +22166,27 @@
     </row>
     <row r="182" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>1372</v>
+        <v>489</v>
       </c>
       <c r="B182" t="s">
         <v>27</v>
       </c>
       <c r="C182" t="str">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
-        <v>y</v>
+        <v>n</v>
       </c>
       <c r="D182" t="s">
-        <v>1463</v>
+        <v>1465</v>
       </c>
       <c r="E182" t="s">
-        <v>770</v>
+        <v>1472</v>
       </c>
       <c r="F182" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
-        <v>parent field</v>
+        <v>simple field</v>
       </c>
       <c r="G182" t="s">
-        <v>1402</v>
+        <v>5</v>
       </c>
       <c r="H182" t="s">
         <v>193</v>
@@ -22194,13 +22201,13 @@
         <v>294</v>
       </c>
       <c r="L182" t="s">
-        <v>501</v>
+        <v>606</v>
       </c>
       <c r="M182" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="N182" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="O182" t="s">
         <v>27</v>
@@ -22212,36 +22219,36 @@
         <v>5</v>
       </c>
       <c r="R182" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="S182" t="s">
-        <v>143</v>
+        <v>73</v>
       </c>
       <c r="T182" t="s">
         <v>27</v>
       </c>
       <c r="U182" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="V182" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="W182" t="s">
-        <v>27</v>
+        <v>151</v>
       </c>
       <c r="X182" t="s">
-        <v>1399</v>
+        <v>519</v>
       </c>
       <c r="Y182" t="s">
         <v>5</v>
       </c>
-      <c r="Z182" s="8">
+      <c r="Z182">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA182">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AB182" t="s">
         <v>5</v>
@@ -22252,27 +22259,27 @@
     </row>
     <row r="183" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>1401</v>
+        <v>491</v>
       </c>
       <c r="B183" t="s">
-        <v>1372</v>
+        <v>27</v>
       </c>
       <c r="C183" t="str">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
         <v>n</v>
       </c>
-      <c r="D183" s="9" t="s">
-        <v>1466</v>
+      <c r="D183" t="s">
+        <v>1465</v>
       </c>
       <c r="E183" t="s">
-        <v>770</v>
+        <v>1472</v>
       </c>
       <c r="F183" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
-        <v>field element</v>
+        <v>simple field</v>
       </c>
       <c r="G183" t="s">
-        <v>1402</v>
+        <v>5</v>
       </c>
       <c r="H183" t="s">
         <v>193</v>
@@ -22284,16 +22291,16 @@
         <v>1332</v>
       </c>
       <c r="K183" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L183" t="s">
-        <v>501</v>
+        <v>607</v>
       </c>
       <c r="M183" t="s">
         <v>27</v>
       </c>
       <c r="N183" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="O183" t="s">
         <v>27</v>
@@ -22305,36 +22312,36 @@
         <v>5</v>
       </c>
       <c r="R183" t="s">
-        <v>1335</v>
+        <v>82</v>
       </c>
       <c r="S183" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="T183" t="s">
         <v>27</v>
       </c>
       <c r="U183" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="V183" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="W183" t="s">
-        <v>27</v>
+        <v>151</v>
       </c>
       <c r="X183" t="s">
-        <v>1399</v>
+        <v>519</v>
       </c>
       <c r="Y183" t="s">
-        <v>1483</v>
-      </c>
-      <c r="Z183" s="8">
+        <v>5</v>
+      </c>
+      <c r="Z183">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA183">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="AB183" t="s">
         <v>5</v>
@@ -22345,24 +22352,24 @@
     </row>
     <row r="184" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>1400</v>
+        <v>1372</v>
       </c>
       <c r="B184" t="s">
-        <v>1372</v>
+        <v>27</v>
       </c>
       <c r="C184" t="str">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
-        <v>n</v>
+        <v>y</v>
       </c>
       <c r="D184" t="s">
-        <v>1467</v>
+        <v>1463</v>
       </c>
       <c r="E184" t="s">
-        <v>1475</v>
+        <v>770</v>
       </c>
       <c r="F184" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
-        <v>field element</v>
+        <v>parent field</v>
       </c>
       <c r="G184" t="s">
         <v>1402</v>
@@ -22377,13 +22384,13 @@
         <v>1332</v>
       </c>
       <c r="K184" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="L184" t="s">
-        <v>446</v>
+        <v>501</v>
       </c>
       <c r="M184" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="N184" t="s">
         <v>27</v>
@@ -22392,22 +22399,22 @@
         <v>27</v>
       </c>
       <c r="P184" t="s">
-        <v>398</v>
+        <v>27</v>
       </c>
       <c r="Q184" t="s">
         <v>5</v>
       </c>
       <c r="R184" t="s">
-        <v>1398</v>
+        <v>93</v>
       </c>
       <c r="S184" t="s">
-        <v>27</v>
+        <v>143</v>
       </c>
       <c r="T184" t="s">
-        <v>5</v>
-      </c>
-      <c r="U184" s="16" t="s">
-        <v>142</v>
+        <v>27</v>
+      </c>
+      <c r="U184" t="s">
+        <v>27</v>
       </c>
       <c r="V184" t="s">
         <v>27</v>
@@ -22427,7 +22434,7 @@
       </c>
       <c r="AA184">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="AB184" t="s">
         <v>5</v>
@@ -22437,28 +22444,28 @@
       </c>
     </row>
     <row r="185" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A185" s="20" t="s">
-        <v>1371</v>
+      <c r="A185" t="s">
+        <v>1401</v>
       </c>
       <c r="B185" t="s">
-        <v>27</v>
+        <v>1372</v>
       </c>
       <c r="C185" t="str">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
         <v>n</v>
       </c>
-      <c r="D185" t="s">
-        <v>1465</v>
+      <c r="D185" s="9" t="s">
+        <v>1466</v>
       </c>
       <c r="E185" t="s">
-        <v>1472</v>
+        <v>770</v>
       </c>
       <c r="F185" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
-        <v>simple field</v>
+        <v>field element</v>
       </c>
       <c r="G185" t="s">
-        <v>5</v>
+        <v>1402</v>
       </c>
       <c r="H185" t="s">
         <v>193</v>
@@ -22470,16 +22477,16 @@
         <v>1332</v>
       </c>
       <c r="K185" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="L185" t="s">
-        <v>608</v>
+        <v>501</v>
       </c>
       <c r="M185" t="s">
         <v>27</v>
       </c>
       <c r="N185" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="O185" t="s">
         <v>27</v>
@@ -22491,36 +22498,36 @@
         <v>5</v>
       </c>
       <c r="R185" t="s">
-        <v>65</v>
+        <v>1335</v>
       </c>
       <c r="S185" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="T185" t="s">
         <v>27</v>
       </c>
       <c r="U185" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="V185" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="W185" t="s">
-        <v>151</v>
+        <v>27</v>
       </c>
       <c r="X185" t="s">
-        <v>519</v>
+        <v>1399</v>
       </c>
       <c r="Y185" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z185">
+        <v>1483</v>
+      </c>
+      <c r="Z185" s="8">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
         <v>0</v>
       </c>
       <c r="AA185">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="AB185" t="s">
         <v>5</v>
@@ -22530,31 +22537,31 @@
       </c>
     </row>
     <row r="186" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A186" s="9" t="s">
-        <v>1102</v>
+      <c r="A186" t="s">
+        <v>1400</v>
       </c>
       <c r="B186" t="s">
-        <v>27</v>
+        <v>1372</v>
       </c>
       <c r="C186" t="str">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
-        <v>y</v>
+        <v>n</v>
       </c>
       <c r="D186" t="s">
-        <v>1463</v>
+        <v>1467</v>
       </c>
       <c r="E186" t="s">
-        <v>770</v>
+        <v>1475</v>
       </c>
       <c r="F186" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
-        <v>parent field</v>
+        <v>field element</v>
       </c>
       <c r="G186" t="s">
-        <v>972</v>
-      </c>
-      <c r="H186" s="9" t="s">
-        <v>1111</v>
+        <v>1402</v>
+      </c>
+      <c r="H186" t="s">
+        <v>193</v>
       </c>
       <c r="I186" t="s">
         <v>2</v>
@@ -22563,13 +22570,13 @@
         <v>1332</v>
       </c>
       <c r="K186" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="L186" t="s">
-        <v>501</v>
+        <v>446</v>
       </c>
       <c r="M186" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="N186" t="s">
         <v>27</v>
@@ -22578,76 +22585,76 @@
         <v>27</v>
       </c>
       <c r="P186" t="s">
-        <v>27</v>
+        <v>398</v>
       </c>
       <c r="Q186" t="s">
         <v>5</v>
       </c>
       <c r="R186" t="s">
-        <v>1025</v>
+        <v>1398</v>
       </c>
       <c r="S186" t="s">
-        <v>440</v>
+        <v>27</v>
       </c>
       <c r="T186" t="s">
-        <v>207</v>
-      </c>
-      <c r="U186" s="9" t="s">
-        <v>1109</v>
+        <v>5</v>
+      </c>
+      <c r="U186" s="16" t="s">
+        <v>142</v>
       </c>
       <c r="V186" t="s">
         <v>27</v>
       </c>
       <c r="W186" t="s">
-        <v>356</v>
-      </c>
-      <c r="X186" s="9" t="s">
-        <v>1110</v>
+        <v>27</v>
+      </c>
+      <c r="X186" t="s">
+        <v>1399</v>
       </c>
       <c r="Y186" t="s">
-        <v>617</v>
-      </c>
-      <c r="Z186" s="15">
+        <v>5</v>
+      </c>
+      <c r="Z186" s="8">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
         <v>0</v>
       </c>
-      <c r="AA186" s="9">
+      <c r="AA186">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AB186" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC186" s="9" t="s">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="AB186" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC186" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="187" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A187" s="9" t="s">
-        <v>1103</v>
-      </c>
-      <c r="B187" s="9" t="s">
-        <v>1102</v>
-      </c>
-      <c r="C187" s="9" t="str">
+      <c r="A187" s="20" t="s">
+        <v>1371</v>
+      </c>
+      <c r="B187" t="s">
+        <v>27</v>
+      </c>
+      <c r="C187" t="str">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
         <v>n</v>
       </c>
-      <c r="D187" s="9" t="s">
-        <v>1467</v>
-      </c>
-      <c r="E187" s="9" t="s">
-        <v>1473</v>
-      </c>
-      <c r="F187" s="9" t="str">
+      <c r="D187" t="s">
+        <v>1465</v>
+      </c>
+      <c r="E187" t="s">
+        <v>1472</v>
+      </c>
+      <c r="F187" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
-        <v>field element</v>
+        <v>simple field</v>
       </c>
       <c r="G187" t="s">
-        <v>972</v>
-      </c>
-      <c r="H187" s="9" t="s">
-        <v>1111</v>
+        <v>5</v>
+      </c>
+      <c r="H187" t="s">
+        <v>193</v>
       </c>
       <c r="I187" t="s">
         <v>2</v>
@@ -22656,83 +22663,85 @@
         <v>1332</v>
       </c>
       <c r="K187" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L187" t="s">
-        <v>985</v>
+        <v>608</v>
       </c>
       <c r="M187" t="s">
         <v>27</v>
       </c>
       <c r="N187" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="O187" t="s">
         <v>27</v>
       </c>
       <c r="P187" t="s">
-        <v>1108</v>
+        <v>27</v>
       </c>
       <c r="Q187" t="s">
-        <v>981</v>
+        <v>5</v>
       </c>
       <c r="R187" t="s">
-        <v>1027</v>
+        <v>65</v>
       </c>
       <c r="S187" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="T187" t="s">
-        <v>207</v>
-      </c>
-      <c r="U187" s="9" t="s">
-        <v>27</v>
+        <v>27</v>
+      </c>
+      <c r="U187" t="s">
+        <v>68</v>
       </c>
       <c r="V187" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="W187" t="s">
-        <v>356</v>
-      </c>
-      <c r="X187" s="9" t="s">
-        <v>1110</v>
+        <v>151</v>
+      </c>
+      <c r="X187" t="s">
+        <v>519</v>
       </c>
       <c r="Y187" t="s">
-        <v>617</v>
-      </c>
-      <c r="Z187" s="15">
+        <v>5</v>
+      </c>
+      <c r="Z187">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
         <v>0</v>
       </c>
-      <c r="AA187" s="9">
+      <c r="AA187">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>3</v>
-      </c>
-      <c r="AB187" s="9"/>
-      <c r="AC187" s="9" t="s">
-        <v>3</v>
+        <v>19</v>
+      </c>
+      <c r="AB187" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC187" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="188" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A188" s="9" t="s">
-        <v>1340</v>
-      </c>
-      <c r="B188" s="9" t="s">
         <v>1102</v>
       </c>
-      <c r="C188" s="9" t="str">
+      <c r="B188" t="s">
+        <v>27</v>
+      </c>
+      <c r="C188" t="str">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
-        <v>n</v>
-      </c>
-      <c r="D188" s="9" t="s">
-        <v>1466</v>
+        <v>y</v>
+      </c>
+      <c r="D188" t="s">
+        <v>1463</v>
       </c>
       <c r="E188" t="s">
         <v>770</v>
       </c>
-      <c r="F188" s="9" t="str">
+      <c r="F188" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
-        <v>field element</v>
+        <v>parent field</v>
       </c>
       <c r="G188" t="s">
         <v>972</v>
@@ -22747,13 +22756,13 @@
         <v>1332</v>
       </c>
       <c r="K188" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L188" t="s">
         <v>501</v>
       </c>
       <c r="M188" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="N188" t="s">
         <v>27</v>
@@ -22768,16 +22777,16 @@
         <v>5</v>
       </c>
       <c r="R188" t="s">
-        <v>1335</v>
+        <v>1025</v>
       </c>
       <c r="S188" t="s">
-        <v>1322</v>
+        <v>440</v>
       </c>
       <c r="T188" t="s">
-        <v>27</v>
+        <v>207</v>
       </c>
       <c r="U188" s="9" t="s">
-        <v>27</v>
+        <v>1109</v>
       </c>
       <c r="V188" t="s">
         <v>27</v>
@@ -22786,10 +22795,10 @@
         <v>356</v>
       </c>
       <c r="X188" s="9" t="s">
-        <v>1337</v>
+        <v>1110</v>
       </c>
       <c r="Y188" t="s">
-        <v>1039</v>
+        <v>617</v>
       </c>
       <c r="Z188" s="15">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
@@ -22797,7 +22806,7 @@
       </c>
       <c r="AA188" s="9">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB188" s="9" t="s">
         <v>2</v>
@@ -22808,7 +22817,7 @@
     </row>
     <row r="189" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A189" s="9" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="B189" s="9" t="s">
         <v>1102</v>
@@ -22840,10 +22849,10 @@
         <v>1332</v>
       </c>
       <c r="K189" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L189" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="M189" t="s">
         <v>27</v>
@@ -22858,10 +22867,10 @@
         <v>1108</v>
       </c>
       <c r="Q189" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="R189" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="S189" t="s">
         <v>27</v>
@@ -22870,7 +22879,7 @@
         <v>207</v>
       </c>
       <c r="U189" s="9" t="s">
-        <v>1109</v>
+        <v>27</v>
       </c>
       <c r="V189" t="s">
         <v>27</v>
@@ -22890,7 +22899,7 @@
       </c>
       <c r="AA189" s="9">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="AB189" s="9"/>
       <c r="AC189" s="9" t="s">
@@ -22899,7 +22908,7 @@
     </row>
     <row r="190" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A190" s="9" t="s">
-        <v>1105</v>
+        <v>1340</v>
       </c>
       <c r="B190" s="9" t="s">
         <v>1102</v>
@@ -22909,10 +22918,10 @@
         <v>n</v>
       </c>
       <c r="D190" s="9" t="s">
-        <v>1467</v>
-      </c>
-      <c r="E190" s="9" t="s">
-        <v>1473</v>
+        <v>1466</v>
+      </c>
+      <c r="E190" t="s">
+        <v>770</v>
       </c>
       <c r="F190" s="9" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
@@ -22934,7 +22943,7 @@
         <v>295</v>
       </c>
       <c r="L190" t="s">
-        <v>443</v>
+        <v>501</v>
       </c>
       <c r="M190" t="s">
         <v>27</v>
@@ -22952,16 +22961,16 @@
         <v>5</v>
       </c>
       <c r="R190" t="s">
-        <v>1031</v>
+        <v>1335</v>
       </c>
       <c r="S190" t="s">
-        <v>27</v>
+        <v>1322</v>
       </c>
       <c r="T190" t="s">
-        <v>207</v>
-      </c>
-      <c r="U190" s="24" t="s">
-        <v>1109</v>
+        <v>27</v>
+      </c>
+      <c r="U190" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="V190" t="s">
         <v>27</v>
@@ -22970,10 +22979,10 @@
         <v>356</v>
       </c>
       <c r="X190" s="9" t="s">
-        <v>1110</v>
+        <v>1337</v>
       </c>
       <c r="Y190" t="s">
-        <v>617</v>
+        <v>1039</v>
       </c>
       <c r="Z190" s="15">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
@@ -22981,16 +22990,18 @@
       </c>
       <c r="AA190" s="9">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>3</v>
-      </c>
-      <c r="AB190" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="AB190" s="9" t="s">
+        <v>2</v>
+      </c>
       <c r="AC190" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="191" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A191" s="9" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="B191" s="9" t="s">
         <v>1102</v>
@@ -23022,10 +23033,10 @@
         <v>1332</v>
       </c>
       <c r="K191" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="L191" t="s">
-        <v>443</v>
+        <v>986</v>
       </c>
       <c r="M191" t="s">
         <v>27</v>
@@ -23040,10 +23051,10 @@
         <v>1108</v>
       </c>
       <c r="Q191" t="s">
-        <v>1007</v>
+        <v>983</v>
       </c>
       <c r="R191" t="s">
-        <v>1033</v>
+        <v>1029</v>
       </c>
       <c r="S191" t="s">
         <v>27</v>
@@ -23072,7 +23083,7 @@
       </c>
       <c r="AA191" s="9">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="AB191" s="9"/>
       <c r="AC191" s="9" t="s">
@@ -23081,7 +23092,7 @@
     </row>
     <row r="192" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A192" s="9" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="B192" s="9" t="s">
         <v>1102</v>
@@ -23090,11 +23101,11 @@
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
         <v>n</v>
       </c>
-      <c r="D192" t="s">
-        <v>1464</v>
-      </c>
-      <c r="E192" t="s">
-        <v>770</v>
+      <c r="D192" s="9" t="s">
+        <v>1467</v>
+      </c>
+      <c r="E192" s="9" t="s">
+        <v>1473</v>
       </c>
       <c r="F192" s="9" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
@@ -23113,10 +23124,10 @@
         <v>1332</v>
       </c>
       <c r="K192" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L192" t="s">
-        <v>501</v>
+        <v>443</v>
       </c>
       <c r="M192" t="s">
         <v>27</v>
@@ -23134,16 +23145,16 @@
         <v>5</v>
       </c>
       <c r="R192" t="s">
-        <v>979</v>
+        <v>1031</v>
       </c>
       <c r="S192" t="s">
-        <v>980</v>
+        <v>27</v>
       </c>
       <c r="T192" t="s">
-        <v>27</v>
-      </c>
-      <c r="U192" s="9" t="s">
-        <v>27</v>
+        <v>207</v>
+      </c>
+      <c r="U192" s="24" t="s">
+        <v>1109</v>
       </c>
       <c r="V192" t="s">
         <v>27</v>
@@ -23163,7 +23174,7 @@
       </c>
       <c r="AA192" s="9">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AB192" s="9"/>
       <c r="AC192" s="9" t="s">
@@ -23172,30 +23183,30 @@
     </row>
     <row r="193" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A193" s="9" t="s">
-        <v>197</v>
+        <v>1106</v>
       </c>
       <c r="B193" s="9" t="s">
-        <v>27</v>
+        <v>1102</v>
       </c>
       <c r="C193" s="9" t="str">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
-        <v>y</v>
-      </c>
-      <c r="D193" t="s">
-        <v>1463</v>
-      </c>
-      <c r="E193" t="s">
-        <v>770</v>
+        <v>n</v>
+      </c>
+      <c r="D193" s="9" t="s">
+        <v>1467</v>
+      </c>
+      <c r="E193" s="9" t="s">
+        <v>1473</v>
       </c>
       <c r="F193" s="9" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
-        <v>parent field</v>
+        <v>field element</v>
       </c>
       <c r="G193" t="s">
-        <v>5</v>
+        <v>972</v>
       </c>
       <c r="H193" s="9" t="s">
-        <v>199</v>
+        <v>1111</v>
       </c>
       <c r="I193" t="s">
         <v>2</v>
@@ -23204,13 +23215,13 @@
         <v>1332</v>
       </c>
       <c r="K193" t="s">
-        <v>316</v>
+        <v>295</v>
       </c>
       <c r="L193" t="s">
-        <v>501</v>
+        <v>443</v>
       </c>
       <c r="M193" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="N193" t="s">
         <v>27</v>
@@ -23219,22 +23230,22 @@
         <v>27</v>
       </c>
       <c r="P193" t="s">
-        <v>27</v>
+        <v>1108</v>
       </c>
       <c r="Q193" t="s">
-        <v>5</v>
+        <v>1007</v>
       </c>
       <c r="R193" t="s">
-        <v>1319</v>
+        <v>1033</v>
       </c>
       <c r="S193" t="s">
         <v>27</v>
       </c>
       <c r="T193" t="s">
-        <v>27</v>
-      </c>
-      <c r="U193" s="16" t="s">
-        <v>203</v>
+        <v>207</v>
+      </c>
+      <c r="U193" s="9" t="s">
+        <v>1109</v>
       </c>
       <c r="V193" t="s">
         <v>27</v>
@@ -23243,10 +23254,10 @@
         <v>356</v>
       </c>
       <c r="X193" s="9" t="s">
-        <v>1320</v>
+        <v>1110</v>
       </c>
       <c r="Y193" t="s">
-        <v>1321</v>
+        <v>617</v>
       </c>
       <c r="Z193" s="15">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
@@ -23254,41 +23265,39 @@
       </c>
       <c r="AA193" s="9">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AB193" s="9" t="s">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AB193" s="9"/>
       <c r="AC193" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="194" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
-        <v>1328</v>
-      </c>
-      <c r="B194" t="s">
-        <v>197</v>
-      </c>
-      <c r="C194" t="str">
+      <c r="A194" s="9" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B194" s="9" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C194" s="9" t="str">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
         <v>n</v>
       </c>
-      <c r="D194" s="9" t="s">
-        <v>1466</v>
+      <c r="D194" t="s">
+        <v>1464</v>
       </c>
       <c r="E194" t="s">
         <v>770</v>
       </c>
-      <c r="F194" t="str">
+      <c r="F194" s="9" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
         <v>field element</v>
       </c>
       <c r="G194" t="s">
-        <v>5</v>
-      </c>
-      <c r="H194" t="s">
-        <v>199</v>
+        <v>972</v>
+      </c>
+      <c r="H194" s="9" t="s">
+        <v>1111</v>
       </c>
       <c r="I194" t="s">
         <v>2</v>
@@ -23297,7 +23306,7 @@
         <v>1332</v>
       </c>
       <c r="K194" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="L194" t="s">
         <v>501</v>
@@ -23314,16 +23323,19 @@
       <c r="P194" t="s">
         <v>27</v>
       </c>
+      <c r="Q194" t="s">
+        <v>5</v>
+      </c>
       <c r="R194" t="s">
-        <v>1335</v>
+        <v>979</v>
       </c>
       <c r="S194" t="s">
-        <v>1322</v>
+        <v>980</v>
       </c>
       <c r="T194" t="s">
         <v>27</v>
       </c>
-      <c r="U194" t="s">
+      <c r="U194" s="9" t="s">
         <v>27</v>
       </c>
       <c r="V194" t="s">
@@ -23332,420 +23344,415 @@
       <c r="W194" t="s">
         <v>356</v>
       </c>
-      <c r="X194" t="s">
-        <v>1337</v>
+      <c r="X194" s="9" t="s">
+        <v>1110</v>
       </c>
       <c r="Y194" t="s">
-        <v>1341</v>
-      </c>
-      <c r="Z194" s="8">
+        <v>617</v>
+      </c>
+      <c r="Z194" s="15">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
         <v>0</v>
       </c>
-      <c r="AA194">
+      <c r="AA194" s="9">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
         <v>1</v>
       </c>
-      <c r="AB194" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC194" t="s">
+      <c r="AB194" s="9"/>
+      <c r="AC194" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="195" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
-        <v>611</v>
-      </c>
-      <c r="B195" t="s">
+      <c r="A195" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="C195" t="str">
+      <c r="B195" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C195" s="9" t="str">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
-        <v>n</v>
+        <v>y</v>
       </c>
       <c r="D195" t="s">
-        <v>1467</v>
+        <v>1463</v>
       </c>
       <c r="E195" t="s">
-        <v>1474</v>
-      </c>
-      <c r="F195" t="str">
+        <v>770</v>
+      </c>
+      <c r="F195" s="9" t="str">
+        <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
+        <v>parent field</v>
+      </c>
+      <c r="G195" t="s">
+        <v>5</v>
+      </c>
+      <c r="H195" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="I195" t="s">
+        <v>2</v>
+      </c>
+      <c r="J195" t="s">
+        <v>1332</v>
+      </c>
+      <c r="K195" t="s">
+        <v>316</v>
+      </c>
+      <c r="L195" t="s">
+        <v>501</v>
+      </c>
+      <c r="M195" t="s">
+        <v>3</v>
+      </c>
+      <c r="N195" t="s">
+        <v>27</v>
+      </c>
+      <c r="O195" t="s">
+        <v>27</v>
+      </c>
+      <c r="P195" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q195" t="s">
+        <v>5</v>
+      </c>
+      <c r="R195" t="s">
+        <v>1319</v>
+      </c>
+      <c r="S195" t="s">
+        <v>27</v>
+      </c>
+      <c r="T195" t="s">
+        <v>27</v>
+      </c>
+      <c r="U195" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="V195" t="s">
+        <v>27</v>
+      </c>
+      <c r="W195" t="s">
+        <v>356</v>
+      </c>
+      <c r="X195" s="9" t="s">
+        <v>1320</v>
+      </c>
+      <c r="Y195" t="s">
+        <v>1321</v>
+      </c>
+      <c r="Z195" s="15">
+        <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA195" s="9">
+        <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB195" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC195" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="196" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B196" t="s">
+        <v>197</v>
+      </c>
+      <c r="C196" t="str">
+        <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
+        <v>n</v>
+      </c>
+      <c r="D196" s="9" t="s">
+        <v>1466</v>
+      </c>
+      <c r="E196" t="s">
+        <v>770</v>
+      </c>
+      <c r="F196" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
         <v>field element</v>
       </c>
-      <c r="G195" t="s">
-        <v>5</v>
-      </c>
-      <c r="H195" t="s">
+      <c r="G196" t="s">
+        <v>5</v>
+      </c>
+      <c r="H196" t="s">
         <v>199</v>
       </c>
-      <c r="I195" t="s">
-        <v>2</v>
-      </c>
-      <c r="J195" t="s">
+      <c r="I196" t="s">
+        <v>2</v>
+      </c>
+      <c r="J196" t="s">
         <v>1332</v>
       </c>
-      <c r="K195" t="s">
+      <c r="K196" t="s">
+        <v>295</v>
+      </c>
+      <c r="L196" t="s">
+        <v>501</v>
+      </c>
+      <c r="M196" t="s">
+        <v>27</v>
+      </c>
+      <c r="N196" t="s">
+        <v>27</v>
+      </c>
+      <c r="O196" t="s">
+        <v>27</v>
+      </c>
+      <c r="P196" t="s">
+        <v>27</v>
+      </c>
+      <c r="R196" t="s">
+        <v>1335</v>
+      </c>
+      <c r="S196" t="s">
+        <v>1322</v>
+      </c>
+      <c r="T196" t="s">
+        <v>27</v>
+      </c>
+      <c r="U196" t="s">
+        <v>27</v>
+      </c>
+      <c r="V196" t="s">
+        <v>27</v>
+      </c>
+      <c r="W196" t="s">
+        <v>356</v>
+      </c>
+      <c r="X196" t="s">
+        <v>1337</v>
+      </c>
+      <c r="Y196" t="s">
+        <v>1341</v>
+      </c>
+      <c r="Z196" s="8">
+        <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA196">
+        <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AB196" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC196" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="197" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>611</v>
+      </c>
+      <c r="B197" t="s">
+        <v>197</v>
+      </c>
+      <c r="C197" t="str">
+        <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
+        <v>n</v>
+      </c>
+      <c r="D197" t="s">
+        <v>1467</v>
+      </c>
+      <c r="E197" t="s">
+        <v>1474</v>
+      </c>
+      <c r="F197" t="str">
+        <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
+        <v>field element</v>
+      </c>
+      <c r="G197" t="s">
+        <v>5</v>
+      </c>
+      <c r="H197" t="s">
+        <v>199</v>
+      </c>
+      <c r="I197" t="s">
+        <v>2</v>
+      </c>
+      <c r="J197" t="s">
+        <v>1332</v>
+      </c>
+      <c r="K197" t="s">
         <v>296</v>
       </c>
-      <c r="L195" t="s">
+      <c r="L197" t="s">
         <v>443</v>
       </c>
-      <c r="M195" t="s">
-        <v>27</v>
-      </c>
-      <c r="N195" t="s">
-        <v>27</v>
-      </c>
-      <c r="O195" t="s">
+      <c r="M197" t="s">
+        <v>27</v>
+      </c>
+      <c r="N197" t="s">
+        <v>27</v>
+      </c>
+      <c r="O197" t="s">
         <v>502</v>
       </c>
-      <c r="P195" t="s">
+      <c r="P197" t="s">
         <v>602</v>
       </c>
-      <c r="Q195" t="s">
-        <v>5</v>
-      </c>
-      <c r="R195" t="s">
+      <c r="Q197" t="s">
+        <v>5</v>
+      </c>
+      <c r="R197" t="s">
         <v>612</v>
       </c>
-      <c r="S195" t="s">
-        <v>5</v>
-      </c>
-      <c r="T195" t="s">
+      <c r="S197" t="s">
+        <v>5</v>
+      </c>
+      <c r="T197" t="s">
         <v>613</v>
       </c>
-      <c r="U195" t="s">
+      <c r="U197" t="s">
         <v>203</v>
       </c>
-      <c r="V195" t="s">
-        <v>27</v>
-      </c>
-      <c r="W195" t="s">
+      <c r="V197" t="s">
+        <v>27</v>
+      </c>
+      <c r="W197" t="s">
         <v>356</v>
       </c>
-      <c r="X195" s="9" t="s">
+      <c r="X197" s="9" t="s">
         <v>1320</v>
       </c>
-      <c r="Y195" t="s">
+      <c r="Y197" t="s">
         <v>1321</v>
       </c>
-      <c r="Z195" s="8">
+      <c r="Z197" s="8">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
         <v>0</v>
       </c>
-      <c r="AA195">
+      <c r="AA197">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
         <v>1</v>
       </c>
-      <c r="AB195" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC195" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="196" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
+      <c r="AB197" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC197" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="198" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
         <v>1323</v>
       </c>
-      <c r="B196" t="s">
-        <v>27</v>
-      </c>
-      <c r="C196" t="str">
+      <c r="B198" t="s">
+        <v>27</v>
+      </c>
+      <c r="C198" t="str">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
         <v>n</v>
       </c>
-      <c r="D196" t="s">
+      <c r="D198" t="s">
         <v>1465</v>
       </c>
-      <c r="E196" t="s">
+      <c r="E198" t="s">
         <v>1472</v>
       </c>
-      <c r="F196" t="str">
+      <c r="F198" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
         <v>simple field</v>
       </c>
-      <c r="G196" t="s">
-        <v>5</v>
-      </c>
-      <c r="H196" t="s">
+      <c r="G198" t="s">
+        <v>5</v>
+      </c>
+      <c r="H198" t="s">
         <v>199</v>
       </c>
-      <c r="I196" t="s">
-        <v>2</v>
-      </c>
-      <c r="J196" t="s">
+      <c r="I198" t="s">
+        <v>2</v>
+      </c>
+      <c r="J198" t="s">
         <v>1332</v>
       </c>
-      <c r="K196" t="s">
+      <c r="K198" t="s">
         <v>296</v>
       </c>
-      <c r="L196" t="s">
+      <c r="L198" t="s">
         <v>1471</v>
       </c>
-      <c r="M196" t="s">
-        <v>27</v>
-      </c>
-      <c r="N196" t="s">
-        <v>27</v>
-      </c>
-      <c r="O196" t="s">
-        <v>27</v>
-      </c>
-      <c r="P196" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q196" t="s">
-        <v>27</v>
-      </c>
-      <c r="R196" t="s">
+      <c r="M198" t="s">
+        <v>27</v>
+      </c>
+      <c r="N198" t="s">
+        <v>27</v>
+      </c>
+      <c r="O198" t="s">
+        <v>27</v>
+      </c>
+      <c r="P198" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q198" t="s">
+        <v>27</v>
+      </c>
+      <c r="R198" t="s">
         <v>1324</v>
       </c>
-      <c r="S196" t="s">
+      <c r="S198" t="s">
         <v>1325</v>
       </c>
-      <c r="T196" t="s">
+      <c r="T198" t="s">
         <v>613</v>
       </c>
-      <c r="U196" t="s">
+      <c r="U198" t="s">
         <v>614</v>
       </c>
-      <c r="V196" t="s">
-        <v>27</v>
-      </c>
-      <c r="W196" t="s">
+      <c r="V198" t="s">
+        <v>27</v>
+      </c>
+      <c r="W198" t="s">
         <v>356</v>
       </c>
-      <c r="X196" s="9" t="s">
+      <c r="X198" s="9" t="s">
         <v>1326</v>
       </c>
-      <c r="Y196" t="s">
+      <c r="Y198" t="s">
         <v>1321</v>
       </c>
-      <c r="Z196" s="8">
+      <c r="Z198" s="8">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
         <v>0</v>
       </c>
-      <c r="AA196">
+      <c r="AA198">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
         <v>1</v>
       </c>
-      <c r="AB196" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC196" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="197" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
+      <c r="AB198" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC198" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="199" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
         <v>874</v>
       </c>
-      <c r="B197" t="s">
-        <v>27</v>
-      </c>
-      <c r="C197" t="str">
+      <c r="B199" t="s">
+        <v>27</v>
+      </c>
+      <c r="C199" t="str">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
         <v>y</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D199" t="s">
         <v>1463</v>
       </c>
-      <c r="E197" t="s">
+      <c r="E199" t="s">
         <v>770</v>
       </c>
-      <c r="F197" t="str">
+      <c r="F199" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
         <v>parent field</v>
       </c>
-      <c r="G197" t="s">
-        <v>5</v>
-      </c>
-      <c r="H197" t="s">
-        <v>199</v>
-      </c>
-      <c r="I197" t="s">
-        <v>2</v>
-      </c>
-      <c r="J197" t="s">
-        <v>1332</v>
-      </c>
-      <c r="K197" t="s">
-        <v>294</v>
-      </c>
-      <c r="L197" t="s">
-        <v>501</v>
-      </c>
-      <c r="M197" t="s">
-        <v>3</v>
-      </c>
-      <c r="N197" t="s">
-        <v>27</v>
-      </c>
-      <c r="O197" t="s">
-        <v>27</v>
-      </c>
-      <c r="P197" t="s">
-        <v>880</v>
-      </c>
-      <c r="Q197" t="s">
-        <v>5</v>
-      </c>
-      <c r="R197" t="s">
-        <v>881</v>
-      </c>
-      <c r="S197" t="s">
-        <v>5</v>
-      </c>
-      <c r="T197" t="s">
-        <v>27</v>
-      </c>
-      <c r="U197" t="s">
-        <v>610</v>
-      </c>
-      <c r="V197" t="s">
-        <v>27</v>
-      </c>
-      <c r="W197" t="s">
-        <v>356</v>
-      </c>
-      <c r="X197" t="s">
-        <v>882</v>
-      </c>
-      <c r="Y197" t="s">
-        <v>883</v>
-      </c>
-      <c r="Z197" s="8">
-        <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AA197">
-        <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AB197" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC197" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="198" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
-        <v>879</v>
-      </c>
-      <c r="B198" t="s">
-        <v>874</v>
-      </c>
-      <c r="C198" t="str">
-        <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
-        <v>n</v>
-      </c>
-      <c r="D198" t="s">
-        <v>1464</v>
-      </c>
-      <c r="E198" t="s">
-        <v>770</v>
-      </c>
-      <c r="F198" t="str">
-        <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
-        <v>field element</v>
-      </c>
-      <c r="G198" t="s">
-        <v>5</v>
-      </c>
-      <c r="H198" t="s">
-        <v>199</v>
-      </c>
-      <c r="I198" t="s">
-        <v>2</v>
-      </c>
-      <c r="J198" t="s">
-        <v>1332</v>
-      </c>
-      <c r="K198" t="s">
-        <v>295</v>
-      </c>
-      <c r="L198" t="s">
-        <v>501</v>
-      </c>
-      <c r="M198" t="s">
-        <v>27</v>
-      </c>
-      <c r="N198" t="s">
-        <v>27</v>
-      </c>
-      <c r="O198" t="s">
-        <v>27</v>
-      </c>
-      <c r="P198" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q198" t="s">
-        <v>5</v>
-      </c>
-      <c r="R198" t="s">
-        <v>890</v>
-      </c>
-      <c r="S198" t="s">
-        <v>891</v>
-      </c>
-      <c r="T198" t="s">
-        <v>27</v>
-      </c>
-      <c r="U198" t="s">
-        <v>27</v>
-      </c>
-      <c r="V198" t="s">
-        <v>27</v>
-      </c>
-      <c r="W198" t="s">
-        <v>356</v>
-      </c>
-      <c r="X198" t="s">
-        <v>882</v>
-      </c>
-      <c r="Y198" t="s">
-        <v>883</v>
-      </c>
-      <c r="Z198" s="8">
-        <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AA198">
-        <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>4</v>
-      </c>
-      <c r="AB198" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC198" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="199" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
-        <v>878</v>
-      </c>
-      <c r="B199" t="s">
-        <v>874</v>
-      </c>
-      <c r="C199" t="str">
-        <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
-        <v>n</v>
-      </c>
-      <c r="D199" t="s">
-        <v>1467</v>
-      </c>
-      <c r="E199" t="s">
-        <v>1476</v>
-      </c>
-      <c r="F199" t="str">
-        <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
-        <v>field element</v>
-      </c>
       <c r="G199" t="s">
         <v>5</v>
       </c>
@@ -23759,13 +23766,13 @@
         <v>1332</v>
       </c>
       <c r="K199" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L199" t="s">
-        <v>443</v>
+        <v>501</v>
       </c>
       <c r="M199" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="N199" t="s">
         <v>27</v>
@@ -23774,22 +23781,22 @@
         <v>27</v>
       </c>
       <c r="P199" t="s">
-        <v>27</v>
+        <v>880</v>
       </c>
       <c r="Q199" t="s">
         <v>5</v>
       </c>
       <c r="R199" t="s">
-        <v>889</v>
+        <v>881</v>
       </c>
       <c r="S199" t="s">
         <v>5</v>
       </c>
       <c r="T199" t="s">
-        <v>207</v>
+        <v>27</v>
       </c>
       <c r="U199" t="s">
-        <v>27</v>
+        <v>610</v>
       </c>
       <c r="V199" t="s">
         <v>27</v>
@@ -23809,7 +23816,7 @@
       </c>
       <c r="AA199">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB199" t="s">
         <v>2</v>
@@ -23820,7 +23827,7 @@
     </row>
     <row r="200" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>992</v>
+        <v>879</v>
       </c>
       <c r="B200" t="s">
         <v>874</v>
@@ -23855,7 +23862,7 @@
         <v>295</v>
       </c>
       <c r="L200" t="s">
-        <v>444</v>
+        <v>501</v>
       </c>
       <c r="M200" t="s">
         <v>27</v>
@@ -23867,16 +23874,16 @@
         <v>27</v>
       </c>
       <c r="P200" t="s">
-        <v>880</v>
+        <v>27</v>
       </c>
       <c r="Q200" t="s">
-        <v>993</v>
+        <v>5</v>
       </c>
       <c r="R200" t="s">
-        <v>994</v>
+        <v>890</v>
       </c>
       <c r="S200" t="s">
-        <v>5</v>
+        <v>891</v>
       </c>
       <c r="T200" t="s">
         <v>27</v>
@@ -23902,7 +23909,7 @@
       </c>
       <c r="AA200">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AB200" t="s">
         <v>2</v>
@@ -23913,7 +23920,7 @@
     </row>
     <row r="201" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c r="B201" t="s">
         <v>874</v>
@@ -23923,10 +23930,10 @@
         <v>n</v>
       </c>
       <c r="D201" t="s">
-        <v>1465</v>
+        <v>1467</v>
       </c>
       <c r="E201" t="s">
-        <v>1472</v>
+        <v>1476</v>
       </c>
       <c r="F201" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
@@ -23948,7 +23955,7 @@
         <v>295</v>
       </c>
       <c r="L201" t="s">
-        <v>501</v>
+        <v>443</v>
       </c>
       <c r="M201" t="s">
         <v>27</v>
@@ -23960,19 +23967,19 @@
         <v>27</v>
       </c>
       <c r="P201" t="s">
-        <v>880</v>
+        <v>27</v>
       </c>
       <c r="Q201" t="s">
-        <v>888</v>
+        <v>5</v>
       </c>
       <c r="R201" t="s">
-        <v>886</v>
+        <v>889</v>
       </c>
       <c r="S201" t="s">
         <v>5</v>
       </c>
       <c r="T201" t="s">
-        <v>27</v>
+        <v>207</v>
       </c>
       <c r="U201" t="s">
         <v>27</v>
@@ -23995,7 +24002,7 @@
       </c>
       <c r="AA201">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AB201" t="s">
         <v>2</v>
@@ -24006,7 +24013,7 @@
     </row>
     <row r="202" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>875</v>
+        <v>992</v>
       </c>
       <c r="B202" t="s">
         <v>874</v>
@@ -24041,7 +24048,7 @@
         <v>295</v>
       </c>
       <c r="L202" t="s">
-        <v>501</v>
+        <v>444</v>
       </c>
       <c r="M202" t="s">
         <v>27</v>
@@ -24053,13 +24060,13 @@
         <v>27</v>
       </c>
       <c r="P202" t="s">
-        <v>27</v>
+        <v>880</v>
       </c>
       <c r="Q202" t="s">
-        <v>884</v>
+        <v>993</v>
       </c>
       <c r="R202" t="s">
-        <v>885</v>
+        <v>994</v>
       </c>
       <c r="S202" t="s">
         <v>5</v>
@@ -24088,7 +24095,7 @@
       </c>
       <c r="AA202">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AB202" t="s">
         <v>2</v>
@@ -24099,7 +24106,7 @@
     </row>
     <row r="203" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="B203" t="s">
         <v>874</v>
@@ -24109,10 +24116,10 @@
         <v>n</v>
       </c>
       <c r="D203" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
       <c r="E203" t="s">
-        <v>1476</v>
+        <v>1472</v>
       </c>
       <c r="F203" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
@@ -24131,10 +24138,10 @@
         <v>1332</v>
       </c>
       <c r="K203" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L203" t="s">
-        <v>443</v>
+        <v>501</v>
       </c>
       <c r="M203" t="s">
         <v>27</v>
@@ -24152,13 +24159,13 @@
         <v>888</v>
       </c>
       <c r="R203" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="S203" t="s">
         <v>5</v>
       </c>
       <c r="T203" t="s">
-        <v>207</v>
+        <v>27</v>
       </c>
       <c r="U203" t="s">
         <v>27</v>
@@ -24181,7 +24188,7 @@
       </c>
       <c r="AA203">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AB203" t="s">
         <v>2</v>
@@ -24192,30 +24199,30 @@
     </row>
     <row r="204" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>271</v>
+        <v>875</v>
       </c>
       <c r="B204" t="s">
-        <v>27</v>
+        <v>874</v>
       </c>
       <c r="C204" t="str">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
-        <v>y</v>
+        <v>n</v>
       </c>
       <c r="D204" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="E204" t="s">
         <v>770</v>
       </c>
       <c r="F204" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
-        <v>parent field</v>
+        <v>field element</v>
       </c>
       <c r="G204" t="s">
-        <v>285</v>
+        <v>5</v>
       </c>
       <c r="H204" t="s">
-        <v>259</v>
+        <v>199</v>
       </c>
       <c r="I204" t="s">
         <v>2</v>
@@ -24224,13 +24231,13 @@
         <v>1332</v>
       </c>
       <c r="K204" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="L204" t="s">
-        <v>444</v>
+        <v>501</v>
       </c>
       <c r="M204" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="N204" t="s">
         <v>27</v>
@@ -24239,16 +24246,16 @@
         <v>27</v>
       </c>
       <c r="P204" t="s">
-        <v>620</v>
+        <v>27</v>
       </c>
       <c r="Q204" t="s">
-        <v>5</v>
+        <v>884</v>
       </c>
       <c r="R204" t="s">
-        <v>621</v>
+        <v>885</v>
       </c>
       <c r="S204" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="T204" t="s">
         <v>27</v>
@@ -24257,16 +24264,16 @@
         <v>27</v>
       </c>
       <c r="V204" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="W204" t="s">
-        <v>1182</v>
+        <v>356</v>
       </c>
       <c r="X204" t="s">
-        <v>563</v>
+        <v>882</v>
       </c>
       <c r="Y204" t="s">
-        <v>624</v>
+        <v>883</v>
       </c>
       <c r="Z204" s="8">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
@@ -24274,41 +24281,41 @@
       </c>
       <c r="AA204">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AB204" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AC204" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="205" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>1179</v>
+        <v>877</v>
       </c>
       <c r="B205" t="s">
-        <v>271</v>
+        <v>874</v>
       </c>
       <c r="C205" t="str">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
         <v>n</v>
       </c>
       <c r="D205" t="s">
-        <v>1465</v>
+        <v>1467</v>
       </c>
       <c r="E205" t="s">
-        <v>1472</v>
+        <v>1476</v>
       </c>
       <c r="F205" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
         <v>field element</v>
       </c>
       <c r="G205" t="s">
-        <v>285</v>
+        <v>5</v>
       </c>
       <c r="H205" t="s">
-        <v>259</v>
+        <v>199</v>
       </c>
       <c r="I205" t="s">
         <v>2</v>
@@ -24317,13 +24324,13 @@
         <v>1332</v>
       </c>
       <c r="K205" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="L205" t="s">
-        <v>501</v>
+        <v>443</v>
       </c>
       <c r="M205" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="N205" t="s">
         <v>27</v>
@@ -24332,34 +24339,34 @@
         <v>27</v>
       </c>
       <c r="P205" t="s">
-        <v>620</v>
+        <v>880</v>
       </c>
       <c r="Q205" t="s">
-        <v>5</v>
+        <v>888</v>
       </c>
       <c r="R205" t="s">
-        <v>276</v>
+        <v>887</v>
       </c>
       <c r="S205" t="s">
-        <v>623</v>
+        <v>5</v>
       </c>
       <c r="T205" t="s">
-        <v>27</v>
+        <v>207</v>
       </c>
       <c r="U205" t="s">
         <v>27</v>
       </c>
       <c r="V205" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="W205" t="s">
-        <v>1182</v>
+        <v>356</v>
       </c>
       <c r="X205" t="s">
-        <v>563</v>
+        <v>882</v>
       </c>
       <c r="Y205" t="s">
-        <v>624</v>
+        <v>883</v>
       </c>
       <c r="Z205" s="8">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
@@ -24367,35 +24374,35 @@
       </c>
       <c r="AA205">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AB205" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AC205" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="206" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>1180</v>
+        <v>271</v>
       </c>
       <c r="B206" t="s">
-        <v>271</v>
+        <v>27</v>
       </c>
       <c r="C206" t="str">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
-        <v>n</v>
+        <v>y</v>
       </c>
       <c r="D206" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="E206" t="s">
         <v>770</v>
       </c>
       <c r="F206" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
-        <v>field element</v>
+        <v>parent field</v>
       </c>
       <c r="G206" t="s">
         <v>285</v>
@@ -24410,13 +24417,13 @@
         <v>1332</v>
       </c>
       <c r="K206" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="L206" t="s">
-        <v>501</v>
+        <v>444</v>
       </c>
       <c r="M206" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="N206" t="s">
         <v>27</v>
@@ -24431,7 +24438,7 @@
         <v>5</v>
       </c>
       <c r="R206" t="s">
-        <v>1181</v>
+        <v>621</v>
       </c>
       <c r="S206" t="s">
         <v>27</v>
@@ -24443,7 +24450,7 @@
         <v>27</v>
       </c>
       <c r="V206" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="W206" t="s">
         <v>1182</v>
@@ -24460,7 +24467,7 @@
       </c>
       <c r="AA206">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB206" t="s">
         <v>5</v>
@@ -24471,7 +24478,7 @@
     </row>
     <row r="207" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>619</v>
+        <v>1179</v>
       </c>
       <c r="B207" t="s">
         <v>271</v>
@@ -24481,10 +24488,10 @@
         <v>n</v>
       </c>
       <c r="D207" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="E207" t="s">
-        <v>770</v>
+        <v>1472</v>
       </c>
       <c r="F207" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
@@ -24503,13 +24510,13 @@
         <v>1332</v>
       </c>
       <c r="K207" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="L207" t="s">
-        <v>444</v>
+        <v>501</v>
       </c>
       <c r="M207" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="N207" t="s">
         <v>27</v>
@@ -24524,19 +24531,19 @@
         <v>5</v>
       </c>
       <c r="R207" t="s">
-        <v>622</v>
+        <v>276</v>
       </c>
       <c r="S207" t="s">
-        <v>274</v>
+        <v>623</v>
       </c>
       <c r="T207" t="s">
         <v>27</v>
       </c>
-      <c r="U207" s="23" t="s">
-        <v>275</v>
+      <c r="U207" t="s">
+        <v>27</v>
       </c>
       <c r="V207" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="W207" t="s">
         <v>1182</v>
@@ -24553,7 +24560,7 @@
       </c>
       <c r="AA207">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB207" t="s">
         <v>5</v>
@@ -24564,81 +24571,81 @@
     </row>
     <row r="208" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>324</v>
+        <v>1180</v>
       </c>
       <c r="B208" t="s">
-        <v>27</v>
+        <v>271</v>
       </c>
       <c r="C208" t="str">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
-        <v>y</v>
+        <v>n</v>
       </c>
       <c r="D208" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="E208" t="s">
         <v>770</v>
       </c>
       <c r="F208" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
-        <v>parent field</v>
+        <v>field element</v>
       </c>
       <c r="G208" t="s">
-        <v>5</v>
+        <v>285</v>
       </c>
       <c r="H208" t="s">
-        <v>324</v>
+        <v>259</v>
       </c>
       <c r="I208" t="s">
         <v>2</v>
       </c>
       <c r="J208" t="s">
-        <v>54</v>
+        <v>1332</v>
       </c>
       <c r="K208" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="L208" t="s">
         <v>501</v>
       </c>
       <c r="M208" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="N208" t="s">
         <v>27</v>
       </c>
       <c r="O208" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="P208" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="Q208" t="s">
         <v>5</v>
       </c>
       <c r="R208" t="s">
-        <v>5</v>
+        <v>1181</v>
       </c>
       <c r="S208" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="T208" t="s">
         <v>27</v>
       </c>
       <c r="U208" t="s">
-        <v>325</v>
+        <v>27</v>
       </c>
       <c r="V208" t="s">
         <v>27</v>
       </c>
       <c r="W208" t="s">
-        <v>5</v>
+        <v>1182</v>
       </c>
       <c r="X208" t="s">
-        <v>519</v>
+        <v>563</v>
       </c>
       <c r="Y208" t="s">
-        <v>5</v>
+        <v>624</v>
       </c>
       <c r="Z208" s="8">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
@@ -24646,21 +24653,21 @@
       </c>
       <c r="AA208">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB208" t="s">
         <v>5</v>
       </c>
       <c r="AC208" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="209" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>323</v>
+        <v>619</v>
       </c>
       <c r="B209" t="s">
-        <v>324</v>
+        <v>271</v>
       </c>
       <c r="C209" t="str">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
@@ -24677,22 +24684,22 @@
         <v>field element</v>
       </c>
       <c r="G209" t="s">
-        <v>5</v>
+        <v>285</v>
       </c>
       <c r="H209" t="s">
-        <v>324</v>
+        <v>259</v>
       </c>
       <c r="I209" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J209" t="s">
-        <v>54</v>
+        <v>1332</v>
       </c>
       <c r="K209" t="s">
         <v>296</v>
       </c>
       <c r="L209" t="s">
-        <v>501</v>
+        <v>444</v>
       </c>
       <c r="M209" t="s">
         <v>27</v>
@@ -24704,34 +24711,34 @@
         <v>27</v>
       </c>
       <c r="P209" t="s">
-        <v>27</v>
+        <v>620</v>
       </c>
       <c r="Q209" t="s">
         <v>5</v>
       </c>
       <c r="R209" t="s">
-        <v>332</v>
+        <v>622</v>
       </c>
       <c r="S209" t="s">
-        <v>333</v>
+        <v>274</v>
       </c>
       <c r="T209" t="s">
         <v>27</v>
       </c>
-      <c r="U209" s="16" t="s">
-        <v>27</v>
+      <c r="U209" s="23" t="s">
+        <v>275</v>
       </c>
       <c r="V209" t="s">
         <v>27</v>
       </c>
       <c r="W209" t="s">
-        <v>5</v>
+        <v>1182</v>
       </c>
       <c r="X209" t="s">
-        <v>519</v>
+        <v>563</v>
       </c>
       <c r="Y209" t="s">
-        <v>5</v>
+        <v>624</v>
       </c>
       <c r="Z209" s="8">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
@@ -24739,35 +24746,35 @@
       </c>
       <c r="AA209">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB209" t="s">
         <v>5</v>
       </c>
       <c r="AC209" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="210" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="B210" t="s">
-        <v>324</v>
+        <v>27</v>
       </c>
       <c r="C210" t="str">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
-        <v>n</v>
+        <v>y</v>
       </c>
       <c r="D210" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="E210" t="s">
         <v>770</v>
       </c>
       <c r="F210" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
-        <v>field element</v>
+        <v>parent field</v>
       </c>
       <c r="G210" t="s">
         <v>5</v>
@@ -24782,13 +24789,13 @@
         <v>54</v>
       </c>
       <c r="K210" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="L210" t="s">
         <v>501</v>
       </c>
       <c r="M210" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="N210" t="s">
         <v>27</v>
@@ -24803,16 +24810,16 @@
         <v>5</v>
       </c>
       <c r="R210" t="s">
-        <v>328</v>
+        <v>5</v>
       </c>
       <c r="S210" t="s">
-        <v>329</v>
+        <v>5</v>
       </c>
       <c r="T210" t="s">
         <v>27</v>
       </c>
       <c r="U210" t="s">
-        <v>27</v>
+        <v>325</v>
       </c>
       <c r="V210" t="s">
         <v>27</v>
@@ -24832,7 +24839,7 @@
       </c>
       <c r="AA210">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB210" t="s">
         <v>5</v>
@@ -24843,7 +24850,7 @@
     </row>
     <row r="211" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B211" t="s">
         <v>324</v>
@@ -24853,10 +24860,10 @@
         <v>n</v>
       </c>
       <c r="D211" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="E211" t="s">
-        <v>1472</v>
+        <v>770</v>
       </c>
       <c r="F211" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
@@ -24869,7 +24876,7 @@
         <v>324</v>
       </c>
       <c r="I211" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J211" t="s">
         <v>54</v>
@@ -24887,19 +24894,19 @@
         <v>27</v>
       </c>
       <c r="O211" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="P211" t="s">
-        <v>625</v>
+        <v>27</v>
       </c>
       <c r="Q211" t="s">
         <v>5</v>
       </c>
       <c r="R211" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="S211" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="T211" t="s">
         <v>27</v>
@@ -24925,7 +24932,7 @@
       </c>
       <c r="AA211">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AB211" t="s">
         <v>5</v>
@@ -24936,7 +24943,7 @@
     </row>
     <row r="212" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>1422</v>
+        <v>321</v>
       </c>
       <c r="B212" t="s">
         <v>324</v>
@@ -24980,24 +24987,24 @@
         <v>27</v>
       </c>
       <c r="O212" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="P212" t="s">
-        <v>27</v>
+        <v>625</v>
       </c>
       <c r="Q212" t="s">
         <v>5</v>
       </c>
       <c r="R212" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="S212" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="T212" t="s">
         <v>27</v>
       </c>
-      <c r="U212" s="16" t="s">
+      <c r="U212" t="s">
         <v>27</v>
       </c>
       <c r="V212" t="s">
@@ -25018,7 +25025,7 @@
       </c>
       <c r="AA212">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AB212" t="s">
         <v>5</v>
@@ -25029,22 +25036,22 @@
     </row>
     <row r="213" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>1484</v>
+        <v>322</v>
       </c>
       <c r="B213" t="s">
         <v>324</v>
       </c>
-      <c r="C213" s="8" t="str">
+      <c r="C213" t="str">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
         <v>n</v>
       </c>
       <c r="D213" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="E213" t="s">
-        <v>770</v>
-      </c>
-      <c r="F213" s="8" t="str">
+        <v>1472</v>
+      </c>
+      <c r="F213" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
         <v>field element</v>
       </c>
@@ -25061,7 +25068,7 @@
         <v>54</v>
       </c>
       <c r="K213" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="L213" t="s">
         <v>501</v>
@@ -25073,25 +25080,25 @@
         <v>27</v>
       </c>
       <c r="O213" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="P213" t="s">
-        <v>27</v>
+        <v>625</v>
       </c>
       <c r="Q213" t="s">
         <v>5</v>
       </c>
       <c r="R213" t="s">
-        <v>1485</v>
+        <v>330</v>
       </c>
       <c r="S213" t="s">
-        <v>1486</v>
+        <v>331</v>
       </c>
       <c r="T213" t="s">
         <v>27</v>
       </c>
       <c r="U213" s="16" t="s">
-        <v>1487</v>
+        <v>27</v>
       </c>
       <c r="V213" t="s">
         <v>27</v>
@@ -25111,10 +25118,10 @@
       </c>
       <c r="AA213">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB213" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AC213" t="s">
         <v>5</v>
@@ -25122,10 +25129,10 @@
     </row>
     <row r="214" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>299</v>
+        <v>1422</v>
       </c>
       <c r="B214" t="s">
-        <v>27</v>
+        <v>324</v>
       </c>
       <c r="C214" t="str">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
@@ -25139,13 +25146,13 @@
       </c>
       <c r="F214" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
-        <v>simple field</v>
+        <v>field element</v>
       </c>
       <c r="G214" t="s">
         <v>5</v>
       </c>
       <c r="H214" t="s">
-        <v>259</v>
+        <v>324</v>
       </c>
       <c r="I214" t="s">
         <v>2</v>
@@ -25154,10 +25161,10 @@
         <v>54</v>
       </c>
       <c r="K214" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="L214" t="s">
-        <v>444</v>
+        <v>501</v>
       </c>
       <c r="M214" t="s">
         <v>27</v>
@@ -25172,25 +25179,25 @@
         <v>27</v>
       </c>
       <c r="Q214" t="s">
-        <v>626</v>
+        <v>5</v>
       </c>
       <c r="R214" t="s">
-        <v>300</v>
+        <v>326</v>
       </c>
       <c r="S214" t="s">
-        <v>301</v>
+        <v>327</v>
       </c>
       <c r="T214" t="s">
-        <v>67</v>
-      </c>
-      <c r="U214" t="s">
+        <v>27</v>
+      </c>
+      <c r="U214" s="16" t="s">
         <v>27</v>
       </c>
       <c r="V214" t="s">
         <v>27</v>
       </c>
       <c r="W214" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="X214" t="s">
         <v>519</v>
@@ -25204,10 +25211,10 @@
       </c>
       <c r="AA214">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AB214" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AC214" t="s">
         <v>5</v>
@@ -25215,12 +25222,12 @@
     </row>
     <row r="215" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>284</v>
+        <v>1484</v>
       </c>
       <c r="B215" t="s">
-        <v>27</v>
-      </c>
-      <c r="C215" t="str">
+        <v>324</v>
+      </c>
+      <c r="C215" s="8" t="str">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
         <v>n</v>
       </c>
@@ -25230,79 +25237,265 @@
       <c r="E215" t="s">
         <v>770</v>
       </c>
-      <c r="F215" t="str">
+      <c r="F215" s="8" t="str">
+        <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
+        <v>field element</v>
+      </c>
+      <c r="G215" t="s">
+        <v>5</v>
+      </c>
+      <c r="H215" t="s">
+        <v>324</v>
+      </c>
+      <c r="I215" t="s">
+        <v>2</v>
+      </c>
+      <c r="J215" t="s">
+        <v>54</v>
+      </c>
+      <c r="K215" t="s">
+        <v>295</v>
+      </c>
+      <c r="L215" t="s">
+        <v>501</v>
+      </c>
+      <c r="M215" t="s">
+        <v>27</v>
+      </c>
+      <c r="N215" t="s">
+        <v>27</v>
+      </c>
+      <c r="O215" t="s">
+        <v>27</v>
+      </c>
+      <c r="P215" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q215" t="s">
+        <v>5</v>
+      </c>
+      <c r="R215" t="s">
+        <v>1485</v>
+      </c>
+      <c r="S215" t="s">
+        <v>1486</v>
+      </c>
+      <c r="T215" t="s">
+        <v>27</v>
+      </c>
+      <c r="U215" s="16" t="s">
+        <v>1487</v>
+      </c>
+      <c r="V215" t="s">
+        <v>27</v>
+      </c>
+      <c r="W215" t="s">
+        <v>5</v>
+      </c>
+      <c r="X215" t="s">
+        <v>519</v>
+      </c>
+      <c r="Y215" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z215" s="8">
+        <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA215">
+        <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB215" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC215" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="216" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>299</v>
+      </c>
+      <c r="B216" t="s">
+        <v>27</v>
+      </c>
+      <c r="C216" t="str">
+        <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
+        <v>n</v>
+      </c>
+      <c r="D216" t="s">
+        <v>1464</v>
+      </c>
+      <c r="E216" t="s">
+        <v>770</v>
+      </c>
+      <c r="F216" t="str">
         <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
         <v>simple field</v>
       </c>
-      <c r="G215" t="s">
-        <v>5</v>
-      </c>
-      <c r="H215" t="s">
+      <c r="G216" t="s">
+        <v>5</v>
+      </c>
+      <c r="H216" t="s">
+        <v>259</v>
+      </c>
+      <c r="I216" t="s">
+        <v>2</v>
+      </c>
+      <c r="J216" t="s">
+        <v>54</v>
+      </c>
+      <c r="K216" t="s">
+        <v>294</v>
+      </c>
+      <c r="L216" t="s">
+        <v>444</v>
+      </c>
+      <c r="M216" t="s">
+        <v>27</v>
+      </c>
+      <c r="N216" t="s">
+        <v>27</v>
+      </c>
+      <c r="O216" t="s">
+        <v>27</v>
+      </c>
+      <c r="P216" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q216" t="s">
+        <v>626</v>
+      </c>
+      <c r="R216" t="s">
+        <v>300</v>
+      </c>
+      <c r="S216" t="s">
+        <v>301</v>
+      </c>
+      <c r="T216" t="s">
+        <v>67</v>
+      </c>
+      <c r="U216" t="s">
+        <v>27</v>
+      </c>
+      <c r="V216" t="s">
+        <v>27</v>
+      </c>
+      <c r="W216" t="s">
+        <v>27</v>
+      </c>
+      <c r="X216" t="s">
+        <v>519</v>
+      </c>
+      <c r="Y216" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z216" s="8">
+        <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA216">
+        <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AB216" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC216" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="217" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>284</v>
+      </c>
+      <c r="B217" t="s">
+        <v>27</v>
+      </c>
+      <c r="C217" t="str">
+        <f>IF(ISNUMBER(MATCH(fields[argot_field],fields[has parent],0)),"y","n")</f>
+        <v>n</v>
+      </c>
+      <c r="D217" t="s">
+        <v>1464</v>
+      </c>
+      <c r="E217" t="s">
+        <v>770</v>
+      </c>
+      <c r="F217" t="str">
+        <f>IF(fields[is parent?]="y","parent field",IF(NOT(fields[has parent]="x"),"field element","simple field"))</f>
+        <v>simple field</v>
+      </c>
+      <c r="G217" t="s">
+        <v>5</v>
+      </c>
+      <c r="H217" t="s">
         <v>344</v>
       </c>
-      <c r="I215" t="s">
-        <v>2</v>
-      </c>
-      <c r="J215" t="s">
+      <c r="I217" t="s">
+        <v>2</v>
+      </c>
+      <c r="J217" t="s">
         <v>54</v>
       </c>
-      <c r="K215" t="s">
+      <c r="K217" t="s">
         <v>294</v>
       </c>
-      <c r="L215" t="s">
+      <c r="L217" t="s">
         <v>345</v>
       </c>
-      <c r="M215" t="s">
-        <v>27</v>
-      </c>
-      <c r="N215" t="s">
+      <c r="M217" t="s">
+        <v>27</v>
+      </c>
+      <c r="N217" t="s">
         <v>628</v>
       </c>
-      <c r="O215" t="s">
-        <v>27</v>
-      </c>
-      <c r="P215" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q215" t="s">
-        <v>27</v>
-      </c>
-      <c r="R215" t="s">
+      <c r="O217" t="s">
+        <v>27</v>
+      </c>
+      <c r="P217" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q217" t="s">
+        <v>27</v>
+      </c>
+      <c r="R217" t="s">
         <v>272</v>
       </c>
-      <c r="S215" t="s">
+      <c r="S217" t="s">
         <v>273</v>
       </c>
-      <c r="T215" t="s">
-        <v>27</v>
-      </c>
-      <c r="U215" t="s">
-        <v>27</v>
-      </c>
-      <c r="V215" t="s">
-        <v>27</v>
-      </c>
-      <c r="W215" t="s">
-        <v>27</v>
-      </c>
-      <c r="X215" t="s">
+      <c r="T217" t="s">
+        <v>27</v>
+      </c>
+      <c r="U217" t="s">
+        <v>27</v>
+      </c>
+      <c r="V217" t="s">
+        <v>27</v>
+      </c>
+      <c r="W217" t="s">
+        <v>27</v>
+      </c>
+      <c r="X217" t="s">
         <v>519</v>
       </c>
-      <c r="Y215" t="s">
+      <c r="Y217" t="s">
         <v>627</v>
       </c>
-      <c r="Z215" s="8">
+      <c r="Z217" s="8">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],issuesfield[field],0)),COUNTIF(issuesfield[field],fields[argot_field]),0)</f>
         <v>0</v>
       </c>
-      <c r="AA215">
+      <c r="AA217">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
         <v>1</v>
       </c>
-      <c r="AB215" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC215" t="s">
+      <c r="AB217" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC217" t="s">
         <v>3</v>
       </c>
     </row>
@@ -25311,8 +25504,9 @@
     <hyperlink ref="Y143" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -25321,8 +25515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q723"/>
   <sheetViews>
-    <sheetView topLeftCell="B41" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView topLeftCell="B579" workbookViewId="0">
+      <selection activeCell="G663" sqref="G663"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
more work on schema
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -5142,10 +5142,23 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="fields" displayName="fields" ref="A1:AD222" totalsRowShown="0">
-  <autoFilter ref="A1:AD222"/>
-  <sortState ref="A2:AD222">
-    <sortCondition ref="A1:A222"/>
-  </sortState>
+  <autoFilter ref="A1:AD222">
+    <filterColumn colId="8">
+      <filters>
+        <filter val="n"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="9">
+      <filters>
+        <filter val="shared"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="29">
+      <filters>
+        <filter val="."/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="30">
     <tableColumn id="1" name="argot_field"/>
     <tableColumn id="2" name="has parent"/>
@@ -5499,9 +5512,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD222"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A171" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD14" sqref="AD14"/>
+      <selection pane="topRight" activeCell="AD190" sqref="AD190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5613,7 +5626,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
@@ -5709,7 +5722,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -5805,7 +5818,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -5901,7 +5914,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -6093,7 +6106,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -6189,7 +6202,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>89</v>
       </c>
@@ -6285,7 +6298,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>93</v>
       </c>
@@ -6381,7 +6394,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>96</v>
       </c>
@@ -6477,7 +6490,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>101</v>
       </c>
@@ -6573,7 +6586,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>111</v>
       </c>
@@ -6669,7 +6682,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>107</v>
       </c>
@@ -6858,7 +6871,7 @@
         <v>73</v>
       </c>
       <c r="AD14" s="3" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
@@ -6954,7 +6967,7 @@
         <v>73</v>
       </c>
       <c r="AD15" s="3" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
@@ -7050,7 +7063,7 @@
         <v>73</v>
       </c>
       <c r="AD16" s="3" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.25">
@@ -7146,7 +7159,7 @@
         <v>32</v>
       </c>
       <c r="AD17" s="3" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.25">
@@ -7242,7 +7255,7 @@
         <v>32</v>
       </c>
       <c r="AD18" s="3" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.25">
@@ -7338,10 +7351,10 @@
         <v>32</v>
       </c>
       <c r="AD19" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>136</v>
       </c>
@@ -7437,7 +7450,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>141</v>
       </c>
@@ -7533,7 +7546,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>146</v>
       </c>
@@ -7629,7 +7642,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
         <v>174</v>
       </c>
@@ -7723,7 +7736,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>149</v>
       </c>
@@ -7819,7 +7832,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>155</v>
       </c>
@@ -7915,7 +7928,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>160</v>
       </c>
@@ -8011,7 +8024,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>164</v>
       </c>
@@ -8107,7 +8120,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>176</v>
       </c>
@@ -10219,7 +10232,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="29" t="s">
         <v>257</v>
       </c>
@@ -11083,7 +11096,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>299</v>
       </c>
@@ -11179,7 +11192,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>303</v>
       </c>
@@ -11275,7 +11288,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>309</v>
       </c>
@@ -11371,7 +11384,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>313</v>
       </c>
@@ -11467,7 +11480,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>316</v>
       </c>
@@ -11563,7 +11576,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>323</v>
       </c>
@@ -11659,7 +11672,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="65" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>327</v>
       </c>
@@ -11755,7 +11768,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>331</v>
       </c>
@@ -11851,7 +11864,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>336</v>
       </c>
@@ -11947,7 +11960,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>342</v>
       </c>
@@ -12043,7 +12056,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="69" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>348</v>
       </c>
@@ -12139,7 +12152,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>351</v>
       </c>
@@ -12331,7 +12344,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="72" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>361</v>
       </c>
@@ -12427,7 +12440,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="73" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>364</v>
       </c>
@@ -12523,7 +12536,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>365</v>
       </c>
@@ -15403,7 +15416,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="104" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>476</v>
       </c>
@@ -15499,7 +15512,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="105" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>479</v>
       </c>
@@ -15595,7 +15608,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="106" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>480</v>
       </c>
@@ -15691,7 +15704,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="107" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>482</v>
       </c>
@@ -15787,7 +15800,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="108" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>485</v>
       </c>
@@ -18091,7 +18104,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="132" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>550</v>
       </c>
@@ -18379,7 +18392,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="135" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>563</v>
       </c>
@@ -18475,7 +18488,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="136" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>565</v>
       </c>
@@ -18571,7 +18584,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="137" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>569</v>
       </c>
@@ -18667,7 +18680,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="138" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:30" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>1515</v>
       </c>
@@ -18763,7 +18776,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="139" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>574</v>
       </c>
@@ -18856,10 +18869,10 @@
         <v>73</v>
       </c>
       <c r="AD139" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="140" spans="1:30" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="140" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>582</v>
       </c>
@@ -18952,10 +18965,10 @@
         <v>73</v>
       </c>
       <c r="AD140" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="141" spans="1:30" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="141" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>583</v>
       </c>
@@ -19048,10 +19061,10 @@
         <v>73</v>
       </c>
       <c r="AD141" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="142" spans="1:30" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="142" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>585</v>
       </c>
@@ -19144,10 +19157,10 @@
         <v>73</v>
       </c>
       <c r="AD142" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="143" spans="1:30" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="143" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>589</v>
       </c>
@@ -19240,10 +19253,10 @@
         <v>73</v>
       </c>
       <c r="AD143" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="144" spans="1:30" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="144" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>590</v>
       </c>
@@ -19336,7 +19349,7 @@
         <v>73</v>
       </c>
       <c r="AD144" s="3" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
     </row>
     <row r="145" spans="1:30" x14ac:dyDescent="0.25">
@@ -21161,7 +21174,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="164" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>646</v>
       </c>
@@ -22889,7 +22902,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="182" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
         <v>693</v>
       </c>
@@ -23654,7 +23667,7 @@
         <v>32</v>
       </c>
       <c r="AD189" s="3" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
     </row>
     <row r="190" spans="1:30" x14ac:dyDescent="0.25">
@@ -23750,7 +23763,7 @@
         <v>32</v>
       </c>
       <c r="AD190" s="3" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
     </row>
     <row r="191" spans="1:30" x14ac:dyDescent="0.25">
@@ -23846,7 +23859,7 @@
         <v>32</v>
       </c>
       <c r="AD191" s="3" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
     </row>
     <row r="192" spans="1:30" x14ac:dyDescent="0.25">
@@ -24617,7 +24630,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="200" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>755</v>
       </c>
@@ -24713,7 +24726,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="201" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
         <v>761</v>
       </c>
@@ -24809,7 +24822,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="202" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
         <v>763</v>
       </c>
@@ -24905,7 +24918,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="203" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
         <v>767</v>
       </c>
@@ -26057,7 +26070,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="215" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="s">
         <v>808</v>
       </c>
@@ -26153,7 +26166,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="216" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="s">
         <v>811</v>
       </c>
@@ -26249,7 +26262,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="217" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
         <v>814</v>
       </c>
@@ -26345,7 +26358,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="218" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
         <v>823</v>
       </c>
@@ -26441,7 +26454,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="219" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
         <v>817</v>
       </c>
@@ -26537,7 +26550,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="220" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
         <v>820</v>
       </c>
@@ -26633,7 +26646,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="221" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
         <v>827</v>
       </c>
@@ -26729,7 +26742,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="222" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
         <v>831</v>
       </c>
@@ -26843,7 +26856,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q716"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
653 i2=4 treated as topical
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="5040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="5040" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14346" uniqueCount="1522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14346" uniqueCount="1523">
   <si>
     <t>argot_field</t>
   </si>
@@ -4593,6 +4593,9 @@
   </si>
   <si>
     <t>title_variant[lang]</t>
+  </si>
+  <si>
+    <t>This *should* map to subject_chronological, BUT too many sloppy catalog records mis-code this 2nd indicator value</t>
   </si>
 </sst>
 </file>
@@ -5214,7 +5217,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="mappings" displayName="mappings" ref="A1:Q720" totalsRowShown="0">
   <autoFilter ref="A1:Q720"/>
   <sortState ref="A2:Q720">
-    <sortCondition ref="A1:A720"/>
+    <sortCondition ref="B1:B720"/>
   </sortState>
   <tableColumns count="17">
     <tableColumn id="1" name="parentfield"/>
@@ -5530,7 +5533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A194" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A194" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="G207" sqref="G207:G214"/>
     </sheetView>
@@ -23677,7 +23680,7 @@
       </c>
       <c r="AA189" s="3">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AB189" s="3" t="s">
         <v>32</v>
@@ -24253,7 +24256,7 @@
       </c>
       <c r="AA195" s="3">
         <f>IF(ISNUMBER(MATCH(fields[argot_field],mappings[field],0)),COUNTIF(mappings[field],fields[argot_field]),0)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AB195" s="3" t="s">
         <v>32</v>
@@ -27163,11 +27166,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q721"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I685" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K692" sqref="K692"/>
+      <selection pane="bottomRight" activeCell="A589" sqref="A589"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37994,7 +37997,7 @@
         <v>426</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>1511</v>
+        <v>1513</v>
       </c>
       <c r="C193" s="3" t="s">
         <v>855</v>
@@ -38008,11 +38011,11 @@
       <c r="F193" s="11">
         <v>510</v>
       </c>
-      <c r="G193" s="3">
-        <v>3</v>
+      <c r="G193" s="3" t="s">
+        <v>897</v>
       </c>
       <c r="H193" s="3" t="s">
-        <v>850</v>
+        <v>1519</v>
       </c>
       <c r="I193" s="3" t="s">
         <v>862</v>
@@ -38021,11 +38024,11 @@
         <v>29</v>
       </c>
       <c r="K193" s="3" t="s">
-        <v>411</v>
+        <v>29</v>
       </c>
       <c r="L193" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>note_cited_in[label]GEN5103none</v>
+        <v>note_cited_in[indexed_value]GEN510abc$u OR $x present</v>
       </c>
       <c r="M193" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -38051,7 +38054,7 @@
         <v>426</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="C194" s="3" t="s">
         <v>855</v>
@@ -38065,8 +38068,8 @@
       <c r="F194" s="11">
         <v>510</v>
       </c>
-      <c r="G194" s="3" t="s">
-        <v>1517</v>
+      <c r="G194" s="3">
+        <v>3</v>
       </c>
       <c r="H194" s="3" t="s">
         <v>850</v>
@@ -38075,14 +38078,14 @@
         <v>862</v>
       </c>
       <c r="J194" s="3" t="s">
-        <v>1518</v>
+        <v>29</v>
       </c>
       <c r="K194" s="3" t="s">
-        <v>29</v>
+        <v>411</v>
       </c>
       <c r="L194" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>note_cited_in[value]GEN510abcuxnone</v>
+        <v>note_cited_in[label]GEN5103none</v>
       </c>
       <c r="M194" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -38108,7 +38111,7 @@
         <v>426</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="C195" s="3" t="s">
         <v>855</v>
@@ -38123,23 +38126,23 @@
         <v>510</v>
       </c>
       <c r="G195" s="3" t="s">
-        <v>897</v>
+        <v>1517</v>
       </c>
       <c r="H195" s="3" t="s">
-        <v>1519</v>
+        <v>850</v>
       </c>
       <c r="I195" s="3" t="s">
         <v>862</v>
       </c>
       <c r="J195" s="3" t="s">
-        <v>29</v>
+        <v>1518</v>
       </c>
       <c r="K195" s="3" t="s">
         <v>29</v>
       </c>
       <c r="L195" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>note_cited_in[indexed_value]GEN510abc$u OR $x present</v>
+        <v>note_cited_in[value]GEN510abcuxnone</v>
       </c>
       <c r="M195" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -40370,7 +40373,7 @@
         <v>473</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C237" s="3" t="s">
         <v>855</v>
@@ -40382,26 +40385,26 @@
         <v>841</v>
       </c>
       <c r="F237" s="11">
-        <v>541</v>
+        <v>790</v>
       </c>
       <c r="G237" s="3" t="s">
-        <v>849</v>
+        <v>31</v>
       </c>
       <c r="H237" s="3" t="s">
         <v>850</v>
       </c>
       <c r="I237" s="3" t="s">
-        <v>847</v>
+        <v>1042</v>
       </c>
       <c r="J237" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K237" s="3" t="s">
-        <v>32</v>
+        <v>1261</v>
       </c>
       <c r="L237" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>note_local[indexed_value]UNC541anone</v>
+        <v>note_local[indexed]UNC790{na}none</v>
       </c>
       <c r="M237" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -40415,19 +40418,15 @@
         <f>IF(ISNUMBER(MATCH(mappings[field],#REF!,0)),"y","n")</f>
         <v>n</v>
       </c>
-      <c r="P237" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q237" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="P237" s="3"/>
+      <c r="Q237" s="3"/>
     </row>
     <row r="238" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A238" s="3" t="s">
         <v>473</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="C238" s="3" t="s">
         <v>855</v>
@@ -40436,27 +40435,29 @@
         <v>33</v>
       </c>
       <c r="E238" s="3" t="s">
-        <v>856</v>
+        <v>841</v>
       </c>
       <c r="F238" s="11">
-        <v>561</v>
+        <v>791</v>
       </c>
       <c r="G238" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H238" s="3" t="s">
-        <v>1053</v>
+        <v>850</v>
       </c>
       <c r="I238" s="3" t="s">
-        <v>883</v>
+        <v>1042</v>
       </c>
       <c r="J238" s="3" t="s">
-        <v>1476</v>
-      </c>
-      <c r="K238" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="K238" s="3" t="s">
+        <v>1261</v>
+      </c>
       <c r="L238" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>note_local[label]GEN561{na}ind1 != 0 and $3 NOT present</v>
+        <v>note_local[indexed]UNC791{na}none</v>
       </c>
       <c r="M238" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -40478,7 +40479,7 @@
         <v>473</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C239" s="3" t="s">
         <v>855</v>
@@ -40487,29 +40488,29 @@
         <v>33</v>
       </c>
       <c r="E239" s="3" t="s">
-        <v>856</v>
+        <v>841</v>
       </c>
       <c r="F239" s="11">
-        <v>561</v>
-      </c>
-      <c r="G239" s="3">
-        <v>3</v>
+        <v>541</v>
+      </c>
+      <c r="G239" s="3" t="s">
+        <v>849</v>
       </c>
       <c r="H239" s="3" t="s">
-        <v>1052</v>
+        <v>850</v>
       </c>
       <c r="I239" s="3" t="s">
-        <v>862</v>
+        <v>847</v>
       </c>
       <c r="J239" s="3" t="s">
-        <v>1477</v>
+        <v>32</v>
       </c>
       <c r="K239" s="3" t="s">
         <v>32</v>
       </c>
       <c r="L239" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>note_local[label]GEN5613ind1 != 0 and $3 present</v>
+        <v>note_local[indexed_value]UNC541anone</v>
       </c>
       <c r="M239" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -40523,8 +40524,12 @@
         <f>IF(ISNUMBER(MATCH(mappings[field],#REF!,0)),"y","n")</f>
         <v>n</v>
       </c>
-      <c r="P239" s="3"/>
-      <c r="Q239" s="3"/>
+      <c r="P239" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q239" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="240" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A240" s="3" t="s">
@@ -40540,29 +40545,27 @@
         <v>33</v>
       </c>
       <c r="E240" s="3" t="s">
-        <v>841</v>
+        <v>856</v>
       </c>
       <c r="F240" s="11">
-        <v>541</v>
+        <v>561</v>
       </c>
       <c r="G240" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H240" s="3" t="s">
-        <v>850</v>
+        <v>1053</v>
       </c>
       <c r="I240" s="3" t="s">
         <v>883</v>
       </c>
       <c r="J240" s="3" t="s">
-        <v>1490</v>
-      </c>
-      <c r="K240" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>1476</v>
+      </c>
+      <c r="K240" s="3"/>
       <c r="L240" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>note_local[label]UNC541{na}none</v>
+        <v>note_local[label]GEN561{na}ind1 != 0 and $3 NOT present</v>
       </c>
       <c r="M240" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -40596,26 +40599,26 @@
         <v>856</v>
       </c>
       <c r="F241" s="11">
-        <v>500</v>
+        <v>561</v>
       </c>
       <c r="G241" s="3">
         <v>3</v>
       </c>
       <c r="H241" s="3" t="s">
-        <v>1049</v>
+        <v>1052</v>
       </c>
       <c r="I241" s="3" t="s">
         <v>862</v>
       </c>
       <c r="J241" s="3" t="s">
-        <v>32</v>
+        <v>1477</v>
       </c>
       <c r="K241" s="3" t="s">
         <v>32</v>
       </c>
       <c r="L241" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>note_local[label]GEN5003field contains whitelisted $5 value</v>
+        <v>note_local[label]GEN5613ind1 != 0 and $3 present</v>
       </c>
       <c r="M241" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -40629,19 +40632,15 @@
         <f>IF(ISNUMBER(MATCH(mappings[field],#REF!,0)),"y","n")</f>
         <v>n</v>
       </c>
-      <c r="P241" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q241" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="P241" s="3"/>
+      <c r="Q241" s="3"/>
     </row>
     <row r="242" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A242" s="3" t="s">
         <v>473</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="C242" s="3" t="s">
         <v>855</v>
@@ -40650,29 +40649,29 @@
         <v>33</v>
       </c>
       <c r="E242" s="3" t="s">
-        <v>856</v>
+        <v>841</v>
       </c>
       <c r="F242" s="11">
-        <v>500</v>
+        <v>541</v>
       </c>
       <c r="G242" s="3" t="s">
-        <v>849</v>
+        <v>31</v>
       </c>
       <c r="H242" s="3" t="s">
-        <v>1049</v>
+        <v>850</v>
       </c>
       <c r="I242" s="3" t="s">
-        <v>862</v>
+        <v>883</v>
       </c>
       <c r="J242" s="3" t="s">
-        <v>32</v>
+        <v>1490</v>
       </c>
       <c r="K242" s="3" t="s">
         <v>32</v>
       </c>
       <c r="L242" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>note_local[value]GEN500afield contains whitelisted $5 value</v>
+        <v>note_local[label]UNC541{na}none</v>
       </c>
       <c r="M242" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -40686,19 +40685,15 @@
         <f>IF(ISNUMBER(MATCH(mappings[field],#REF!,0)),"y","n")</f>
         <v>n</v>
       </c>
-      <c r="P242" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q242" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="P242" s="3"/>
+      <c r="Q242" s="3"/>
     </row>
     <row r="243" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A243" s="3" t="s">
         <v>473</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="C243" s="3" t="s">
         <v>855</v>
@@ -40710,13 +40705,13 @@
         <v>856</v>
       </c>
       <c r="F243" s="11">
-        <v>561</v>
-      </c>
-      <c r="G243" s="3" t="s">
-        <v>849</v>
+        <v>500</v>
+      </c>
+      <c r="G243" s="3">
+        <v>3</v>
       </c>
       <c r="H243" s="3" t="s">
-        <v>1054</v>
+        <v>1049</v>
       </c>
       <c r="I243" s="3" t="s">
         <v>862</v>
@@ -40729,7 +40724,7 @@
       </c>
       <c r="L243" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>note_local[value]GEN561aind1 != 0</v>
+        <v>note_local[label]GEN5003field contains whitelisted $5 value</v>
       </c>
       <c r="M243" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -40767,13 +40762,13 @@
         <v>856</v>
       </c>
       <c r="F244" s="11">
-        <v>590</v>
+        <v>500</v>
       </c>
       <c r="G244" s="3" t="s">
         <v>849</v>
       </c>
       <c r="H244" s="3" t="s">
-        <v>850</v>
+        <v>1049</v>
       </c>
       <c r="I244" s="3" t="s">
         <v>862</v>
@@ -40786,7 +40781,7 @@
       </c>
       <c r="L244" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>note_local[value]GEN590anone</v>
+        <v>note_local[value]GEN500afield contains whitelisted $5 value</v>
       </c>
       <c r="M244" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -40821,29 +40816,29 @@
         <v>33</v>
       </c>
       <c r="E245" s="3" t="s">
-        <v>841</v>
+        <v>856</v>
       </c>
       <c r="F245" s="11">
-        <v>541</v>
+        <v>561</v>
       </c>
       <c r="G245" s="3" t="s">
-        <v>1050</v>
+        <v>849</v>
       </c>
       <c r="H245" s="3" t="s">
-        <v>850</v>
+        <v>1054</v>
       </c>
       <c r="I245" s="3" t="s">
         <v>862</v>
       </c>
       <c r="J245" s="3" t="s">
-        <v>1051</v>
+        <v>32</v>
       </c>
       <c r="K245" s="3" t="s">
         <v>32</v>
       </c>
       <c r="L245" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>note_local[value]UNC541abcdefhno3none</v>
+        <v>note_local[value]GEN561aind1 != 0</v>
       </c>
       <c r="M245" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -40878,29 +40873,29 @@
         <v>33</v>
       </c>
       <c r="E246" s="3" t="s">
-        <v>841</v>
+        <v>856</v>
       </c>
       <c r="F246" s="11">
-        <v>790</v>
+        <v>590</v>
       </c>
       <c r="G246" s="3" t="s">
-        <v>860</v>
+        <v>849</v>
       </c>
       <c r="H246" s="3" t="s">
-        <v>861</v>
+        <v>850</v>
       </c>
       <c r="I246" s="3" t="s">
         <v>862</v>
       </c>
       <c r="J246" s="3" t="s">
-        <v>863</v>
+        <v>32</v>
       </c>
       <c r="K246" s="3" t="s">
         <v>32</v>
       </c>
       <c r="L246" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>note_local[value]UNC790abcdgquind 1 = 0</v>
+        <v>note_local[value]GEN590anone</v>
       </c>
       <c r="M246" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -40915,10 +40910,10 @@
         <v>n</v>
       </c>
       <c r="P246" s="3" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="Q246" s="3" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
     </row>
     <row r="247" spans="1:17" x14ac:dyDescent="0.25">
@@ -40938,26 +40933,26 @@
         <v>841</v>
       </c>
       <c r="F247" s="11">
-        <v>791</v>
+        <v>541</v>
       </c>
       <c r="G247" s="3" t="s">
-        <v>864</v>
+        <v>1050</v>
       </c>
       <c r="H247" s="3" t="s">
-        <v>865</v>
+        <v>850</v>
       </c>
       <c r="I247" s="3" t="s">
         <v>862</v>
       </c>
       <c r="J247" t="s">
-        <v>866</v>
+        <v>1051</v>
       </c>
       <c r="K247" s="3" t="s">
         <v>32</v>
       </c>
       <c r="L247" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>note_local[value]UNC791abcdfgind 1 = 2</v>
+        <v>note_local[value]UNC541abcdefhno3none</v>
       </c>
       <c r="M247" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -40972,10 +40967,10 @@
         <v>n</v>
       </c>
       <c r="P247" s="3" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="Q247" s="3" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
     </row>
     <row r="248" spans="1:17" x14ac:dyDescent="0.25">
@@ -40983,7 +40978,7 @@
         <v>473</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="C248" s="3" t="s">
         <v>855</v>
@@ -40998,23 +40993,23 @@
         <v>790</v>
       </c>
       <c r="G248" s="3" t="s">
-        <v>31</v>
+        <v>860</v>
       </c>
       <c r="H248" s="3" t="s">
-        <v>850</v>
+        <v>861</v>
       </c>
       <c r="I248" s="3" t="s">
-        <v>1042</v>
+        <v>862</v>
       </c>
       <c r="J248" s="3" t="s">
-        <v>29</v>
+        <v>863</v>
       </c>
       <c r="K248" s="3" t="s">
-        <v>1261</v>
+        <v>32</v>
       </c>
       <c r="L248" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>note_local[indexed]UNC790{na}none</v>
+        <v>note_local[value]UNC790abcdgquind 1 = 0</v>
       </c>
       <c r="M248" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -41028,15 +41023,19 @@
         <f>IF(ISNUMBER(MATCH(mappings[field],#REF!,0)),"y","n")</f>
         <v>n</v>
       </c>
-      <c r="P248" s="3"/>
-      <c r="Q248" s="3"/>
+      <c r="P248" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q248" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="249" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A249" s="3" t="s">
         <v>473</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="C249" s="3" t="s">
         <v>855</v>
@@ -41051,23 +41050,23 @@
         <v>791</v>
       </c>
       <c r="G249" s="3" t="s">
-        <v>31</v>
+        <v>864</v>
       </c>
       <c r="H249" s="3" t="s">
-        <v>850</v>
+        <v>865</v>
       </c>
       <c r="I249" s="3" t="s">
-        <v>1042</v>
+        <v>862</v>
       </c>
       <c r="J249" s="3" t="s">
-        <v>29</v>
+        <v>866</v>
       </c>
       <c r="K249" s="3" t="s">
-        <v>1261</v>
+        <v>32</v>
       </c>
       <c r="L249" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>note_local[indexed]UNC791{na}none</v>
+        <v>note_local[value]UNC791abcdfgind 1 = 2</v>
       </c>
       <c r="M249" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -41081,8 +41080,12 @@
         <f>IF(ISNUMBER(MATCH(mappings[field],#REF!,0)),"y","n")</f>
         <v>n</v>
       </c>
-      <c r="P249" s="3"/>
-      <c r="Q249" s="3"/>
+      <c r="P249" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q249" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="250" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A250" s="3" t="s">
@@ -60234,18 +60237,18 @@
         <v>856</v>
       </c>
       <c r="F589" s="13">
-        <v>653</v>
+        <v>600</v>
       </c>
       <c r="G589" s="24" t="s">
-        <v>849</v>
+        <v>73</v>
       </c>
       <c r="H589" t="s">
-        <v>1174</v>
+        <v>850</v>
       </c>
       <c r="I589" s="24" t="s">
         <v>847</v>
       </c>
-      <c r="J589" s="24" t="s">
+      <c r="J589" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K589" s="24" t="s">
@@ -60253,7 +60256,7 @@
       </c>
       <c r="L589" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronologicalGEN653ai2 = 4</v>
+        <v>subject_chronologicalGEN600ynone</v>
       </c>
       <c r="M589" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -60291,7 +60294,7 @@
         <v>856</v>
       </c>
       <c r="F590" s="13">
-        <v>600</v>
+        <v>610</v>
       </c>
       <c r="G590" s="24" t="s">
         <v>73</v>
@@ -60310,7 +60313,7 @@
       </c>
       <c r="L590" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronologicalGEN600ynone</v>
+        <v>subject_chronologicalGEN610ynone</v>
       </c>
       <c r="M590" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -60348,7 +60351,7 @@
         <v>856</v>
       </c>
       <c r="F591" s="13">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="G591" s="24" t="s">
         <v>73</v>
@@ -60367,7 +60370,7 @@
       </c>
       <c r="L591" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronologicalGEN610ynone</v>
+        <v>subject_chronologicalGEN611ynone</v>
       </c>
       <c r="M591" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -60405,7 +60408,7 @@
         <v>856</v>
       </c>
       <c r="F592" s="13">
-        <v>611</v>
+        <v>630</v>
       </c>
       <c r="G592" s="24" t="s">
         <v>73</v>
@@ -60416,7 +60419,7 @@
       <c r="I592" s="24" t="s">
         <v>847</v>
       </c>
-      <c r="J592" s="3" t="s">
+      <c r="J592" s="24" t="s">
         <v>32</v>
       </c>
       <c r="K592" s="24" t="s">
@@ -60424,7 +60427,7 @@
       </c>
       <c r="L592" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronologicalGEN611ynone</v>
+        <v>subject_chronologicalGEN630ynone</v>
       </c>
       <c r="M592" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -60462,7 +60465,7 @@
         <v>856</v>
       </c>
       <c r="F593" s="13">
-        <v>630</v>
+        <v>650</v>
       </c>
       <c r="G593" s="24" t="s">
         <v>73</v>
@@ -60481,7 +60484,7 @@
       </c>
       <c r="L593" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronologicalGEN630ynone</v>
+        <v>subject_chronologicalGEN650ynone</v>
       </c>
       <c r="M593" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -60519,7 +60522,7 @@
         <v>856</v>
       </c>
       <c r="F594" s="13">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="G594" s="24" t="s">
         <v>73</v>
@@ -60530,7 +60533,7 @@
       <c r="I594" s="24" t="s">
         <v>847</v>
       </c>
-      <c r="J594" s="24" t="s">
+      <c r="J594" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K594" s="24" t="s">
@@ -60538,7 +60541,7 @@
       </c>
       <c r="L594" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronologicalGEN650ynone</v>
+        <v>subject_chronologicalGEN651ynone</v>
       </c>
       <c r="M594" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -60576,7 +60579,7 @@
         <v>856</v>
       </c>
       <c r="F595" s="13">
-        <v>651</v>
+        <v>655</v>
       </c>
       <c r="G595" s="24" t="s">
         <v>73</v>
@@ -60587,7 +60590,7 @@
       <c r="I595" s="24" t="s">
         <v>847</v>
       </c>
-      <c r="J595" s="3" t="s">
+      <c r="J595" s="24" t="s">
         <v>32</v>
       </c>
       <c r="K595" s="24" t="s">
@@ -60595,7 +60598,7 @@
       </c>
       <c r="L595" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronologicalGEN651ynone</v>
+        <v>subject_chronologicalGEN655ynone</v>
       </c>
       <c r="M595" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -60633,7 +60636,7 @@
         <v>856</v>
       </c>
       <c r="F596" s="13">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="G596" s="24" t="s">
         <v>73</v>
@@ -60652,7 +60655,7 @@
       </c>
       <c r="L596" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronologicalGEN655ynone</v>
+        <v>subject_chronologicalGEN656ynone</v>
       </c>
       <c r="M596" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -60690,7 +60693,7 @@
         <v>856</v>
       </c>
       <c r="F597" s="13">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="G597" s="24" t="s">
         <v>73</v>
@@ -60709,7 +60712,7 @@
       </c>
       <c r="L597" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronologicalGEN656ynone</v>
+        <v>subject_chronologicalGEN657ynone</v>
       </c>
       <c r="M597" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -60732,41 +60735,41 @@
     </row>
     <row r="598" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A598" s="24" t="s">
-        <v>703</v>
+        <v>711</v>
       </c>
       <c r="B598" s="24" t="s">
-        <v>703</v>
+        <v>711</v>
       </c>
       <c r="C598" s="24" t="s">
         <v>855</v>
       </c>
       <c r="D598" s="24" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="E598" s="24" t="s">
         <v>856</v>
       </c>
       <c r="F598" s="13">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="G598" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="H598" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
+      </c>
+      <c r="H598" s="24" t="s">
+        <v>869</v>
       </c>
       <c r="I598" s="24" t="s">
         <v>847</v>
       </c>
-      <c r="J598" s="24" t="s">
+      <c r="J598" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K598" s="24" t="s">
-        <v>32</v>
+        <v>1183</v>
       </c>
       <c r="L598" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_chronologicalGEN657ynone</v>
+        <v>subject_genreGEN653ai2 = 6</v>
       </c>
       <c r="M598" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -60774,7 +60777,7 @@
       </c>
       <c r="N598" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O598" s="15" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],#REF!,0)),"y","n")</f>
@@ -60784,7 +60787,7 @@
         <v>73</v>
       </c>
       <c r="Q598" s="15" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
     </row>
     <row r="599" spans="1:17" x14ac:dyDescent="0.25">
@@ -60804,18 +60807,18 @@
         <v>856</v>
       </c>
       <c r="F599" s="13">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="G599" s="24" t="s">
-        <v>849</v>
+        <v>1190</v>
       </c>
       <c r="H599" s="24" t="s">
-        <v>869</v>
+        <v>850</v>
       </c>
       <c r="I599" s="24" t="s">
         <v>847</v>
       </c>
-      <c r="J599" s="3" t="s">
+      <c r="J599" s="24" t="s">
         <v>32</v>
       </c>
       <c r="K599" s="24" t="s">
@@ -60823,7 +60826,7 @@
       </c>
       <c r="L599" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genreGEN653ai2 = 6</v>
+        <v>subject_genreGEN656kvnone</v>
       </c>
       <c r="M599" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -60855,32 +60858,32 @@
         <v>855</v>
       </c>
       <c r="D600" s="24" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="E600" s="24" t="s">
         <v>856</v>
       </c>
       <c r="F600" s="13">
-        <v>656</v>
+        <v>600</v>
       </c>
       <c r="G600" s="24" t="s">
-        <v>1190</v>
-      </c>
-      <c r="H600" s="24" t="s">
+        <v>961</v>
+      </c>
+      <c r="H600" s="3" t="s">
         <v>850</v>
       </c>
       <c r="I600" s="24" t="s">
         <v>847</v>
       </c>
-      <c r="J600" s="24" t="s">
+      <c r="J600" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K600" s="24" t="s">
-        <v>1183</v>
+        <v>32</v>
       </c>
       <c r="L600" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genreGEN656kvnone</v>
+        <v>subject_genreGEN600vnone</v>
       </c>
       <c r="M600" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -60898,7 +60901,7 @@
         <v>73</v>
       </c>
       <c r="Q600" s="15" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
     </row>
     <row r="601" spans="1:17" x14ac:dyDescent="0.25">
@@ -60918,7 +60921,7 @@
         <v>856</v>
       </c>
       <c r="F601" s="13">
-        <v>600</v>
+        <v>610</v>
       </c>
       <c r="G601" s="24" t="s">
         <v>961</v>
@@ -60929,7 +60932,7 @@
       <c r="I601" s="24" t="s">
         <v>847</v>
       </c>
-      <c r="J601" s="3" t="s">
+      <c r="J601" s="24" t="s">
         <v>32</v>
       </c>
       <c r="K601" s="24" t="s">
@@ -60937,7 +60940,7 @@
       </c>
       <c r="L601" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genreGEN600vnone</v>
+        <v>subject_genreGEN610vnone</v>
       </c>
       <c r="M601" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -60975,7 +60978,7 @@
         <v>856</v>
       </c>
       <c r="F602" s="13">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="G602" s="24" t="s">
         <v>961</v>
@@ -60994,7 +60997,7 @@
       </c>
       <c r="L602" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genreGEN610vnone</v>
+        <v>subject_genreGEN611vnone</v>
       </c>
       <c r="M602" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -61032,7 +61035,7 @@
         <v>856</v>
       </c>
       <c r="F603" s="13">
-        <v>611</v>
+        <v>630</v>
       </c>
       <c r="G603" s="24" t="s">
         <v>961</v>
@@ -61051,7 +61054,7 @@
       </c>
       <c r="L603" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genreGEN611vnone</v>
+        <v>subject_genreGEN630vnone</v>
       </c>
       <c r="M603" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -61083,13 +61086,13 @@
         <v>855</v>
       </c>
       <c r="D604" s="24" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="E604" s="24" t="s">
         <v>856</v>
       </c>
       <c r="F604" s="13">
-        <v>630</v>
+        <v>647</v>
       </c>
       <c r="G604" s="24" t="s">
         <v>961</v>
@@ -61104,11 +61107,11 @@
         <v>32</v>
       </c>
       <c r="K604" s="24" t="s">
-        <v>32</v>
+        <v>1181</v>
       </c>
       <c r="L604" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genreGEN630vnone</v>
+        <v>subject_genreGEN647vnone</v>
       </c>
       <c r="M604" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -61146,7 +61149,7 @@
         <v>856</v>
       </c>
       <c r="F605" s="13">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="G605" s="24" t="s">
         <v>961</v>
@@ -61157,15 +61160,15 @@
       <c r="I605" s="24" t="s">
         <v>847</v>
       </c>
-      <c r="J605" s="24" t="s">
+      <c r="J605" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K605" s="24" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="L605" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genreGEN647vnone</v>
+        <v>subject_genreGEN648vnone</v>
       </c>
       <c r="M605" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -61197,13 +61200,13 @@
         <v>855</v>
       </c>
       <c r="D606" s="24" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="E606" s="24" t="s">
         <v>856</v>
       </c>
       <c r="F606" s="13">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="G606" s="24" t="s">
         <v>961</v>
@@ -61214,15 +61217,15 @@
       <c r="I606" s="24" t="s">
         <v>847</v>
       </c>
-      <c r="J606" s="3" t="s">
+      <c r="J606" s="24" t="s">
         <v>32</v>
       </c>
       <c r="K606" s="24" t="s">
-        <v>1182</v>
+        <v>32</v>
       </c>
       <c r="L606" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genreGEN648vnone</v>
+        <v>subject_genreGEN650vnone</v>
       </c>
       <c r="M606" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -61260,7 +61263,7 @@
         <v>856</v>
       </c>
       <c r="F607" s="13">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="G607" s="24" t="s">
         <v>961</v>
@@ -61271,7 +61274,7 @@
       <c r="I607" s="24" t="s">
         <v>847</v>
       </c>
-      <c r="J607" s="24" t="s">
+      <c r="J607" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K607" s="24" t="s">
@@ -61279,7 +61282,7 @@
       </c>
       <c r="L607" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genreGEN650vnone</v>
+        <v>subject_genreGEN651vnone</v>
       </c>
       <c r="M607" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -61301,10 +61304,10 @@
       </c>
     </row>
     <row r="608" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A608" s="24" t="s">
+      <c r="A608" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="B608" s="24" t="s">
+      <c r="B608" s="3" t="s">
         <v>711</v>
       </c>
       <c r="C608" s="24" t="s">
@@ -61316,13 +61319,13 @@
       <c r="E608" s="24" t="s">
         <v>856</v>
       </c>
-      <c r="F608" s="13">
-        <v>651</v>
-      </c>
-      <c r="G608" s="24" t="s">
+      <c r="F608" s="11">
+        <v>655</v>
+      </c>
+      <c r="G608" s="3" t="s">
         <v>961</v>
       </c>
-      <c r="H608" s="3" t="s">
+      <c r="H608" s="24" t="s">
         <v>850</v>
       </c>
       <c r="I608" s="24" t="s">
@@ -61331,52 +61334,52 @@
       <c r="J608" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K608" s="24" t="s">
+      <c r="K608" s="3" t="s">
         <v>32</v>
       </c>
       <c r="L608" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genreGEN651vnone</v>
-      </c>
-      <c r="M608" s="24">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="N608" s="24">
+        <v>subject_genreGEN655vnone</v>
+      </c>
+      <c r="M608" s="3">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N608" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
         <v>2</v>
       </c>
-      <c r="O608" s="15" t="str">
-        <f>IF(ISNUMBER(MATCH(mappings[field],#REF!,0)),"y","n")</f>
-        <v>n</v>
-      </c>
-      <c r="P608" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q608" s="15" t="s">
+      <c r="O608" s="3" t="str">
+        <f>IF(ISNUMBER(MATCH(mappings[field],#REF!,0)),"y","n")</f>
+        <v>n</v>
+      </c>
+      <c r="P608" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q608" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="609" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A609" s="3" t="s">
+      <c r="A609" s="24" t="s">
         <v>711</v>
       </c>
-      <c r="B609" s="3" t="s">
+      <c r="B609" s="24" t="s">
         <v>711</v>
       </c>
       <c r="C609" s="24" t="s">
         <v>855</v>
       </c>
       <c r="D609" s="24" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="E609" s="24" t="s">
         <v>856</v>
       </c>
-      <c r="F609" s="11">
-        <v>655</v>
-      </c>
-      <c r="G609" s="3" t="s">
+      <c r="F609" s="13">
+        <v>657</v>
+      </c>
+      <c r="G609" s="24" t="s">
         <v>961</v>
       </c>
       <c r="H609" s="24" t="s">
@@ -61388,29 +61391,29 @@
       <c r="J609" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K609" s="3" t="s">
-        <v>32</v>
+      <c r="K609" s="24" t="s">
+        <v>1183</v>
       </c>
       <c r="L609" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genreGEN655vnone</v>
-      </c>
-      <c r="M609" s="3">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="N609" s="3">
+        <v>subject_genreGEN657vnone</v>
+      </c>
+      <c r="M609" s="24">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N609" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
         <v>2</v>
       </c>
-      <c r="O609" s="3" t="str">
-        <f>IF(ISNUMBER(MATCH(mappings[field],#REF!,0)),"y","n")</f>
-        <v>n</v>
-      </c>
-      <c r="P609" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q609" s="3" t="s">
+      <c r="O609" s="15" t="str">
+        <f>IF(ISNUMBER(MATCH(mappings[field],#REF!,0)),"y","n")</f>
+        <v>n</v>
+      </c>
+      <c r="P609" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q609" s="15" t="s">
         <v>32</v>
       </c>
     </row>
@@ -61425,32 +61428,32 @@
         <v>855</v>
       </c>
       <c r="D610" s="24" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="E610" s="24" t="s">
         <v>856</v>
       </c>
       <c r="F610" s="13">
-        <v>657</v>
-      </c>
-      <c r="G610" s="24" t="s">
-        <v>961</v>
+        <v>6</v>
+      </c>
+      <c r="G610" s="24">
+        <v>17</v>
       </c>
       <c r="H610" s="24" t="s">
-        <v>850</v>
+        <v>1175</v>
       </c>
       <c r="I610" s="24" t="s">
         <v>847</v>
       </c>
       <c r="J610" s="3" t="s">
-        <v>32</v>
+        <v>1177</v>
       </c>
       <c r="K610" s="24" t="s">
-        <v>1183</v>
+        <v>1178</v>
       </c>
       <c r="L610" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genreGEN657vnone</v>
+        <v>subject_genreGEN617006/00 =~ [at]</v>
       </c>
       <c r="M610" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -61468,7 +61471,7 @@
         <v>73</v>
       </c>
       <c r="Q610" s="15" t="s">
-        <v>32</v>
+        <v>927</v>
       </c>
     </row>
     <row r="611" spans="1:17" x14ac:dyDescent="0.25">
@@ -61488,18 +61491,18 @@
         <v>856</v>
       </c>
       <c r="F611" s="13">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G611" s="24">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="H611" s="24" t="s">
-        <v>1175</v>
+        <v>1179</v>
       </c>
       <c r="I611" s="24" t="s">
         <v>847</v>
       </c>
-      <c r="J611" s="3" t="s">
+      <c r="J611" s="24" t="s">
         <v>1177</v>
       </c>
       <c r="K611" s="24" t="s">
@@ -61507,7 +61510,7 @@
       </c>
       <c r="L611" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genreGEN617006/00 =~ [at]</v>
+        <v>subject_genreGEN834LDR/06 = a AND LDR/07 =~ [acdm]</v>
       </c>
       <c r="M611" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -61525,7 +61528,7 @@
         <v>73</v>
       </c>
       <c r="Q611" s="15" t="s">
-        <v>927</v>
+        <v>73</v>
       </c>
     </row>
     <row r="612" spans="1:17" x14ac:dyDescent="0.25">
@@ -61545,26 +61548,26 @@
         <v>856</v>
       </c>
       <c r="F612" s="13">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G612" s="24">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="H612" s="24" t="s">
-        <v>1179</v>
+        <v>1175</v>
       </c>
       <c r="I612" s="24" t="s">
         <v>847</v>
       </c>
       <c r="J612" s="24" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="K612" s="24" t="s">
-        <v>1178</v>
+        <v>32</v>
       </c>
       <c r="L612" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genreGEN834LDR/06 = a AND LDR/07 =~ [acdm]</v>
+        <v>subject_genreGEN616006/00 =~ [at]</v>
       </c>
       <c r="M612" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -61602,13 +61605,13 @@
         <v>856</v>
       </c>
       <c r="F613" s="13">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G613" s="24">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="H613" s="24" t="s">
-        <v>1175</v>
+        <v>1179</v>
       </c>
       <c r="I613" s="24" t="s">
         <v>847</v>
@@ -61621,7 +61624,7 @@
       </c>
       <c r="L613" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genreGEN616006/00 =~ [at]</v>
+        <v>subject_genreGEN833LDR/06 = a AND LDR/07 =~ [acdm]</v>
       </c>
       <c r="M613" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -61639,7 +61642,7 @@
         <v>73</v>
       </c>
       <c r="Q613" s="15" t="s">
-        <v>73</v>
+        <v>927</v>
       </c>
     </row>
     <row r="614" spans="1:17" x14ac:dyDescent="0.25">
@@ -61653,32 +61656,32 @@
         <v>855</v>
       </c>
       <c r="D614" s="24" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="E614" s="24" t="s">
         <v>856</v>
       </c>
       <c r="F614" s="13">
-        <v>8</v>
-      </c>
-      <c r="G614" s="24">
-        <v>33</v>
-      </c>
-      <c r="H614" s="24" t="s">
-        <v>1179</v>
+        <v>655</v>
+      </c>
+      <c r="G614" s="24" t="s">
+        <v>1184</v>
+      </c>
+      <c r="H614" s="3" t="s">
+        <v>850</v>
       </c>
       <c r="I614" s="24" t="s">
-        <v>847</v>
-      </c>
-      <c r="J614" s="24" t="s">
-        <v>1176</v>
+        <v>862</v>
+      </c>
+      <c r="J614" s="3" t="s">
+        <v>1185</v>
       </c>
       <c r="K614" s="24" t="s">
-        <v>32</v>
+        <v>1186</v>
       </c>
       <c r="L614" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genreGEN833LDR/06 = a AND LDR/07 =~ [acdm]</v>
+        <v>subject_genreGEN655axnone</v>
       </c>
       <c r="M614" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -61696,7 +61699,7 @@
         <v>73</v>
       </c>
       <c r="Q614" s="15" t="s">
-        <v>927</v>
+        <v>73</v>
       </c>
     </row>
     <row r="615" spans="1:17" x14ac:dyDescent="0.25">
@@ -61721,21 +61724,21 @@
       <c r="G615" s="24" t="s">
         <v>1184</v>
       </c>
-      <c r="H615" s="3" t="s">
-        <v>850</v>
+      <c r="H615" s="24" t="s">
+        <v>1187</v>
       </c>
       <c r="I615" s="24" t="s">
         <v>862</v>
       </c>
-      <c r="J615" t="s">
-        <v>1185</v>
+      <c r="J615" s="24" t="s">
+        <v>1188</v>
       </c>
       <c r="K615" s="24" t="s">
-        <v>1186</v>
+        <v>1189</v>
       </c>
       <c r="L615" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genreGEN655axnone</v>
+        <v>subject_genreGEN655axi2=7 AND $2 =~ /rbbin|rbgenr|rbmscv|rbpap|rbpri|rbprov|rbpub|rbtyp/</v>
       </c>
       <c r="M615" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -61773,43 +61776,39 @@
         <v>856</v>
       </c>
       <c r="F616" s="13">
-        <v>655</v>
+        <v>384</v>
       </c>
       <c r="G616" s="24" t="s">
-        <v>1184</v>
+        <v>849</v>
       </c>
       <c r="H616" s="24" t="s">
-        <v>1187</v>
+        <v>850</v>
       </c>
       <c r="I616" s="24" t="s">
-        <v>862</v>
+        <v>847</v>
       </c>
       <c r="J616" s="24" t="s">
-        <v>1188</v>
+        <v>29</v>
       </c>
       <c r="K616" s="24" t="s">
-        <v>1189</v>
-      </c>
-      <c r="L616" s="24" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genreGEN655axi2=7 AND $2 =~ /rbbin|rbgenr|rbmscv|rbpap|rbpri|rbprov|rbpub|rbtyp/</v>
-      </c>
-      <c r="M616" s="24">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="N616" s="24">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>2</v>
-      </c>
-      <c r="O616" s="15" t="str">
-        <f>IF(ISNUMBER(MATCH(mappings[field],#REF!,0)),"y","n")</f>
-        <v>n</v>
-      </c>
-      <c r="P616" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q616" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="L616" s="15" t="s">
+        <v>1180</v>
+      </c>
+      <c r="M616" s="15">
+        <v>0</v>
+      </c>
+      <c r="N616" s="15">
+        <v>3</v>
+      </c>
+      <c r="O616" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="P616" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q616" s="3" t="s">
         <v>73</v>
       </c>
     </row>
@@ -61830,10 +61829,10 @@
         <v>856</v>
       </c>
       <c r="F617" s="13">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="G617" s="24" t="s">
-        <v>849</v>
+        <v>868</v>
       </c>
       <c r="H617" s="24" t="s">
         <v>850</v>
@@ -61847,70 +61846,74 @@
       <c r="K617" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="L617" s="15" t="s">
-        <v>1180</v>
+      <c r="L617" s="15" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>subject_genreGEN382abdpnone</v>
       </c>
       <c r="M617" s="15">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
         <v>0</v>
       </c>
       <c r="N617" s="15">
-        <v>3</v>
-      </c>
-      <c r="O617" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="P617" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q617" s="3" t="s">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>2</v>
+      </c>
+      <c r="O617" s="15" t="str">
+        <f>IF(ISNUMBER(MATCH(mappings[field],#REF!,0)),"y","n")</f>
+        <v>n</v>
+      </c>
+      <c r="P617" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q617" s="15" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="618" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A618" s="24" t="s">
-        <v>711</v>
+        <v>718</v>
       </c>
       <c r="B618" s="24" t="s">
-        <v>711</v>
+        <v>718</v>
       </c>
       <c r="C618" s="24" t="s">
         <v>855</v>
       </c>
       <c r="D618" s="24" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="E618" s="24" t="s">
         <v>856</v>
       </c>
       <c r="F618" s="13">
-        <v>382</v>
+        <v>653</v>
       </c>
       <c r="G618" s="24" t="s">
-        <v>868</v>
+        <v>849</v>
       </c>
       <c r="H618" s="24" t="s">
-        <v>850</v>
+        <v>1193</v>
       </c>
       <c r="I618" s="24" t="s">
         <v>847</v>
       </c>
-      <c r="J618" s="24" t="s">
-        <v>29</v>
+      <c r="J618" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="K618" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="L618" s="15" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_genreGEN382abdpnone</v>
-      </c>
-      <c r="M618" s="15">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="N618" s="15">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>2</v>
+        <v>32</v>
+      </c>
+      <c r="L618" s="24" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>subject_geographicGEN653ai2 = 5</v>
+      </c>
+      <c r="M618" s="24">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N618" s="24">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>1</v>
       </c>
       <c r="O618" s="15" t="str">
         <f>IF(ISNUMBER(MATCH(mappings[field],#REF!,0)),"y","n")</f>
@@ -61920,7 +61923,7 @@
         <v>73</v>
       </c>
       <c r="Q618" s="15" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
     </row>
     <row r="619" spans="1:17" x14ac:dyDescent="0.25">
@@ -61940,13 +61943,13 @@
         <v>856</v>
       </c>
       <c r="F619" s="13">
-        <v>653</v>
+        <v>662</v>
       </c>
       <c r="G619" s="24" t="s">
-        <v>849</v>
+        <v>1194</v>
       </c>
       <c r="H619" s="24" t="s">
-        <v>1193</v>
+        <v>850</v>
       </c>
       <c r="I619" s="24" t="s">
         <v>847</v>
@@ -61957,15 +61960,15 @@
       <c r="K619" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="L619" s="24" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographicGEN653ai2 = 5</v>
-      </c>
-      <c r="M619" s="24">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="N619" s="24">
+      <c r="L619" s="15" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>subject_geographicGEN662abcdfghnone</v>
+      </c>
+      <c r="M619" s="15">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N619" s="15">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
         <v>1</v>
       </c>
@@ -61977,7 +61980,7 @@
         <v>73</v>
       </c>
       <c r="Q619" s="15" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
     </row>
     <row r="620" spans="1:17" x14ac:dyDescent="0.25">
@@ -61997,10 +62000,10 @@
         <v>856</v>
       </c>
       <c r="F620" s="13">
-        <v>662</v>
+        <v>600</v>
       </c>
       <c r="G620" s="24" t="s">
-        <v>1194</v>
+        <v>926</v>
       </c>
       <c r="H620" s="24" t="s">
         <v>850</v>
@@ -62008,21 +62011,21 @@
       <c r="I620" s="24" t="s">
         <v>847</v>
       </c>
-      <c r="J620" s="3" t="s">
+      <c r="J620" s="24" t="s">
         <v>32</v>
       </c>
       <c r="K620" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="L620" s="15" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographicGEN662abcdfghnone</v>
-      </c>
-      <c r="M620" s="15">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="N620" s="15">
+      <c r="L620" s="24" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>subject_geographicGEN600znone</v>
+      </c>
+      <c r="M620" s="24">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N620" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
         <v>1</v>
       </c>
@@ -62034,7 +62037,7 @@
         <v>73</v>
       </c>
       <c r="Q620" s="15" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
     </row>
     <row r="621" spans="1:17" x14ac:dyDescent="0.25">
@@ -62054,7 +62057,7 @@
         <v>856</v>
       </c>
       <c r="F621" s="13">
-        <v>600</v>
+        <v>610</v>
       </c>
       <c r="G621" s="24" t="s">
         <v>926</v>
@@ -62073,7 +62076,7 @@
       </c>
       <c r="L621" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographicGEN600znone</v>
+        <v>subject_geographicGEN610znone</v>
       </c>
       <c r="M621" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -62111,7 +62114,7 @@
         <v>856</v>
       </c>
       <c r="F622" s="13">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="G622" s="24" t="s">
         <v>926</v>
@@ -62119,10 +62122,10 @@
       <c r="H622" s="24" t="s">
         <v>850</v>
       </c>
-      <c r="I622" s="24" t="s">
+      <c r="I622" s="3" t="s">
         <v>847</v>
       </c>
-      <c r="J622" s="24" t="s">
+      <c r="J622" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K622" s="24" t="s">
@@ -62130,7 +62133,7 @@
       </c>
       <c r="L622" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographicGEN610znone</v>
+        <v>subject_geographicGEN611znone</v>
       </c>
       <c r="M622" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -62168,7 +62171,7 @@
         <v>856</v>
       </c>
       <c r="F623" s="13">
-        <v>611</v>
+        <v>630</v>
       </c>
       <c r="G623" s="24" t="s">
         <v>926</v>
@@ -62176,10 +62179,10 @@
       <c r="H623" s="24" t="s">
         <v>850</v>
       </c>
-      <c r="I623" s="3" t="s">
+      <c r="I623" s="24" t="s">
         <v>847</v>
       </c>
-      <c r="J623" s="3" t="s">
+      <c r="J623" s="24" t="s">
         <v>32</v>
       </c>
       <c r="K623" s="24" t="s">
@@ -62187,7 +62190,7 @@
       </c>
       <c r="L623" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographicGEN611znone</v>
+        <v>subject_geographicGEN630znone</v>
       </c>
       <c r="M623" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -62219,13 +62222,13 @@
         <v>855</v>
       </c>
       <c r="D624" s="24" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="E624" s="24" t="s">
         <v>856</v>
       </c>
       <c r="F624" s="13">
-        <v>630</v>
+        <v>648</v>
       </c>
       <c r="G624" s="24" t="s">
         <v>926</v>
@@ -62240,11 +62243,11 @@
         <v>32</v>
       </c>
       <c r="K624" s="24" t="s">
-        <v>32</v>
+        <v>1182</v>
       </c>
       <c r="L624" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographicGEN630znone</v>
+        <v>subject_geographicGEN648znone</v>
       </c>
       <c r="M624" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -62276,13 +62279,13 @@
         <v>855</v>
       </c>
       <c r="D625" s="24" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="E625" s="24" t="s">
         <v>856</v>
       </c>
       <c r="F625" s="13">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="G625" s="24" t="s">
         <v>926</v>
@@ -62297,11 +62300,11 @@
         <v>32</v>
       </c>
       <c r="K625" s="24" t="s">
-        <v>1182</v>
+        <v>32</v>
       </c>
       <c r="L625" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographicGEN648znone</v>
+        <v>subject_geographicGEN650znone</v>
       </c>
       <c r="M625" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -62339,7 +62342,7 @@
         <v>856</v>
       </c>
       <c r="F626" s="13">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="G626" s="24" t="s">
         <v>926</v>
@@ -62350,7 +62353,7 @@
       <c r="I626" s="24" t="s">
         <v>847</v>
       </c>
-      <c r="J626" s="24" t="s">
+      <c r="J626" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K626" s="24" t="s">
@@ -62358,7 +62361,7 @@
       </c>
       <c r="L626" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographicGEN650znone</v>
+        <v>subject_geographicGEN651znone</v>
       </c>
       <c r="M626" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -62396,7 +62399,7 @@
         <v>856</v>
       </c>
       <c r="F627" s="13">
-        <v>651</v>
+        <v>655</v>
       </c>
       <c r="G627" s="24" t="s">
         <v>926</v>
@@ -62415,7 +62418,7 @@
       </c>
       <c r="L627" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographicGEN651znone</v>
+        <v>subject_geographicGEN655znone</v>
       </c>
       <c r="M627" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -62453,7 +62456,7 @@
         <v>856</v>
       </c>
       <c r="F628" s="13">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="G628" s="24" t="s">
         <v>926</v>
@@ -62472,7 +62475,7 @@
       </c>
       <c r="L628" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographicGEN655znone</v>
+        <v>subject_geographicGEN656znone</v>
       </c>
       <c r="M628" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -62510,7 +62513,7 @@
         <v>856</v>
       </c>
       <c r="F629" s="13">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="G629" s="24" t="s">
         <v>926</v>
@@ -62529,7 +62532,7 @@
       </c>
       <c r="L629" s="24" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographicGEN656znone</v>
+        <v>subject_geographicGEN657znone</v>
       </c>
       <c r="M629" s="24">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -62567,32 +62570,32 @@
         <v>856</v>
       </c>
       <c r="F630" s="13">
-        <v>657</v>
+        <v>651</v>
       </c>
       <c r="G630" s="24" t="s">
-        <v>926</v>
+        <v>1191</v>
       </c>
       <c r="H630" s="24" t="s">
         <v>850</v>
       </c>
       <c r="I630" s="24" t="s">
-        <v>847</v>
+        <v>862</v>
       </c>
       <c r="J630" t="s">
-        <v>32</v>
+        <v>1192</v>
       </c>
       <c r="K630" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="L630" s="24" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographicGEN657znone</v>
-      </c>
-      <c r="M630" s="24">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="N630" s="24">
+      <c r="L630" s="15" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>subject_geographicGEN651agnone</v>
+      </c>
+      <c r="M630" s="15">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N630" s="15">
         <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
         <v>1</v>
       </c>
@@ -62604,63 +62607,63 @@
         <v>73</v>
       </c>
       <c r="Q630" s="15" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
     </row>
     <row r="631" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A631" s="24" t="s">
-        <v>718</v>
-      </c>
-      <c r="B631" s="24" t="s">
-        <v>718</v>
+      <c r="A631" s="3" t="s">
+        <v>724</v>
+      </c>
+      <c r="B631" s="3" t="s">
+        <v>729</v>
       </c>
       <c r="C631" s="24" t="s">
         <v>855</v>
       </c>
       <c r="D631" s="24" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="E631" s="24" t="s">
         <v>856</v>
       </c>
-      <c r="F631" s="13">
-        <v>651</v>
-      </c>
-      <c r="G631" s="24" t="s">
-        <v>1191</v>
-      </c>
-      <c r="H631" s="24" t="s">
-        <v>850</v>
-      </c>
-      <c r="I631" s="24" t="s">
-        <v>862</v>
+      <c r="F631" s="11">
+        <v>653</v>
+      </c>
+      <c r="G631" s="3" t="s">
+        <v>849</v>
+      </c>
+      <c r="H631" s="3" t="s">
+        <v>1202</v>
+      </c>
+      <c r="I631" s="3" t="s">
+        <v>847</v>
       </c>
       <c r="J631" s="3" t="s">
-        <v>1192</v>
-      </c>
-      <c r="K631" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="L631" s="15" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_geographicGEN651agnone</v>
-      </c>
-      <c r="M631" s="15">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="N631" s="15">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>1</v>
-      </c>
-      <c r="O631" s="15" t="str">
-        <f>IF(ISNUMBER(MATCH(mappings[field],#REF!,0)),"y","n")</f>
-        <v>n</v>
-      </c>
-      <c r="P631" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q631" s="15" t="s">
+        <v>870</v>
+      </c>
+      <c r="K631" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L631" s="3" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>subject_headings[value]GEN653ai2 =~ /[ 012345]/</v>
+      </c>
+      <c r="M631" s="3">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N631" s="3">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O631" s="3" t="str">
+        <f>IF(ISNUMBER(MATCH(mappings[field],#REF!,0)),"y","n")</f>
+        <v>n</v>
+      </c>
+      <c r="P631" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q631" s="3" t="s">
         <v>73</v>
       </c>
     </row>
@@ -62681,16 +62684,16 @@
         <v>856</v>
       </c>
       <c r="F632" s="11">
-        <v>653</v>
+        <v>662</v>
       </c>
       <c r="G632" s="3" t="s">
-        <v>849</v>
+        <v>1194</v>
       </c>
       <c r="H632" t="s">
-        <v>1202</v>
+        <v>850</v>
       </c>
       <c r="I632" s="3" t="s">
-        <v>847</v>
+        <v>862</v>
       </c>
       <c r="J632" t="s">
         <v>870</v>
@@ -62700,7 +62703,7 @@
       </c>
       <c r="L632" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_headings[value]GEN653ai2 =~ /[ 012345]/</v>
+        <v>subject_headings[value]GEN662abcdfghnone</v>
       </c>
       <c r="M632" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -62738,10 +62741,10 @@
         <v>856</v>
       </c>
       <c r="F633" s="11">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="G633" s="3" t="s">
-        <v>1194</v>
+        <v>1203</v>
       </c>
       <c r="H633" t="s">
         <v>850</v>
@@ -62757,7 +62760,7 @@
       </c>
       <c r="L633" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_headings[value]GEN662abcdfghnone</v>
+        <v>subject_headings[value]GEN656akvxyznone</v>
       </c>
       <c r="M633" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -62795,10 +62798,10 @@
         <v>856</v>
       </c>
       <c r="F634" s="11">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="G634" s="3" t="s">
-        <v>1203</v>
+        <v>871</v>
       </c>
       <c r="H634" t="s">
         <v>850</v>
@@ -62814,7 +62817,7 @@
       </c>
       <c r="L634" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_headings[value]GEN656akvxyznone</v>
+        <v>subject_headings[value]GEN657avxyznone</v>
       </c>
       <c r="M634" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -62852,10 +62855,10 @@
         <v>856</v>
       </c>
       <c r="F635" s="11">
-        <v>657</v>
+        <v>600</v>
       </c>
       <c r="G635" s="3" t="s">
-        <v>871</v>
+        <v>1195</v>
       </c>
       <c r="H635" t="s">
         <v>850</v>
@@ -62864,14 +62867,14 @@
         <v>862</v>
       </c>
       <c r="J635" s="3" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
       <c r="K635" s="3" t="s">
         <v>32</v>
       </c>
       <c r="L635" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_headings[value]GEN657avxyznone</v>
+        <v>subject_headings[value]GEN600abcdfghjklmnopqrstuvxyznone</v>
       </c>
       <c r="M635" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -62909,10 +62912,10 @@
         <v>856</v>
       </c>
       <c r="F636" s="11">
-        <v>600</v>
+        <v>610</v>
       </c>
       <c r="G636" s="3" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="H636" t="s">
         <v>850</v>
@@ -62928,7 +62931,7 @@
       </c>
       <c r="L636" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_headings[value]GEN600abcdfghjklmnopqrstuvxyznone</v>
+        <v>subject_headings[value]GEN610abcdfghklmnoprstuvxyznone</v>
       </c>
       <c r="M636" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -62966,10 +62969,10 @@
         <v>856</v>
       </c>
       <c r="F637" s="11">
-        <v>610</v>
+        <v>650</v>
       </c>
       <c r="G637" s="3" t="s">
-        <v>1196</v>
+        <v>1200</v>
       </c>
       <c r="H637" t="s">
         <v>850</v>
@@ -62985,7 +62988,7 @@
       </c>
       <c r="L637" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_headings[value]GEN610abcdfghklmnoprstuvxyznone</v>
+        <v>subject_headings[value]GEN650abcdgvxyznone</v>
       </c>
       <c r="M637" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -63023,10 +63026,10 @@
         <v>856</v>
       </c>
       <c r="F638" s="11">
-        <v>650</v>
+        <v>611</v>
       </c>
       <c r="G638" s="3" t="s">
-        <v>1200</v>
+        <v>1197</v>
       </c>
       <c r="H638" t="s">
         <v>850</v>
@@ -63042,7 +63045,7 @@
       </c>
       <c r="L638" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_headings[value]GEN650abcdgvxyznone</v>
+        <v>subject_headings[value]GEN611acdefghklnpqstuvxyznone</v>
       </c>
       <c r="M638" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -63080,10 +63083,10 @@
         <v>856</v>
       </c>
       <c r="F639" s="11">
-        <v>611</v>
+        <v>647</v>
       </c>
       <c r="G639" s="3" t="s">
-        <v>1197</v>
+        <v>1199</v>
       </c>
       <c r="H639" t="s">
         <v>850</v>
@@ -63099,7 +63102,7 @@
       </c>
       <c r="L639" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_headings[value]GEN611acdefghklnpqstuvxyznone</v>
+        <v>subject_headings[value]GEN647acdgvxyznone</v>
       </c>
       <c r="M639" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -63137,10 +63140,10 @@
         <v>856</v>
       </c>
       <c r="F640" s="11">
-        <v>647</v>
+        <v>630</v>
       </c>
       <c r="G640" s="3" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="H640" s="3" t="s">
         <v>850</v>
@@ -63156,7 +63159,7 @@
       </c>
       <c r="L640" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_headings[value]GEN647acdgvxyznone</v>
+        <v>subject_headings[value]GEN630adfghklmnoprstvxyznone</v>
       </c>
       <c r="M640" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -63194,10 +63197,10 @@
         <v>856</v>
       </c>
       <c r="F641" s="11">
-        <v>630</v>
+        <v>651</v>
       </c>
       <c r="G641" s="3" t="s">
-        <v>1198</v>
+        <v>1201</v>
       </c>
       <c r="H641" s="3" t="s">
         <v>850</v>
@@ -63213,7 +63216,7 @@
       </c>
       <c r="L641" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_headings[value]GEN630adfghklmnoprstvxyznone</v>
+        <v>subject_headings[value]GEN651agvxyznone</v>
       </c>
       <c r="M641" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -63251,10 +63254,10 @@
         <v>856</v>
       </c>
       <c r="F642" s="11">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="G642" s="3" t="s">
-        <v>1201</v>
+        <v>871</v>
       </c>
       <c r="H642" s="3" t="s">
         <v>850</v>
@@ -63270,7 +63273,7 @@
       </c>
       <c r="L642" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_headings[value]GEN651agvxyznone</v>
+        <v>subject_headings[value]GEN648avxyznone</v>
       </c>
       <c r="M642" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -63292,60 +63295,60 @@
       </c>
     </row>
     <row r="643" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A643" s="3" t="s">
-        <v>724</v>
-      </c>
-      <c r="B643" s="3" t="s">
-        <v>729</v>
+      <c r="A643" s="24" t="s">
+        <v>732</v>
+      </c>
+      <c r="B643" s="24" t="s">
+        <v>732</v>
       </c>
       <c r="C643" s="24" t="s">
         <v>855</v>
       </c>
       <c r="D643" s="24" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="E643" s="24" t="s">
         <v>856</v>
       </c>
-      <c r="F643" s="11">
-        <v>648</v>
-      </c>
-      <c r="G643" t="s">
-        <v>871</v>
+      <c r="F643" s="13">
+        <v>653</v>
+      </c>
+      <c r="G643" s="24" t="s">
+        <v>849</v>
       </c>
       <c r="H643" s="3" t="s">
-        <v>850</v>
-      </c>
-      <c r="I643" s="3" t="s">
-        <v>862</v>
-      </c>
-      <c r="J643" t="s">
-        <v>872</v>
-      </c>
-      <c r="K643" t="s">
-        <v>32</v>
-      </c>
-      <c r="L643" t="str">
-        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>subject_headings[value]GEN648avxyznone</v>
-      </c>
-      <c r="M643">
-        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="N643">
-        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O643" s="3" t="str">
-        <f>IF(ISNUMBER(MATCH(mappings[field],#REF!,0)),"y","n")</f>
-        <v>n</v>
-      </c>
-      <c r="P643" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q643" s="3" t="s">
-        <v>73</v>
+        <v>1174</v>
+      </c>
+      <c r="I643" s="24" t="s">
+        <v>847</v>
+      </c>
+      <c r="J643" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="K643" s="24" t="s">
+        <v>1522</v>
+      </c>
+      <c r="L643" s="24" t="str">
+        <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
+        <v>subject_topicalGEN653ai2 = 4</v>
+      </c>
+      <c r="M643" s="24">
+        <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N643" s="24">
+        <f>IF(ISNUMBER(MATCH(mappings[field],issuesfield[field],0)),COUNTIF(issuesfield[field],mappings[field]),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O643" s="15" t="str">
+        <f>IF(ISNUMBER(MATCH(mappings[field],#REF!,0)),"y","n")</f>
+        <v>n</v>
+      </c>
+      <c r="P643" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q643" s="15" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="644" spans="1:17" x14ac:dyDescent="0.25">
@@ -67058,7 +67061,7 @@
         <v>804</v>
       </c>
       <c r="B709" s="3" t="s">
-        <v>1506</v>
+        <v>807</v>
       </c>
       <c r="C709" s="3" t="s">
         <v>855</v>
@@ -67073,23 +67076,23 @@
         <v>856</v>
       </c>
       <c r="G709" s="3" t="s">
-        <v>31</v>
+        <v>1252</v>
       </c>
       <c r="H709" s="3" t="s">
-        <v>1251</v>
-      </c>
-      <c r="I709" s="3" t="s">
-        <v>883</v>
+        <v>850</v>
+      </c>
+      <c r="I709" s="24" t="s">
+        <v>847</v>
       </c>
       <c r="J709" t="s">
-        <v>1407</v>
+        <v>1253</v>
       </c>
       <c r="K709" s="3" t="s">
         <v>29</v>
       </c>
       <c r="L709" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>url[restricted]UNC856{na}$u does not meet criteria to be coded as restricted (see other mappings)</v>
+        <v>url[href]UNC856unone</v>
       </c>
       <c r="M709" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -67129,20 +67132,20 @@
         <v>31</v>
       </c>
       <c r="H710" s="3" t="s">
-        <v>1249</v>
+        <v>1251</v>
       </c>
       <c r="I710" s="3" t="s">
-        <v>1042</v>
+        <v>883</v>
       </c>
       <c r="J710" s="3" t="s">
-        <v>29</v>
+        <v>1407</v>
       </c>
       <c r="K710" s="3" t="s">
-        <v>1509</v>
+        <v>29</v>
       </c>
       <c r="L710" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>url[restricted]UNC856{na}$u.include?('libproxy.lib.unc')</v>
+        <v>url[restricted]UNC856{na}$u does not meet criteria to be coded as restricted (see other mappings)</v>
       </c>
       <c r="M710" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -67182,7 +67185,7 @@
         <v>31</v>
       </c>
       <c r="H711" s="3" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="I711" s="3" t="s">
         <v>1042</v>
@@ -67195,7 +67198,7 @@
       </c>
       <c r="L711" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>url[restricted]UNC856{na}$u.include?('unc.kanopystreaming.com')</v>
+        <v>url[restricted]UNC856{na}$u.include?('libproxy.lib.unc')</v>
       </c>
       <c r="M711" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>
@@ -67217,7 +67220,7 @@
         <v>804</v>
       </c>
       <c r="B712" s="3" t="s">
-        <v>807</v>
+        <v>1506</v>
       </c>
       <c r="C712" s="3" t="s">
         <v>855</v>
@@ -67232,23 +67235,23 @@
         <v>856</v>
       </c>
       <c r="G712" s="3" t="s">
-        <v>1252</v>
+        <v>31</v>
       </c>
       <c r="H712" s="3" t="s">
-        <v>850</v>
-      </c>
-      <c r="I712" s="24" t="s">
-        <v>847</v>
+        <v>1250</v>
+      </c>
+      <c r="I712" s="3" t="s">
+        <v>1042</v>
       </c>
       <c r="J712" s="3" t="s">
-        <v>1253</v>
+        <v>29</v>
       </c>
       <c r="K712" s="3" t="s">
-        <v>29</v>
+        <v>1509</v>
       </c>
       <c r="L712" s="3" t="str">
         <f>mappings[field]&amp;mappings[institution]&amp;mappings[element/field]&amp;mappings[subelement/field(s)]&amp;mappings[constraints]</f>
-        <v>url[href]UNC856unone</v>
+        <v>url[restricted]UNC856{na}$u.include?('unc.kanopystreaming.com')</v>
       </c>
       <c r="M712" s="3">
         <f>IF(ISNUMBER(MATCH(mappings[mapping_id],issuesmap[mappingID],0)),COUNTIF(issuesmap[mappingID],mappings[mapping_id]),0)</f>

</xml_diff>

<commit_message>
add to schema: imprint_main, imprint_multiple
</commit_message>
<xml_diff>
--- a/argot/argot.xlsx
+++ b/argot/argot.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="5040" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="5040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="elements" sheetId="1" r:id="rId1"/>
@@ -5440,7 +5440,14 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="fields" displayName="fields" ref="A1:AE246" totalsRowShown="0">
-  <autoFilter ref="A1:AE246"/>
+  <autoFilter ref="A1:AE246">
+    <filterColumn colId="30">
+      <filters>
+        <filter val="."/>
+        <filter val="n"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="31">
     <tableColumn id="1" name="argot element"/>
     <tableColumn id="2" name="parent element"/>
@@ -5802,9 +5809,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM246"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AE37" sqref="AE37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5927,7 +5934,7 @@
       <c r="AF1"/>
       <c r="AM1"/>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -6028,7 +6035,7 @@
       <c r="AF2"/>
       <c r="AM2"/>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -6331,7 +6338,7 @@
       <c r="AF5"/>
       <c r="AM5"/>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>54</v>
       </c>
@@ -6836,7 +6843,7 @@
       <c r="AF10"/>
       <c r="AM10"/>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>89</v>
       </c>
@@ -6937,7 +6944,7 @@
       <c r="AF11"/>
       <c r="AM11"/>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>93</v>
       </c>
@@ -7038,7 +7045,7 @@
       <c r="AF12"/>
       <c r="AM12"/>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>102</v>
       </c>
@@ -7139,7 +7146,7 @@
       <c r="AF13"/>
       <c r="AM13"/>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>99</v>
       </c>
@@ -7240,7 +7247,7 @@
       <c r="AF14"/>
       <c r="AM14"/>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>105</v>
       </c>
@@ -7341,7 +7348,7 @@
       <c r="AF15"/>
       <c r="AM15"/>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>110</v>
       </c>
@@ -7442,7 +7449,7 @@
       <c r="AF16"/>
       <c r="AM16"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>111</v>
       </c>
@@ -7543,7 +7550,7 @@
       <c r="AF17"/>
       <c r="AM17"/>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>114</v>
       </c>
@@ -7644,7 +7651,7 @@
       <c r="AF18"/>
       <c r="AM18"/>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>121</v>
       </c>
@@ -7745,7 +7752,7 @@
       <c r="AF19"/>
       <c r="AM19"/>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>123</v>
       </c>
@@ -8752,7 +8759,7 @@
       <c r="AF29"/>
       <c r="AM29"/>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>166</v>
       </c>
@@ -8949,7 +8956,7 @@
         <v>28</v>
       </c>
       <c r="AE31" s="3" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="AF31"/>
       <c r="AM31"/>
@@ -9050,7 +9057,7 @@
         <v>28</v>
       </c>
       <c r="AE32" s="3" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="AF32"/>
       <c r="AM32"/>
@@ -9151,7 +9158,7 @@
         <v>28</v>
       </c>
       <c r="AE33" s="3" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="AF33"/>
       <c r="AM33"/>
@@ -9252,7 +9259,7 @@
         <v>28</v>
       </c>
       <c r="AE34" s="3" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="AF34"/>
       <c r="AM34"/>
@@ -9353,7 +9360,7 @@
         <v>28</v>
       </c>
       <c r="AE35" s="3" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="AF35"/>
       <c r="AM35"/>
@@ -9454,7 +9461,7 @@
         <v>28</v>
       </c>
       <c r="AE36" s="3" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="AF36"/>
       <c r="AM36"/>
@@ -9555,7 +9562,7 @@
         <v>28</v>
       </c>
       <c r="AE37" s="3" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="AF37"/>
       <c r="AM37"/>
@@ -9656,7 +9663,7 @@
         <v>28</v>
       </c>
       <c r="AE38" s="3" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="AF38"/>
       <c r="AM38"/>
@@ -10974,7 +10981,7 @@
       <c r="AF51"/>
       <c r="AM51"/>
     </row>
-    <row r="52" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="23" t="s">
         <v>246</v>
       </c>
@@ -21147,7 +21154,7 @@
       <c r="AF152"/>
       <c r="AM152"/>
     </row>
-    <row r="153" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>1315</v>
       </c>
@@ -21248,7 +21255,7 @@
       <c r="AF153"/>
       <c r="AM153"/>
     </row>
-    <row r="154" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
         <v>559</v>
       </c>
@@ -21349,7 +21356,7 @@
       <c r="AF154"/>
       <c r="AM154"/>
     </row>
-    <row r="155" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:39" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>567</v>
       </c>
@@ -21448,7 +21455,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="156" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
         <v>1498</v>
       </c>
@@ -21549,7 +21556,7 @@
       <c r="AF156"/>
       <c r="AM156"/>
     </row>
-    <row r="157" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>568</v>
       </c>
@@ -21650,7 +21657,7 @@
       <c r="AF157"/>
       <c r="AM157"/>
     </row>
-    <row r="158" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>570</v>
       </c>
@@ -21751,7 +21758,7 @@
       <c r="AF158"/>
       <c r="AM158"/>
     </row>
-    <row r="159" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>574</v>
       </c>
@@ -21852,7 +21859,7 @@
       <c r="AF159"/>
       <c r="AM159"/>
     </row>
-    <row r="160" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>575</v>
       </c>
@@ -26879,7 +26886,7 @@
       <c r="AF209"/>
       <c r="AM209"/>
     </row>
-    <row r="210" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="s">
         <v>710</v>
       </c>
@@ -26980,7 +26987,7 @@
       <c r="AF210"/>
       <c r="AM210"/>
     </row>
-    <row r="211" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:39" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
         <v>713</v>
       </c>
@@ -27079,7 +27086,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="212" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
         <v>715</v>
       </c>
@@ -28188,7 +28195,7 @@
       <c r="AF222"/>
       <c r="AM222"/>
     </row>
-    <row r="223" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="23" t="s">
         <v>737</v>
       </c>
@@ -28289,7 +28296,7 @@
       <c r="AF223"/>
       <c r="AM223"/>
     </row>
-    <row r="224" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
         <v>743</v>
       </c>
@@ -28390,7 +28397,7 @@
       <c r="AF224"/>
       <c r="AM224"/>
     </row>
-    <row r="225" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
         <v>745</v>
       </c>
@@ -28491,7 +28498,7 @@
       <c r="AF225"/>
       <c r="AM225"/>
     </row>
-    <row r="226" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:39" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="3" t="s">
         <v>749</v>
       </c>
@@ -30622,7 +30629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V749"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C660" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>